<commit_message>
added support for vpc domain configuration
</commit_message>
<xml_diff>
--- a/Terraform/aci/base-configs/aci-fabric-deploy-Input-Spreadsheet.xlsx
+++ b/Terraform/aci/base-configs/aci-fabric-deploy-Input-Spreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\tyscott\terraform-aci-fabric-deploy\Terraform\aci\base-configs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{720C99E4-7311-490F-B58F-984BB9309CE8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ADCB25F-03E5-4431-9FFA-05C59423E1C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="227">
   <si>
     <t>Type</t>
   </si>
@@ -862,6 +862,27 @@
   </si>
   <si>
     <t>is it needed, I don't know</t>
+  </si>
+  <si>
+    <t>VPC Pairs</t>
+  </si>
+  <si>
+    <t>vpc_pair</t>
+  </si>
+  <si>
+    <t>VPC ID</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>Node ID 1</t>
+  </si>
+  <si>
+    <t>Node ID 2</t>
+  </si>
+  <si>
+    <t>leaf201-202-vpc</t>
   </si>
 </sst>
 </file>
@@ -1681,7 +1702,25 @@
     <xf numFmtId="49" fontId="20" fillId="34" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="18" fillId="34" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="16" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="20" fillId="34" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="33" borderId="8" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="33" borderId="8" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="34" borderId="8" xfId="3" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="34" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="33" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="18" fillId="0" borderId="25" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1690,19 +1729,55 @@
     <xf numFmtId="49" fontId="18" fillId="0" borderId="26" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="20" fillId="34" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="20" fillId="34" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="20" fillId="34" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="20" fillId="34" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="34" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="34" borderId="8" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="34" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="18" fillId="0" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="16" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="20" fillId="34" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="20" fillId="34" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="36" borderId="8" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="18" fillId="0" borderId="11" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="16" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="20" fillId="34" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="20" fillId="34" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="20" fillId="34" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="20" fillId="34" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="20" fillId="34" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="20" fillId="34" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="20" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1714,64 +1789,10 @@
     <xf numFmtId="49" fontId="20" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="17" fillId="36" borderId="8" xfId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="34" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="20" fillId="34" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="20" fillId="34" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="20" fillId="34" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="20" fillId="34" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="34" borderId="8" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="33" borderId="8" xfId="2" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="34" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="33" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="20" fillId="34" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="20" fillId="34" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="20" fillId="34" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="33" borderId="8" xfId="2" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="34" borderId="8" xfId="3" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="16" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="20" fillId="34" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="1" fontId="20" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="20" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="20" fillId="34" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2130,10 +2151,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P121"/>
+  <dimension ref="A1:P131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C80" sqref="C80:E80"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2158,21 +2179,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="6" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="22" t="s">
         <v>99</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
-      <c r="J1" s="44"/>
-      <c r="K1" s="44"/>
-      <c r="L1" s="44"/>
-      <c r="M1" s="44"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
     </row>
     <row r="2" spans="1:13" s="3" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
@@ -2213,38 +2234,38 @@
       <c r="M3" s="13"/>
     </row>
     <row r="5" spans="1:13" s="6" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="44" t="s">
+      <c r="A5" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="B5" s="44"/>
-      <c r="C5" s="44"/>
-      <c r="D5" s="44"/>
-      <c r="E5" s="44"/>
-      <c r="F5" s="44"/>
-      <c r="G5" s="44"/>
-      <c r="H5" s="44"/>
-      <c r="I5" s="44"/>
-      <c r="J5" s="44"/>
-      <c r="K5" s="44"/>
-      <c r="L5" s="44"/>
-      <c r="M5" s="44"/>
+      <c r="B5" s="22"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="22"/>
+      <c r="J5" s="22"/>
+      <c r="K5" s="22"/>
+      <c r="L5" s="22"/>
+      <c r="M5" s="22"/>
     </row>
     <row r="6" spans="1:13" s="6" customFormat="1" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="45" t="s">
+      <c r="A6" s="24" t="s">
         <v>149</v>
       </c>
-      <c r="B6" s="45"/>
-      <c r="C6" s="45"/>
-      <c r="D6" s="45"/>
-      <c r="E6" s="45"/>
-      <c r="F6" s="45"/>
-      <c r="G6" s="45"/>
-      <c r="H6" s="45"/>
-      <c r="I6" s="45"/>
-      <c r="J6" s="45"/>
-      <c r="K6" s="45"/>
-      <c r="L6" s="45"/>
-      <c r="M6" s="45"/>
+      <c r="B6" s="24"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="24"/>
+      <c r="J6" s="24"/>
+      <c r="K6" s="24"/>
+      <c r="L6" s="24"/>
+      <c r="M6" s="24"/>
     </row>
     <row r="7" spans="1:13" s="3" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
@@ -2567,642 +2588,588 @@
       <c r="L21" s="11"/>
       <c r="M21" s="11"/>
     </row>
-    <row r="23" spans="1:13" s="6" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="44" t="s">
+    <row r="23" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="22" t="s">
+        <v>220</v>
+      </c>
+      <c r="B23" s="22"/>
+      <c r="C23" s="22"/>
+      <c r="D23" s="22"/>
+      <c r="E23" s="22"/>
+      <c r="F23" s="22"/>
+      <c r="G23" s="22"/>
+      <c r="H23" s="22"/>
+      <c r="I23" s="22"/>
+      <c r="J23" s="22"/>
+      <c r="K23" s="22"/>
+      <c r="L23" s="22"/>
+      <c r="M23" s="22"/>
+    </row>
+    <row r="24" spans="1:13" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>222</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>224</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="F24" s="8"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="8"/>
+      <c r="I24" s="8"/>
+      <c r="J24" s="8"/>
+      <c r="K24" s="8"/>
+      <c r="L24" s="8"/>
+      <c r="M24" s="8"/>
+    </row>
+    <row r="25" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="13" t="s">
+        <v>221</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>223</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>226</v>
+      </c>
+      <c r="D25" s="14">
+        <v>201</v>
+      </c>
+      <c r="E25" s="14">
+        <v>202</v>
+      </c>
+      <c r="F25" s="13"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="14"/>
+      <c r="I25" s="13"/>
+      <c r="J25" s="13"/>
+      <c r="K25" s="13"/>
+      <c r="L25" s="13"/>
+      <c r="M25" s="13"/>
+    </row>
+    <row r="26" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="11"/>
+      <c r="B26" s="11"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="11"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="12"/>
+      <c r="I26" s="11"/>
+      <c r="J26" s="11"/>
+      <c r="K26" s="11"/>
+      <c r="L26" s="11"/>
+      <c r="M26" s="11"/>
+    </row>
+    <row r="27" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="13"/>
+      <c r="B27" s="13"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="14"/>
+      <c r="H27" s="14"/>
+      <c r="I27" s="13"/>
+      <c r="J27" s="13"/>
+      <c r="K27" s="13"/>
+      <c r="L27" s="13"/>
+      <c r="M27" s="13"/>
+    </row>
+    <row r="28" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="11"/>
+      <c r="B28" s="11"/>
+      <c r="C28" s="11"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="12"/>
+      <c r="I28" s="11"/>
+      <c r="J28" s="11"/>
+      <c r="K28" s="11"/>
+      <c r="L28" s="11"/>
+      <c r="M28" s="11"/>
+    </row>
+    <row r="29" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="13"/>
+      <c r="B29" s="13"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="14"/>
+      <c r="H29" s="14"/>
+      <c r="I29" s="13"/>
+      <c r="J29" s="13"/>
+      <c r="K29" s="13"/>
+      <c r="L29" s="13"/>
+      <c r="M29" s="13"/>
+    </row>
+    <row r="30" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="11"/>
+      <c r="B30" s="11"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="12"/>
+      <c r="E30" s="12"/>
+      <c r="F30" s="11"/>
+      <c r="G30" s="12"/>
+      <c r="H30" s="12"/>
+      <c r="I30" s="11"/>
+      <c r="J30" s="11"/>
+      <c r="K30" s="11"/>
+      <c r="L30" s="11"/>
+      <c r="M30" s="11"/>
+    </row>
+    <row r="31" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="13"/>
+      <c r="B31" s="13"/>
+      <c r="C31" s="13"/>
+      <c r="D31" s="14"/>
+      <c r="E31" s="14"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="14"/>
+      <c r="H31" s="14"/>
+      <c r="I31" s="13"/>
+      <c r="J31" s="13"/>
+      <c r="K31" s="13"/>
+      <c r="L31" s="13"/>
+      <c r="M31" s="13"/>
+    </row>
+    <row r="33" spans="1:13" s="6" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="22" t="s">
         <v>141</v>
       </c>
-      <c r="B23" s="44"/>
-      <c r="C23" s="44"/>
-      <c r="D23" s="44"/>
-      <c r="E23" s="44"/>
-      <c r="F23" s="44"/>
-      <c r="G23" s="44"/>
-      <c r="H23" s="44"/>
-      <c r="I23" s="44"/>
-      <c r="J23" s="44"/>
-      <c r="K23" s="44"/>
-      <c r="L23" s="44"/>
-      <c r="M23" s="44"/>
-    </row>
-    <row r="24" spans="1:13" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="39" t="s">
+      <c r="B33" s="22"/>
+      <c r="C33" s="22"/>
+      <c r="D33" s="22"/>
+      <c r="E33" s="22"/>
+      <c r="F33" s="22"/>
+      <c r="G33" s="22"/>
+      <c r="H33" s="22"/>
+      <c r="I33" s="22"/>
+      <c r="J33" s="22"/>
+      <c r="K33" s="22"/>
+      <c r="L33" s="22"/>
+      <c r="M33" s="22"/>
+    </row>
+    <row r="34" spans="1:13" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="25" t="s">
         <v>143</v>
       </c>
-      <c r="B24" s="39"/>
-      <c r="C24" s="39"/>
-      <c r="D24" s="39"/>
-      <c r="E24" s="39"/>
-      <c r="F24" s="39"/>
-      <c r="G24" s="39"/>
-      <c r="H24" s="39"/>
-      <c r="I24" s="39"/>
-      <c r="J24" s="39"/>
-      <c r="K24" s="39"/>
-      <c r="L24" s="39"/>
-      <c r="M24" s="39"/>
-    </row>
-    <row r="25" spans="1:13" s="3" customFormat="1" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B25" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="C25" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="D25" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="E25" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="F25" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="G25" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="H25" s="8" t="s">
-        <v>212</v>
-      </c>
-      <c r="I25" s="8" t="s">
-        <v>214</v>
-      </c>
-      <c r="J25" s="8" t="s">
-        <v>213</v>
-      </c>
-      <c r="K25" s="8"/>
-      <c r="L25" s="8"/>
-      <c r="M25" s="8"/>
-    </row>
-    <row r="26" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="B26" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="C26" s="13">
-        <v>1</v>
-      </c>
-      <c r="D26" s="14">
-        <v>1</v>
-      </c>
-      <c r="E26" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="F26" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="G26" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="H26" s="14" t="s">
-        <v>107</v>
-      </c>
-      <c r="I26" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="J26" s="13" t="s">
-        <v>107</v>
-      </c>
-      <c r="K26" s="13"/>
-      <c r="L26" s="13"/>
-      <c r="M26" s="13"/>
-    </row>
-    <row r="27" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="11"/>
-      <c r="B27" s="11"/>
-      <c r="C27" s="11"/>
-      <c r="D27" s="12"/>
-      <c r="E27" s="11"/>
-      <c r="F27" s="11"/>
-      <c r="G27" s="12"/>
-      <c r="H27" s="12"/>
-      <c r="I27" s="11"/>
-      <c r="J27" s="11"/>
-      <c r="K27" s="11"/>
-      <c r="L27" s="11"/>
-      <c r="M27" s="11"/>
-    </row>
-    <row r="28" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="13"/>
-      <c r="B28" s="13"/>
-      <c r="C28" s="13"/>
-      <c r="D28" s="14"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="14"/>
-      <c r="H28" s="14"/>
-      <c r="I28" s="13"/>
-      <c r="J28" s="13"/>
-      <c r="K28" s="13"/>
-      <c r="L28" s="13"/>
-      <c r="M28" s="13"/>
-    </row>
-    <row r="29" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="11"/>
-      <c r="B29" s="11"/>
-      <c r="C29" s="11"/>
-      <c r="D29" s="12"/>
-      <c r="E29" s="11"/>
-      <c r="F29" s="11"/>
-      <c r="G29" s="12"/>
-      <c r="H29" s="12"/>
-      <c r="I29" s="11"/>
-      <c r="J29" s="11"/>
-      <c r="K29" s="11"/>
-      <c r="L29" s="11"/>
-      <c r="M29" s="11"/>
-    </row>
-    <row r="30" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="13"/>
-      <c r="B30" s="13"/>
-      <c r="C30" s="13"/>
-      <c r="D30" s="14"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="14"/>
-      <c r="H30" s="14"/>
-      <c r="I30" s="13"/>
-      <c r="J30" s="13"/>
-      <c r="K30" s="13"/>
-      <c r="L30" s="13"/>
-      <c r="M30" s="13"/>
-    </row>
-    <row r="31" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="11"/>
-      <c r="B31" s="11"/>
-      <c r="C31" s="11"/>
-      <c r="D31" s="12"/>
-      <c r="E31" s="11"/>
-      <c r="F31" s="11"/>
-      <c r="G31" s="12"/>
-      <c r="H31" s="12"/>
-      <c r="I31" s="11"/>
-      <c r="J31" s="11"/>
-      <c r="K31" s="11"/>
-      <c r="L31" s="11"/>
-      <c r="M31" s="11"/>
-    </row>
-    <row r="32" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="13"/>
-      <c r="B32" s="13"/>
-      <c r="C32" s="13"/>
-      <c r="D32" s="14"/>
-      <c r="E32" s="13"/>
-      <c r="F32" s="13"/>
-      <c r="G32" s="14"/>
-      <c r="H32" s="14"/>
-      <c r="I32" s="13"/>
-      <c r="J32" s="13"/>
-      <c r="K32" s="13"/>
-      <c r="L32" s="13"/>
-      <c r="M32" s="13"/>
-    </row>
-    <row r="34" spans="1:13" s="6" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="44" t="s">
-        <v>140</v>
-      </c>
-      <c r="B34" s="44"/>
-      <c r="C34" s="44"/>
-      <c r="D34" s="44"/>
-      <c r="E34" s="44"/>
-      <c r="F34" s="44"/>
-      <c r="G34" s="44"/>
-      <c r="H34" s="44"/>
-      <c r="I34" s="44"/>
-      <c r="J34" s="44"/>
-      <c r="K34" s="44"/>
-      <c r="L34" s="44"/>
-      <c r="M34" s="44"/>
-    </row>
-    <row r="35" spans="1:13" s="3" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="25"/>
+      <c r="C34" s="25"/>
+      <c r="D34" s="25"/>
+      <c r="E34" s="25"/>
+      <c r="F34" s="25"/>
+      <c r="G34" s="25"/>
+      <c r="H34" s="25"/>
+      <c r="I34" s="25"/>
+      <c r="J34" s="25"/>
+      <c r="K34" s="25"/>
+      <c r="L34" s="25"/>
+      <c r="M34" s="25"/>
+    </row>
+    <row r="35" spans="1:13" s="3" customFormat="1" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C35" s="8"/>
-      <c r="D35" s="8"/>
-      <c r="E35" s="8"/>
-      <c r="F35" s="8"/>
-      <c r="G35" s="8"/>
-      <c r="H35" s="8"/>
-      <c r="I35" s="8"/>
-      <c r="J35" s="8"/>
+        <v>139</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="E35" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="F35" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="G35" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="H35" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="I35" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="J35" s="8" t="s">
+        <v>213</v>
+      </c>
       <c r="K35" s="8"/>
       <c r="L35" s="8"/>
       <c r="M35" s="8"/>
     </row>
     <row r="36" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="B36" s="13">
-        <v>65513</v>
-      </c>
-      <c r="C36" s="13"/>
-      <c r="D36" s="14"/>
-      <c r="E36" s="13"/>
-      <c r="F36" s="13"/>
-      <c r="G36" s="14"/>
-      <c r="H36" s="14"/>
-      <c r="I36" s="13"/>
-      <c r="J36" s="13"/>
+        <v>23</v>
+      </c>
+      <c r="B36" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C36" s="13">
+        <v>1</v>
+      </c>
+      <c r="D36" s="14">
+        <v>1</v>
+      </c>
+      <c r="E36" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="F36" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="G36" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="H36" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="I36" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="J36" s="13" t="s">
+        <v>107</v>
+      </c>
       <c r="K36" s="13"/>
       <c r="L36" s="13"/>
       <c r="M36" s="13"/>
     </row>
-    <row r="38" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="38" t="s">
+    <row r="37" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="11"/>
+      <c r="B37" s="11"/>
+      <c r="C37" s="11"/>
+      <c r="D37" s="12"/>
+      <c r="E37" s="11"/>
+      <c r="F37" s="11"/>
+      <c r="G37" s="12"/>
+      <c r="H37" s="12"/>
+      <c r="I37" s="11"/>
+      <c r="J37" s="11"/>
+      <c r="K37" s="11"/>
+      <c r="L37" s="11"/>
+      <c r="M37" s="11"/>
+    </row>
+    <row r="38" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="13"/>
+      <c r="B38" s="13"/>
+      <c r="C38" s="13"/>
+      <c r="D38" s="14"/>
+      <c r="E38" s="13"/>
+      <c r="F38" s="13"/>
+      <c r="G38" s="14"/>
+      <c r="H38" s="14"/>
+      <c r="I38" s="13"/>
+      <c r="J38" s="13"/>
+      <c r="K38" s="13"/>
+      <c r="L38" s="13"/>
+      <c r="M38" s="13"/>
+    </row>
+    <row r="39" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="11"/>
+      <c r="B39" s="11"/>
+      <c r="C39" s="11"/>
+      <c r="D39" s="12"/>
+      <c r="E39" s="11"/>
+      <c r="F39" s="11"/>
+      <c r="G39" s="12"/>
+      <c r="H39" s="12"/>
+      <c r="I39" s="11"/>
+      <c r="J39" s="11"/>
+      <c r="K39" s="11"/>
+      <c r="L39" s="11"/>
+      <c r="M39" s="11"/>
+    </row>
+    <row r="40" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="13"/>
+      <c r="B40" s="13"/>
+      <c r="C40" s="13"/>
+      <c r="D40" s="14"/>
+      <c r="E40" s="13"/>
+      <c r="F40" s="13"/>
+      <c r="G40" s="14"/>
+      <c r="H40" s="14"/>
+      <c r="I40" s="13"/>
+      <c r="J40" s="13"/>
+      <c r="K40" s="13"/>
+      <c r="L40" s="13"/>
+      <c r="M40" s="13"/>
+    </row>
+    <row r="41" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="11"/>
+      <c r="B41" s="11"/>
+      <c r="C41" s="11"/>
+      <c r="D41" s="12"/>
+      <c r="E41" s="11"/>
+      <c r="F41" s="11"/>
+      <c r="G41" s="12"/>
+      <c r="H41" s="12"/>
+      <c r="I41" s="11"/>
+      <c r="J41" s="11"/>
+      <c r="K41" s="11"/>
+      <c r="L41" s="11"/>
+      <c r="M41" s="11"/>
+    </row>
+    <row r="42" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="13"/>
+      <c r="B42" s="13"/>
+      <c r="C42" s="13"/>
+      <c r="D42" s="14"/>
+      <c r="E42" s="13"/>
+      <c r="F42" s="13"/>
+      <c r="G42" s="14"/>
+      <c r="H42" s="14"/>
+      <c r="I42" s="13"/>
+      <c r="J42" s="13"/>
+      <c r="K42" s="13"/>
+      <c r="L42" s="13"/>
+      <c r="M42" s="13"/>
+    </row>
+    <row r="44" spans="1:13" s="6" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="22" t="s">
+        <v>140</v>
+      </c>
+      <c r="B44" s="22"/>
+      <c r="C44" s="22"/>
+      <c r="D44" s="22"/>
+      <c r="E44" s="22"/>
+      <c r="F44" s="22"/>
+      <c r="G44" s="22"/>
+      <c r="H44" s="22"/>
+      <c r="I44" s="22"/>
+      <c r="J44" s="22"/>
+      <c r="K44" s="22"/>
+      <c r="L44" s="22"/>
+      <c r="M44" s="22"/>
+    </row>
+    <row r="45" spans="1:13" s="3" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B45" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C45" s="8"/>
+      <c r="D45" s="8"/>
+      <c r="E45" s="8"/>
+      <c r="F45" s="8"/>
+      <c r="G45" s="8"/>
+      <c r="H45" s="8"/>
+      <c r="I45" s="8"/>
+      <c r="J45" s="8"/>
+      <c r="K45" s="8"/>
+      <c r="L45" s="8"/>
+      <c r="M45" s="8"/>
+    </row>
+    <row r="46" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B46" s="13">
+        <v>65513</v>
+      </c>
+      <c r="C46" s="13"/>
+      <c r="D46" s="14"/>
+      <c r="E46" s="13"/>
+      <c r="F46" s="13"/>
+      <c r="G46" s="14"/>
+      <c r="H46" s="14"/>
+      <c r="I46" s="13"/>
+      <c r="J46" s="13"/>
+      <c r="K46" s="13"/>
+      <c r="L46" s="13"/>
+      <c r="M46" s="13"/>
+    </row>
+    <row r="48" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="23" t="s">
         <v>142</v>
       </c>
-      <c r="B38" s="38"/>
-      <c r="C38" s="38"/>
-      <c r="D38" s="38"/>
-      <c r="E38" s="38"/>
-      <c r="F38" s="38"/>
-      <c r="G38" s="38"/>
-      <c r="H38" s="38"/>
-      <c r="I38" s="38"/>
-      <c r="J38" s="38"/>
-      <c r="K38" s="38"/>
-      <c r="L38" s="38"/>
-      <c r="M38" s="38"/>
-    </row>
-    <row r="39" spans="1:13" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="39" t="s">
+      <c r="B48" s="23"/>
+      <c r="C48" s="23"/>
+      <c r="D48" s="23"/>
+      <c r="E48" s="23"/>
+      <c r="F48" s="23"/>
+      <c r="G48" s="23"/>
+      <c r="H48" s="23"/>
+      <c r="I48" s="23"/>
+      <c r="J48" s="23"/>
+      <c r="K48" s="23"/>
+      <c r="L48" s="23"/>
+      <c r="M48" s="23"/>
+    </row>
+    <row r="49" spans="1:16" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="25" t="s">
         <v>144</v>
       </c>
-      <c r="B39" s="39"/>
-      <c r="C39" s="39"/>
-      <c r="D39" s="39"/>
-      <c r="E39" s="39"/>
-      <c r="F39" s="39"/>
-      <c r="G39" s="39"/>
-      <c r="H39" s="39"/>
-      <c r="I39" s="39"/>
-      <c r="J39" s="39"/>
-      <c r="K39" s="39"/>
-      <c r="L39" s="39"/>
-      <c r="M39" s="39"/>
-    </row>
-    <row r="40" spans="1:13" s="3" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="8" t="s">
+      <c r="B49" s="25"/>
+      <c r="C49" s="25"/>
+      <c r="D49" s="25"/>
+      <c r="E49" s="25"/>
+      <c r="F49" s="25"/>
+      <c r="G49" s="25"/>
+      <c r="H49" s="25"/>
+      <c r="I49" s="25"/>
+      <c r="J49" s="25"/>
+      <c r="K49" s="25"/>
+      <c r="L49" s="25"/>
+      <c r="M49" s="25"/>
+    </row>
+    <row r="50" spans="1:16" s="3" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B40" s="8" t="s">
+      <c r="B50" s="8" t="s">
         <v>132</v>
       </c>
-      <c r="C40" s="8" t="s">
+      <c r="C50" s="8" t="s">
         <v>133</v>
       </c>
-      <c r="D40" s="8"/>
-      <c r="E40" s="8"/>
-      <c r="F40" s="8"/>
-      <c r="G40" s="8"/>
-      <c r="H40" s="8"/>
-      <c r="I40" s="8"/>
-      <c r="J40" s="8"/>
-      <c r="K40" s="8"/>
-      <c r="L40" s="8"/>
-      <c r="M40" s="8"/>
-    </row>
-    <row r="41" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="13" t="s">
+      <c r="D50" s="8"/>
+      <c r="E50" s="8"/>
+      <c r="F50" s="8"/>
+      <c r="G50" s="8"/>
+      <c r="H50" s="8"/>
+      <c r="I50" s="8"/>
+      <c r="J50" s="8"/>
+      <c r="K50" s="8"/>
+      <c r="L50" s="8"/>
+      <c r="M50" s="8"/>
+    </row>
+    <row r="51" spans="1:16" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B41" s="13" t="s">
+      <c r="B51" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="C41" s="13">
+      <c r="C51" s="13">
         <v>101</v>
       </c>
-      <c r="D41" s="14"/>
-      <c r="E41" s="13"/>
-      <c r="F41" s="13"/>
-      <c r="G41" s="14"/>
-      <c r="H41" s="14"/>
-      <c r="I41" s="13"/>
-      <c r="J41" s="13"/>
-      <c r="K41" s="13"/>
-      <c r="L41" s="13"/>
-      <c r="M41" s="13"/>
-    </row>
-    <row r="43" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="38" t="s">
+      <c r="D51" s="14"/>
+      <c r="E51" s="13"/>
+      <c r="F51" s="13"/>
+      <c r="G51" s="14"/>
+      <c r="H51" s="14"/>
+      <c r="I51" s="13"/>
+      <c r="J51" s="13"/>
+      <c r="K51" s="13"/>
+      <c r="L51" s="13"/>
+      <c r="M51" s="13"/>
+    </row>
+    <row r="53" spans="1:16" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="23" t="s">
         <v>145</v>
       </c>
-      <c r="B43" s="38"/>
-      <c r="C43" s="38"/>
-      <c r="D43" s="38"/>
-      <c r="E43" s="38"/>
-      <c r="F43" s="38"/>
-      <c r="G43" s="38"/>
-      <c r="H43" s="38"/>
-      <c r="I43" s="38"/>
-      <c r="J43" s="38"/>
-      <c r="K43" s="38"/>
-      <c r="L43" s="38"/>
-      <c r="M43" s="38"/>
-    </row>
-    <row r="44" spans="1:13" s="3" customFormat="1" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="8" t="s">
+      <c r="B53" s="23"/>
+      <c r="C53" s="23"/>
+      <c r="D53" s="23"/>
+      <c r="E53" s="23"/>
+      <c r="F53" s="23"/>
+      <c r="G53" s="23"/>
+      <c r="H53" s="23"/>
+      <c r="I53" s="23"/>
+      <c r="J53" s="23"/>
+      <c r="K53" s="23"/>
+      <c r="L53" s="23"/>
+      <c r="M53" s="23"/>
+    </row>
+    <row r="54" spans="1:16" s="3" customFormat="1" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B44" s="9" t="s">
+      <c r="B54" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="C44" s="46"/>
-      <c r="D44" s="8"/>
-      <c r="E44" s="8"/>
-      <c r="F44" s="8"/>
-      <c r="G44" s="8"/>
-      <c r="H44" s="8"/>
-      <c r="I44" s="8"/>
-      <c r="J44" s="8"/>
-      <c r="K44" s="8"/>
-      <c r="L44" s="8"/>
-      <c r="M44" s="8"/>
-    </row>
-    <row r="45" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="13" t="s">
+      <c r="C54" s="20"/>
+      <c r="D54" s="8"/>
+      <c r="E54" s="8"/>
+      <c r="F54" s="8"/>
+      <c r="G54" s="8"/>
+      <c r="H54" s="8"/>
+      <c r="I54" s="8"/>
+      <c r="J54" s="8"/>
+      <c r="K54" s="8"/>
+      <c r="L54" s="8"/>
+      <c r="M54" s="8"/>
+    </row>
+    <row r="55" spans="1:16" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="B45" s="15" t="s">
+      <c r="B55" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="C45" s="47"/>
-      <c r="D45" s="14"/>
-      <c r="E45" s="13"/>
-      <c r="F45" s="13"/>
-      <c r="G45" s="14"/>
-      <c r="H45" s="14"/>
-      <c r="I45" s="13"/>
-      <c r="J45" s="13"/>
-      <c r="K45" s="13"/>
-      <c r="L45" s="13"/>
-      <c r="M45" s="13"/>
-    </row>
-    <row r="47" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="38" t="s">
+      <c r="C55" s="21"/>
+      <c r="D55" s="14"/>
+      <c r="E55" s="13"/>
+      <c r="F55" s="13"/>
+      <c r="G55" s="14"/>
+      <c r="H55" s="14"/>
+      <c r="I55" s="13"/>
+      <c r="J55" s="13"/>
+      <c r="K55" s="13"/>
+      <c r="L55" s="13"/>
+      <c r="M55" s="13"/>
+    </row>
+    <row r="57" spans="1:16" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="23" t="s">
         <v>146</v>
       </c>
-      <c r="B47" s="38"/>
-      <c r="C47" s="38"/>
-      <c r="D47" s="38"/>
-      <c r="E47" s="38"/>
-      <c r="F47" s="38"/>
-      <c r="G47" s="38"/>
-      <c r="H47" s="38"/>
-      <c r="I47" s="38"/>
-      <c r="J47" s="38"/>
-      <c r="K47" s="38"/>
-      <c r="L47" s="38"/>
-      <c r="M47" s="38"/>
-    </row>
-    <row r="48" spans="1:13" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="39" t="s">
+      <c r="B57" s="23"/>
+      <c r="C57" s="23"/>
+      <c r="D57" s="23"/>
+      <c r="E57" s="23"/>
+      <c r="F57" s="23"/>
+      <c r="G57" s="23"/>
+      <c r="H57" s="23"/>
+      <c r="I57" s="23"/>
+      <c r="J57" s="23"/>
+      <c r="K57" s="23"/>
+      <c r="L57" s="23"/>
+      <c r="M57" s="23"/>
+    </row>
+    <row r="58" spans="1:16" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="25" t="s">
         <v>147</v>
       </c>
-      <c r="B48" s="39"/>
-      <c r="C48" s="39"/>
-      <c r="D48" s="39"/>
-      <c r="E48" s="39"/>
-      <c r="F48" s="39"/>
-      <c r="G48" s="39"/>
-      <c r="H48" s="39"/>
-      <c r="I48" s="39"/>
-      <c r="J48" s="39"/>
-      <c r="K48" s="39"/>
-      <c r="L48" s="39"/>
-      <c r="M48" s="39"/>
-    </row>
-    <row r="49" spans="1:16" s="3" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B49" s="8" t="s">
-        <v>158</v>
-      </c>
-      <c r="C49" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D49" s="8"/>
-      <c r="E49" s="8"/>
-      <c r="F49" s="8"/>
-      <c r="G49" s="8"/>
-      <c r="H49" s="8"/>
-      <c r="I49" s="8"/>
-      <c r="J49" s="8"/>
-      <c r="K49" s="8"/>
-      <c r="L49" s="8"/>
-      <c r="M49" s="8"/>
-    </row>
-    <row r="50" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="B50" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="C50" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="D50" s="14"/>
-      <c r="E50" s="13"/>
-      <c r="F50" s="13"/>
-      <c r="G50" s="14"/>
-      <c r="H50" s="14"/>
-      <c r="I50" s="13"/>
-      <c r="J50" s="13"/>
-      <c r="K50" s="13"/>
-      <c r="L50" s="13"/>
-      <c r="M50" s="13"/>
-    </row>
-    <row r="51" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="B51" s="11" t="s">
-        <v>152</v>
-      </c>
-      <c r="C51" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="D51" s="12"/>
-      <c r="E51" s="11"/>
-      <c r="F51" s="11"/>
-      <c r="G51" s="12"/>
-      <c r="H51" s="12"/>
-      <c r="I51" s="11"/>
-      <c r="J51" s="11"/>
-      <c r="K51" s="11"/>
-      <c r="L51" s="11"/>
-      <c r="M51" s="11"/>
-    </row>
-    <row r="53" spans="1:16" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="40" t="s">
-        <v>148</v>
-      </c>
-      <c r="B53" s="40"/>
-      <c r="C53" s="40"/>
-      <c r="D53" s="40"/>
-      <c r="E53" s="40"/>
-      <c r="F53" s="40"/>
-      <c r="G53" s="40"/>
-      <c r="H53" s="40"/>
-      <c r="I53" s="40"/>
-      <c r="J53" s="40"/>
-      <c r="K53" s="40"/>
-      <c r="L53" s="40"/>
-      <c r="M53" s="40"/>
-      <c r="N53" s="40"/>
-      <c r="O53" s="40"/>
-      <c r="P53" s="40"/>
-    </row>
-    <row r="54" spans="1:16" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="20" t="s">
-        <v>170</v>
-      </c>
-      <c r="B54" s="20"/>
-      <c r="C54" s="20"/>
-      <c r="D54" s="20"/>
-      <c r="E54" s="20"/>
-      <c r="F54" s="20"/>
-      <c r="G54" s="20"/>
-      <c r="H54" s="20"/>
-      <c r="I54" s="20"/>
-      <c r="J54" s="20"/>
-      <c r="K54" s="20"/>
-      <c r="L54" s="20"/>
-      <c r="M54" s="20"/>
-      <c r="N54" s="20"/>
-      <c r="O54" s="20"/>
-      <c r="P54" s="20"/>
-    </row>
-    <row r="55" spans="1:16" s="3" customFormat="1" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B55" s="8" t="s">
-        <v>160</v>
-      </c>
-      <c r="C55" s="8" t="s">
-        <v>161</v>
-      </c>
-      <c r="D55" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="E55" s="21" t="s">
-        <v>162</v>
-      </c>
-      <c r="F55" s="22"/>
-      <c r="G55" s="21" t="s">
-        <v>163</v>
-      </c>
-      <c r="H55" s="22"/>
-      <c r="I55" s="21" t="s">
-        <v>164</v>
-      </c>
-      <c r="J55" s="22"/>
-      <c r="K55" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="L55" s="8" t="s">
-        <v>216</v>
-      </c>
-      <c r="M55" s="18" t="s">
-        <v>166</v>
-      </c>
-      <c r="N55" s="8" t="s">
-        <v>167</v>
-      </c>
-      <c r="O55" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="P55" s="8" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="56" spans="1:16" s="4" customFormat="1" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="B56" s="13">
-        <v>25</v>
-      </c>
-      <c r="C56" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="D56" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="E56" s="35" t="s">
-        <v>37</v>
-      </c>
-      <c r="F56" s="36"/>
-      <c r="G56" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="H56" s="24"/>
-      <c r="I56" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="J56" s="24"/>
-      <c r="K56" s="14" t="s">
-        <v>100</v>
-      </c>
-      <c r="L56" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="M56" s="19" t="s">
-        <v>217</v>
-      </c>
-      <c r="N56" s="13">
-        <v>5555555</v>
-      </c>
-      <c r="O56" s="13">
-        <v>5555555</v>
-      </c>
-      <c r="P56" s="13">
-        <v>555555</v>
-      </c>
-    </row>
-    <row r="57" spans="1:16" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="58" spans="1:16" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="38" t="s">
-        <v>154</v>
-      </c>
-      <c r="B58" s="38"/>
-      <c r="C58" s="38"/>
-      <c r="D58" s="38"/>
-      <c r="E58" s="38"/>
-      <c r="F58" s="38"/>
-      <c r="G58" s="38"/>
-      <c r="H58" s="38"/>
-      <c r="I58" s="38"/>
-      <c r="J58" s="38"/>
-      <c r="K58" s="38"/>
-      <c r="L58" s="38"/>
-      <c r="M58" s="38"/>
-    </row>
-    <row r="59" spans="1:16" s="3" customFormat="1" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B58" s="25"/>
+      <c r="C58" s="25"/>
+      <c r="D58" s="25"/>
+      <c r="E58" s="25"/>
+      <c r="F58" s="25"/>
+      <c r="G58" s="25"/>
+      <c r="H58" s="25"/>
+      <c r="I58" s="25"/>
+      <c r="J58" s="25"/>
+      <c r="K58" s="25"/>
+      <c r="L58" s="25"/>
+      <c r="M58" s="25"/>
+    </row>
+    <row r="59" spans="1:16" s="3" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>171</v>
+        <v>158</v>
       </c>
       <c r="C59" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="D59" s="8" t="s">
-        <v>131</v>
-      </c>
+      <c r="D59" s="8"/>
       <c r="E59" s="8"/>
       <c r="F59" s="8"/>
       <c r="G59" s="8"/>
@@ -3215,17 +3182,15 @@
     </row>
     <row r="60" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="13" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="B60" s="13" t="s">
-        <v>153</v>
+        <v>78</v>
       </c>
       <c r="C60" s="13" t="s">
-        <v>150</v>
-      </c>
-      <c r="D60" s="14" t="s">
-        <v>30</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="D60" s="14"/>
       <c r="E60" s="13"/>
       <c r="F60" s="13"/>
       <c r="G60" s="14"/>
@@ -3238,17 +3203,15 @@
     </row>
     <row r="61" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="11" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="B61" s="11" t="s">
-        <v>88</v>
+        <v>152</v>
       </c>
       <c r="C61" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="D61" s="12" t="s">
-        <v>30</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="D61" s="12"/>
       <c r="E61" s="11"/>
       <c r="F61" s="11"/>
       <c r="G61" s="12"/>
@@ -3259,112 +3222,161 @@
       <c r="L61" s="11"/>
       <c r="M61" s="11"/>
     </row>
-    <row r="63" spans="1:16" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="38" t="s">
-        <v>155</v>
-      </c>
-      <c r="B63" s="38"/>
-      <c r="C63" s="38"/>
-      <c r="D63" s="38"/>
-      <c r="E63" s="38"/>
-      <c r="F63" s="38"/>
-      <c r="G63" s="38"/>
-      <c r="H63" s="38"/>
-      <c r="I63" s="38"/>
-      <c r="J63" s="38"/>
-      <c r="K63" s="38"/>
-      <c r="L63" s="38"/>
-      <c r="M63" s="38"/>
-    </row>
-    <row r="64" spans="1:16" s="3" customFormat="1" ht="31.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="8" t="s">
+    <row r="63" spans="1:16" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="26" t="s">
+        <v>148</v>
+      </c>
+      <c r="B63" s="26"/>
+      <c r="C63" s="26"/>
+      <c r="D63" s="26"/>
+      <c r="E63" s="26"/>
+      <c r="F63" s="26"/>
+      <c r="G63" s="26"/>
+      <c r="H63" s="26"/>
+      <c r="I63" s="26"/>
+      <c r="J63" s="26"/>
+      <c r="K63" s="26"/>
+      <c r="L63" s="26"/>
+      <c r="M63" s="26"/>
+      <c r="N63" s="26"/>
+      <c r="O63" s="26"/>
+      <c r="P63" s="26"/>
+    </row>
+    <row r="64" spans="1:16" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="33" t="s">
+        <v>170</v>
+      </c>
+      <c r="B64" s="33"/>
+      <c r="C64" s="33"/>
+      <c r="D64" s="33"/>
+      <c r="E64" s="33"/>
+      <c r="F64" s="33"/>
+      <c r="G64" s="33"/>
+      <c r="H64" s="33"/>
+      <c r="I64" s="33"/>
+      <c r="J64" s="33"/>
+      <c r="K64" s="33"/>
+      <c r="L64" s="33"/>
+      <c r="M64" s="33"/>
+      <c r="N64" s="33"/>
+      <c r="O64" s="33"/>
+      <c r="P64" s="33"/>
+    </row>
+    <row r="65" spans="1:16" s="3" customFormat="1" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B64" s="25" t="s">
-        <v>41</v>
-      </c>
-      <c r="C64" s="27"/>
-      <c r="D64" s="25" t="s">
-        <v>156</v>
-      </c>
-      <c r="E64" s="27"/>
-      <c r="F64" s="8"/>
-      <c r="G64" s="8"/>
-      <c r="H64" s="8"/>
-      <c r="I64" s="8"/>
-      <c r="J64" s="8"/>
-      <c r="K64" s="8"/>
-      <c r="L64" s="8"/>
-      <c r="M64" s="8"/>
-    </row>
-    <row r="65" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="B65" s="33" t="s">
-        <v>43</v>
-      </c>
-      <c r="C65" s="34"/>
-      <c r="D65" s="41" t="s">
-        <v>34</v>
-      </c>
-      <c r="E65" s="43"/>
-      <c r="F65" s="13"/>
-      <c r="G65" s="14"/>
-      <c r="H65" s="14"/>
-      <c r="I65" s="13"/>
-      <c r="J65" s="13"/>
-      <c r="K65" s="13"/>
-      <c r="L65" s="13"/>
-      <c r="M65" s="13"/>
-    </row>
-    <row r="66" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="B66" s="28" t="s">
-        <v>159</v>
-      </c>
-      <c r="C66" s="30"/>
-      <c r="D66" s="48" t="s">
-        <v>33</v>
-      </c>
-      <c r="E66" s="49"/>
-      <c r="F66" s="11"/>
-      <c r="G66" s="12"/>
-      <c r="H66" s="12"/>
-      <c r="I66" s="11"/>
-      <c r="J66" s="11"/>
-      <c r="K66" s="11"/>
-      <c r="L66" s="11"/>
-      <c r="M66" s="11"/>
-    </row>
-    <row r="68" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="38" t="s">
-        <v>157</v>
-      </c>
-      <c r="B68" s="38"/>
-      <c r="C68" s="38"/>
-      <c r="D68" s="38"/>
-      <c r="E68" s="38"/>
-      <c r="F68" s="38"/>
-      <c r="G68" s="38"/>
-      <c r="H68" s="38"/>
-      <c r="I68" s="38"/>
-      <c r="J68" s="38"/>
-      <c r="K68" s="38"/>
-      <c r="L68" s="38"/>
-      <c r="M68" s="38"/>
-    </row>
-    <row r="69" spans="1:13" s="3" customFormat="1" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B65" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="C65" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="D65" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="E65" s="27" t="s">
+        <v>162</v>
+      </c>
+      <c r="F65" s="28"/>
+      <c r="G65" s="27" t="s">
+        <v>163</v>
+      </c>
+      <c r="H65" s="28"/>
+      <c r="I65" s="27" t="s">
+        <v>164</v>
+      </c>
+      <c r="J65" s="28"/>
+      <c r="K65" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="L65" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="M65" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="N65" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="O65" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="P65" s="8" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="66" spans="1:16" s="4" customFormat="1" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B66" s="13">
+        <v>25</v>
+      </c>
+      <c r="C66" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="D66" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E66" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="F66" s="30"/>
+      <c r="G66" s="44" t="s">
+        <v>38</v>
+      </c>
+      <c r="H66" s="45"/>
+      <c r="I66" s="44" t="s">
+        <v>38</v>
+      </c>
+      <c r="J66" s="45"/>
+      <c r="K66" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="L66" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="M66" s="19" t="s">
+        <v>217</v>
+      </c>
+      <c r="N66" s="13">
+        <v>5555555</v>
+      </c>
+      <c r="O66" s="13">
+        <v>5555555</v>
+      </c>
+      <c r="P66" s="13">
+        <v>555555</v>
+      </c>
+    </row>
+    <row r="67" spans="1:16" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
+    <row r="68" spans="1:16" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="23" t="s">
+        <v>154</v>
+      </c>
+      <c r="B68" s="23"/>
+      <c r="C68" s="23"/>
+      <c r="D68" s="23"/>
+      <c r="E68" s="23"/>
+      <c r="F68" s="23"/>
+      <c r="G68" s="23"/>
+      <c r="H68" s="23"/>
+      <c r="I68" s="23"/>
+      <c r="J68" s="23"/>
+      <c r="K68" s="23"/>
+      <c r="L68" s="23"/>
+      <c r="M68" s="23"/>
+    </row>
+    <row r="69" spans="1:16" s="3" customFormat="1" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B69" s="8" t="s">
-        <v>207</v>
+        <v>171</v>
       </c>
       <c r="C69" s="8" t="s">
-        <v>208</v>
+        <v>31</v>
       </c>
       <c r="D69" s="8" t="s">
         <v>131</v>
@@ -3379,15 +3391,15 @@
       <c r="L69" s="8"/>
       <c r="M69" s="8"/>
     </row>
-    <row r="70" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="13" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B70" s="13" t="s">
-        <v>45</v>
+        <v>153</v>
       </c>
       <c r="C70" s="13" t="s">
-        <v>46</v>
+        <v>150</v>
       </c>
       <c r="D70" s="14" t="s">
         <v>30</v>
@@ -3402,15 +3414,15 @@
       <c r="L70" s="13"/>
       <c r="M70" s="13"/>
     </row>
-    <row r="71" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="11" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B71" s="11" t="s">
-        <v>47</v>
+        <v>88</v>
       </c>
       <c r="C71" s="11" t="s">
-        <v>48</v>
+        <v>151</v>
       </c>
       <c r="D71" s="12" t="s">
         <v>30</v>
@@ -3425,36 +3437,36 @@
       <c r="L71" s="11"/>
       <c r="M71" s="11"/>
     </row>
-    <row r="73" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="38" t="s">
-        <v>180</v>
-      </c>
-      <c r="B73" s="38"/>
-      <c r="C73" s="38"/>
-      <c r="D73" s="38"/>
-      <c r="E73" s="38"/>
-      <c r="F73" s="38"/>
-      <c r="G73" s="38"/>
-      <c r="H73" s="38"/>
-      <c r="I73" s="38"/>
-      <c r="J73" s="38"/>
-      <c r="K73" s="38"/>
-      <c r="L73" s="38"/>
-      <c r="M73" s="38"/>
-    </row>
-    <row r="74" spans="1:13" s="3" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:16" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="23" t="s">
+        <v>155</v>
+      </c>
+      <c r="B73" s="23"/>
+      <c r="C73" s="23"/>
+      <c r="D73" s="23"/>
+      <c r="E73" s="23"/>
+      <c r="F73" s="23"/>
+      <c r="G73" s="23"/>
+      <c r="H73" s="23"/>
+      <c r="I73" s="23"/>
+      <c r="J73" s="23"/>
+      <c r="K73" s="23"/>
+      <c r="L73" s="23"/>
+      <c r="M73" s="23"/>
+    </row>
+    <row r="74" spans="1:16" s="3" customFormat="1" ht="31.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B74" s="26" t="s">
-        <v>178</v>
-      </c>
-      <c r="C74" s="26"/>
-      <c r="D74" s="25" t="s">
-        <v>179</v>
-      </c>
-      <c r="E74" s="26"/>
-      <c r="F74" s="27"/>
+      <c r="B74" s="34" t="s">
+        <v>41</v>
+      </c>
+      <c r="C74" s="35"/>
+      <c r="D74" s="34" t="s">
+        <v>156</v>
+      </c>
+      <c r="E74" s="35"/>
+      <c r="F74" s="8"/>
       <c r="G74" s="8"/>
       <c r="H74" s="8"/>
       <c r="I74" s="8"/>
@@ -3463,19 +3475,19 @@
       <c r="L74" s="8"/>
       <c r="M74" s="8"/>
     </row>
-    <row r="75" spans="1:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="B75" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="C75" s="34"/>
-      <c r="D75" s="41" t="s">
-        <v>50</v>
+        <v>42</v>
+      </c>
+      <c r="B75" s="36" t="s">
+        <v>43</v>
+      </c>
+      <c r="C75" s="37"/>
+      <c r="D75" s="40" t="s">
+        <v>34</v>
       </c>
       <c r="E75" s="42"/>
-      <c r="F75" s="43"/>
+      <c r="F75" s="13"/>
       <c r="G75" s="14"/>
       <c r="H75" s="14"/>
       <c r="I75" s="13"/>
@@ -3484,55 +3496,58 @@
       <c r="L75" s="13"/>
       <c r="M75" s="13"/>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B76" s="7"/>
-    </row>
-    <row r="77" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="38" t="s">
-        <v>172</v>
-      </c>
-      <c r="B77" s="38"/>
-      <c r="C77" s="38"/>
-      <c r="D77" s="38"/>
-      <c r="E77" s="38"/>
-      <c r="F77" s="38"/>
-      <c r="G77" s="38"/>
-      <c r="H77" s="38"/>
-      <c r="I77" s="38"/>
-      <c r="J77" s="38"/>
-      <c r="K77" s="38"/>
-      <c r="L77" s="38"/>
-      <c r="M77" s="38"/>
-    </row>
-    <row r="78" spans="1:13" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="39" t="s">
-        <v>173</v>
-      </c>
-      <c r="B78" s="39"/>
-      <c r="C78" s="39"/>
-      <c r="D78" s="39"/>
-      <c r="E78" s="39"/>
-      <c r="F78" s="39"/>
-      <c r="G78" s="39"/>
-      <c r="H78" s="39"/>
-      <c r="I78" s="39"/>
-      <c r="J78" s="39"/>
-      <c r="K78" s="39"/>
-      <c r="L78" s="39"/>
-      <c r="M78" s="39"/>
-    </row>
-    <row r="79" spans="1:13" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B76" s="46" t="s">
+        <v>159</v>
+      </c>
+      <c r="C76" s="48"/>
+      <c r="D76" s="49" t="s">
+        <v>33</v>
+      </c>
+      <c r="E76" s="50"/>
+      <c r="F76" s="11"/>
+      <c r="G76" s="12"/>
+      <c r="H76" s="12"/>
+      <c r="I76" s="11"/>
+      <c r="J76" s="11"/>
+      <c r="K76" s="11"/>
+      <c r="L76" s="11"/>
+      <c r="M76" s="11"/>
+    </row>
+    <row r="78" spans="1:16" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A78" s="23" t="s">
+        <v>157</v>
+      </c>
+      <c r="B78" s="23"/>
+      <c r="C78" s="23"/>
+      <c r="D78" s="23"/>
+      <c r="E78" s="23"/>
+      <c r="F78" s="23"/>
+      <c r="G78" s="23"/>
+      <c r="H78" s="23"/>
+      <c r="I78" s="23"/>
+      <c r="J78" s="23"/>
+      <c r="K78" s="23"/>
+      <c r="L78" s="23"/>
+      <c r="M78" s="23"/>
+    </row>
+    <row r="79" spans="1:16" s="3" customFormat="1" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B79" s="8" t="s">
-        <v>209</v>
-      </c>
-      <c r="C79" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="D79" s="26"/>
-      <c r="E79" s="27"/>
+        <v>207</v>
+      </c>
+      <c r="C79" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="D79" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="E79" s="8"/>
       <c r="F79" s="8"/>
       <c r="G79" s="8"/>
       <c r="H79" s="8"/>
@@ -3542,18 +3557,20 @@
       <c r="L79" s="8"/>
       <c r="M79" s="8"/>
     </row>
-    <row r="80" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" s="13" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="B80" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="C80" s="33" t="s">
-        <v>219</v>
-      </c>
-      <c r="D80" s="50"/>
-      <c r="E80" s="34"/>
+        <v>45</v>
+      </c>
+      <c r="C80" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="D80" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E80" s="13"/>
       <c r="F80" s="13"/>
       <c r="G80" s="14"/>
       <c r="H80" s="14"/>
@@ -3563,16 +3580,20 @@
       <c r="L80" s="13"/>
       <c r="M80" s="13"/>
     </row>
-    <row r="81" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" s="11" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="B81" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="C81" s="28"/>
-      <c r="D81" s="29"/>
-      <c r="E81" s="30"/>
+        <v>47</v>
+      </c>
+      <c r="C81" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D81" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="E81" s="11"/>
       <c r="F81" s="11"/>
       <c r="G81" s="12"/>
       <c r="H81" s="12"/>
@@ -3582,1034 +3603,1199 @@
       <c r="L81" s="11"/>
       <c r="M81" s="11"/>
     </row>
-    <row r="82" spans="1:13" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
     <row r="83" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="40" t="s">
+      <c r="A83" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="B83" s="23"/>
+      <c r="C83" s="23"/>
+      <c r="D83" s="23"/>
+      <c r="E83" s="23"/>
+      <c r="F83" s="23"/>
+      <c r="G83" s="23"/>
+      <c r="H83" s="23"/>
+      <c r="I83" s="23"/>
+      <c r="J83" s="23"/>
+      <c r="K83" s="23"/>
+      <c r="L83" s="23"/>
+      <c r="M83" s="23"/>
+    </row>
+    <row r="84" spans="1:13" s="3" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A84" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B84" s="39" t="s">
+        <v>178</v>
+      </c>
+      <c r="C84" s="39"/>
+      <c r="D84" s="34" t="s">
+        <v>179</v>
+      </c>
+      <c r="E84" s="39"/>
+      <c r="F84" s="35"/>
+      <c r="G84" s="8"/>
+      <c r="H84" s="8"/>
+      <c r="I84" s="8"/>
+      <c r="J84" s="8"/>
+      <c r="K84" s="8"/>
+      <c r="L84" s="8"/>
+      <c r="M84" s="8"/>
+    </row>
+    <row r="85" spans="1:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A85" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="B85" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="C85" s="37"/>
+      <c r="D85" s="40" t="s">
+        <v>50</v>
+      </c>
+      <c r="E85" s="41"/>
+      <c r="F85" s="42"/>
+      <c r="G85" s="14"/>
+      <c r="H85" s="14"/>
+      <c r="I85" s="13"/>
+      <c r="J85" s="13"/>
+      <c r="K85" s="13"/>
+      <c r="L85" s="13"/>
+      <c r="M85" s="13"/>
+    </row>
+    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B86" s="7"/>
+    </row>
+    <row r="87" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A87" s="23" t="s">
+        <v>172</v>
+      </c>
+      <c r="B87" s="23"/>
+      <c r="C87" s="23"/>
+      <c r="D87" s="23"/>
+      <c r="E87" s="23"/>
+      <c r="F87" s="23"/>
+      <c r="G87" s="23"/>
+      <c r="H87" s="23"/>
+      <c r="I87" s="23"/>
+      <c r="J87" s="23"/>
+      <c r="K87" s="23"/>
+      <c r="L87" s="23"/>
+      <c r="M87" s="23"/>
+    </row>
+    <row r="88" spans="1:13" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A88" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="B88" s="25"/>
+      <c r="C88" s="25"/>
+      <c r="D88" s="25"/>
+      <c r="E88" s="25"/>
+      <c r="F88" s="25"/>
+      <c r="G88" s="25"/>
+      <c r="H88" s="25"/>
+      <c r="I88" s="25"/>
+      <c r="J88" s="25"/>
+      <c r="K88" s="25"/>
+      <c r="L88" s="25"/>
+      <c r="M88" s="25"/>
+    </row>
+    <row r="89" spans="1:13" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A89" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B89" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="C89" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="D89" s="39"/>
+      <c r="E89" s="35"/>
+      <c r="F89" s="8"/>
+      <c r="G89" s="8"/>
+      <c r="H89" s="8"/>
+      <c r="I89" s="8"/>
+      <c r="J89" s="8"/>
+      <c r="K89" s="8"/>
+      <c r="L89" s="8"/>
+      <c r="M89" s="8"/>
+    </row>
+    <row r="90" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A90" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="B90" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="C90" s="36" t="s">
+        <v>219</v>
+      </c>
+      <c r="D90" s="43"/>
+      <c r="E90" s="37"/>
+      <c r="F90" s="13"/>
+      <c r="G90" s="14"/>
+      <c r="H90" s="14"/>
+      <c r="I90" s="13"/>
+      <c r="J90" s="13"/>
+      <c r="K90" s="13"/>
+      <c r="L90" s="13"/>
+      <c r="M90" s="13"/>
+    </row>
+    <row r="91" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A91" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="B91" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="C91" s="46"/>
+      <c r="D91" s="47"/>
+      <c r="E91" s="48"/>
+      <c r="F91" s="11"/>
+      <c r="G91" s="12"/>
+      <c r="H91" s="12"/>
+      <c r="I91" s="11"/>
+      <c r="J91" s="11"/>
+      <c r="K91" s="11"/>
+      <c r="L91" s="11"/>
+      <c r="M91" s="11"/>
+    </row>
+    <row r="92" spans="1:13" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
+    <row r="93" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A93" s="26" t="s">
         <v>181</v>
       </c>
-      <c r="B83" s="40"/>
-      <c r="C83" s="40"/>
-      <c r="D83" s="40"/>
-      <c r="E83" s="40"/>
-      <c r="F83" s="40"/>
-      <c r="G83" s="40"/>
-      <c r="H83" s="40"/>
-      <c r="I83" s="40"/>
-      <c r="J83" s="40"/>
-      <c r="K83" s="40"/>
-      <c r="L83" s="40"/>
-      <c r="M83" s="40"/>
-    </row>
-    <row r="84" spans="1:13" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A84" s="39" t="s">
+      <c r="B93" s="26"/>
+      <c r="C93" s="26"/>
+      <c r="D93" s="26"/>
+      <c r="E93" s="26"/>
+      <c r="F93" s="26"/>
+      <c r="G93" s="26"/>
+      <c r="H93" s="26"/>
+      <c r="I93" s="26"/>
+      <c r="J93" s="26"/>
+      <c r="K93" s="26"/>
+      <c r="L93" s="26"/>
+      <c r="M93" s="26"/>
+    </row>
+    <row r="94" spans="1:13" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A94" s="25" t="s">
         <v>185</v>
       </c>
-      <c r="B84" s="39"/>
-      <c r="C84" s="39"/>
-      <c r="D84" s="39"/>
-      <c r="E84" s="39"/>
-      <c r="F84" s="39"/>
-      <c r="G84" s="39"/>
-      <c r="H84" s="39"/>
-      <c r="I84" s="39"/>
-      <c r="J84" s="39"/>
-      <c r="K84" s="39"/>
-      <c r="L84" s="39"/>
-      <c r="M84" s="39"/>
-    </row>
-    <row r="85" spans="1:13" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="8" t="s">
+      <c r="B94" s="25"/>
+      <c r="C94" s="25"/>
+      <c r="D94" s="25"/>
+      <c r="E94" s="25"/>
+      <c r="F94" s="25"/>
+      <c r="G94" s="25"/>
+      <c r="H94" s="25"/>
+      <c r="I94" s="25"/>
+      <c r="J94" s="25"/>
+      <c r="K94" s="25"/>
+      <c r="L94" s="25"/>
+      <c r="M94" s="25"/>
+    </row>
+    <row r="95" spans="1:13" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A95" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B85" s="8" t="s">
+      <c r="B95" s="8" t="s">
         <v>175</v>
       </c>
-      <c r="C85" s="8" t="s">
+      <c r="C95" s="8" t="s">
         <v>174</v>
       </c>
-      <c r="D85" s="8" t="s">
+      <c r="D95" s="8" t="s">
         <v>176</v>
       </c>
-      <c r="E85" s="8" t="s">
+      <c r="E95" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="F85" s="8" t="s">
+      <c r="F95" s="8" t="s">
         <v>177</v>
       </c>
-      <c r="G85" s="8" t="s">
+      <c r="G95" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="H85" s="8"/>
-      <c r="I85" s="8"/>
-      <c r="J85" s="8"/>
-      <c r="K85" s="8"/>
-      <c r="L85" s="8"/>
-      <c r="M85" s="8"/>
-    </row>
-    <row r="86" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="13" t="s">
+      <c r="H95" s="8"/>
+      <c r="I95" s="8"/>
+      <c r="J95" s="8"/>
+      <c r="K95" s="8"/>
+      <c r="L95" s="8"/>
+      <c r="M95" s="8"/>
+    </row>
+    <row r="96" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A96" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="B86" s="13" t="s">
+      <c r="B96" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="C86" s="13">
+      <c r="C96" s="13">
         <v>162</v>
       </c>
-      <c r="D86" s="14" t="s">
+      <c r="D96" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="E86" s="13" t="s">
+      <c r="E96" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="F86" s="13" t="s">
+      <c r="F96" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="G86" s="14" t="s">
+      <c r="G96" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="H86" s="14"/>
-      <c r="I86" s="13"/>
-      <c r="J86" s="13"/>
-      <c r="K86" s="13"/>
-      <c r="L86" s="13"/>
-      <c r="M86" s="13"/>
-    </row>
-    <row r="87" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="11" t="s">
+      <c r="H96" s="14"/>
+      <c r="I96" s="13"/>
+      <c r="J96" s="13"/>
+      <c r="K96" s="13"/>
+      <c r="L96" s="13"/>
+      <c r="M96" s="13"/>
+    </row>
+    <row r="97" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A97" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="B87" s="11" t="s">
+      <c r="B97" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="C87" s="11">
+      <c r="C97" s="11">
         <v>162</v>
       </c>
-      <c r="D87" s="12" t="s">
+      <c r="D97" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="E87" s="11" t="s">
+      <c r="E97" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="F87" s="11" t="s">
+      <c r="F97" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="G87" s="12" t="s">
+      <c r="G97" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="H87" s="12"/>
-      <c r="I87" s="11"/>
-      <c r="J87" s="11"/>
-      <c r="K87" s="11"/>
-      <c r="L87" s="11"/>
-      <c r="M87" s="11"/>
-    </row>
-    <row r="88" spans="1:13" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="89" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A89" s="38" t="s">
+      <c r="H97" s="12"/>
+      <c r="I97" s="11"/>
+      <c r="J97" s="11"/>
+      <c r="K97" s="11"/>
+      <c r="L97" s="11"/>
+      <c r="M97" s="11"/>
+    </row>
+    <row r="98" spans="1:13" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
+    <row r="99" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A99" s="23" t="s">
         <v>182</v>
       </c>
-      <c r="B89" s="38"/>
-      <c r="C89" s="38"/>
-      <c r="D89" s="38"/>
-      <c r="E89" s="38"/>
-      <c r="F89" s="38"/>
-      <c r="G89" s="38"/>
-      <c r="H89" s="38"/>
-      <c r="I89" s="38"/>
-      <c r="J89" s="38"/>
-      <c r="K89" s="38"/>
-      <c r="L89" s="38"/>
-      <c r="M89" s="38"/>
-    </row>
-    <row r="90" spans="1:13" s="3" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="39" t="s">
+      <c r="B99" s="23"/>
+      <c r="C99" s="23"/>
+      <c r="D99" s="23"/>
+      <c r="E99" s="23"/>
+      <c r="F99" s="23"/>
+      <c r="G99" s="23"/>
+      <c r="H99" s="23"/>
+      <c r="I99" s="23"/>
+      <c r="J99" s="23"/>
+      <c r="K99" s="23"/>
+      <c r="L99" s="23"/>
+      <c r="M99" s="23"/>
+    </row>
+    <row r="100" spans="1:13" s="3" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A100" s="25" t="s">
         <v>183</v>
       </c>
-      <c r="B90" s="39"/>
-      <c r="C90" s="39"/>
-      <c r="D90" s="39"/>
-      <c r="E90" s="39"/>
-      <c r="F90" s="39"/>
-      <c r="G90" s="39"/>
-      <c r="H90" s="39"/>
-      <c r="I90" s="39"/>
-      <c r="J90" s="39"/>
-      <c r="K90" s="39"/>
-      <c r="L90" s="39"/>
-      <c r="M90" s="39"/>
-    </row>
-    <row r="91" spans="1:13" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A91" s="8" t="s">
+      <c r="B100" s="25"/>
+      <c r="C100" s="25"/>
+      <c r="D100" s="25"/>
+      <c r="E100" s="25"/>
+      <c r="F100" s="25"/>
+      <c r="G100" s="25"/>
+      <c r="H100" s="25"/>
+      <c r="I100" s="25"/>
+      <c r="J100" s="25"/>
+      <c r="K100" s="25"/>
+      <c r="L100" s="25"/>
+      <c r="M100" s="25"/>
+    </row>
+    <row r="101" spans="1:13" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A101" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B91" s="8" t="s">
+      <c r="B101" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="C91" s="8" t="s">
+      <c r="C101" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="D91" s="8" t="s">
+      <c r="D101" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="E91" s="8" t="s">
+      <c r="E101" s="8" t="s">
         <v>184</v>
       </c>
-      <c r="F91" s="8" t="s">
+      <c r="F101" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="G91" s="8"/>
-      <c r="H91" s="8"/>
-      <c r="I91" s="8"/>
-      <c r="J91" s="8"/>
-      <c r="K91" s="8"/>
-      <c r="L91" s="8"/>
-      <c r="M91" s="8"/>
-    </row>
-    <row r="92" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A92" s="13" t="s">
+      <c r="G101" s="8"/>
+      <c r="H101" s="8"/>
+      <c r="I101" s="8"/>
+      <c r="J101" s="8"/>
+      <c r="K101" s="8"/>
+      <c r="L101" s="8"/>
+      <c r="M101" s="8"/>
+    </row>
+    <row r="102" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A102" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="B92" s="13" t="s">
+      <c r="B102" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="C92" s="13" t="s">
+      <c r="C102" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="D92" s="14" t="s">
+      <c r="D102" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="E92" s="13" t="s">
+      <c r="E102" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="F92" s="13" t="s">
+      <c r="F102" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="G92" s="14"/>
-      <c r="H92" s="14"/>
-      <c r="I92" s="13"/>
-      <c r="J92" s="13"/>
-      <c r="K92" s="13"/>
-      <c r="L92" s="13"/>
-      <c r="M92" s="13"/>
-    </row>
-    <row r="93" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A93" s="11" t="s">
+      <c r="G102" s="14"/>
+      <c r="H102" s="14"/>
+      <c r="I102" s="13"/>
+      <c r="J102" s="13"/>
+      <c r="K102" s="13"/>
+      <c r="L102" s="13"/>
+      <c r="M102" s="13"/>
+    </row>
+    <row r="103" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A103" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="B93" s="11" t="s">
+      <c r="B103" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="C93" s="11" t="s">
+      <c r="C103" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="D93" s="12" t="s">
+      <c r="D103" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="E93" s="11" t="s">
+      <c r="E103" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="F93" s="11" t="s">
+      <c r="F103" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="G93" s="12"/>
-      <c r="H93" s="12"/>
-      <c r="I93" s="11"/>
-      <c r="J93" s="11"/>
-      <c r="K93" s="11"/>
-      <c r="L93" s="11"/>
-      <c r="M93" s="11"/>
-    </row>
-    <row r="94" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A94" s="13" t="s">
+      <c r="G103" s="12"/>
+      <c r="H103" s="12"/>
+      <c r="I103" s="11"/>
+      <c r="J103" s="11"/>
+      <c r="K103" s="11"/>
+      <c r="L103" s="11"/>
+      <c r="M103" s="11"/>
+    </row>
+    <row r="104" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A104" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="B94" s="13" t="s">
+      <c r="B104" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="C94" s="13" t="s">
+      <c r="C104" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="D94" s="14"/>
-      <c r="E94" s="13" t="s">
+      <c r="D104" s="14"/>
+      <c r="E104" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="F94" s="13" t="s">
+      <c r="F104" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="G94" s="14"/>
-      <c r="H94" s="14"/>
-      <c r="I94" s="13"/>
-      <c r="J94" s="13"/>
-      <c r="K94" s="13"/>
-      <c r="L94" s="13"/>
-      <c r="M94" s="13"/>
-    </row>
-    <row r="95" spans="1:13" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="96" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A96" s="38" t="s">
+      <c r="G104" s="14"/>
+      <c r="H104" s="14"/>
+      <c r="I104" s="13"/>
+      <c r="J104" s="13"/>
+      <c r="K104" s="13"/>
+      <c r="L104" s="13"/>
+      <c r="M104" s="13"/>
+    </row>
+    <row r="105" spans="1:13" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
+    <row r="106" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A106" s="23" t="s">
         <v>186</v>
       </c>
-      <c r="B96" s="38"/>
-      <c r="C96" s="38"/>
-      <c r="D96" s="38"/>
-      <c r="E96" s="38"/>
-      <c r="F96" s="38"/>
-      <c r="G96" s="38"/>
-      <c r="H96" s="38"/>
-      <c r="I96" s="38"/>
-      <c r="J96" s="38"/>
-      <c r="K96" s="38"/>
-      <c r="L96" s="38"/>
-      <c r="M96" s="38"/>
-    </row>
-    <row r="97" spans="1:13" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A97" s="8" t="s">
+      <c r="B106" s="23"/>
+      <c r="C106" s="23"/>
+      <c r="D106" s="23"/>
+      <c r="E106" s="23"/>
+      <c r="F106" s="23"/>
+      <c r="G106" s="23"/>
+      <c r="H106" s="23"/>
+      <c r="I106" s="23"/>
+      <c r="J106" s="23"/>
+      <c r="K106" s="23"/>
+      <c r="L106" s="23"/>
+      <c r="M106" s="23"/>
+    </row>
+    <row r="107" spans="1:13" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A107" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B97" s="8" t="s">
+      <c r="B107" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="C97" s="8" t="s">
+      <c r="C107" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="D97" s="8" t="s">
+      <c r="D107" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="E97" s="8" t="s">
+      <c r="E107" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="F97" s="8" t="s">
+      <c r="F107" s="8" t="s">
         <v>192</v>
       </c>
-      <c r="G97" s="8" t="s">
+      <c r="G107" s="8" t="s">
         <v>191</v>
       </c>
-      <c r="H97" s="8" t="s">
+      <c r="H107" s="8" t="s">
         <v>190</v>
       </c>
-      <c r="I97" s="8" t="s">
+      <c r="I107" s="8" t="s">
         <v>189</v>
       </c>
-      <c r="J97" s="8" t="s">
+      <c r="J107" s="8" t="s">
         <v>188</v>
       </c>
-      <c r="K97" s="8"/>
-      <c r="L97" s="8"/>
-      <c r="M97" s="8"/>
-    </row>
-    <row r="98" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="13" t="s">
+      <c r="K107" s="8"/>
+      <c r="L107" s="8"/>
+      <c r="M107" s="8"/>
+    </row>
+    <row r="108" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A108" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="B98" s="13" t="s">
+      <c r="B108" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="C98" s="13">
+      <c r="C108" s="13">
         <v>514</v>
       </c>
-      <c r="D98" s="14" t="s">
+      <c r="D108" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="E98" s="13" t="s">
+      <c r="E108" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="F98" s="13" t="s">
+      <c r="F108" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="G98" s="14" t="s">
+      <c r="G108" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="H98" s="14" t="s">
+      <c r="H108" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="I98" s="13" t="s">
+      <c r="I108" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="J98" s="13" t="s">
+      <c r="J108" s="13" t="s">
         <v>187</v>
       </c>
-      <c r="K98" s="13"/>
-      <c r="L98" s="13"/>
-      <c r="M98" s="13"/>
-    </row>
-    <row r="99" spans="1:13" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="100" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A100" s="38" t="s">
+      <c r="K108" s="13"/>
+      <c r="L108" s="13"/>
+      <c r="M108" s="13"/>
+    </row>
+    <row r="109" spans="1:13" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
+    <row r="110" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A110" s="23" t="s">
         <v>194</v>
       </c>
-      <c r="B100" s="38"/>
-      <c r="C100" s="38"/>
-      <c r="D100" s="38"/>
-      <c r="E100" s="38"/>
-      <c r="F100" s="38"/>
-      <c r="G100" s="38"/>
-      <c r="H100" s="38"/>
-      <c r="I100" s="38"/>
-      <c r="J100" s="38"/>
-      <c r="K100" s="38"/>
-      <c r="L100" s="38"/>
-      <c r="M100" s="38"/>
-    </row>
-    <row r="101" spans="1:13" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="32" t="s">
+      <c r="B110" s="23"/>
+      <c r="C110" s="23"/>
+      <c r="D110" s="23"/>
+      <c r="E110" s="23"/>
+      <c r="F110" s="23"/>
+      <c r="G110" s="23"/>
+      <c r="H110" s="23"/>
+      <c r="I110" s="23"/>
+      <c r="J110" s="23"/>
+      <c r="K110" s="23"/>
+      <c r="L110" s="23"/>
+      <c r="M110" s="23"/>
+    </row>
+    <row r="111" spans="1:13" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A111" s="31" t="s">
         <v>200</v>
       </c>
-      <c r="B101" s="32"/>
-      <c r="C101" s="32"/>
-      <c r="D101" s="32"/>
-      <c r="E101" s="32"/>
-      <c r="F101" s="32"/>
-      <c r="G101" s="32"/>
-      <c r="H101" s="32"/>
-      <c r="I101" s="32"/>
-      <c r="J101" s="32"/>
-      <c r="K101" s="32"/>
-      <c r="L101" s="32"/>
-      <c r="M101" s="32"/>
-    </row>
-    <row r="102" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="20" t="s">
+      <c r="B111" s="31"/>
+      <c r="C111" s="31"/>
+      <c r="D111" s="31"/>
+      <c r="E111" s="31"/>
+      <c r="F111" s="31"/>
+      <c r="G111" s="31"/>
+      <c r="H111" s="31"/>
+      <c r="I111" s="31"/>
+      <c r="J111" s="31"/>
+      <c r="K111" s="31"/>
+      <c r="L111" s="31"/>
+      <c r="M111" s="31"/>
+    </row>
+    <row r="112" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A112" s="33" t="s">
         <v>108</v>
       </c>
-      <c r="B102" s="20"/>
-      <c r="C102" s="20"/>
-      <c r="D102" s="20"/>
-      <c r="E102" s="20"/>
-      <c r="F102" s="20"/>
-      <c r="G102" s="20"/>
-      <c r="H102" s="20"/>
-      <c r="I102" s="20"/>
-      <c r="J102" s="20"/>
-      <c r="K102" s="20"/>
-      <c r="L102" s="20"/>
-      <c r="M102" s="20"/>
-    </row>
-    <row r="103" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A103" s="37" t="s">
+      <c r="B112" s="33"/>
+      <c r="C112" s="33"/>
+      <c r="D112" s="33"/>
+      <c r="E112" s="33"/>
+      <c r="F112" s="33"/>
+      <c r="G112" s="33"/>
+      <c r="H112" s="33"/>
+      <c r="I112" s="33"/>
+      <c r="J112" s="33"/>
+      <c r="K112" s="33"/>
+      <c r="L112" s="33"/>
+      <c r="M112" s="33"/>
+    </row>
+    <row r="113" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A113" s="32" t="s">
         <v>201</v>
       </c>
-      <c r="B103" s="37"/>
-      <c r="C103" s="37"/>
-      <c r="D103" s="37"/>
-      <c r="E103" s="37"/>
-      <c r="F103" s="37"/>
-      <c r="G103" s="37"/>
-      <c r="H103" s="37"/>
-      <c r="I103" s="37"/>
-      <c r="J103" s="37"/>
-      <c r="K103" s="37"/>
-      <c r="L103" s="37"/>
-      <c r="M103" s="37"/>
-    </row>
-    <row r="104" spans="1:13" s="4" customFormat="1" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A104" s="8" t="s">
+      <c r="B113" s="32"/>
+      <c r="C113" s="32"/>
+      <c r="D113" s="32"/>
+      <c r="E113" s="32"/>
+      <c r="F113" s="32"/>
+      <c r="G113" s="32"/>
+      <c r="H113" s="32"/>
+      <c r="I113" s="32"/>
+      <c r="J113" s="32"/>
+      <c r="K113" s="32"/>
+      <c r="L113" s="32"/>
+      <c r="M113" s="32"/>
+    </row>
+    <row r="114" spans="1:13" s="4" customFormat="1" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A114" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B104" s="8" t="s">
+      <c r="B114" s="8" t="s">
         <v>197</v>
       </c>
-      <c r="C104" s="8" t="s">
+      <c r="C114" s="8" t="s">
         <v>198</v>
       </c>
-      <c r="D104" s="8" t="s">
+      <c r="D114" s="8" t="s">
         <v>199</v>
       </c>
-      <c r="E104" s="8" t="s">
+      <c r="E114" s="8" t="s">
         <v>206</v>
       </c>
-      <c r="F104" s="8" t="s">
+      <c r="F114" s="8" t="s">
         <v>196</v>
       </c>
-      <c r="G104" s="8" t="s">
+      <c r="G114" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="H104" s="8" t="s">
+      <c r="H114" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="I104" s="8" t="s">
+      <c r="I114" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="J104" s="8"/>
-      <c r="K104" s="8"/>
-      <c r="L104" s="8"/>
-      <c r="M104" s="8"/>
-    </row>
-    <row r="105" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A105" s="13" t="s">
+      <c r="J114" s="8"/>
+      <c r="K114" s="8"/>
+      <c r="L114" s="8"/>
+      <c r="M114" s="8"/>
+    </row>
+    <row r="115" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A115" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="B105" s="13" t="s">
+      <c r="B115" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="C105" s="13" t="s">
+      <c r="C115" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="D105" s="14">
+      <c r="D115" s="14">
         <v>1812</v>
       </c>
-      <c r="E105" s="13" t="s">
+      <c r="E115" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="F105" s="13" t="s">
+      <c r="F115" s="13" t="s">
         <v>195</v>
       </c>
-      <c r="G105" s="14">
+      <c r="G115" s="14">
         <v>5</v>
       </c>
-      <c r="H105" s="14">
+      <c r="H115" s="14">
         <v>5</v>
       </c>
-      <c r="I105" s="13" t="s">
+      <c r="I115" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="J105" s="13"/>
-      <c r="K105" s="13"/>
-      <c r="L105" s="13"/>
-      <c r="M105" s="13"/>
-    </row>
-    <row r="106" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A106" s="11" t="s">
+      <c r="J115" s="13"/>
+      <c r="K115" s="13"/>
+      <c r="L115" s="13"/>
+      <c r="M115" s="13"/>
+    </row>
+    <row r="116" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A116" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="B106" s="11" t="s">
+      <c r="B116" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="C106" s="11" t="s">
+      <c r="C116" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="D106" s="12">
+      <c r="D116" s="12">
         <v>1812</v>
       </c>
-      <c r="E106" s="11" t="s">
+      <c r="E116" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="F106" s="11" t="s">
+      <c r="F116" s="11" t="s">
         <v>195</v>
       </c>
-      <c r="G106" s="12">
+      <c r="G116" s="12">
         <v>5</v>
       </c>
-      <c r="H106" s="12">
+      <c r="H116" s="12">
         <v>5</v>
       </c>
-      <c r="I106" s="11" t="s">
+      <c r="I116" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="J106" s="11"/>
-      <c r="K106" s="11"/>
-      <c r="L106" s="11"/>
-      <c r="M106" s="11"/>
-    </row>
-    <row r="107" spans="1:13" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="108" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A108" s="38" t="s">
+      <c r="J116" s="11"/>
+      <c r="K116" s="11"/>
+      <c r="L116" s="11"/>
+      <c r="M116" s="11"/>
+    </row>
+    <row r="117" spans="1:13" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
+    <row r="118" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A118" s="23" t="s">
         <v>210</v>
       </c>
-      <c r="B108" s="38"/>
-      <c r="C108" s="38"/>
-      <c r="D108" s="38"/>
-      <c r="E108" s="38"/>
-      <c r="F108" s="38"/>
-      <c r="G108" s="38"/>
-      <c r="H108" s="38"/>
-      <c r="I108" s="38"/>
-      <c r="J108" s="38"/>
-      <c r="K108" s="38"/>
-      <c r="L108" s="38"/>
-      <c r="M108" s="38"/>
-    </row>
-    <row r="109" spans="1:13" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="32" t="s">
+      <c r="B118" s="23"/>
+      <c r="C118" s="23"/>
+      <c r="D118" s="23"/>
+      <c r="E118" s="23"/>
+      <c r="F118" s="23"/>
+      <c r="G118" s="23"/>
+      <c r="H118" s="23"/>
+      <c r="I118" s="23"/>
+      <c r="J118" s="23"/>
+      <c r="K118" s="23"/>
+      <c r="L118" s="23"/>
+      <c r="M118" s="23"/>
+    </row>
+    <row r="119" spans="1:13" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A119" s="31" t="s">
         <v>200</v>
       </c>
-      <c r="B109" s="32"/>
-      <c r="C109" s="32"/>
-      <c r="D109" s="32"/>
-      <c r="E109" s="32"/>
-      <c r="F109" s="32"/>
-      <c r="G109" s="32"/>
-      <c r="H109" s="32"/>
-      <c r="I109" s="32"/>
-      <c r="J109" s="32"/>
-      <c r="K109" s="32"/>
-      <c r="L109" s="32"/>
-      <c r="M109" s="32"/>
-    </row>
-    <row r="110" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="20" t="s">
+      <c r="B119" s="31"/>
+      <c r="C119" s="31"/>
+      <c r="D119" s="31"/>
+      <c r="E119" s="31"/>
+      <c r="F119" s="31"/>
+      <c r="G119" s="31"/>
+      <c r="H119" s="31"/>
+      <c r="I119" s="31"/>
+      <c r="J119" s="31"/>
+      <c r="K119" s="31"/>
+      <c r="L119" s="31"/>
+      <c r="M119" s="31"/>
+    </row>
+    <row r="120" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A120" s="33" t="s">
         <v>108</v>
       </c>
-      <c r="B110" s="20"/>
-      <c r="C110" s="20"/>
-      <c r="D110" s="20"/>
-      <c r="E110" s="20"/>
-      <c r="F110" s="20"/>
-      <c r="G110" s="20"/>
-      <c r="H110" s="20"/>
-      <c r="I110" s="20"/>
-      <c r="J110" s="20"/>
-      <c r="K110" s="20"/>
-      <c r="L110" s="20"/>
-      <c r="M110" s="20"/>
-    </row>
-    <row r="111" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A111" s="37" t="s">
+      <c r="B120" s="33"/>
+      <c r="C120" s="33"/>
+      <c r="D120" s="33"/>
+      <c r="E120" s="33"/>
+      <c r="F120" s="33"/>
+      <c r="G120" s="33"/>
+      <c r="H120" s="33"/>
+      <c r="I120" s="33"/>
+      <c r="J120" s="33"/>
+      <c r="K120" s="33"/>
+      <c r="L120" s="33"/>
+      <c r="M120" s="33"/>
+    </row>
+    <row r="121" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A121" s="32" t="s">
         <v>202</v>
       </c>
-      <c r="B111" s="37"/>
-      <c r="C111" s="37"/>
-      <c r="D111" s="37"/>
-      <c r="E111" s="37"/>
-      <c r="F111" s="37"/>
-      <c r="G111" s="37"/>
-      <c r="H111" s="37"/>
-      <c r="I111" s="37"/>
-      <c r="J111" s="37"/>
-      <c r="K111" s="37"/>
-      <c r="L111" s="37"/>
-      <c r="M111" s="37"/>
-    </row>
-    <row r="112" spans="1:13" s="4" customFormat="1" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A112" s="10" t="s">
+      <c r="B121" s="32"/>
+      <c r="C121" s="32"/>
+      <c r="D121" s="32"/>
+      <c r="E121" s="32"/>
+      <c r="F121" s="32"/>
+      <c r="G121" s="32"/>
+      <c r="H121" s="32"/>
+      <c r="I121" s="32"/>
+      <c r="J121" s="32"/>
+      <c r="K121" s="32"/>
+      <c r="L121" s="32"/>
+      <c r="M121" s="32"/>
+    </row>
+    <row r="122" spans="1:13" s="4" customFormat="1" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A122" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B112" s="10" t="s">
+      <c r="B122" s="10" t="s">
         <v>197</v>
       </c>
-      <c r="C112" s="10" t="s">
+      <c r="C122" s="10" t="s">
         <v>205</v>
       </c>
-      <c r="D112" s="10" t="s">
+      <c r="D122" s="10" t="s">
         <v>204</v>
       </c>
-      <c r="E112" s="10" t="s">
+      <c r="E122" s="10" t="s">
         <v>206</v>
       </c>
-      <c r="F112" s="10" t="s">
+      <c r="F122" s="10" t="s">
         <v>203</v>
       </c>
-      <c r="G112" s="10" t="s">
+      <c r="G122" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="H112" s="10" t="s">
+      <c r="H122" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="I112" s="10" t="s">
+      <c r="I122" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="J112" s="10"/>
-      <c r="K112" s="10"/>
-      <c r="L112" s="10"/>
-      <c r="M112" s="10"/>
-    </row>
-    <row r="113" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A113" s="13" t="s">
+      <c r="J122" s="10"/>
+      <c r="K122" s="10"/>
+      <c r="L122" s="10"/>
+      <c r="M122" s="10"/>
+    </row>
+    <row r="123" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A123" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="B113" s="13" t="s">
+      <c r="B123" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="C113" s="13" t="s">
+      <c r="C123" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="D113" s="14">
+      <c r="D123" s="14">
         <v>49</v>
       </c>
-      <c r="E113" s="13" t="s">
+      <c r="E123" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="F113" s="13" t="s">
+      <c r="F123" s="13" t="s">
         <v>195</v>
       </c>
-      <c r="G113" s="14">
+      <c r="G123" s="14">
         <v>5</v>
       </c>
-      <c r="H113" s="14">
+      <c r="H123" s="14">
         <v>5</v>
       </c>
-      <c r="I113" s="13" t="s">
+      <c r="I123" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="J113" s="13"/>
-      <c r="K113" s="13"/>
-      <c r="L113" s="13"/>
-      <c r="M113" s="13"/>
-    </row>
-    <row r="114" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A114" s="11" t="s">
+      <c r="J123" s="13"/>
+      <c r="K123" s="13"/>
+      <c r="L123" s="13"/>
+      <c r="M123" s="13"/>
+    </row>
+    <row r="124" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A124" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="B114" s="11" t="s">
+      <c r="B124" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="C114" s="11" t="s">
+      <c r="C124" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="D114" s="12">
+      <c r="D124" s="12">
         <v>49</v>
       </c>
-      <c r="E114" s="11" t="s">
+      <c r="E124" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="F114" s="11" t="s">
+      <c r="F124" s="11" t="s">
         <v>195</v>
       </c>
-      <c r="G114" s="12">
+      <c r="G124" s="12">
         <v>5</v>
       </c>
-      <c r="H114" s="12">
+      <c r="H124" s="12">
         <v>5</v>
       </c>
-      <c r="I114" s="11" t="s">
+      <c r="I124" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="J114" s="11"/>
-      <c r="K114" s="11"/>
-      <c r="L114" s="11"/>
-      <c r="M114" s="11"/>
-    </row>
-    <row r="116" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A116" s="31" t="s">
+      <c r="J124" s="11"/>
+      <c r="K124" s="11"/>
+      <c r="L124" s="11"/>
+      <c r="M124" s="11"/>
+    </row>
+    <row r="126" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A126" s="38" t="s">
         <v>218</v>
       </c>
-      <c r="B116" s="31"/>
-      <c r="C116" s="31"/>
-      <c r="D116" s="31"/>
-      <c r="E116" s="31"/>
-      <c r="F116" s="31"/>
-      <c r="G116" s="31"/>
-      <c r="H116" s="31"/>
-      <c r="I116" s="31"/>
-      <c r="J116" s="31"/>
-      <c r="K116" s="31"/>
-      <c r="L116" s="31"/>
-      <c r="M116" s="31"/>
-    </row>
-    <row r="117" spans="1:13" s="3" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A117" s="32" t="s">
+      <c r="B126" s="38"/>
+      <c r="C126" s="38"/>
+      <c r="D126" s="38"/>
+      <c r="E126" s="38"/>
+      <c r="F126" s="38"/>
+      <c r="G126" s="38"/>
+      <c r="H126" s="38"/>
+      <c r="I126" s="38"/>
+      <c r="J126" s="38"/>
+      <c r="K126" s="38"/>
+      <c r="L126" s="38"/>
+      <c r="M126" s="38"/>
+    </row>
+    <row r="127" spans="1:13" s="3" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A127" s="31" t="s">
         <v>215</v>
       </c>
-      <c r="B117" s="32"/>
-      <c r="C117" s="32"/>
-      <c r="D117" s="32"/>
-      <c r="E117" s="32"/>
-      <c r="F117" s="32"/>
-      <c r="G117" s="32"/>
-      <c r="H117" s="32"/>
-      <c r="I117" s="32"/>
-      <c r="J117" s="32"/>
-      <c r="K117" s="32"/>
-      <c r="L117" s="32"/>
-      <c r="M117" s="32"/>
-    </row>
-    <row r="118" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A118" s="20" t="s">
+      <c r="B127" s="31"/>
+      <c r="C127" s="31"/>
+      <c r="D127" s="31"/>
+      <c r="E127" s="31"/>
+      <c r="F127" s="31"/>
+      <c r="G127" s="31"/>
+      <c r="H127" s="31"/>
+      <c r="I127" s="31"/>
+      <c r="J127" s="31"/>
+      <c r="K127" s="31"/>
+      <c r="L127" s="31"/>
+      <c r="M127" s="31"/>
+    </row>
+    <row r="128" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A128" s="33" t="s">
         <v>211</v>
       </c>
-      <c r="B118" s="20"/>
-      <c r="C118" s="20"/>
-      <c r="D118" s="20"/>
-      <c r="E118" s="20"/>
-      <c r="F118" s="20"/>
-      <c r="G118" s="20"/>
-      <c r="H118" s="20"/>
-      <c r="I118" s="20"/>
-      <c r="J118" s="20"/>
-      <c r="K118" s="20"/>
-      <c r="L118" s="20"/>
-      <c r="M118" s="20"/>
-    </row>
-    <row r="119" spans="1:13" s="4" customFormat="1" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A119" s="8" t="s">
+      <c r="B128" s="33"/>
+      <c r="C128" s="33"/>
+      <c r="D128" s="33"/>
+      <c r="E128" s="33"/>
+      <c r="F128" s="33"/>
+      <c r="G128" s="33"/>
+      <c r="H128" s="33"/>
+      <c r="I128" s="33"/>
+      <c r="J128" s="33"/>
+      <c r="K128" s="33"/>
+      <c r="L128" s="33"/>
+      <c r="M128" s="33"/>
+    </row>
+    <row r="129" spans="1:13" s="4" customFormat="1" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A129" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B119" s="8" t="s">
+      <c r="B129" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="C119" s="8" t="s">
+      <c r="C129" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="D119" s="8" t="s">
+      <c r="D129" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="E119" s="8"/>
-      <c r="F119" s="8"/>
-      <c r="G119" s="8"/>
-      <c r="H119" s="8"/>
-      <c r="I119" s="8"/>
-      <c r="J119" s="8"/>
-      <c r="K119" s="8"/>
-      <c r="L119" s="8"/>
-      <c r="M119" s="8"/>
-    </row>
-    <row r="120" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A120" s="16" t="s">
+      <c r="E129" s="8"/>
+      <c r="F129" s="8"/>
+      <c r="G129" s="8"/>
+      <c r="H129" s="8"/>
+      <c r="I129" s="8"/>
+      <c r="J129" s="8"/>
+      <c r="K129" s="8"/>
+      <c r="L129" s="8"/>
+      <c r="M129" s="8"/>
+    </row>
+    <row r="130" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A130" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="B120" s="16" t="s">
+      <c r="B130" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="C120" s="16" t="s">
+      <c r="C130" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="D120" s="16" t="s">
+      <c r="D130" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="E120" s="16"/>
-      <c r="F120" s="16"/>
-      <c r="G120" s="16"/>
-      <c r="H120" s="16"/>
-      <c r="I120" s="16"/>
-      <c r="J120" s="16"/>
-      <c r="K120" s="16"/>
-      <c r="L120" s="16"/>
-      <c r="M120" s="16"/>
-    </row>
-    <row r="121" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A121" s="17" t="s">
+      <c r="E130" s="16"/>
+      <c r="F130" s="16"/>
+      <c r="G130" s="16"/>
+      <c r="H130" s="16"/>
+      <c r="I130" s="16"/>
+      <c r="J130" s="16"/>
+      <c r="K130" s="16"/>
+      <c r="L130" s="16"/>
+      <c r="M130" s="16"/>
+    </row>
+    <row r="131" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A131" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="B121" s="17" t="s">
+      <c r="B131" s="17" t="s">
         <v>97</v>
       </c>
-      <c r="C121" s="17"/>
-      <c r="D121" s="17" t="s">
+      <c r="C131" s="17"/>
+      <c r="D131" s="17" t="s">
         <v>98</v>
       </c>
-      <c r="E121" s="17"/>
-      <c r="F121" s="17"/>
-      <c r="G121" s="17"/>
-      <c r="H121" s="17"/>
-      <c r="I121" s="17"/>
-      <c r="J121" s="17"/>
-      <c r="K121" s="17"/>
-      <c r="L121" s="17"/>
-      <c r="M121" s="17"/>
+      <c r="E131" s="17"/>
+      <c r="F131" s="17"/>
+      <c r="G131" s="17"/>
+      <c r="H131" s="17"/>
+      <c r="I131" s="17"/>
+      <c r="J131" s="17"/>
+      <c r="K131" s="17"/>
+      <c r="L131" s="17"/>
+      <c r="M131" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="54">
+  <mergeCells count="55">
+    <mergeCell ref="A64:P64"/>
+    <mergeCell ref="I65:J65"/>
+    <mergeCell ref="I66:J66"/>
+    <mergeCell ref="C89:E89"/>
+    <mergeCell ref="C91:E91"/>
+    <mergeCell ref="A83:M83"/>
+    <mergeCell ref="A68:M68"/>
+    <mergeCell ref="A73:M73"/>
+    <mergeCell ref="A78:M78"/>
+    <mergeCell ref="B76:C76"/>
+    <mergeCell ref="G65:H65"/>
+    <mergeCell ref="G66:H66"/>
+    <mergeCell ref="D75:E75"/>
+    <mergeCell ref="D76:E76"/>
+    <mergeCell ref="A126:M126"/>
+    <mergeCell ref="A127:M127"/>
+    <mergeCell ref="A128:M128"/>
+    <mergeCell ref="B84:C84"/>
+    <mergeCell ref="B85:C85"/>
+    <mergeCell ref="A88:M88"/>
+    <mergeCell ref="A93:M93"/>
+    <mergeCell ref="A99:M99"/>
+    <mergeCell ref="A100:M100"/>
+    <mergeCell ref="A94:M94"/>
+    <mergeCell ref="D84:F84"/>
+    <mergeCell ref="D85:F85"/>
+    <mergeCell ref="C90:E90"/>
+    <mergeCell ref="E65:F65"/>
+    <mergeCell ref="E66:F66"/>
+    <mergeCell ref="A119:M119"/>
+    <mergeCell ref="A121:M121"/>
+    <mergeCell ref="A120:M120"/>
+    <mergeCell ref="A112:M112"/>
+    <mergeCell ref="D74:E74"/>
+    <mergeCell ref="B74:C74"/>
+    <mergeCell ref="B75:C75"/>
+    <mergeCell ref="A106:M106"/>
+    <mergeCell ref="A110:M110"/>
+    <mergeCell ref="A111:M111"/>
+    <mergeCell ref="A113:M113"/>
+    <mergeCell ref="A118:M118"/>
+    <mergeCell ref="A87:M87"/>
+    <mergeCell ref="A49:M49"/>
+    <mergeCell ref="A57:M57"/>
+    <mergeCell ref="A58:M58"/>
+    <mergeCell ref="A63:P63"/>
+    <mergeCell ref="A53:M53"/>
     <mergeCell ref="A5:M5"/>
     <mergeCell ref="A1:M1"/>
+    <mergeCell ref="A33:M33"/>
+    <mergeCell ref="A44:M44"/>
+    <mergeCell ref="A48:M48"/>
+    <mergeCell ref="A6:M6"/>
+    <mergeCell ref="A34:M34"/>
     <mergeCell ref="A23:M23"/>
-    <mergeCell ref="A34:M34"/>
-    <mergeCell ref="A38:M38"/>
-    <mergeCell ref="A6:M6"/>
-    <mergeCell ref="A24:M24"/>
-    <mergeCell ref="A39:M39"/>
-    <mergeCell ref="A47:M47"/>
-    <mergeCell ref="A48:M48"/>
-    <mergeCell ref="A53:P53"/>
-    <mergeCell ref="A43:M43"/>
-    <mergeCell ref="E55:F55"/>
-    <mergeCell ref="E56:F56"/>
-    <mergeCell ref="A109:M109"/>
-    <mergeCell ref="A111:M111"/>
-    <mergeCell ref="A110:M110"/>
-    <mergeCell ref="A102:M102"/>
-    <mergeCell ref="D64:E64"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="A96:M96"/>
-    <mergeCell ref="A100:M100"/>
-    <mergeCell ref="A101:M101"/>
-    <mergeCell ref="A103:M103"/>
-    <mergeCell ref="A108:M108"/>
-    <mergeCell ref="A77:M77"/>
-    <mergeCell ref="A116:M116"/>
-    <mergeCell ref="A117:M117"/>
-    <mergeCell ref="A118:M118"/>
-    <mergeCell ref="B74:C74"/>
-    <mergeCell ref="B75:C75"/>
-    <mergeCell ref="A78:M78"/>
-    <mergeCell ref="A83:M83"/>
-    <mergeCell ref="A89:M89"/>
-    <mergeCell ref="A90:M90"/>
-    <mergeCell ref="A84:M84"/>
-    <mergeCell ref="D74:F74"/>
-    <mergeCell ref="D75:F75"/>
-    <mergeCell ref="C80:E80"/>
-    <mergeCell ref="A54:P54"/>
-    <mergeCell ref="I55:J55"/>
-    <mergeCell ref="I56:J56"/>
-    <mergeCell ref="C79:E79"/>
-    <mergeCell ref="C81:E81"/>
-    <mergeCell ref="A73:M73"/>
-    <mergeCell ref="A58:M58"/>
-    <mergeCell ref="A63:M63"/>
-    <mergeCell ref="A68:M68"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="G55:H55"/>
-    <mergeCell ref="G56:H56"/>
-    <mergeCell ref="D65:E65"/>
-    <mergeCell ref="D66:E66"/>
   </mergeCells>
-  <dataValidations count="50">
+  <dataValidations count="52">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A3" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"inband_vlan"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E8:E21" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"unspecified,remote-leaf-wan"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G8:G21" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G8:G21 G25:G31" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>switch_role</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H8:H21" xr:uid="{00000000-0002-0000-0000-000003000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H8:H21 H25:H31" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>INDIRECT(G8)</formula1>
     </dataValidation>
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Inband VLAN" error="VLAN must be between 5 and 3097" sqref="B3" xr:uid="{00000000-0002-0000-0000-000004000000}">
       <formula1>5</formula1>
       <formula2>3097</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Node ID" error="Valid Node ID is between 101 and 4000" sqref="C41 D8:D21" xr:uid="{00000000-0002-0000-0000-000005000000}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Node ID" error="Valid Node ID is between 101 and 4000" sqref="C51 D8:D21 D25:E31" xr:uid="{00000000-0002-0000-0000-000005000000}">
       <formula1>101</formula1>
       <formula2>4000</formula2>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A8:A21" xr:uid="{00000000-0002-0000-0000-000006000000}">
       <formula1>"switch"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A26:A32" xr:uid="{00000000-0002-0000-0000-000007000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A36:A42" xr:uid="{00000000-0002-0000-0000-000007000000}">
       <formula1>"apic_inb"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A36" xr:uid="{00000000-0002-0000-0000-000008000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A46" xr:uid="{00000000-0002-0000-0000-000008000000}">
       <formula1>"bgp_as"</formula1>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="BGP ASN" error="BGP ASN Must be between 1 and 4294967295" sqref="B36" xr:uid="{00000000-0002-0000-0000-000009000000}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="BGP ASN" error="BGP ASN Must be between 1 and 4294967295" sqref="B46" xr:uid="{00000000-0002-0000-0000-000009000000}">
       <formula1>1</formula1>
       <formula2>4294967295</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Pod ID" error="Pod Id must be between 1 and 12!" sqref="D26:D32 F8:F21" xr:uid="{00000000-0002-0000-0000-00000A000000}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Pod ID" error="Pod Id must be between 1 and 12!" sqref="D36:D42 F8:F21 F25:F31" xr:uid="{00000000-0002-0000-0000-00000A000000}">
       <formula1>1</formula1>
       <formula2>12</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="APIC Node ID" error="APIC Node ID must be between 1 and 7" sqref="C26:C32" xr:uid="{00000000-0002-0000-0000-00000B000000}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="APIC Node ID" error="APIC Node ID must be between 1 and 7" sqref="C36:C42" xr:uid="{00000000-0002-0000-0000-00000B000000}">
       <formula1>1</formula1>
       <formula2>7</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A41" xr:uid="{00000000-0002-0000-0000-00000C000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A51" xr:uid="{00000000-0002-0000-0000-00000C000000}">
       <formula1>"bgp_rr"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B45 D60:D61 D70:D71 G86:G87 D98 I105:I106 I113:I114 D56" xr:uid="{00000000-0002-0000-0000-00000D000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B55 D70:D71 D80:D81 G96:G97 D108 I115:I116 I123:I124 D66" xr:uid="{00000000-0002-0000-0000-00000D000000}">
       <formula1>"inband,oob"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A45" xr:uid="{00000000-0002-0000-0000-00000E000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A55" xr:uid="{00000000-0002-0000-0000-00000E000000}">
       <formula1>"dns_mgmt"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A50:A51" xr:uid="{00000000-0002-0000-0000-00000F000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A60:A61" xr:uid="{00000000-0002-0000-0000-00000F000000}">
       <formula1>"dns"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C50:C51 D65:D66" xr:uid="{00000000-0002-0000-0000-000010000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C60:C61 D75:D76" xr:uid="{00000000-0002-0000-0000-000010000000}">
       <formula1>"no,yes"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A56" xr:uid="{00000000-0002-0000-0000-000011000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A66" xr:uid="{00000000-0002-0000-0000-000011000000}">
       <formula1>"smartcallhome"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C60:C61" xr:uid="{00000000-0002-0000-0000-000012000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C70:C71" xr:uid="{00000000-0002-0000-0000-000012000000}">
       <formula1>"false,true"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A65:A66" xr:uid="{00000000-0002-0000-0000-000013000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A75:A76" xr:uid="{00000000-0002-0000-0000-000013000000}">
       <formula1>"search_domain"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A60:A61" xr:uid="{00000000-0002-0000-0000-000014000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A70:A71" xr:uid="{00000000-0002-0000-0000-000014000000}">
       <formula1>"ntp"</formula1>
     </dataValidation>
-    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Community String" error="The SNMP Community can be 1 to 32 characters and contain letters, numbers, and [.\-]. No other special characters" sqref="B80:B81" xr:uid="{00000000-0002-0000-0000-000015000000}">
+    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Community String" error="The SNMP Community can be 1 to 32 characters and contain letters, numbers, and [.\-]. No other special characters" sqref="B90:B91" xr:uid="{00000000-0002-0000-0000-000015000000}">
       <formula1>1</formula1>
       <formula2>32</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A75" xr:uid="{00000000-0002-0000-0000-000016000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A85" xr:uid="{00000000-0002-0000-0000-000016000000}">
       <formula1>"snmp_info"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A80:A81" xr:uid="{00000000-0002-0000-0000-000017000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A90:A91" xr:uid="{00000000-0002-0000-0000-000017000000}">
       <formula1>"snmp_comm"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C92:C94" xr:uid="{00000000-0002-0000-0000-000018000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C102:C104" xr:uid="{00000000-0002-0000-0000-000018000000}">
       <formula1>"aes-128,des,none"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E92:E94" xr:uid="{00000000-0002-0000-0000-000019000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E102:E104" xr:uid="{00000000-0002-0000-0000-000019000000}">
       <formula1>"md5,sha1"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D86:D87" xr:uid="{00000000-0002-0000-0000-00001A000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D96:D97" xr:uid="{00000000-0002-0000-0000-00001A000000}">
       <formula1>"v1,v2c,v3"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A92:A94" xr:uid="{00000000-0002-0000-0000-00001B000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A102:A104" xr:uid="{00000000-0002-0000-0000-00001B000000}">
       <formula1>"snmp_user"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E98 H98" xr:uid="{00000000-0002-0000-0000-00001C000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E108 H108" xr:uid="{00000000-0002-0000-0000-00001C000000}">
       <formula1>"emergencies,alerts,critical,errors,warnings,notifications,information,debugging"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F98" xr:uid="{00000000-0002-0000-0000-00001D000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F108" xr:uid="{00000000-0002-0000-0000-00001D000000}">
       <formula1>"local0,local1,local2,local3,local4,local5,local6,local7"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G98 I98" xr:uid="{00000000-0002-0000-0000-00001E000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G108 I108" xr:uid="{00000000-0002-0000-0000-00001E000000}">
       <formula1>"enabled,disabled"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J98" xr:uid="{00000000-0002-0000-0000-00001F000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J108" xr:uid="{00000000-0002-0000-0000-00001F000000}">
       <formula1>"emergencies,alerts,critical"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A98" xr:uid="{00000000-0002-0000-0000-000020000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A108" xr:uid="{00000000-0002-0000-0000-000020000000}">
       <formula1>"syslog"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F105:F106 F113:F114" xr:uid="{00000000-0002-0000-0000-000021000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F115:F116 F123:F124" xr:uid="{00000000-0002-0000-0000-000021000000}">
       <formula1>"chap,mschap,pap"</formula1>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="RADIUS Timeout" error="Timeout should be between 5 and 60 and be a Factor of 5.  Default is 5" sqref="G105:G106" xr:uid="{00000000-0002-0000-0000-000022000000}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="RADIUS Timeout" error="Timeout should be between 5 and 60 and be a Factor of 5.  Default is 5" sqref="G115:G116" xr:uid="{00000000-0002-0000-0000-000022000000}">
       <formula1>5</formula1>
       <formula2>60</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="RADIUS Retry" error="Retry should be a number between 1 and 5.  Default is 1" sqref="H105:H106" xr:uid="{00000000-0002-0000-0000-000023000000}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="RADIUS Retry" error="Retry should be a number between 1 and 5.  Default is 1" sqref="H115:H116" xr:uid="{00000000-0002-0000-0000-000023000000}">
       <formula1>1</formula1>
       <formula2>5</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="TACACS Timeout" error="Timeout should be between 5 and 60 and be a Factor of 5.  Default is 5" sqref="G113:G114" xr:uid="{00000000-0002-0000-0000-000024000000}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="TACACS Timeout" error="Timeout should be between 5 and 60 and be a Factor of 5.  Default is 5" sqref="G123:G124" xr:uid="{00000000-0002-0000-0000-000024000000}">
       <formula1>5</formula1>
       <formula2>60</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="TACACS Retry" error="Retry should be a number between 1 and 5.  Default is 1" sqref="H113:H114" xr:uid="{00000000-0002-0000-0000-000025000000}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="TACACS Retry" error="Retry should be a number between 1 and 5.  Default is 1" sqref="H123:H124" xr:uid="{00000000-0002-0000-0000-000025000000}">
       <formula1>1</formula1>
       <formula2>5</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Syslog Port" error="Valid Port Range is between 1 and 65535.  Default is 514" sqref="C98" xr:uid="{00000000-0002-0000-0000-000026000000}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Syslog Port" error="Valid Port Range is between 1 and 65535.  Default is 514" sqref="C108" xr:uid="{00000000-0002-0000-0000-000026000000}">
       <formula1>1</formula1>
       <formula2>65535</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="RADIUS Port" error="Valid Port Range is between 1 and 65535. Default is 1812" sqref="D105:D106" xr:uid="{00000000-0002-0000-0000-000027000000}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="RADIUS Port" error="Valid Port Range is between 1 and 65535. Default is 1812" sqref="D115:D116" xr:uid="{00000000-0002-0000-0000-000027000000}">
       <formula1>1</formula1>
       <formula2>65535</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="TACACS Port" error="Valid Port Range is between 1 and 65535. Default is 49" sqref="D113:D114" xr:uid="{00000000-0002-0000-0000-000028000000}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="TACACS Port" error="Valid Port Range is between 1 and 65535. Default is 49" sqref="D123:D124" xr:uid="{00000000-0002-0000-0000-000028000000}">
       <formula1>1</formula1>
       <formula2>65535</formula2>
     </dataValidation>
-    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Login Domain" error="Maximum length is 10 Alpha Numberic Characters or an underscore &quot;_&quot;.  But it must not begin with a underscore &quot;_&quot;." sqref="B113:B114" xr:uid="{00000000-0002-0000-0000-000029000000}">
+    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Login Domain" error="Maximum length is 10 Alpha Numberic Characters or an underscore &quot;_&quot;.  But it must not begin with a underscore &quot;_&quot;." sqref="B123:B124" xr:uid="{00000000-0002-0000-0000-000029000000}">
       <formula1>1</formula1>
       <formula2>10</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A113:A114" xr:uid="{00000000-0002-0000-0000-00002A000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A123:A124" xr:uid="{00000000-0002-0000-0000-00002A000000}">
       <formula1>"tacacs"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A105:A106" xr:uid="{00000000-0002-0000-0000-00002B000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A115:A116" xr:uid="{00000000-0002-0000-0000-00002B000000}">
       <formula1>"radius"</formula1>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SNMP Trap Port" error="Valid Port Range is between 1 and 65535.  Default is 162" sqref="C86:C87" xr:uid="{00000000-0002-0000-0000-00002C000000}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SNMP Trap Port" error="Valid Port Range is between 1 and 65535.  Default is 162" sqref="C96:C97" xr:uid="{00000000-0002-0000-0000-00002C000000}">
       <formula1>1</formula1>
       <formula2>65535</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A86:A87" xr:uid="{00000000-0002-0000-0000-00002D000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A96:A97" xr:uid="{00000000-0002-0000-0000-00002D000000}">
       <formula1>"snmp_trap"</formula1>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SMTP Port" error="Valid Port Range is between 1 and 65535.  Default is 25" sqref="B56" xr:uid="{00000000-0002-0000-0000-00002E000000}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SMTP Port" error="Valid Port Range is between 1 and 65535.  Default is 25" sqref="B66" xr:uid="{00000000-0002-0000-0000-00002E000000}">
       <formula1>1</formula1>
       <formula2>65535</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Login Domain Type" error="The Login Domain Type can be [local|ldap|radius|tacacs|rsa|saml].  SAML is not supported for Console Authentication" sqref="D120:D121" xr:uid="{00000000-0002-0000-0000-00002F000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Login Domain Type" error="The Login Domain Type can be [local|ldap|radius|tacacs|rsa|saml].  SAML is not supported for Console Authentication" sqref="D130:D131" xr:uid="{00000000-0002-0000-0000-00002F000000}">
       <formula1>"local,ldap,radius,tacacs,rsa,saml"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B120:B121" xr:uid="{00000000-0002-0000-0000-000030000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B130:B131" xr:uid="{00000000-0002-0000-0000-000030000000}">
       <formula1>"console,default"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A120:A121" xr:uid="{00000000-0002-0000-0000-000031000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A130:A131" xr:uid="{00000000-0002-0000-0000-000031000000}">
       <formula1>"realm"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A25:A31" xr:uid="{A2F55667-432D-4009-90B0-3CBF96713B99}">
+      <formula1>"vpc_pair"</formula1>
+    </dataValidation>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="VPC ID" error="The VPC ID must be a number between 1 and 1000" sqref="B25:B31" xr:uid="{2DB049D3-4D1F-4770-AA8C-B1564D6B004B}">
+      <formula1>1</formula1>
+      <formula2>1000</formula2>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
modified OOB IPv4 to be Optional
</commit_message>
<xml_diff>
--- a/Terraform/aci/base-configs/aci-fabric-deploy-Input-Spreadsheet.xlsx
+++ b/Terraform/aci/base-configs/aci-fabric-deploy-Input-Spreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\tyscott\terraform-aci-fabric-deploy\Terraform\aci\base-configs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ADCB25F-03E5-4431-9FFA-05C59423E1C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{710CA232-1FD5-4857-800D-E8EE3501BBA6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="226">
   <si>
     <t>Type</t>
   </si>
@@ -864,18 +864,12 @@
     <t>is it needed, I don't know</t>
   </si>
   <si>
-    <t>VPC Pairs</t>
-  </si>
-  <si>
     <t>vpc_pair</t>
   </si>
   <si>
     <t>VPC ID</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
     <t>Node ID 1</t>
   </si>
   <si>
@@ -883,6 +877,9 @@
   </si>
   <si>
     <t>leaf201-202-vpc</t>
+  </si>
+  <si>
+    <t>VPC Pairs - It is Recommended to use the 1st Node Id for the VPC ID unless you are using Node ID's &gt; 1000</t>
   </si>
 </sst>
 </file>
@@ -1708,19 +1705,7 @@
     <xf numFmtId="49" fontId="20" fillId="34" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="17" fillId="33" borderId="8" xfId="2" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="33" borderId="8" xfId="2" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="34" borderId="8" xfId="3" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="34" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="33" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="18" fillId="34" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="18" fillId="0" borderId="25" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1729,55 +1714,19 @@
     <xf numFmtId="49" fontId="18" fillId="0" borderId="26" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="20" fillId="34" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="20" fillId="34" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="20" fillId="34" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="34" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="34" borderId="8" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="34" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="20" fillId="34" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="18" fillId="0" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="16" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="20" fillId="34" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="20" fillId="34" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="36" borderId="8" xfId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="18" fillId="0" borderId="11" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="20" fillId="34" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="20" fillId="34" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="20" fillId="34" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="20" fillId="34" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="20" fillId="34" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="20" fillId="34" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="16" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="20" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1789,11 +1738,59 @@
     <xf numFmtId="49" fontId="20" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="17" fillId="33" borderId="8" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="20" fillId="34" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="20" fillId="34" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="1" fontId="20" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="20" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="36" borderId="8" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="34" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="20" fillId="34" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="20" fillId="34" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="34" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="33" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="20" fillId="34" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="20" fillId="34" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="20" fillId="34" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="20" fillId="34" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="34" borderId="8" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="33" borderId="8" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="34" borderId="8" xfId="3" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -2153,8 +2150,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2179,21 +2176,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="6" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="49" t="s">
         <v>99</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22"/>
-      <c r="M1" s="22"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="49"/>
+      <c r="J1" s="49"/>
+      <c r="K1" s="49"/>
+      <c r="L1" s="49"/>
+      <c r="M1" s="49"/>
     </row>
     <row r="2" spans="1:13" s="3" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
@@ -2234,38 +2231,38 @@
       <c r="M3" s="13"/>
     </row>
     <row r="5" spans="1:13" s="6" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="49" t="s">
         <v>109</v>
       </c>
-      <c r="B5" s="22"/>
-      <c r="C5" s="22"/>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22"/>
-      <c r="F5" s="22"/>
-      <c r="G5" s="22"/>
-      <c r="H5" s="22"/>
-      <c r="I5" s="22"/>
-      <c r="J5" s="22"/>
-      <c r="K5" s="22"/>
-      <c r="L5" s="22"/>
-      <c r="M5" s="22"/>
+      <c r="B5" s="49"/>
+      <c r="C5" s="49"/>
+      <c r="D5" s="49"/>
+      <c r="E5" s="49"/>
+      <c r="F5" s="49"/>
+      <c r="G5" s="49"/>
+      <c r="H5" s="49"/>
+      <c r="I5" s="49"/>
+      <c r="J5" s="49"/>
+      <c r="K5" s="49"/>
+      <c r="L5" s="49"/>
+      <c r="M5" s="49"/>
     </row>
     <row r="6" spans="1:13" s="6" customFormat="1" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="50" t="s">
         <v>149</v>
       </c>
-      <c r="B6" s="24"/>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="24"/>
-      <c r="I6" s="24"/>
-      <c r="J6" s="24"/>
-      <c r="K6" s="24"/>
-      <c r="L6" s="24"/>
-      <c r="M6" s="24"/>
+      <c r="B6" s="50"/>
+      <c r="C6" s="50"/>
+      <c r="D6" s="50"/>
+      <c r="E6" s="50"/>
+      <c r="F6" s="50"/>
+      <c r="G6" s="50"/>
+      <c r="H6" s="50"/>
+      <c r="I6" s="50"/>
+      <c r="J6" s="50"/>
+      <c r="K6" s="50"/>
+      <c r="L6" s="50"/>
+      <c r="M6" s="50"/>
     </row>
     <row r="7" spans="1:13" s="3" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
@@ -2589,37 +2586,37 @@
       <c r="M21" s="11"/>
     </row>
     <row r="23" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="22" t="s">
-        <v>220</v>
-      </c>
-      <c r="B23" s="22"/>
-      <c r="C23" s="22"/>
-      <c r="D23" s="22"/>
-      <c r="E23" s="22"/>
-      <c r="F23" s="22"/>
-      <c r="G23" s="22"/>
-      <c r="H23" s="22"/>
-      <c r="I23" s="22"/>
-      <c r="J23" s="22"/>
-      <c r="K23" s="22"/>
-      <c r="L23" s="22"/>
-      <c r="M23" s="22"/>
+      <c r="A23" s="49" t="s">
+        <v>225</v>
+      </c>
+      <c r="B23" s="49"/>
+      <c r="C23" s="49"/>
+      <c r="D23" s="49"/>
+      <c r="E23" s="49"/>
+      <c r="F23" s="49"/>
+      <c r="G23" s="49"/>
+      <c r="H23" s="49"/>
+      <c r="I23" s="49"/>
+      <c r="J23" s="49"/>
+      <c r="K23" s="49"/>
+      <c r="L23" s="49"/>
+      <c r="M23" s="49"/>
     </row>
     <row r="24" spans="1:13" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C24" s="8" t="s">
         <v>3</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="F24" s="8"/>
       <c r="G24" s="8"/>
@@ -2632,13 +2629,13 @@
     </row>
     <row r="25" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="13" t="s">
-        <v>221</v>
-      </c>
-      <c r="B25" s="13" t="s">
-        <v>223</v>
+        <v>220</v>
+      </c>
+      <c r="B25" s="14">
+        <v>201</v>
       </c>
       <c r="C25" s="13" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D25" s="14">
         <v>201</v>
@@ -2657,7 +2654,7 @@
     </row>
     <row r="26" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="11"/>
-      <c r="B26" s="11"/>
+      <c r="B26" s="12"/>
       <c r="C26" s="11"/>
       <c r="D26" s="12"/>
       <c r="E26" s="12"/>
@@ -2672,7 +2669,7 @@
     </row>
     <row r="27" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="13"/>
-      <c r="B27" s="13"/>
+      <c r="B27" s="14"/>
       <c r="C27" s="13"/>
       <c r="D27" s="14"/>
       <c r="E27" s="14"/>
@@ -2687,7 +2684,7 @@
     </row>
     <row r="28" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="11"/>
-      <c r="B28" s="11"/>
+      <c r="B28" s="12"/>
       <c r="C28" s="11"/>
       <c r="D28" s="12"/>
       <c r="E28" s="12"/>
@@ -2702,7 +2699,7 @@
     </row>
     <row r="29" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="13"/>
-      <c r="B29" s="13"/>
+      <c r="B29" s="14"/>
       <c r="C29" s="13"/>
       <c r="D29" s="14"/>
       <c r="E29" s="14"/>
@@ -2717,7 +2714,7 @@
     </row>
     <row r="30" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="11"/>
-      <c r="B30" s="11"/>
+      <c r="B30" s="12"/>
       <c r="C30" s="11"/>
       <c r="D30" s="12"/>
       <c r="E30" s="12"/>
@@ -2732,7 +2729,7 @@
     </row>
     <row r="31" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="13"/>
-      <c r="B31" s="13"/>
+      <c r="B31" s="14"/>
       <c r="C31" s="13"/>
       <c r="D31" s="14"/>
       <c r="E31" s="14"/>
@@ -2746,38 +2743,38 @@
       <c r="M31" s="13"/>
     </row>
     <row r="33" spans="1:13" s="6" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="22" t="s">
+      <c r="A33" s="49" t="s">
         <v>141</v>
       </c>
-      <c r="B33" s="22"/>
-      <c r="C33" s="22"/>
-      <c r="D33" s="22"/>
-      <c r="E33" s="22"/>
-      <c r="F33" s="22"/>
-      <c r="G33" s="22"/>
-      <c r="H33" s="22"/>
-      <c r="I33" s="22"/>
-      <c r="J33" s="22"/>
-      <c r="K33" s="22"/>
-      <c r="L33" s="22"/>
-      <c r="M33" s="22"/>
+      <c r="B33" s="49"/>
+      <c r="C33" s="49"/>
+      <c r="D33" s="49"/>
+      <c r="E33" s="49"/>
+      <c r="F33" s="49"/>
+      <c r="G33" s="49"/>
+      <c r="H33" s="49"/>
+      <c r="I33" s="49"/>
+      <c r="J33" s="49"/>
+      <c r="K33" s="49"/>
+      <c r="L33" s="49"/>
+      <c r="M33" s="49"/>
     </row>
     <row r="34" spans="1:13" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="25" t="s">
+      <c r="A34" s="42" t="s">
         <v>143</v>
       </c>
-      <c r="B34" s="25"/>
-      <c r="C34" s="25"/>
-      <c r="D34" s="25"/>
-      <c r="E34" s="25"/>
-      <c r="F34" s="25"/>
-      <c r="G34" s="25"/>
-      <c r="H34" s="25"/>
-      <c r="I34" s="25"/>
-      <c r="J34" s="25"/>
-      <c r="K34" s="25"/>
-      <c r="L34" s="25"/>
-      <c r="M34" s="25"/>
+      <c r="B34" s="42"/>
+      <c r="C34" s="42"/>
+      <c r="D34" s="42"/>
+      <c r="E34" s="42"/>
+      <c r="F34" s="42"/>
+      <c r="G34" s="42"/>
+      <c r="H34" s="42"/>
+      <c r="I34" s="42"/>
+      <c r="J34" s="42"/>
+      <c r="K34" s="42"/>
+      <c r="L34" s="42"/>
+      <c r="M34" s="42"/>
     </row>
     <row r="35" spans="1:13" s="3" customFormat="1" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="8" t="s">
@@ -2940,21 +2937,21 @@
       <c r="M42" s="13"/>
     </row>
     <row r="44" spans="1:13" s="6" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="22" t="s">
+      <c r="A44" s="49" t="s">
         <v>140</v>
       </c>
-      <c r="B44" s="22"/>
-      <c r="C44" s="22"/>
-      <c r="D44" s="22"/>
-      <c r="E44" s="22"/>
-      <c r="F44" s="22"/>
-      <c r="G44" s="22"/>
-      <c r="H44" s="22"/>
-      <c r="I44" s="22"/>
-      <c r="J44" s="22"/>
-      <c r="K44" s="22"/>
-      <c r="L44" s="22"/>
-      <c r="M44" s="22"/>
+      <c r="B44" s="49"/>
+      <c r="C44" s="49"/>
+      <c r="D44" s="49"/>
+      <c r="E44" s="49"/>
+      <c r="F44" s="49"/>
+      <c r="G44" s="49"/>
+      <c r="H44" s="49"/>
+      <c r="I44" s="49"/>
+      <c r="J44" s="49"/>
+      <c r="K44" s="49"/>
+      <c r="L44" s="49"/>
+      <c r="M44" s="49"/>
     </row>
     <row r="45" spans="1:13" s="3" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="8" t="s">
@@ -2995,38 +2992,38 @@
       <c r="M46" s="13"/>
     </row>
     <row r="48" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="23" t="s">
+      <c r="A48" s="33" t="s">
         <v>142</v>
       </c>
-      <c r="B48" s="23"/>
-      <c r="C48" s="23"/>
-      <c r="D48" s="23"/>
-      <c r="E48" s="23"/>
-      <c r="F48" s="23"/>
-      <c r="G48" s="23"/>
-      <c r="H48" s="23"/>
-      <c r="I48" s="23"/>
-      <c r="J48" s="23"/>
-      <c r="K48" s="23"/>
-      <c r="L48" s="23"/>
-      <c r="M48" s="23"/>
+      <c r="B48" s="33"/>
+      <c r="C48" s="33"/>
+      <c r="D48" s="33"/>
+      <c r="E48" s="33"/>
+      <c r="F48" s="33"/>
+      <c r="G48" s="33"/>
+      <c r="H48" s="33"/>
+      <c r="I48" s="33"/>
+      <c r="J48" s="33"/>
+      <c r="K48" s="33"/>
+      <c r="L48" s="33"/>
+      <c r="M48" s="33"/>
     </row>
     <row r="49" spans="1:16" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="25" t="s">
+      <c r="A49" s="42" t="s">
         <v>144</v>
       </c>
-      <c r="B49" s="25"/>
-      <c r="C49" s="25"/>
-      <c r="D49" s="25"/>
-      <c r="E49" s="25"/>
-      <c r="F49" s="25"/>
-      <c r="G49" s="25"/>
-      <c r="H49" s="25"/>
-      <c r="I49" s="25"/>
-      <c r="J49" s="25"/>
-      <c r="K49" s="25"/>
-      <c r="L49" s="25"/>
-      <c r="M49" s="25"/>
+      <c r="B49" s="42"/>
+      <c r="C49" s="42"/>
+      <c r="D49" s="42"/>
+      <c r="E49" s="42"/>
+      <c r="F49" s="42"/>
+      <c r="G49" s="42"/>
+      <c r="H49" s="42"/>
+      <c r="I49" s="42"/>
+      <c r="J49" s="42"/>
+      <c r="K49" s="42"/>
+      <c r="L49" s="42"/>
+      <c r="M49" s="42"/>
     </row>
     <row r="50" spans="1:16" s="3" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="8" t="s">
@@ -3071,21 +3068,21 @@
       <c r="M51" s="13"/>
     </row>
     <row r="53" spans="1:16" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="23" t="s">
+      <c r="A53" s="33" t="s">
         <v>145</v>
       </c>
-      <c r="B53" s="23"/>
-      <c r="C53" s="23"/>
-      <c r="D53" s="23"/>
-      <c r="E53" s="23"/>
-      <c r="F53" s="23"/>
-      <c r="G53" s="23"/>
-      <c r="H53" s="23"/>
-      <c r="I53" s="23"/>
-      <c r="J53" s="23"/>
-      <c r="K53" s="23"/>
-      <c r="L53" s="23"/>
-      <c r="M53" s="23"/>
+      <c r="B53" s="33"/>
+      <c r="C53" s="33"/>
+      <c r="D53" s="33"/>
+      <c r="E53" s="33"/>
+      <c r="F53" s="33"/>
+      <c r="G53" s="33"/>
+      <c r="H53" s="33"/>
+      <c r="I53" s="33"/>
+      <c r="J53" s="33"/>
+      <c r="K53" s="33"/>
+      <c r="L53" s="33"/>
+      <c r="M53" s="33"/>
     </row>
     <row r="54" spans="1:16" s="3" customFormat="1" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="8" t="s">
@@ -3126,38 +3123,38 @@
       <c r="M55" s="13"/>
     </row>
     <row r="57" spans="1:16" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="23" t="s">
+      <c r="A57" s="33" t="s">
         <v>146</v>
       </c>
-      <c r="B57" s="23"/>
-      <c r="C57" s="23"/>
-      <c r="D57" s="23"/>
-      <c r="E57" s="23"/>
-      <c r="F57" s="23"/>
-      <c r="G57" s="23"/>
-      <c r="H57" s="23"/>
-      <c r="I57" s="23"/>
-      <c r="J57" s="23"/>
-      <c r="K57" s="23"/>
-      <c r="L57" s="23"/>
-      <c r="M57" s="23"/>
+      <c r="B57" s="33"/>
+      <c r="C57" s="33"/>
+      <c r="D57" s="33"/>
+      <c r="E57" s="33"/>
+      <c r="F57" s="33"/>
+      <c r="G57" s="33"/>
+      <c r="H57" s="33"/>
+      <c r="I57" s="33"/>
+      <c r="J57" s="33"/>
+      <c r="K57" s="33"/>
+      <c r="L57" s="33"/>
+      <c r="M57" s="33"/>
     </row>
     <row r="58" spans="1:16" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="25" t="s">
+      <c r="A58" s="42" t="s">
         <v>147</v>
       </c>
-      <c r="B58" s="25"/>
-      <c r="C58" s="25"/>
-      <c r="D58" s="25"/>
-      <c r="E58" s="25"/>
-      <c r="F58" s="25"/>
-      <c r="G58" s="25"/>
-      <c r="H58" s="25"/>
-      <c r="I58" s="25"/>
-      <c r="J58" s="25"/>
-      <c r="K58" s="25"/>
-      <c r="L58" s="25"/>
-      <c r="M58" s="25"/>
+      <c r="B58" s="42"/>
+      <c r="C58" s="42"/>
+      <c r="D58" s="42"/>
+      <c r="E58" s="42"/>
+      <c r="F58" s="42"/>
+      <c r="G58" s="42"/>
+      <c r="H58" s="42"/>
+      <c r="I58" s="42"/>
+      <c r="J58" s="42"/>
+      <c r="K58" s="42"/>
+      <c r="L58" s="42"/>
+      <c r="M58" s="42"/>
     </row>
     <row r="59" spans="1:16" s="3" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="8" t="s">
@@ -3223,44 +3220,44 @@
       <c r="M61" s="11"/>
     </row>
     <row r="63" spans="1:16" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="26" t="s">
+      <c r="A63" s="43" t="s">
         <v>148</v>
       </c>
-      <c r="B63" s="26"/>
-      <c r="C63" s="26"/>
-      <c r="D63" s="26"/>
-      <c r="E63" s="26"/>
-      <c r="F63" s="26"/>
-      <c r="G63" s="26"/>
-      <c r="H63" s="26"/>
-      <c r="I63" s="26"/>
-      <c r="J63" s="26"/>
-      <c r="K63" s="26"/>
-      <c r="L63" s="26"/>
-      <c r="M63" s="26"/>
-      <c r="N63" s="26"/>
-      <c r="O63" s="26"/>
-      <c r="P63" s="26"/>
+      <c r="B63" s="43"/>
+      <c r="C63" s="43"/>
+      <c r="D63" s="43"/>
+      <c r="E63" s="43"/>
+      <c r="F63" s="43"/>
+      <c r="G63" s="43"/>
+      <c r="H63" s="43"/>
+      <c r="I63" s="43"/>
+      <c r="J63" s="43"/>
+      <c r="K63" s="43"/>
+      <c r="L63" s="43"/>
+      <c r="M63" s="43"/>
+      <c r="N63" s="43"/>
+      <c r="O63" s="43"/>
+      <c r="P63" s="43"/>
     </row>
     <row r="64" spans="1:16" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="33" t="s">
+      <c r="A64" s="22" t="s">
         <v>170</v>
       </c>
-      <c r="B64" s="33"/>
-      <c r="C64" s="33"/>
-      <c r="D64" s="33"/>
-      <c r="E64" s="33"/>
-      <c r="F64" s="33"/>
-      <c r="G64" s="33"/>
-      <c r="H64" s="33"/>
-      <c r="I64" s="33"/>
-      <c r="J64" s="33"/>
-      <c r="K64" s="33"/>
-      <c r="L64" s="33"/>
-      <c r="M64" s="33"/>
-      <c r="N64" s="33"/>
-      <c r="O64" s="33"/>
-      <c r="P64" s="33"/>
+      <c r="B64" s="22"/>
+      <c r="C64" s="22"/>
+      <c r="D64" s="22"/>
+      <c r="E64" s="22"/>
+      <c r="F64" s="22"/>
+      <c r="G64" s="22"/>
+      <c r="H64" s="22"/>
+      <c r="I64" s="22"/>
+      <c r="J64" s="22"/>
+      <c r="K64" s="22"/>
+      <c r="L64" s="22"/>
+      <c r="M64" s="22"/>
+      <c r="N64" s="22"/>
+      <c r="O64" s="22"/>
+      <c r="P64" s="22"/>
     </row>
     <row r="65" spans="1:16" s="3" customFormat="1" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="8" t="s">
@@ -3275,18 +3272,18 @@
       <c r="D65" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="E65" s="27" t="s">
+      <c r="E65" s="23" t="s">
         <v>162</v>
       </c>
-      <c r="F65" s="28"/>
-      <c r="G65" s="27" t="s">
+      <c r="F65" s="24"/>
+      <c r="G65" s="23" t="s">
         <v>163</v>
       </c>
-      <c r="H65" s="28"/>
-      <c r="I65" s="27" t="s">
+      <c r="H65" s="24"/>
+      <c r="I65" s="23" t="s">
         <v>164</v>
       </c>
-      <c r="J65" s="28"/>
+      <c r="J65" s="24"/>
       <c r="K65" s="8" t="s">
         <v>165</v>
       </c>
@@ -3319,18 +3316,18 @@
       <c r="D66" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="E66" s="29" t="s">
+      <c r="E66" s="46" t="s">
         <v>37</v>
       </c>
-      <c r="F66" s="30"/>
-      <c r="G66" s="44" t="s">
+      <c r="F66" s="47"/>
+      <c r="G66" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="H66" s="45"/>
-      <c r="I66" s="44" t="s">
+      <c r="H66" s="26"/>
+      <c r="I66" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="J66" s="45"/>
+      <c r="J66" s="26"/>
       <c r="K66" s="14" t="s">
         <v>100</v>
       </c>
@@ -3352,21 +3349,21 @@
     </row>
     <row r="67" spans="1:16" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
     <row r="68" spans="1:16" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="23" t="s">
+      <c r="A68" s="33" t="s">
         <v>154</v>
       </c>
-      <c r="B68" s="23"/>
-      <c r="C68" s="23"/>
-      <c r="D68" s="23"/>
-      <c r="E68" s="23"/>
-      <c r="F68" s="23"/>
-      <c r="G68" s="23"/>
-      <c r="H68" s="23"/>
-      <c r="I68" s="23"/>
-      <c r="J68" s="23"/>
-      <c r="K68" s="23"/>
-      <c r="L68" s="23"/>
-      <c r="M68" s="23"/>
+      <c r="B68" s="33"/>
+      <c r="C68" s="33"/>
+      <c r="D68" s="33"/>
+      <c r="E68" s="33"/>
+      <c r="F68" s="33"/>
+      <c r="G68" s="33"/>
+      <c r="H68" s="33"/>
+      <c r="I68" s="33"/>
+      <c r="J68" s="33"/>
+      <c r="K68" s="33"/>
+      <c r="L68" s="33"/>
+      <c r="M68" s="33"/>
     </row>
     <row r="69" spans="1:16" s="3" customFormat="1" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="8" t="s">
@@ -3438,34 +3435,34 @@
       <c r="M71" s="11"/>
     </row>
     <row r="73" spans="1:16" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="23" t="s">
+      <c r="A73" s="33" t="s">
         <v>155</v>
       </c>
-      <c r="B73" s="23"/>
-      <c r="C73" s="23"/>
-      <c r="D73" s="23"/>
-      <c r="E73" s="23"/>
-      <c r="F73" s="23"/>
-      <c r="G73" s="23"/>
-      <c r="H73" s="23"/>
-      <c r="I73" s="23"/>
-      <c r="J73" s="23"/>
-      <c r="K73" s="23"/>
-      <c r="L73" s="23"/>
-      <c r="M73" s="23"/>
+      <c r="B73" s="33"/>
+      <c r="C73" s="33"/>
+      <c r="D73" s="33"/>
+      <c r="E73" s="33"/>
+      <c r="F73" s="33"/>
+      <c r="G73" s="33"/>
+      <c r="H73" s="33"/>
+      <c r="I73" s="33"/>
+      <c r="J73" s="33"/>
+      <c r="K73" s="33"/>
+      <c r="L73" s="33"/>
+      <c r="M73" s="33"/>
     </row>
     <row r="74" spans="1:16" s="3" customFormat="1" ht="31.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B74" s="34" t="s">
+      <c r="B74" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="C74" s="35"/>
-      <c r="D74" s="34" t="s">
+      <c r="C74" s="29"/>
+      <c r="D74" s="27" t="s">
         <v>156</v>
       </c>
-      <c r="E74" s="35"/>
+      <c r="E74" s="29"/>
       <c r="F74" s="8"/>
       <c r="G74" s="8"/>
       <c r="H74" s="8"/>
@@ -3479,14 +3476,14 @@
       <c r="A75" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="B75" s="36" t="s">
+      <c r="B75" s="40" t="s">
         <v>43</v>
       </c>
-      <c r="C75" s="37"/>
-      <c r="D75" s="40" t="s">
+      <c r="C75" s="41"/>
+      <c r="D75" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="E75" s="42"/>
+      <c r="E75" s="35"/>
       <c r="F75" s="13"/>
       <c r="G75" s="14"/>
       <c r="H75" s="14"/>
@@ -3500,14 +3497,14 @@
       <c r="A76" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="B76" s="46" t="s">
+      <c r="B76" s="30" t="s">
         <v>159</v>
       </c>
-      <c r="C76" s="48"/>
-      <c r="D76" s="49" t="s">
+      <c r="C76" s="32"/>
+      <c r="D76" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="E76" s="50"/>
+      <c r="E76" s="37"/>
       <c r="F76" s="11"/>
       <c r="G76" s="12"/>
       <c r="H76" s="12"/>
@@ -3518,21 +3515,21 @@
       <c r="M76" s="11"/>
     </row>
     <row r="78" spans="1:16" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="23" t="s">
+      <c r="A78" s="33" t="s">
         <v>157</v>
       </c>
-      <c r="B78" s="23"/>
-      <c r="C78" s="23"/>
-      <c r="D78" s="23"/>
-      <c r="E78" s="23"/>
-      <c r="F78" s="23"/>
-      <c r="G78" s="23"/>
-      <c r="H78" s="23"/>
-      <c r="I78" s="23"/>
-      <c r="J78" s="23"/>
-      <c r="K78" s="23"/>
-      <c r="L78" s="23"/>
-      <c r="M78" s="23"/>
+      <c r="B78" s="33"/>
+      <c r="C78" s="33"/>
+      <c r="D78" s="33"/>
+      <c r="E78" s="33"/>
+      <c r="F78" s="33"/>
+      <c r="G78" s="33"/>
+      <c r="H78" s="33"/>
+      <c r="I78" s="33"/>
+      <c r="J78" s="33"/>
+      <c r="K78" s="33"/>
+      <c r="L78" s="33"/>
+      <c r="M78" s="33"/>
     </row>
     <row r="79" spans="1:16" s="3" customFormat="1" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="8" t="s">
@@ -3604,35 +3601,35 @@
       <c r="M81" s="11"/>
     </row>
     <row r="83" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="23" t="s">
+      <c r="A83" s="33" t="s">
         <v>180</v>
       </c>
-      <c r="B83" s="23"/>
-      <c r="C83" s="23"/>
-      <c r="D83" s="23"/>
-      <c r="E83" s="23"/>
-      <c r="F83" s="23"/>
-      <c r="G83" s="23"/>
-      <c r="H83" s="23"/>
-      <c r="I83" s="23"/>
-      <c r="J83" s="23"/>
-      <c r="K83" s="23"/>
-      <c r="L83" s="23"/>
-      <c r="M83" s="23"/>
+      <c r="B83" s="33"/>
+      <c r="C83" s="33"/>
+      <c r="D83" s="33"/>
+      <c r="E83" s="33"/>
+      <c r="F83" s="33"/>
+      <c r="G83" s="33"/>
+      <c r="H83" s="33"/>
+      <c r="I83" s="33"/>
+      <c r="J83" s="33"/>
+      <c r="K83" s="33"/>
+      <c r="L83" s="33"/>
+      <c r="M83" s="33"/>
     </row>
     <row r="84" spans="1:13" s="3" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A84" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B84" s="39" t="s">
+      <c r="B84" s="28" t="s">
         <v>178</v>
       </c>
-      <c r="C84" s="39"/>
-      <c r="D84" s="34" t="s">
+      <c r="C84" s="28"/>
+      <c r="D84" s="27" t="s">
         <v>179</v>
       </c>
-      <c r="E84" s="39"/>
-      <c r="F84" s="35"/>
+      <c r="E84" s="28"/>
+      <c r="F84" s="29"/>
       <c r="G84" s="8"/>
       <c r="H84" s="8"/>
       <c r="I84" s="8"/>
@@ -3645,15 +3642,15 @@
       <c r="A85" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="B85" s="36" t="s">
+      <c r="B85" s="40" t="s">
         <v>38</v>
       </c>
-      <c r="C85" s="37"/>
-      <c r="D85" s="40" t="s">
+      <c r="C85" s="41"/>
+      <c r="D85" s="34" t="s">
         <v>50</v>
       </c>
-      <c r="E85" s="41"/>
-      <c r="F85" s="42"/>
+      <c r="E85" s="44"/>
+      <c r="F85" s="35"/>
       <c r="G85" s="14"/>
       <c r="H85" s="14"/>
       <c r="I85" s="13"/>
@@ -3666,38 +3663,38 @@
       <c r="B86" s="7"/>
     </row>
     <row r="87" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="23" t="s">
+      <c r="A87" s="33" t="s">
         <v>172</v>
       </c>
-      <c r="B87" s="23"/>
-      <c r="C87" s="23"/>
-      <c r="D87" s="23"/>
-      <c r="E87" s="23"/>
-      <c r="F87" s="23"/>
-      <c r="G87" s="23"/>
-      <c r="H87" s="23"/>
-      <c r="I87" s="23"/>
-      <c r="J87" s="23"/>
-      <c r="K87" s="23"/>
-      <c r="L87" s="23"/>
-      <c r="M87" s="23"/>
+      <c r="B87" s="33"/>
+      <c r="C87" s="33"/>
+      <c r="D87" s="33"/>
+      <c r="E87" s="33"/>
+      <c r="F87" s="33"/>
+      <c r="G87" s="33"/>
+      <c r="H87" s="33"/>
+      <c r="I87" s="33"/>
+      <c r="J87" s="33"/>
+      <c r="K87" s="33"/>
+      <c r="L87" s="33"/>
+      <c r="M87" s="33"/>
     </row>
     <row r="88" spans="1:13" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="25" t="s">
+      <c r="A88" s="42" t="s">
         <v>173</v>
       </c>
-      <c r="B88" s="25"/>
-      <c r="C88" s="25"/>
-      <c r="D88" s="25"/>
-      <c r="E88" s="25"/>
-      <c r="F88" s="25"/>
-      <c r="G88" s="25"/>
-      <c r="H88" s="25"/>
-      <c r="I88" s="25"/>
-      <c r="J88" s="25"/>
-      <c r="K88" s="25"/>
-      <c r="L88" s="25"/>
-      <c r="M88" s="25"/>
+      <c r="B88" s="42"/>
+      <c r="C88" s="42"/>
+      <c r="D88" s="42"/>
+      <c r="E88" s="42"/>
+      <c r="F88" s="42"/>
+      <c r="G88" s="42"/>
+      <c r="H88" s="42"/>
+      <c r="I88" s="42"/>
+      <c r="J88" s="42"/>
+      <c r="K88" s="42"/>
+      <c r="L88" s="42"/>
+      <c r="M88" s="42"/>
     </row>
     <row r="89" spans="1:13" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A89" s="8" t="s">
@@ -3706,11 +3703,11 @@
       <c r="B89" s="8" t="s">
         <v>209</v>
       </c>
-      <c r="C89" s="34" t="s">
+      <c r="C89" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="D89" s="39"/>
-      <c r="E89" s="35"/>
+      <c r="D89" s="28"/>
+      <c r="E89" s="29"/>
       <c r="F89" s="8"/>
       <c r="G89" s="8"/>
       <c r="H89" s="8"/>
@@ -3727,11 +3724,11 @@
       <c r="B90" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="C90" s="36" t="s">
+      <c r="C90" s="40" t="s">
         <v>219</v>
       </c>
-      <c r="D90" s="43"/>
-      <c r="E90" s="37"/>
+      <c r="D90" s="45"/>
+      <c r="E90" s="41"/>
       <c r="F90" s="13"/>
       <c r="G90" s="14"/>
       <c r="H90" s="14"/>
@@ -3748,9 +3745,9 @@
       <c r="B91" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="C91" s="46"/>
-      <c r="D91" s="47"/>
-      <c r="E91" s="48"/>
+      <c r="C91" s="30"/>
+      <c r="D91" s="31"/>
+      <c r="E91" s="32"/>
       <c r="F91" s="11"/>
       <c r="G91" s="12"/>
       <c r="H91" s="12"/>
@@ -3762,38 +3759,38 @@
     </row>
     <row r="92" spans="1:13" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
     <row r="93" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A93" s="26" t="s">
+      <c r="A93" s="43" t="s">
         <v>181</v>
       </c>
-      <c r="B93" s="26"/>
-      <c r="C93" s="26"/>
-      <c r="D93" s="26"/>
-      <c r="E93" s="26"/>
-      <c r="F93" s="26"/>
-      <c r="G93" s="26"/>
-      <c r="H93" s="26"/>
-      <c r="I93" s="26"/>
-      <c r="J93" s="26"/>
-      <c r="K93" s="26"/>
-      <c r="L93" s="26"/>
-      <c r="M93" s="26"/>
+      <c r="B93" s="43"/>
+      <c r="C93" s="43"/>
+      <c r="D93" s="43"/>
+      <c r="E93" s="43"/>
+      <c r="F93" s="43"/>
+      <c r="G93" s="43"/>
+      <c r="H93" s="43"/>
+      <c r="I93" s="43"/>
+      <c r="J93" s="43"/>
+      <c r="K93" s="43"/>
+      <c r="L93" s="43"/>
+      <c r="M93" s="43"/>
     </row>
     <row r="94" spans="1:13" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A94" s="25" t="s">
+      <c r="A94" s="42" t="s">
         <v>185</v>
       </c>
-      <c r="B94" s="25"/>
-      <c r="C94" s="25"/>
-      <c r="D94" s="25"/>
-      <c r="E94" s="25"/>
-      <c r="F94" s="25"/>
-      <c r="G94" s="25"/>
-      <c r="H94" s="25"/>
-      <c r="I94" s="25"/>
-      <c r="J94" s="25"/>
-      <c r="K94" s="25"/>
-      <c r="L94" s="25"/>
-      <c r="M94" s="25"/>
+      <c r="B94" s="42"/>
+      <c r="C94" s="42"/>
+      <c r="D94" s="42"/>
+      <c r="E94" s="42"/>
+      <c r="F94" s="42"/>
+      <c r="G94" s="42"/>
+      <c r="H94" s="42"/>
+      <c r="I94" s="42"/>
+      <c r="J94" s="42"/>
+      <c r="K94" s="42"/>
+      <c r="L94" s="42"/>
+      <c r="M94" s="42"/>
     </row>
     <row r="95" spans="1:13" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A95" s="8" t="s">
@@ -3884,38 +3881,38 @@
     </row>
     <row r="98" spans="1:13" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
     <row r="99" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A99" s="23" t="s">
+      <c r="A99" s="33" t="s">
         <v>182</v>
       </c>
-      <c r="B99" s="23"/>
-      <c r="C99" s="23"/>
-      <c r="D99" s="23"/>
-      <c r="E99" s="23"/>
-      <c r="F99" s="23"/>
-      <c r="G99" s="23"/>
-      <c r="H99" s="23"/>
-      <c r="I99" s="23"/>
-      <c r="J99" s="23"/>
-      <c r="K99" s="23"/>
-      <c r="L99" s="23"/>
-      <c r="M99" s="23"/>
+      <c r="B99" s="33"/>
+      <c r="C99" s="33"/>
+      <c r="D99" s="33"/>
+      <c r="E99" s="33"/>
+      <c r="F99" s="33"/>
+      <c r="G99" s="33"/>
+      <c r="H99" s="33"/>
+      <c r="I99" s="33"/>
+      <c r="J99" s="33"/>
+      <c r="K99" s="33"/>
+      <c r="L99" s="33"/>
+      <c r="M99" s="33"/>
     </row>
     <row r="100" spans="1:13" s="3" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A100" s="25" t="s">
+      <c r="A100" s="42" t="s">
         <v>183</v>
       </c>
-      <c r="B100" s="25"/>
-      <c r="C100" s="25"/>
-      <c r="D100" s="25"/>
-      <c r="E100" s="25"/>
-      <c r="F100" s="25"/>
-      <c r="G100" s="25"/>
-      <c r="H100" s="25"/>
-      <c r="I100" s="25"/>
-      <c r="J100" s="25"/>
-      <c r="K100" s="25"/>
-      <c r="L100" s="25"/>
-      <c r="M100" s="25"/>
+      <c r="B100" s="42"/>
+      <c r="C100" s="42"/>
+      <c r="D100" s="42"/>
+      <c r="E100" s="42"/>
+      <c r="F100" s="42"/>
+      <c r="G100" s="42"/>
+      <c r="H100" s="42"/>
+      <c r="I100" s="42"/>
+      <c r="J100" s="42"/>
+      <c r="K100" s="42"/>
+      <c r="L100" s="42"/>
+      <c r="M100" s="42"/>
     </row>
     <row r="101" spans="1:13" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A101" s="8" t="s">
@@ -4025,21 +4022,21 @@
     </row>
     <row r="105" spans="1:13" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
     <row r="106" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A106" s="23" t="s">
+      <c r="A106" s="33" t="s">
         <v>186</v>
       </c>
-      <c r="B106" s="23"/>
-      <c r="C106" s="23"/>
-      <c r="D106" s="23"/>
-      <c r="E106" s="23"/>
-      <c r="F106" s="23"/>
-      <c r="G106" s="23"/>
-      <c r="H106" s="23"/>
-      <c r="I106" s="23"/>
-      <c r="J106" s="23"/>
-      <c r="K106" s="23"/>
-      <c r="L106" s="23"/>
-      <c r="M106" s="23"/>
+      <c r="B106" s="33"/>
+      <c r="C106" s="33"/>
+      <c r="D106" s="33"/>
+      <c r="E106" s="33"/>
+      <c r="F106" s="33"/>
+      <c r="G106" s="33"/>
+      <c r="H106" s="33"/>
+      <c r="I106" s="33"/>
+      <c r="J106" s="33"/>
+      <c r="K106" s="33"/>
+      <c r="L106" s="33"/>
+      <c r="M106" s="33"/>
     </row>
     <row r="107" spans="1:13" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A107" s="8" t="s">
@@ -4113,72 +4110,72 @@
     </row>
     <row r="109" spans="1:13" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
     <row r="110" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A110" s="23" t="s">
+      <c r="A110" s="33" t="s">
         <v>194</v>
       </c>
-      <c r="B110" s="23"/>
-      <c r="C110" s="23"/>
-      <c r="D110" s="23"/>
-      <c r="E110" s="23"/>
-      <c r="F110" s="23"/>
-      <c r="G110" s="23"/>
-      <c r="H110" s="23"/>
-      <c r="I110" s="23"/>
-      <c r="J110" s="23"/>
-      <c r="K110" s="23"/>
-      <c r="L110" s="23"/>
-      <c r="M110" s="23"/>
+      <c r="B110" s="33"/>
+      <c r="C110" s="33"/>
+      <c r="D110" s="33"/>
+      <c r="E110" s="33"/>
+      <c r="F110" s="33"/>
+      <c r="G110" s="33"/>
+      <c r="H110" s="33"/>
+      <c r="I110" s="33"/>
+      <c r="J110" s="33"/>
+      <c r="K110" s="33"/>
+      <c r="L110" s="33"/>
+      <c r="M110" s="33"/>
     </row>
     <row r="111" spans="1:13" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="31" t="s">
+      <c r="A111" s="39" t="s">
         <v>200</v>
       </c>
-      <c r="B111" s="31"/>
-      <c r="C111" s="31"/>
-      <c r="D111" s="31"/>
-      <c r="E111" s="31"/>
-      <c r="F111" s="31"/>
-      <c r="G111" s="31"/>
-      <c r="H111" s="31"/>
-      <c r="I111" s="31"/>
-      <c r="J111" s="31"/>
-      <c r="K111" s="31"/>
-      <c r="L111" s="31"/>
-      <c r="M111" s="31"/>
+      <c r="B111" s="39"/>
+      <c r="C111" s="39"/>
+      <c r="D111" s="39"/>
+      <c r="E111" s="39"/>
+      <c r="F111" s="39"/>
+      <c r="G111" s="39"/>
+      <c r="H111" s="39"/>
+      <c r="I111" s="39"/>
+      <c r="J111" s="39"/>
+      <c r="K111" s="39"/>
+      <c r="L111" s="39"/>
+      <c r="M111" s="39"/>
     </row>
     <row r="112" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="33" t="s">
+      <c r="A112" s="22" t="s">
         <v>108</v>
       </c>
-      <c r="B112" s="33"/>
-      <c r="C112" s="33"/>
-      <c r="D112" s="33"/>
-      <c r="E112" s="33"/>
-      <c r="F112" s="33"/>
-      <c r="G112" s="33"/>
-      <c r="H112" s="33"/>
-      <c r="I112" s="33"/>
-      <c r="J112" s="33"/>
-      <c r="K112" s="33"/>
-      <c r="L112" s="33"/>
-      <c r="M112" s="33"/>
+      <c r="B112" s="22"/>
+      <c r="C112" s="22"/>
+      <c r="D112" s="22"/>
+      <c r="E112" s="22"/>
+      <c r="F112" s="22"/>
+      <c r="G112" s="22"/>
+      <c r="H112" s="22"/>
+      <c r="I112" s="22"/>
+      <c r="J112" s="22"/>
+      <c r="K112" s="22"/>
+      <c r="L112" s="22"/>
+      <c r="M112" s="22"/>
     </row>
     <row r="113" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A113" s="32" t="s">
+      <c r="A113" s="48" t="s">
         <v>201</v>
       </c>
-      <c r="B113" s="32"/>
-      <c r="C113" s="32"/>
-      <c r="D113" s="32"/>
-      <c r="E113" s="32"/>
-      <c r="F113" s="32"/>
-      <c r="G113" s="32"/>
-      <c r="H113" s="32"/>
-      <c r="I113" s="32"/>
-      <c r="J113" s="32"/>
-      <c r="K113" s="32"/>
-      <c r="L113" s="32"/>
-      <c r="M113" s="32"/>
+      <c r="B113" s="48"/>
+      <c r="C113" s="48"/>
+      <c r="D113" s="48"/>
+      <c r="E113" s="48"/>
+      <c r="F113" s="48"/>
+      <c r="G113" s="48"/>
+      <c r="H113" s="48"/>
+      <c r="I113" s="48"/>
+      <c r="J113" s="48"/>
+      <c r="K113" s="48"/>
+      <c r="L113" s="48"/>
+      <c r="M113" s="48"/>
     </row>
     <row r="114" spans="1:13" s="4" customFormat="1" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A114" s="8" t="s">
@@ -4281,72 +4278,72 @@
     </row>
     <row r="117" spans="1:13" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
     <row r="118" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A118" s="23" t="s">
+      <c r="A118" s="33" t="s">
         <v>210</v>
       </c>
-      <c r="B118" s="23"/>
-      <c r="C118" s="23"/>
-      <c r="D118" s="23"/>
-      <c r="E118" s="23"/>
-      <c r="F118" s="23"/>
-      <c r="G118" s="23"/>
-      <c r="H118" s="23"/>
-      <c r="I118" s="23"/>
-      <c r="J118" s="23"/>
-      <c r="K118" s="23"/>
-      <c r="L118" s="23"/>
-      <c r="M118" s="23"/>
+      <c r="B118" s="33"/>
+      <c r="C118" s="33"/>
+      <c r="D118" s="33"/>
+      <c r="E118" s="33"/>
+      <c r="F118" s="33"/>
+      <c r="G118" s="33"/>
+      <c r="H118" s="33"/>
+      <c r="I118" s="33"/>
+      <c r="J118" s="33"/>
+      <c r="K118" s="33"/>
+      <c r="L118" s="33"/>
+      <c r="M118" s="33"/>
     </row>
     <row r="119" spans="1:13" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="31" t="s">
+      <c r="A119" s="39" t="s">
         <v>200</v>
       </c>
-      <c r="B119" s="31"/>
-      <c r="C119" s="31"/>
-      <c r="D119" s="31"/>
-      <c r="E119" s="31"/>
-      <c r="F119" s="31"/>
-      <c r="G119" s="31"/>
-      <c r="H119" s="31"/>
-      <c r="I119" s="31"/>
-      <c r="J119" s="31"/>
-      <c r="K119" s="31"/>
-      <c r="L119" s="31"/>
-      <c r="M119" s="31"/>
+      <c r="B119" s="39"/>
+      <c r="C119" s="39"/>
+      <c r="D119" s="39"/>
+      <c r="E119" s="39"/>
+      <c r="F119" s="39"/>
+      <c r="G119" s="39"/>
+      <c r="H119" s="39"/>
+      <c r="I119" s="39"/>
+      <c r="J119" s="39"/>
+      <c r="K119" s="39"/>
+      <c r="L119" s="39"/>
+      <c r="M119" s="39"/>
     </row>
     <row r="120" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="33" t="s">
+      <c r="A120" s="22" t="s">
         <v>108</v>
       </c>
-      <c r="B120" s="33"/>
-      <c r="C120" s="33"/>
-      <c r="D120" s="33"/>
-      <c r="E120" s="33"/>
-      <c r="F120" s="33"/>
-      <c r="G120" s="33"/>
-      <c r="H120" s="33"/>
-      <c r="I120" s="33"/>
-      <c r="J120" s="33"/>
-      <c r="K120" s="33"/>
-      <c r="L120" s="33"/>
-      <c r="M120" s="33"/>
+      <c r="B120" s="22"/>
+      <c r="C120" s="22"/>
+      <c r="D120" s="22"/>
+      <c r="E120" s="22"/>
+      <c r="F120" s="22"/>
+      <c r="G120" s="22"/>
+      <c r="H120" s="22"/>
+      <c r="I120" s="22"/>
+      <c r="J120" s="22"/>
+      <c r="K120" s="22"/>
+      <c r="L120" s="22"/>
+      <c r="M120" s="22"/>
     </row>
     <row r="121" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A121" s="32" t="s">
+      <c r="A121" s="48" t="s">
         <v>202</v>
       </c>
-      <c r="B121" s="32"/>
-      <c r="C121" s="32"/>
-      <c r="D121" s="32"/>
-      <c r="E121" s="32"/>
-      <c r="F121" s="32"/>
-      <c r="G121" s="32"/>
-      <c r="H121" s="32"/>
-      <c r="I121" s="32"/>
-      <c r="J121" s="32"/>
-      <c r="K121" s="32"/>
-      <c r="L121" s="32"/>
-      <c r="M121" s="32"/>
+      <c r="B121" s="48"/>
+      <c r="C121" s="48"/>
+      <c r="D121" s="48"/>
+      <c r="E121" s="48"/>
+      <c r="F121" s="48"/>
+      <c r="G121" s="48"/>
+      <c r="H121" s="48"/>
+      <c r="I121" s="48"/>
+      <c r="J121" s="48"/>
+      <c r="K121" s="48"/>
+      <c r="L121" s="48"/>
+      <c r="M121" s="48"/>
     </row>
     <row r="122" spans="1:13" s="4" customFormat="1" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A122" s="10" t="s">
@@ -4465,38 +4462,38 @@
       <c r="M126" s="38"/>
     </row>
     <row r="127" spans="1:13" s="3" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A127" s="31" t="s">
+      <c r="A127" s="39" t="s">
         <v>215</v>
       </c>
-      <c r="B127" s="31"/>
-      <c r="C127" s="31"/>
-      <c r="D127" s="31"/>
-      <c r="E127" s="31"/>
-      <c r="F127" s="31"/>
-      <c r="G127" s="31"/>
-      <c r="H127" s="31"/>
-      <c r="I127" s="31"/>
-      <c r="J127" s="31"/>
-      <c r="K127" s="31"/>
-      <c r="L127" s="31"/>
-      <c r="M127" s="31"/>
+      <c r="B127" s="39"/>
+      <c r="C127" s="39"/>
+      <c r="D127" s="39"/>
+      <c r="E127" s="39"/>
+      <c r="F127" s="39"/>
+      <c r="G127" s="39"/>
+      <c r="H127" s="39"/>
+      <c r="I127" s="39"/>
+      <c r="J127" s="39"/>
+      <c r="K127" s="39"/>
+      <c r="L127" s="39"/>
+      <c r="M127" s="39"/>
     </row>
     <row r="128" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A128" s="33" t="s">
+      <c r="A128" s="22" t="s">
         <v>211</v>
       </c>
-      <c r="B128" s="33"/>
-      <c r="C128" s="33"/>
-      <c r="D128" s="33"/>
-      <c r="E128" s="33"/>
-      <c r="F128" s="33"/>
-      <c r="G128" s="33"/>
-      <c r="H128" s="33"/>
-      <c r="I128" s="33"/>
-      <c r="J128" s="33"/>
-      <c r="K128" s="33"/>
-      <c r="L128" s="33"/>
-      <c r="M128" s="33"/>
+      <c r="B128" s="22"/>
+      <c r="C128" s="22"/>
+      <c r="D128" s="22"/>
+      <c r="E128" s="22"/>
+      <c r="F128" s="22"/>
+      <c r="G128" s="22"/>
+      <c r="H128" s="22"/>
+      <c r="I128" s="22"/>
+      <c r="J128" s="22"/>
+      <c r="K128" s="22"/>
+      <c r="L128" s="22"/>
+      <c r="M128" s="22"/>
     </row>
     <row r="129" spans="1:13" s="4" customFormat="1" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A129" s="8" t="s">
@@ -4567,6 +4564,45 @@
     </row>
   </sheetData>
   <mergeCells count="55">
+    <mergeCell ref="A5:M5"/>
+    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="A33:M33"/>
+    <mergeCell ref="A44:M44"/>
+    <mergeCell ref="A48:M48"/>
+    <mergeCell ref="A6:M6"/>
+    <mergeCell ref="A34:M34"/>
+    <mergeCell ref="A23:M23"/>
+    <mergeCell ref="A113:M113"/>
+    <mergeCell ref="A118:M118"/>
+    <mergeCell ref="A87:M87"/>
+    <mergeCell ref="A49:M49"/>
+    <mergeCell ref="A57:M57"/>
+    <mergeCell ref="A58:M58"/>
+    <mergeCell ref="A63:P63"/>
+    <mergeCell ref="A53:M53"/>
+    <mergeCell ref="A112:M112"/>
+    <mergeCell ref="D74:E74"/>
+    <mergeCell ref="B74:C74"/>
+    <mergeCell ref="B75:C75"/>
+    <mergeCell ref="A106:M106"/>
+    <mergeCell ref="A110:M110"/>
+    <mergeCell ref="A111:M111"/>
+    <mergeCell ref="A126:M126"/>
+    <mergeCell ref="A127:M127"/>
+    <mergeCell ref="A128:M128"/>
+    <mergeCell ref="B84:C84"/>
+    <mergeCell ref="B85:C85"/>
+    <mergeCell ref="A88:M88"/>
+    <mergeCell ref="A93:M93"/>
+    <mergeCell ref="A99:M99"/>
+    <mergeCell ref="A100:M100"/>
+    <mergeCell ref="A94:M94"/>
+    <mergeCell ref="D84:F84"/>
+    <mergeCell ref="D85:F85"/>
+    <mergeCell ref="C90:E90"/>
+    <mergeCell ref="A119:M119"/>
+    <mergeCell ref="A121:M121"/>
+    <mergeCell ref="A120:M120"/>
     <mergeCell ref="A64:P64"/>
     <mergeCell ref="I65:J65"/>
     <mergeCell ref="I66:J66"/>
@@ -4581,47 +4617,8 @@
     <mergeCell ref="G66:H66"/>
     <mergeCell ref="D75:E75"/>
     <mergeCell ref="D76:E76"/>
-    <mergeCell ref="A126:M126"/>
-    <mergeCell ref="A127:M127"/>
-    <mergeCell ref="A128:M128"/>
-    <mergeCell ref="B84:C84"/>
-    <mergeCell ref="B85:C85"/>
-    <mergeCell ref="A88:M88"/>
-    <mergeCell ref="A93:M93"/>
-    <mergeCell ref="A99:M99"/>
-    <mergeCell ref="A100:M100"/>
-    <mergeCell ref="A94:M94"/>
-    <mergeCell ref="D84:F84"/>
-    <mergeCell ref="D85:F85"/>
-    <mergeCell ref="C90:E90"/>
     <mergeCell ref="E65:F65"/>
     <mergeCell ref="E66:F66"/>
-    <mergeCell ref="A119:M119"/>
-    <mergeCell ref="A121:M121"/>
-    <mergeCell ref="A120:M120"/>
-    <mergeCell ref="A112:M112"/>
-    <mergeCell ref="D74:E74"/>
-    <mergeCell ref="B74:C74"/>
-    <mergeCell ref="B75:C75"/>
-    <mergeCell ref="A106:M106"/>
-    <mergeCell ref="A110:M110"/>
-    <mergeCell ref="A111:M111"/>
-    <mergeCell ref="A113:M113"/>
-    <mergeCell ref="A118:M118"/>
-    <mergeCell ref="A87:M87"/>
-    <mergeCell ref="A49:M49"/>
-    <mergeCell ref="A57:M57"/>
-    <mergeCell ref="A58:M58"/>
-    <mergeCell ref="A63:P63"/>
-    <mergeCell ref="A53:M53"/>
-    <mergeCell ref="A5:M5"/>
-    <mergeCell ref="A1:M1"/>
-    <mergeCell ref="A33:M33"/>
-    <mergeCell ref="A44:M44"/>
-    <mergeCell ref="A48:M48"/>
-    <mergeCell ref="A6:M6"/>
-    <mergeCell ref="A34:M34"/>
-    <mergeCell ref="A23:M23"/>
   </mergeCells>
   <dataValidations count="52">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A3" xr:uid="{00000000-0002-0000-0000-000000000000}">

</xml_diff>

<commit_message>
changed some examples in spreadsheet
</commit_message>
<xml_diff>
--- a/Terraform/aci/base-configs/aci-fabric-deploy-Input-Spreadsheet.xlsx
+++ b/Terraform/aci/base-configs/aci-fabric-deploy-Input-Spreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\tyscott\terraform-aci-fabric-deploy\Terraform\aci\base-configs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{710CA232-1FD5-4857-800D-E8EE3501BBA6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5022D74E-BB54-4AC8-8681-F7AB03CE8651}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,11 +22,21 @@
     <definedName name="switch_role">formulas!$A$2:$A$3</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="225">
   <si>
     <t>Type</t>
   </si>
@@ -55,30 +65,12 @@
     <t>leaf</t>
   </si>
   <si>
-    <t>192.168.85.11/24</t>
-  </si>
-  <si>
-    <t>192.168.85.254</t>
-  </si>
-  <si>
-    <t>192.168.87.11/24</t>
-  </si>
-  <si>
-    <t>192.168.87.254</t>
-  </si>
-  <si>
     <t>TEP-1-102</t>
   </si>
   <si>
     <t>leaf202</t>
   </si>
   <si>
-    <t>192.168.85.12/24</t>
-  </si>
-  <si>
-    <t>192.168.87.12/24</t>
-  </si>
-  <si>
     <t>TEP-1-103</t>
   </si>
   <si>
@@ -88,24 +80,12 @@
     <t>spine</t>
   </si>
   <si>
-    <t>192.168.86.13/24</t>
-  </si>
-  <si>
-    <t>192.168.86.254</t>
-  </si>
-  <si>
-    <t>192.168.87.13/24</t>
-  </si>
-  <si>
     <t>apic_inb</t>
   </si>
   <si>
     <t>apic1</t>
   </si>
   <si>
-    <t>192.168.87.1/24</t>
-  </si>
-  <si>
     <t>AS Number</t>
   </si>
   <si>
@@ -136,18 +116,9 @@
     <t>smartcallhome</t>
   </si>
   <si>
-    <t>cisco-ext.cisco.com</t>
-  </si>
-  <si>
-    <t>asgard-aci@rich.ciscolabs.com</t>
-  </si>
-  <si>
     <t>rich-lab@cisco.com</t>
   </si>
   <si>
-    <t>Richfield Labs</t>
-  </si>
-  <si>
     <t>ntp</t>
   </si>
   <si>
@@ -166,15 +137,9 @@
     <t>snmp-server1</t>
   </si>
   <si>
-    <t>10.0.0.1</t>
-  </si>
-  <si>
     <t>snmp-server2</t>
   </si>
   <si>
-    <t>10.0.0.2</t>
-  </si>
-  <si>
     <t>snmp_info</t>
   </si>
   <si>
@@ -262,9 +227,6 @@
     <t>syslog</t>
   </si>
   <si>
-    <t>1.1.1.1</t>
-  </si>
-  <si>
     <t>warnings</t>
   </si>
   <si>
@@ -292,15 +254,9 @@
     <t>RAD_ISE</t>
   </si>
   <si>
-    <t>1.1.1.5</t>
-  </si>
-  <si>
     <t>cisco1231</t>
   </si>
   <si>
-    <t>1.1.1.6</t>
-  </si>
-  <si>
     <t>tacacs</t>
   </si>
   <si>
@@ -326,9 +282,6 @@
   </si>
   <si>
     <t>Inband VLAN Section (Must be First)</t>
-  </si>
-  <si>
-    <t>+1-408-525-5300</t>
   </si>
   <si>
     <t>Inband VLAN</t>
@@ -541,19 +494,10 @@
     <t>Smart Call Home</t>
   </si>
   <si>
-    <t>Note: Inband Management is Required, OOB Management is Optional</t>
-  </si>
-  <si>
     <t>false</t>
   </si>
   <si>
     <t>true</t>
-  </si>
-  <si>
-    <t>1.1.1.2</t>
-  </si>
-  <si>
-    <t>1.1.1.4</t>
   </si>
   <si>
     <t>NTP Servers IPv4</t>
@@ -855,9 +799,6 @@
     <t>Contact Info</t>
   </si>
   <si>
-    <t>4125 Highlander Pkwy Richfield, OH 44286</t>
-  </si>
-  <si>
     <t>** Authentication Realm - Caution - Make sure to Verify Functionality before configuring default Realm</t>
   </si>
   <si>
@@ -880,13 +821,79 @@
   </si>
   <si>
     <t>VPC Pairs - It is Recommended to use the 1st Node Id for the VPC ID unless you are using Node ID's &gt; 1000</t>
+  </si>
+  <si>
+    <t>Note: Inband Management is Required, OOB Management is Optional - Although Highly Recommended</t>
+  </si>
+  <si>
+    <t>cisco-smtp.example.com</t>
+  </si>
+  <si>
+    <t>cust-aci-fabric@example.com</t>
+  </si>
+  <si>
+    <t>network-ops@example.com</t>
+  </si>
+  <si>
+    <t>+1 408-555-5555</t>
+  </si>
+  <si>
+    <t>Brahma Lab</t>
+  </si>
+  <si>
+    <t>5555 Some Streat Some City, CA 95000</t>
+  </si>
+  <si>
+    <t>198.18.1.201/24</t>
+  </si>
+  <si>
+    <t>198.18.1.1</t>
+  </si>
+  <si>
+    <t>198.18.2.201/24</t>
+  </si>
+  <si>
+    <t>198.18.2.1</t>
+  </si>
+  <si>
+    <t>198.18.1.202/24</t>
+  </si>
+  <si>
+    <t>198.18.2.202/24</t>
+  </si>
+  <si>
+    <t>198.18.1.101/24</t>
+  </si>
+  <si>
+    <t>198.18.2.101/24</t>
+  </si>
+  <si>
+    <t>198.18.2.11</t>
+  </si>
+  <si>
+    <t>198.18.1.51</t>
+  </si>
+  <si>
+    <t>198.18.1.52</t>
+  </si>
+  <si>
+    <t>198.18.1.61</t>
+  </si>
+  <si>
+    <t>198.18.1.62</t>
+  </si>
+  <si>
+    <t>198.18.1.71</t>
+  </si>
+  <si>
+    <t>198.18.1.72</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1041,6 +1048,14 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1599,7 +1614,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="43">
+  <cellStyleXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="49" fontId="17" fillId="33" borderId="8" applyAlignment="0" applyProtection="0"/>
@@ -1643,8 +1658,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="35" borderId="8" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="17" fillId="33" borderId="8" xfId="2" applyNumberFormat="1"/>
@@ -1699,13 +1715,58 @@
     <xf numFmtId="49" fontId="20" fillId="34" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="17" fillId="33" borderId="8" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="33" borderId="8" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="34" borderId="8" xfId="3" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="34" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="34" borderId="8" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="33" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="34" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="18" fillId="0" borderId="16" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="20" fillId="34" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="20" fillId="34" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="18" fillId="34" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="18" fillId="34" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="36" borderId="8" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="11" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="20" fillId="34" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="20" fillId="34" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="20" fillId="34" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="20" fillId="34" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="18" fillId="0" borderId="25" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1714,19 +1775,7 @@
     <xf numFmtId="49" fontId="18" fillId="0" borderId="26" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="20" fillId="34" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="1" fontId="20" fillId="34" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="11" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="16" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="20" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1738,62 +1787,23 @@
     <xf numFmtId="49" fontId="20" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="17" fillId="33" borderId="8" xfId="2" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="20" fillId="34" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="20" fillId="34" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="1" fontId="20" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="20" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="17" fillId="36" borderId="8" xfId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="34" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="20" fillId="34" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="20" fillId="34" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="34" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="33" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="20" fillId="34" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="20" fillId="34" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="20" fillId="34" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="20" fillId="34" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="18" fillId="34" borderId="8" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="21" fillId="34" borderId="22" xfId="43" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="17" fillId="33" borderId="8" xfId="2" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="34" borderId="8" xfId="3" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="1" fontId="21" fillId="34" borderId="22" xfId="43" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="43">
+  <cellStyles count="44">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -1828,6 +1838,7 @@
     <cellStyle name="Heading 2-l" xfId="42" xr:uid="{00000000-0005-0000-0000-00001F000000}"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -2148,10 +2159,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P131"/>
+  <dimension ref="A1:P132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D125" sqref="D125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2176,28 +2187,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="6" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="49" t="s">
-        <v>99</v>
-      </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
-      <c r="G1" s="49"/>
-      <c r="H1" s="49"/>
-      <c r="I1" s="49"/>
-      <c r="J1" s="49"/>
-      <c r="K1" s="49"/>
-      <c r="L1" s="49"/>
-      <c r="M1" s="49"/>
+      <c r="A1" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="20"/>
+      <c r="M1" s="20"/>
     </row>
     <row r="2" spans="1:13" s="3" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>101</v>
+        <v>82</v>
       </c>
       <c r="C2" s="8"/>
       <c r="D2" s="8"/>
@@ -2215,7 +2226,7 @@
       <c r="A3" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="13">
+      <c r="B3" s="14">
         <v>100</v>
       </c>
       <c r="C3" s="13"/>
@@ -2231,38 +2242,38 @@
       <c r="M3" s="13"/>
     </row>
     <row r="5" spans="1:13" s="6" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="49" t="s">
-        <v>109</v>
-      </c>
-      <c r="B5" s="49"/>
-      <c r="C5" s="49"/>
-      <c r="D5" s="49"/>
-      <c r="E5" s="49"/>
-      <c r="F5" s="49"/>
-      <c r="G5" s="49"/>
-      <c r="H5" s="49"/>
-      <c r="I5" s="49"/>
-      <c r="J5" s="49"/>
-      <c r="K5" s="49"/>
-      <c r="L5" s="49"/>
-      <c r="M5" s="49"/>
+      <c r="A5" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="B5" s="20"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="20"/>
+      <c r="K5" s="20"/>
+      <c r="L5" s="20"/>
+      <c r="M5" s="20"/>
     </row>
     <row r="6" spans="1:13" s="6" customFormat="1" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="50" t="s">
-        <v>149</v>
-      </c>
-      <c r="B6" s="50"/>
-      <c r="C6" s="50"/>
-      <c r="D6" s="50"/>
-      <c r="E6" s="50"/>
-      <c r="F6" s="50"/>
-      <c r="G6" s="50"/>
-      <c r="H6" s="50"/>
-      <c r="I6" s="50"/>
-      <c r="J6" s="50"/>
-      <c r="K6" s="50"/>
-      <c r="L6" s="50"/>
-      <c r="M6" s="50"/>
+      <c r="A6" s="22" t="s">
+        <v>203</v>
+      </c>
+      <c r="B6" s="22"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="22"/>
+      <c r="I6" s="22"/>
+      <c r="J6" s="22"/>
+      <c r="K6" s="22"/>
+      <c r="L6" s="22"/>
+      <c r="M6" s="22"/>
     </row>
     <row r="7" spans="1:13" s="3" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
@@ -2275,31 +2286,31 @@
         <v>3</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>133</v>
+        <v>114</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>134</v>
+        <v>115</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>135</v>
+        <v>116</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>136</v>
+        <v>117</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>137</v>
+        <v>118</v>
       </c>
       <c r="J7" s="8" t="s">
-        <v>138</v>
+        <v>119</v>
       </c>
       <c r="K7" s="8" t="s">
-        <v>104</v>
+        <v>85</v>
       </c>
       <c r="L7" s="8" t="s">
-        <v>105</v>
+        <v>86</v>
       </c>
       <c r="M7" s="8"/>
     </row>
@@ -2319,26 +2330,26 @@
       <c r="E8" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="F8" s="13">
+      <c r="F8" s="14">
         <v>1</v>
       </c>
       <c r="G8" s="14" t="s">
         <v>8</v>
       </c>
       <c r="H8" s="14" t="s">
-        <v>130</v>
+        <v>97</v>
       </c>
       <c r="I8" s="13" t="s">
-        <v>9</v>
+        <v>210</v>
       </c>
       <c r="J8" s="13" t="s">
-        <v>10</v>
+        <v>211</v>
       </c>
       <c r="K8" s="13" t="s">
-        <v>11</v>
+        <v>212</v>
       </c>
       <c r="L8" s="13" t="s">
-        <v>12</v>
+        <v>213</v>
       </c>
       <c r="M8" s="13"/>
     </row>
@@ -2347,10 +2358,10 @@
         <v>4</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D9" s="12">
         <v>202</v>
@@ -2358,26 +2369,26 @@
       <c r="E9" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="F9" s="11">
+      <c r="F9" s="12">
         <v>1</v>
       </c>
       <c r="G9" s="12" t="s">
         <v>8</v>
       </c>
       <c r="H9" s="12" t="s">
-        <v>130</v>
+        <v>97</v>
       </c>
       <c r="I9" s="11" t="s">
-        <v>15</v>
+        <v>214</v>
       </c>
       <c r="J9" s="11" t="s">
-        <v>10</v>
+        <v>211</v>
       </c>
       <c r="K9" s="11" t="s">
-        <v>16</v>
+        <v>215</v>
       </c>
       <c r="L9" s="11" t="s">
-        <v>12</v>
+        <v>213</v>
       </c>
       <c r="M9" s="11"/>
     </row>
@@ -2386,10 +2397,10 @@
         <v>4</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D10" s="14">
         <v>101</v>
@@ -2397,26 +2408,26 @@
       <c r="E10" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="F10" s="13">
+      <c r="F10" s="14">
         <v>1</v>
       </c>
       <c r="G10" s="14" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="H10" s="14">
         <v>9508</v>
       </c>
       <c r="I10" s="13" t="s">
-        <v>20</v>
+        <v>216</v>
       </c>
       <c r="J10" s="13" t="s">
-        <v>21</v>
+        <v>211</v>
       </c>
       <c r="K10" s="13" t="s">
-        <v>22</v>
+        <v>217</v>
       </c>
       <c r="L10" s="13" t="s">
-        <v>12</v>
+        <v>213</v>
       </c>
       <c r="M10" s="13"/>
     </row>
@@ -2426,7 +2437,7 @@
       <c r="C11" s="11"/>
       <c r="D11" s="12"/>
       <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
+      <c r="F11" s="12"/>
       <c r="G11" s="12"/>
       <c r="H11" s="12"/>
       <c r="I11" s="11"/>
@@ -2441,7 +2452,7 @@
       <c r="C12" s="13"/>
       <c r="D12" s="14"/>
       <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
+      <c r="F12" s="14"/>
       <c r="G12" s="14"/>
       <c r="H12" s="14"/>
       <c r="I12" s="13"/>
@@ -2456,7 +2467,7 @@
       <c r="C13" s="11"/>
       <c r="D13" s="12"/>
       <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
+      <c r="F13" s="12"/>
       <c r="G13" s="12"/>
       <c r="H13" s="12"/>
       <c r="I13" s="11"/>
@@ -2471,7 +2482,7 @@
       <c r="C14" s="13"/>
       <c r="D14" s="14"/>
       <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
+      <c r="F14" s="14"/>
       <c r="G14" s="14"/>
       <c r="H14" s="14"/>
       <c r="I14" s="13"/>
@@ -2486,7 +2497,7 @@
       <c r="C15" s="11"/>
       <c r="D15" s="12"/>
       <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
+      <c r="F15" s="12"/>
       <c r="G15" s="12"/>
       <c r="H15" s="12"/>
       <c r="I15" s="11"/>
@@ -2501,7 +2512,7 @@
       <c r="C16" s="13"/>
       <c r="D16" s="14"/>
       <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
+      <c r="F16" s="14"/>
       <c r="G16" s="14"/>
       <c r="H16" s="14"/>
       <c r="I16" s="13"/>
@@ -2516,7 +2527,7 @@
       <c r="C17" s="11"/>
       <c r="D17" s="12"/>
       <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
+      <c r="F17" s="12"/>
       <c r="G17" s="12"/>
       <c r="H17" s="12"/>
       <c r="I17" s="11"/>
@@ -2531,7 +2542,7 @@
       <c r="C18" s="13"/>
       <c r="D18" s="14"/>
       <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
+      <c r="F18" s="14"/>
       <c r="G18" s="14"/>
       <c r="H18" s="14"/>
       <c r="I18" s="13"/>
@@ -2546,7 +2557,7 @@
       <c r="C19" s="11"/>
       <c r="D19" s="12"/>
       <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
+      <c r="F19" s="12"/>
       <c r="G19" s="12"/>
       <c r="H19" s="12"/>
       <c r="I19" s="11"/>
@@ -2561,7 +2572,7 @@
       <c r="C20" s="13"/>
       <c r="D20" s="14"/>
       <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
+      <c r="F20" s="14"/>
       <c r="G20" s="14"/>
       <c r="H20" s="14"/>
       <c r="I20" s="13"/>
@@ -2576,7 +2587,7 @@
       <c r="C21" s="11"/>
       <c r="D21" s="12"/>
       <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
+      <c r="F21" s="12"/>
       <c r="G21" s="12"/>
       <c r="H21" s="12"/>
       <c r="I21" s="11"/>
@@ -2586,37 +2597,37 @@
       <c r="M21" s="11"/>
     </row>
     <row r="23" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="49" t="s">
-        <v>225</v>
-      </c>
-      <c r="B23" s="49"/>
-      <c r="C23" s="49"/>
-      <c r="D23" s="49"/>
-      <c r="E23" s="49"/>
-      <c r="F23" s="49"/>
-      <c r="G23" s="49"/>
-      <c r="H23" s="49"/>
-      <c r="I23" s="49"/>
-      <c r="J23" s="49"/>
-      <c r="K23" s="49"/>
-      <c r="L23" s="49"/>
-      <c r="M23" s="49"/>
+      <c r="A23" s="20" t="s">
+        <v>202</v>
+      </c>
+      <c r="B23" s="20"/>
+      <c r="C23" s="20"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="20"/>
+      <c r="H23" s="20"/>
+      <c r="I23" s="20"/>
+      <c r="J23" s="20"/>
+      <c r="K23" s="20"/>
+      <c r="L23" s="20"/>
+      <c r="M23" s="20"/>
     </row>
     <row r="24" spans="1:13" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>221</v>
+        <v>198</v>
       </c>
       <c r="C24" s="8" t="s">
         <v>3</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>222</v>
+        <v>199</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>223</v>
+        <v>200</v>
       </c>
       <c r="F24" s="8"/>
       <c r="G24" s="8"/>
@@ -2629,13 +2640,13 @@
     </row>
     <row r="25" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="13" t="s">
-        <v>220</v>
+        <v>197</v>
       </c>
       <c r="B25" s="14">
         <v>201</v>
       </c>
       <c r="C25" s="13" t="s">
-        <v>224</v>
+        <v>201</v>
       </c>
       <c r="D25" s="14">
         <v>201</v>
@@ -2743,69 +2754,69 @@
       <c r="M31" s="13"/>
     </row>
     <row r="33" spans="1:13" s="6" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="49" t="s">
-        <v>141</v>
-      </c>
-      <c r="B33" s="49"/>
-      <c r="C33" s="49"/>
-      <c r="D33" s="49"/>
-      <c r="E33" s="49"/>
-      <c r="F33" s="49"/>
-      <c r="G33" s="49"/>
-      <c r="H33" s="49"/>
-      <c r="I33" s="49"/>
-      <c r="J33" s="49"/>
-      <c r="K33" s="49"/>
-      <c r="L33" s="49"/>
-      <c r="M33" s="49"/>
+      <c r="A33" s="20" t="s">
+        <v>122</v>
+      </c>
+      <c r="B33" s="20"/>
+      <c r="C33" s="20"/>
+      <c r="D33" s="20"/>
+      <c r="E33" s="20"/>
+      <c r="F33" s="20"/>
+      <c r="G33" s="20"/>
+      <c r="H33" s="20"/>
+      <c r="I33" s="20"/>
+      <c r="J33" s="20"/>
+      <c r="K33" s="20"/>
+      <c r="L33" s="20"/>
+      <c r="M33" s="20"/>
     </row>
     <row r="34" spans="1:13" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="42" t="s">
-        <v>143</v>
-      </c>
-      <c r="B34" s="42"/>
-      <c r="C34" s="42"/>
-      <c r="D34" s="42"/>
-      <c r="E34" s="42"/>
-      <c r="F34" s="42"/>
-      <c r="G34" s="42"/>
-      <c r="H34" s="42"/>
-      <c r="I34" s="42"/>
-      <c r="J34" s="42"/>
-      <c r="K34" s="42"/>
-      <c r="L34" s="42"/>
-      <c r="M34" s="42"/>
+      <c r="A34" s="23" t="s">
+        <v>124</v>
+      </c>
+      <c r="B34" s="23"/>
+      <c r="C34" s="23"/>
+      <c r="D34" s="23"/>
+      <c r="E34" s="23"/>
+      <c r="F34" s="23"/>
+      <c r="G34" s="23"/>
+      <c r="H34" s="23"/>
+      <c r="I34" s="23"/>
+      <c r="J34" s="23"/>
+      <c r="K34" s="23"/>
+      <c r="L34" s="23"/>
+      <c r="M34" s="23"/>
     </row>
     <row r="35" spans="1:13" s="3" customFormat="1" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>139</v>
+        <v>120</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>103</v>
+        <v>84</v>
       </c>
       <c r="E35" s="8" t="s">
-        <v>104</v>
+        <v>85</v>
       </c>
       <c r="F35" s="8" t="s">
-        <v>105</v>
+        <v>86</v>
       </c>
       <c r="G35" s="8" t="s">
-        <v>106</v>
+        <v>87</v>
       </c>
       <c r="H35" s="8" t="s">
-        <v>212</v>
+        <v>190</v>
       </c>
       <c r="I35" s="8" t="s">
-        <v>214</v>
+        <v>192</v>
       </c>
       <c r="J35" s="8" t="s">
-        <v>213</v>
+        <v>191</v>
       </c>
       <c r="K35" s="8"/>
       <c r="L35" s="8"/>
@@ -2813,34 +2824,34 @@
     </row>
     <row r="36" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="13" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="B36" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="C36" s="13">
+        <v>15</v>
+      </c>
+      <c r="C36" s="14">
         <v>1</v>
       </c>
       <c r="D36" s="14">
         <v>1</v>
       </c>
       <c r="E36" s="13" t="s">
-        <v>25</v>
+        <v>218</v>
       </c>
       <c r="F36" s="13" t="s">
-        <v>12</v>
+        <v>213</v>
       </c>
       <c r="G36" s="14" t="s">
         <v>6</v>
       </c>
       <c r="H36" s="14" t="s">
-        <v>107</v>
+        <v>88</v>
       </c>
       <c r="I36" s="13" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="J36" s="13" t="s">
-        <v>107</v>
+        <v>88</v>
       </c>
       <c r="K36" s="13"/>
       <c r="L36" s="13"/>
@@ -2849,7 +2860,7 @@
     <row r="37" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="11"/>
       <c r="B37" s="11"/>
-      <c r="C37" s="11"/>
+      <c r="C37" s="12"/>
       <c r="D37" s="12"/>
       <c r="E37" s="11"/>
       <c r="F37" s="11"/>
@@ -2864,7 +2875,7 @@
     <row r="38" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="13"/>
       <c r="B38" s="13"/>
-      <c r="C38" s="13"/>
+      <c r="C38" s="14"/>
       <c r="D38" s="14"/>
       <c r="E38" s="13"/>
       <c r="F38" s="13"/>
@@ -2879,7 +2890,7 @@
     <row r="39" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="11"/>
       <c r="B39" s="11"/>
-      <c r="C39" s="11"/>
+      <c r="C39" s="12"/>
       <c r="D39" s="12"/>
       <c r="E39" s="11"/>
       <c r="F39" s="11"/>
@@ -2894,7 +2905,7 @@
     <row r="40" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="13"/>
       <c r="B40" s="13"/>
-      <c r="C40" s="13"/>
+      <c r="C40" s="14"/>
       <c r="D40" s="14"/>
       <c r="E40" s="13"/>
       <c r="F40" s="13"/>
@@ -2909,7 +2920,7 @@
     <row r="41" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="11"/>
       <c r="B41" s="11"/>
-      <c r="C41" s="11"/>
+      <c r="C41" s="12"/>
       <c r="D41" s="12"/>
       <c r="E41" s="11"/>
       <c r="F41" s="11"/>
@@ -2924,7 +2935,7 @@
     <row r="42" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="13"/>
       <c r="B42" s="13"/>
-      <c r="C42" s="13"/>
+      <c r="C42" s="14"/>
       <c r="D42" s="14"/>
       <c r="E42" s="13"/>
       <c r="F42" s="13"/>
@@ -2937,28 +2948,28 @@
       <c r="M42" s="13"/>
     </row>
     <row r="44" spans="1:13" s="6" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="49" t="s">
-        <v>140</v>
-      </c>
-      <c r="B44" s="49"/>
-      <c r="C44" s="49"/>
-      <c r="D44" s="49"/>
-      <c r="E44" s="49"/>
-      <c r="F44" s="49"/>
-      <c r="G44" s="49"/>
-      <c r="H44" s="49"/>
-      <c r="I44" s="49"/>
-      <c r="J44" s="49"/>
-      <c r="K44" s="49"/>
-      <c r="L44" s="49"/>
-      <c r="M44" s="49"/>
+      <c r="A44" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="B44" s="20"/>
+      <c r="C44" s="20"/>
+      <c r="D44" s="20"/>
+      <c r="E44" s="20"/>
+      <c r="F44" s="20"/>
+      <c r="G44" s="20"/>
+      <c r="H44" s="20"/>
+      <c r="I44" s="20"/>
+      <c r="J44" s="20"/>
+      <c r="K44" s="20"/>
+      <c r="L44" s="20"/>
+      <c r="M44" s="20"/>
     </row>
     <row r="45" spans="1:13" s="3" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="C45" s="8"/>
       <c r="D45" s="8"/>
@@ -2974,9 +2985,9 @@
     </row>
     <row r="46" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="B46" s="13">
+        <v>17</v>
+      </c>
+      <c r="B46" s="14">
         <v>65513</v>
       </c>
       <c r="C46" s="13"/>
@@ -2992,48 +3003,48 @@
       <c r="M46" s="13"/>
     </row>
     <row r="48" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="33" t="s">
-        <v>142</v>
-      </c>
-      <c r="B48" s="33"/>
-      <c r="C48" s="33"/>
-      <c r="D48" s="33"/>
-      <c r="E48" s="33"/>
-      <c r="F48" s="33"/>
-      <c r="G48" s="33"/>
-      <c r="H48" s="33"/>
-      <c r="I48" s="33"/>
-      <c r="J48" s="33"/>
-      <c r="K48" s="33"/>
-      <c r="L48" s="33"/>
-      <c r="M48" s="33"/>
+      <c r="A48" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="B48" s="21"/>
+      <c r="C48" s="21"/>
+      <c r="D48" s="21"/>
+      <c r="E48" s="21"/>
+      <c r="F48" s="21"/>
+      <c r="G48" s="21"/>
+      <c r="H48" s="21"/>
+      <c r="I48" s="21"/>
+      <c r="J48" s="21"/>
+      <c r="K48" s="21"/>
+      <c r="L48" s="21"/>
+      <c r="M48" s="21"/>
     </row>
     <row r="49" spans="1:16" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="42" t="s">
-        <v>144</v>
-      </c>
-      <c r="B49" s="42"/>
-      <c r="C49" s="42"/>
-      <c r="D49" s="42"/>
-      <c r="E49" s="42"/>
-      <c r="F49" s="42"/>
-      <c r="G49" s="42"/>
-      <c r="H49" s="42"/>
-      <c r="I49" s="42"/>
-      <c r="J49" s="42"/>
-      <c r="K49" s="42"/>
-      <c r="L49" s="42"/>
-      <c r="M49" s="42"/>
+      <c r="A49" s="23" t="s">
+        <v>125</v>
+      </c>
+      <c r="B49" s="23"/>
+      <c r="C49" s="23"/>
+      <c r="D49" s="23"/>
+      <c r="E49" s="23"/>
+      <c r="F49" s="23"/>
+      <c r="G49" s="23"/>
+      <c r="H49" s="23"/>
+      <c r="I49" s="23"/>
+      <c r="J49" s="23"/>
+      <c r="K49" s="23"/>
+      <c r="L49" s="23"/>
+      <c r="M49" s="23"/>
     </row>
     <row r="50" spans="1:16" s="3" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>132</v>
+        <v>113</v>
       </c>
       <c r="C50" s="8" t="s">
-        <v>133</v>
+        <v>114</v>
       </c>
       <c r="D50" s="8"/>
       <c r="E50" s="8"/>
@@ -3048,12 +3059,12 @@
     </row>
     <row r="51" spans="1:16" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="13" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="B51" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="C51" s="13">
+        <v>12</v>
+      </c>
+      <c r="C51" s="14">
         <v>101</v>
       </c>
       <c r="D51" s="14"/>
@@ -3067,1503 +3078,1565 @@
       <c r="L51" s="13"/>
       <c r="M51" s="13"/>
     </row>
-    <row r="53" spans="1:16" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="33" t="s">
+    <row r="52" spans="1:16" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="11"/>
+      <c r="B52" s="11"/>
+      <c r="C52" s="12"/>
+      <c r="D52" s="12"/>
+      <c r="E52" s="11"/>
+      <c r="F52" s="11"/>
+      <c r="G52" s="12"/>
+      <c r="H52" s="12"/>
+      <c r="I52" s="11"/>
+      <c r="J52" s="11"/>
+      <c r="K52" s="11"/>
+      <c r="L52" s="11"/>
+      <c r="M52" s="11"/>
+    </row>
+    <row r="54" spans="1:16" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="B54" s="21"/>
+      <c r="C54" s="21"/>
+      <c r="D54" s="21"/>
+      <c r="E54" s="21"/>
+      <c r="F54" s="21"/>
+      <c r="G54" s="21"/>
+      <c r="H54" s="21"/>
+      <c r="I54" s="21"/>
+      <c r="J54" s="21"/>
+      <c r="K54" s="21"/>
+      <c r="L54" s="21"/>
+      <c r="M54" s="21"/>
+    </row>
+    <row r="55" spans="1:16" s="3" customFormat="1" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B55" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="C55" s="8"/>
+      <c r="D55" s="8"/>
+      <c r="E55" s="8"/>
+      <c r="F55" s="8"/>
+      <c r="G55" s="8"/>
+      <c r="H55" s="8"/>
+      <c r="I55" s="8"/>
+      <c r="J55" s="8"/>
+      <c r="K55" s="8"/>
+      <c r="L55" s="8"/>
+      <c r="M55" s="8"/>
+    </row>
+    <row r="56" spans="1:16" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B56" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C56" s="14"/>
+      <c r="D56" s="14"/>
+      <c r="E56" s="13"/>
+      <c r="F56" s="13"/>
+      <c r="G56" s="14"/>
+      <c r="H56" s="14"/>
+      <c r="I56" s="13"/>
+      <c r="J56" s="13"/>
+      <c r="K56" s="13"/>
+      <c r="L56" s="13"/>
+      <c r="M56" s="13"/>
+    </row>
+    <row r="58" spans="1:16" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="B58" s="21"/>
+      <c r="C58" s="21"/>
+      <c r="D58" s="21"/>
+      <c r="E58" s="21"/>
+      <c r="F58" s="21"/>
+      <c r="G58" s="21"/>
+      <c r="H58" s="21"/>
+      <c r="I58" s="21"/>
+      <c r="J58" s="21"/>
+      <c r="K58" s="21"/>
+      <c r="L58" s="21"/>
+      <c r="M58" s="21"/>
+    </row>
+    <row r="59" spans="1:16" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="23" t="s">
+        <v>128</v>
+      </c>
+      <c r="B59" s="23"/>
+      <c r="C59" s="23"/>
+      <c r="D59" s="23"/>
+      <c r="E59" s="23"/>
+      <c r="F59" s="23"/>
+      <c r="G59" s="23"/>
+      <c r="H59" s="23"/>
+      <c r="I59" s="23"/>
+      <c r="J59" s="23"/>
+      <c r="K59" s="23"/>
+      <c r="L59" s="23"/>
+      <c r="M59" s="23"/>
+    </row>
+    <row r="60" spans="1:16" s="3" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B60" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="C60" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D60" s="8"/>
+      <c r="E60" s="8"/>
+      <c r="F60" s="8"/>
+      <c r="G60" s="8"/>
+      <c r="H60" s="8"/>
+      <c r="I60" s="8"/>
+      <c r="J60" s="8"/>
+      <c r="K60" s="8"/>
+      <c r="L60" s="8"/>
+      <c r="M60" s="8"/>
+    </row>
+    <row r="61" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B61" s="13" t="s">
+        <v>219</v>
+      </c>
+      <c r="C61" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D61" s="14"/>
+      <c r="E61" s="13"/>
+      <c r="F61" s="13"/>
+      <c r="G61" s="14"/>
+      <c r="H61" s="14"/>
+      <c r="I61" s="13"/>
+      <c r="J61" s="13"/>
+      <c r="K61" s="13"/>
+      <c r="L61" s="13"/>
+      <c r="M61" s="13"/>
+    </row>
+    <row r="62" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B62" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="C62" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D62" s="12"/>
+      <c r="E62" s="11"/>
+      <c r="F62" s="11"/>
+      <c r="G62" s="12"/>
+      <c r="H62" s="12"/>
+      <c r="I62" s="11"/>
+      <c r="J62" s="11"/>
+      <c r="K62" s="11"/>
+      <c r="L62" s="11"/>
+      <c r="M62" s="11"/>
+    </row>
+    <row r="64" spans="1:16" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="25" t="s">
+        <v>129</v>
+      </c>
+      <c r="B64" s="25"/>
+      <c r="C64" s="25"/>
+      <c r="D64" s="25"/>
+      <c r="E64" s="25"/>
+      <c r="F64" s="25"/>
+      <c r="G64" s="25"/>
+      <c r="H64" s="25"/>
+      <c r="I64" s="25"/>
+      <c r="J64" s="25"/>
+      <c r="K64" s="25"/>
+      <c r="L64" s="25"/>
+      <c r="M64" s="25"/>
+      <c r="N64" s="25"/>
+      <c r="O64" s="25"/>
+      <c r="P64" s="25"/>
+    </row>
+    <row r="65" spans="1:16" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="26" t="s">
+        <v>148</v>
+      </c>
+      <c r="B65" s="26"/>
+      <c r="C65" s="26"/>
+      <c r="D65" s="26"/>
+      <c r="E65" s="26"/>
+      <c r="F65" s="26"/>
+      <c r="G65" s="26"/>
+      <c r="H65" s="26"/>
+      <c r="I65" s="26"/>
+      <c r="J65" s="26"/>
+      <c r="K65" s="26"/>
+      <c r="L65" s="26"/>
+      <c r="M65" s="26"/>
+      <c r="N65" s="26"/>
+      <c r="O65" s="26"/>
+      <c r="P65" s="26"/>
+    </row>
+    <row r="66" spans="1:16" s="3" customFormat="1" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B66" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="C66" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="D66" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="E66" s="38" t="s">
+        <v>140</v>
+      </c>
+      <c r="F66" s="39"/>
+      <c r="G66" s="38" t="s">
+        <v>141</v>
+      </c>
+      <c r="H66" s="39"/>
+      <c r="I66" s="38" t="s">
+        <v>142</v>
+      </c>
+      <c r="J66" s="39"/>
+      <c r="K66" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="L66" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="M66" s="18" t="s">
+        <v>144</v>
+      </c>
+      <c r="N66" s="8" t="s">
         <v>145</v>
       </c>
-      <c r="B53" s="33"/>
-      <c r="C53" s="33"/>
-      <c r="D53" s="33"/>
-      <c r="E53" s="33"/>
-      <c r="F53" s="33"/>
-      <c r="G53" s="33"/>
-      <c r="H53" s="33"/>
-      <c r="I53" s="33"/>
-      <c r="J53" s="33"/>
-      <c r="K53" s="33"/>
-      <c r="L53" s="33"/>
-      <c r="M53" s="33"/>
-    </row>
-    <row r="54" spans="1:16" s="3" customFormat="1" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="8" t="s">
+      <c r="O66" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="P66" s="8" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="67" spans="1:16" s="4" customFormat="1" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B67" s="14">
+        <v>25</v>
+      </c>
+      <c r="C67" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="D67" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E67" s="47" t="s">
+        <v>205</v>
+      </c>
+      <c r="F67" s="46"/>
+      <c r="G67" s="48" t="s">
+        <v>206</v>
+      </c>
+      <c r="H67" s="40"/>
+      <c r="I67" s="48" t="s">
+        <v>206</v>
+      </c>
+      <c r="J67" s="40"/>
+      <c r="K67" s="13" t="s">
+        <v>207</v>
+      </c>
+      <c r="L67" s="14" t="s">
+        <v>208</v>
+      </c>
+      <c r="M67" s="19" t="s">
+        <v>209</v>
+      </c>
+      <c r="N67" s="13">
+        <v>5555555</v>
+      </c>
+      <c r="O67" s="13">
+        <v>5555555</v>
+      </c>
+      <c r="P67" s="13">
+        <v>555555</v>
+      </c>
+    </row>
+    <row r="68" spans="1:16" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
+    <row r="69" spans="1:16" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="B69" s="21"/>
+      <c r="C69" s="21"/>
+      <c r="D69" s="21"/>
+      <c r="E69" s="21"/>
+      <c r="F69" s="21"/>
+      <c r="G69" s="21"/>
+      <c r="H69" s="21"/>
+      <c r="I69" s="21"/>
+      <c r="J69" s="21"/>
+      <c r="K69" s="21"/>
+      <c r="L69" s="21"/>
+      <c r="M69" s="21"/>
+    </row>
+    <row r="70" spans="1:16" s="3" customFormat="1" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B54" s="9" t="s">
+      <c r="B70" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="C70" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D70" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="E70" s="8"/>
+      <c r="F70" s="8"/>
+      <c r="G70" s="8"/>
+      <c r="H70" s="8"/>
+      <c r="I70" s="8"/>
+      <c r="J70" s="8"/>
+      <c r="K70" s="8"/>
+      <c r="L70" s="8"/>
+      <c r="M70" s="8"/>
+    </row>
+    <row r="71" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B71" s="13" t="s">
+        <v>219</v>
+      </c>
+      <c r="C71" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="D71" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E71" s="13"/>
+      <c r="F71" s="13"/>
+      <c r="G71" s="14"/>
+      <c r="H71" s="14"/>
+      <c r="I71" s="13"/>
+      <c r="J71" s="13"/>
+      <c r="K71" s="13"/>
+      <c r="L71" s="13"/>
+      <c r="M71" s="13"/>
+    </row>
+    <row r="72" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B72" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="C72" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="C54" s="20"/>
-      <c r="D54" s="8"/>
-      <c r="E54" s="8"/>
-      <c r="F54" s="8"/>
-      <c r="G54" s="8"/>
-      <c r="H54" s="8"/>
-      <c r="I54" s="8"/>
-      <c r="J54" s="8"/>
-      <c r="K54" s="8"/>
-      <c r="L54" s="8"/>
-      <c r="M54" s="8"/>
-    </row>
-    <row r="55" spans="1:16" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="13" t="s">
+      <c r="D72" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="E72" s="11"/>
+      <c r="F72" s="11"/>
+      <c r="G72" s="12"/>
+      <c r="H72" s="12"/>
+      <c r="I72" s="11"/>
+      <c r="J72" s="11"/>
+      <c r="K72" s="11"/>
+      <c r="L72" s="11"/>
+      <c r="M72" s="11"/>
+    </row>
+    <row r="74" spans="1:16" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="B74" s="21"/>
+      <c r="C74" s="21"/>
+      <c r="D74" s="21"/>
+      <c r="E74" s="21"/>
+      <c r="F74" s="21"/>
+      <c r="G74" s="21"/>
+      <c r="H74" s="21"/>
+      <c r="I74" s="21"/>
+      <c r="J74" s="21"/>
+      <c r="K74" s="21"/>
+      <c r="L74" s="21"/>
+      <c r="M74" s="21"/>
+    </row>
+    <row r="75" spans="1:16" s="3" customFormat="1" ht="31.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A75" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B75" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="C75" s="28"/>
+      <c r="D75" s="27" t="s">
+        <v>134</v>
+      </c>
+      <c r="E75" s="28"/>
+      <c r="F75" s="8"/>
+      <c r="G75" s="8"/>
+      <c r="H75" s="8"/>
+      <c r="I75" s="8"/>
+      <c r="J75" s="8"/>
+      <c r="K75" s="8"/>
+      <c r="L75" s="8"/>
+      <c r="M75" s="8"/>
+    </row>
+    <row r="76" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="B55" s="15" t="s">
+      <c r="B76" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="C55" s="21"/>
-      <c r="D55" s="14"/>
-      <c r="E55" s="13"/>
-      <c r="F55" s="13"/>
-      <c r="G55" s="14"/>
-      <c r="H55" s="14"/>
-      <c r="I55" s="13"/>
-      <c r="J55" s="13"/>
-      <c r="K55" s="13"/>
-      <c r="L55" s="13"/>
-      <c r="M55" s="13"/>
-    </row>
-    <row r="57" spans="1:16" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="33" t="s">
-        <v>146</v>
-      </c>
-      <c r="B57" s="33"/>
-      <c r="C57" s="33"/>
-      <c r="D57" s="33"/>
-      <c r="E57" s="33"/>
-      <c r="F57" s="33"/>
-      <c r="G57" s="33"/>
-      <c r="H57" s="33"/>
-      <c r="I57" s="33"/>
-      <c r="J57" s="33"/>
-      <c r="K57" s="33"/>
-      <c r="L57" s="33"/>
-      <c r="M57" s="33"/>
-    </row>
-    <row r="58" spans="1:16" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="42" t="s">
-        <v>147</v>
-      </c>
-      <c r="B58" s="42"/>
-      <c r="C58" s="42"/>
-      <c r="D58" s="42"/>
-      <c r="E58" s="42"/>
-      <c r="F58" s="42"/>
-      <c r="G58" s="42"/>
-      <c r="H58" s="42"/>
-      <c r="I58" s="42"/>
-      <c r="J58" s="42"/>
-      <c r="K58" s="42"/>
-      <c r="L58" s="42"/>
-      <c r="M58" s="42"/>
-    </row>
-    <row r="59" spans="1:16" s="3" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="8" t="s">
+      <c r="C76" s="30"/>
+      <c r="D76" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="E76" s="36"/>
+      <c r="F76" s="13"/>
+      <c r="G76" s="14"/>
+      <c r="H76" s="14"/>
+      <c r="I76" s="13"/>
+      <c r="J76" s="13"/>
+      <c r="K76" s="13"/>
+      <c r="L76" s="13"/>
+      <c r="M76" s="13"/>
+    </row>
+    <row r="77" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A77" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B77" s="41" t="s">
+        <v>137</v>
+      </c>
+      <c r="C77" s="43"/>
+      <c r="D77" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="E77" s="45"/>
+      <c r="F77" s="11"/>
+      <c r="G77" s="12"/>
+      <c r="H77" s="12"/>
+      <c r="I77" s="11"/>
+      <c r="J77" s="11"/>
+      <c r="K77" s="11"/>
+      <c r="L77" s="11"/>
+      <c r="M77" s="11"/>
+    </row>
+    <row r="79" spans="1:16" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A79" s="21" t="s">
+        <v>135</v>
+      </c>
+      <c r="B79" s="21"/>
+      <c r="C79" s="21"/>
+      <c r="D79" s="21"/>
+      <c r="E79" s="21"/>
+      <c r="F79" s="21"/>
+      <c r="G79" s="21"/>
+      <c r="H79" s="21"/>
+      <c r="I79" s="21"/>
+      <c r="J79" s="21"/>
+      <c r="K79" s="21"/>
+      <c r="L79" s="21"/>
+      <c r="M79" s="21"/>
+    </row>
+    <row r="80" spans="1:16" s="3" customFormat="1" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A80" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B59" s="8" t="s">
+      <c r="B80" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="C80" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="D80" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="E80" s="8"/>
+      <c r="F80" s="8"/>
+      <c r="G80" s="8"/>
+      <c r="H80" s="8"/>
+      <c r="I80" s="8"/>
+      <c r="J80" s="8"/>
+      <c r="K80" s="8"/>
+      <c r="L80" s="8"/>
+      <c r="M80" s="8"/>
+    </row>
+    <row r="81" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A81" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B81" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C81" s="13" t="s">
+        <v>221</v>
+      </c>
+      <c r="D81" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E81" s="13"/>
+      <c r="F81" s="13"/>
+      <c r="G81" s="14"/>
+      <c r="H81" s="14"/>
+      <c r="I81" s="13"/>
+      <c r="J81" s="13"/>
+      <c r="K81" s="13"/>
+      <c r="L81" s="13"/>
+      <c r="M81" s="13"/>
+    </row>
+    <row r="82" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A82" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B82" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C82" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="D82" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="E82" s="11"/>
+      <c r="F82" s="11"/>
+      <c r="G82" s="12"/>
+      <c r="H82" s="12"/>
+      <c r="I82" s="11"/>
+      <c r="J82" s="11"/>
+      <c r="K82" s="11"/>
+      <c r="L82" s="11"/>
+      <c r="M82" s="11"/>
+    </row>
+    <row r="84" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A84" s="21" t="s">
         <v>158</v>
       </c>
-      <c r="C59" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D59" s="8"/>
-      <c r="E59" s="8"/>
-      <c r="F59" s="8"/>
-      <c r="G59" s="8"/>
-      <c r="H59" s="8"/>
-      <c r="I59" s="8"/>
-      <c r="J59" s="8"/>
-      <c r="K59" s="8"/>
-      <c r="L59" s="8"/>
-      <c r="M59" s="8"/>
-    </row>
-    <row r="60" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="B60" s="13" t="s">
+      <c r="B84" s="21"/>
+      <c r="C84" s="21"/>
+      <c r="D84" s="21"/>
+      <c r="E84" s="21"/>
+      <c r="F84" s="21"/>
+      <c r="G84" s="21"/>
+      <c r="H84" s="21"/>
+      <c r="I84" s="21"/>
+      <c r="J84" s="21"/>
+      <c r="K84" s="21"/>
+      <c r="L84" s="21"/>
+      <c r="M84" s="21"/>
+    </row>
+    <row r="85" spans="1:13" s="3" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A85" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B85" s="33" t="s">
+        <v>156</v>
+      </c>
+      <c r="C85" s="33"/>
+      <c r="D85" s="27" t="s">
+        <v>157</v>
+      </c>
+      <c r="E85" s="33"/>
+      <c r="F85" s="28"/>
+      <c r="G85" s="8"/>
+      <c r="H85" s="8"/>
+      <c r="I85" s="8"/>
+      <c r="J85" s="8"/>
+      <c r="K85" s="8"/>
+      <c r="L85" s="8"/>
+      <c r="M85" s="8"/>
+    </row>
+    <row r="86" spans="1:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A86" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B86" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="C86" s="30"/>
+      <c r="D86" s="34" t="s">
+        <v>35</v>
+      </c>
+      <c r="E86" s="35"/>
+      <c r="F86" s="36"/>
+      <c r="G86" s="14"/>
+      <c r="H86" s="14"/>
+      <c r="I86" s="13"/>
+      <c r="J86" s="13"/>
+      <c r="K86" s="13"/>
+      <c r="L86" s="13"/>
+      <c r="M86" s="13"/>
+    </row>
+    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B87" s="7"/>
+    </row>
+    <row r="88" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A88" s="21" t="s">
+        <v>150</v>
+      </c>
+      <c r="B88" s="21"/>
+      <c r="C88" s="21"/>
+      <c r="D88" s="21"/>
+      <c r="E88" s="21"/>
+      <c r="F88" s="21"/>
+      <c r="G88" s="21"/>
+      <c r="H88" s="21"/>
+      <c r="I88" s="21"/>
+      <c r="J88" s="21"/>
+      <c r="K88" s="21"/>
+      <c r="L88" s="21"/>
+      <c r="M88" s="21"/>
+    </row>
+    <row r="89" spans="1:13" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A89" s="23" t="s">
+        <v>151</v>
+      </c>
+      <c r="B89" s="23"/>
+      <c r="C89" s="23"/>
+      <c r="D89" s="23"/>
+      <c r="E89" s="23"/>
+      <c r="F89" s="23"/>
+      <c r="G89" s="23"/>
+      <c r="H89" s="23"/>
+      <c r="I89" s="23"/>
+      <c r="J89" s="23"/>
+      <c r="K89" s="23"/>
+      <c r="L89" s="23"/>
+      <c r="M89" s="23"/>
+    </row>
+    <row r="90" spans="1:13" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A90" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B90" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="C90" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="D90" s="33"/>
+      <c r="E90" s="28"/>
+      <c r="F90" s="8"/>
+      <c r="G90" s="8"/>
+      <c r="H90" s="8"/>
+      <c r="I90" s="8"/>
+      <c r="J90" s="8"/>
+      <c r="K90" s="8"/>
+      <c r="L90" s="8"/>
+      <c r="M90" s="8"/>
+    </row>
+    <row r="91" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A91" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B91" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C91" s="29" t="s">
+        <v>196</v>
+      </c>
+      <c r="D91" s="37"/>
+      <c r="E91" s="30"/>
+      <c r="F91" s="13"/>
+      <c r="G91" s="14"/>
+      <c r="H91" s="14"/>
+      <c r="I91" s="13"/>
+      <c r="J91" s="13"/>
+      <c r="K91" s="13"/>
+      <c r="L91" s="13"/>
+      <c r="M91" s="13"/>
+    </row>
+    <row r="92" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A92" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B92" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C92" s="41"/>
+      <c r="D92" s="42"/>
+      <c r="E92" s="43"/>
+      <c r="F92" s="11"/>
+      <c r="G92" s="12"/>
+      <c r="H92" s="12"/>
+      <c r="I92" s="11"/>
+      <c r="J92" s="11"/>
+      <c r="K92" s="11"/>
+      <c r="L92" s="11"/>
+      <c r="M92" s="11"/>
+    </row>
+    <row r="93" spans="1:13" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
+    <row r="94" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A94" s="25" t="s">
+        <v>159</v>
+      </c>
+      <c r="B94" s="25"/>
+      <c r="C94" s="25"/>
+      <c r="D94" s="25"/>
+      <c r="E94" s="25"/>
+      <c r="F94" s="25"/>
+      <c r="G94" s="25"/>
+      <c r="H94" s="25"/>
+      <c r="I94" s="25"/>
+      <c r="J94" s="25"/>
+      <c r="K94" s="25"/>
+      <c r="L94" s="25"/>
+      <c r="M94" s="25"/>
+    </row>
+    <row r="95" spans="1:13" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A95" s="23" t="s">
+        <v>163</v>
+      </c>
+      <c r="B95" s="23"/>
+      <c r="C95" s="23"/>
+      <c r="D95" s="23"/>
+      <c r="E95" s="23"/>
+      <c r="F95" s="23"/>
+      <c r="G95" s="23"/>
+      <c r="H95" s="23"/>
+      <c r="I95" s="23"/>
+      <c r="J95" s="23"/>
+      <c r="K95" s="23"/>
+      <c r="L95" s="23"/>
+      <c r="M95" s="23"/>
+    </row>
+    <row r="96" spans="1:13" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A96" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B96" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="C96" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="D96" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E96" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="F96" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="G96" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="H96" s="8"/>
+      <c r="I96" s="8"/>
+      <c r="J96" s="8"/>
+      <c r="K96" s="8"/>
+      <c r="L96" s="8"/>
+      <c r="M96" s="8"/>
+    </row>
+    <row r="97" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A97" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B97" s="13" t="s">
+        <v>221</v>
+      </c>
+      <c r="C97" s="14">
+        <v>162</v>
+      </c>
+      <c r="D97" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="E97" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="F97" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="G97" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="H97" s="14"/>
+      <c r="I97" s="13"/>
+      <c r="J97" s="13"/>
+      <c r="K97" s="13"/>
+      <c r="L97" s="13"/>
+      <c r="M97" s="13"/>
+    </row>
+    <row r="98" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A98" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="B98" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="C98" s="12">
+        <v>162</v>
+      </c>
+      <c r="D98" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="E98" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="F98" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="G98" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="H98" s="12"/>
+      <c r="I98" s="11"/>
+      <c r="J98" s="11"/>
+      <c r="K98" s="11"/>
+      <c r="L98" s="11"/>
+      <c r="M98" s="11"/>
+    </row>
+    <row r="99" spans="1:13" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
+    <row r="100" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A100" s="21" t="s">
+        <v>160</v>
+      </c>
+      <c r="B100" s="21"/>
+      <c r="C100" s="21"/>
+      <c r="D100" s="21"/>
+      <c r="E100" s="21"/>
+      <c r="F100" s="21"/>
+      <c r="G100" s="21"/>
+      <c r="H100" s="21"/>
+      <c r="I100" s="21"/>
+      <c r="J100" s="21"/>
+      <c r="K100" s="21"/>
+      <c r="L100" s="21"/>
+      <c r="M100" s="21"/>
+    </row>
+    <row r="101" spans="1:13" s="3" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A101" s="23" t="s">
+        <v>161</v>
+      </c>
+      <c r="B101" s="23"/>
+      <c r="C101" s="23"/>
+      <c r="D101" s="23"/>
+      <c r="E101" s="23"/>
+      <c r="F101" s="23"/>
+      <c r="G101" s="23"/>
+      <c r="H101" s="23"/>
+      <c r="I101" s="23"/>
+      <c r="J101" s="23"/>
+      <c r="K101" s="23"/>
+      <c r="L101" s="23"/>
+      <c r="M101" s="23"/>
+    </row>
+    <row r="102" spans="1:13" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A102" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B102" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C102" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D102" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="E102" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="F102" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="G102" s="8"/>
+      <c r="H102" s="8"/>
+      <c r="I102" s="8"/>
+      <c r="J102" s="8"/>
+      <c r="K102" s="8"/>
+      <c r="L102" s="8"/>
+      <c r="M102" s="8"/>
+    </row>
+    <row r="103" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A103" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="B103" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C103" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="D103" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="E103" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="F103" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="G103" s="14"/>
+      <c r="H103" s="14"/>
+      <c r="I103" s="13"/>
+      <c r="J103" s="13"/>
+      <c r="K103" s="13"/>
+      <c r="L103" s="13"/>
+      <c r="M103" s="13"/>
+    </row>
+    <row r="104" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A104" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="B104" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C104" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="D104" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="E104" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="F104" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="G104" s="12"/>
+      <c r="H104" s="12"/>
+      <c r="I104" s="11"/>
+      <c r="J104" s="11"/>
+      <c r="K104" s="11"/>
+      <c r="L104" s="11"/>
+      <c r="M104" s="11"/>
+    </row>
+    <row r="105" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A105" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="B105" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="C105" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="D105" s="14"/>
+      <c r="E105" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="F105" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="G105" s="14"/>
+      <c r="H105" s="14"/>
+      <c r="I105" s="13"/>
+      <c r="J105" s="13"/>
+      <c r="K105" s="13"/>
+      <c r="L105" s="13"/>
+      <c r="M105" s="13"/>
+    </row>
+    <row r="106" spans="1:13" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
+    <row r="107" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A107" s="21" t="s">
+        <v>164</v>
+      </c>
+      <c r="B107" s="21"/>
+      <c r="C107" s="21"/>
+      <c r="D107" s="21"/>
+      <c r="E107" s="21"/>
+      <c r="F107" s="21"/>
+      <c r="G107" s="21"/>
+      <c r="H107" s="21"/>
+      <c r="I107" s="21"/>
+      <c r="J107" s="21"/>
+      <c r="K107" s="21"/>
+      <c r="L107" s="21"/>
+      <c r="M107" s="21"/>
+    </row>
+    <row r="108" spans="1:13" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A108" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B108" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="C108" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="D108" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="E108" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="F108" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="G108" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="H108" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="I108" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="J108" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="K108" s="8"/>
+      <c r="L108" s="8"/>
+      <c r="M108" s="8"/>
+    </row>
+    <row r="109" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A109" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="B109" s="13" t="s">
+        <v>221</v>
+      </c>
+      <c r="C109" s="14">
+        <v>514</v>
+      </c>
+      <c r="D109" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E109" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="F109" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="G109" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="H109" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="I109" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="J109" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="K109" s="13"/>
+      <c r="L109" s="13"/>
+      <c r="M109" s="13"/>
+    </row>
+    <row r="110" spans="1:13" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
+    <row r="111" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A111" s="21" t="s">
+        <v>172</v>
+      </c>
+      <c r="B111" s="21"/>
+      <c r="C111" s="21"/>
+      <c r="D111" s="21"/>
+      <c r="E111" s="21"/>
+      <c r="F111" s="21"/>
+      <c r="G111" s="21"/>
+      <c r="H111" s="21"/>
+      <c r="I111" s="21"/>
+      <c r="J111" s="21"/>
+      <c r="K111" s="21"/>
+      <c r="L111" s="21"/>
+      <c r="M111" s="21"/>
+    </row>
+    <row r="112" spans="1:13" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A112" s="31" t="s">
+        <v>178</v>
+      </c>
+      <c r="B112" s="31"/>
+      <c r="C112" s="31"/>
+      <c r="D112" s="31"/>
+      <c r="E112" s="31"/>
+      <c r="F112" s="31"/>
+      <c r="G112" s="31"/>
+      <c r="H112" s="31"/>
+      <c r="I112" s="31"/>
+      <c r="J112" s="31"/>
+      <c r="K112" s="31"/>
+      <c r="L112" s="31"/>
+      <c r="M112" s="31"/>
+    </row>
+    <row r="113" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A113" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="B113" s="26"/>
+      <c r="C113" s="26"/>
+      <c r="D113" s="26"/>
+      <c r="E113" s="26"/>
+      <c r="F113" s="26"/>
+      <c r="G113" s="26"/>
+      <c r="H113" s="26"/>
+      <c r="I113" s="26"/>
+      <c r="J113" s="26"/>
+      <c r="K113" s="26"/>
+      <c r="L113" s="26"/>
+      <c r="M113" s="26"/>
+    </row>
+    <row r="114" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A114" s="24" t="s">
+        <v>179</v>
+      </c>
+      <c r="B114" s="24"/>
+      <c r="C114" s="24"/>
+      <c r="D114" s="24"/>
+      <c r="E114" s="24"/>
+      <c r="F114" s="24"/>
+      <c r="G114" s="24"/>
+      <c r="H114" s="24"/>
+      <c r="I114" s="24"/>
+      <c r="J114" s="24"/>
+      <c r="K114" s="24"/>
+      <c r="L114" s="24"/>
+      <c r="M114" s="24"/>
+    </row>
+    <row r="115" spans="1:13" s="4" customFormat="1" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A115" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B115" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="C115" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="D115" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="E115" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="F115" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="G115" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="H115" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="I115" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="J115" s="8"/>
+      <c r="K115" s="8"/>
+      <c r="L115" s="8"/>
+      <c r="M115" s="8"/>
+    </row>
+    <row r="116" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A116" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="B116" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="C116" s="13" t="s">
+        <v>223</v>
+      </c>
+      <c r="D116" s="14">
+        <v>1812</v>
+      </c>
+      <c r="E116" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="F116" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="G116" s="14">
+        <v>5</v>
+      </c>
+      <c r="H116" s="14">
+        <v>5</v>
+      </c>
+      <c r="I116" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="J116" s="13"/>
+      <c r="K116" s="13"/>
+      <c r="L116" s="13"/>
+      <c r="M116" s="13"/>
+    </row>
+    <row r="117" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A117" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="B117" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="C117" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="D117" s="12">
+        <v>1812</v>
+      </c>
+      <c r="E117" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="F117" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="G117" s="12">
+        <v>5</v>
+      </c>
+      <c r="H117" s="12">
+        <v>5</v>
+      </c>
+      <c r="I117" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="J117" s="11"/>
+      <c r="K117" s="11"/>
+      <c r="L117" s="11"/>
+      <c r="M117" s="11"/>
+    </row>
+    <row r="118" spans="1:13" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
+    <row r="119" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A119" s="21" t="s">
+        <v>188</v>
+      </c>
+      <c r="B119" s="21"/>
+      <c r="C119" s="21"/>
+      <c r="D119" s="21"/>
+      <c r="E119" s="21"/>
+      <c r="F119" s="21"/>
+      <c r="G119" s="21"/>
+      <c r="H119" s="21"/>
+      <c r="I119" s="21"/>
+      <c r="J119" s="21"/>
+      <c r="K119" s="21"/>
+      <c r="L119" s="21"/>
+      <c r="M119" s="21"/>
+    </row>
+    <row r="120" spans="1:13" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A120" s="31" t="s">
+        <v>178</v>
+      </c>
+      <c r="B120" s="31"/>
+      <c r="C120" s="31"/>
+      <c r="D120" s="31"/>
+      <c r="E120" s="31"/>
+      <c r="F120" s="31"/>
+      <c r="G120" s="31"/>
+      <c r="H120" s="31"/>
+      <c r="I120" s="31"/>
+      <c r="J120" s="31"/>
+      <c r="K120" s="31"/>
+      <c r="L120" s="31"/>
+      <c r="M120" s="31"/>
+    </row>
+    <row r="121" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A121" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="B121" s="26"/>
+      <c r="C121" s="26"/>
+      <c r="D121" s="26"/>
+      <c r="E121" s="26"/>
+      <c r="F121" s="26"/>
+      <c r="G121" s="26"/>
+      <c r="H121" s="26"/>
+      <c r="I121" s="26"/>
+      <c r="J121" s="26"/>
+      <c r="K121" s="26"/>
+      <c r="L121" s="26"/>
+      <c r="M121" s="26"/>
+    </row>
+    <row r="122" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A122" s="24" t="s">
+        <v>180</v>
+      </c>
+      <c r="B122" s="24"/>
+      <c r="C122" s="24"/>
+      <c r="D122" s="24"/>
+      <c r="E122" s="24"/>
+      <c r="F122" s="24"/>
+      <c r="G122" s="24"/>
+      <c r="H122" s="24"/>
+      <c r="I122" s="24"/>
+      <c r="J122" s="24"/>
+      <c r="K122" s="24"/>
+      <c r="L122" s="24"/>
+      <c r="M122" s="24"/>
+    </row>
+    <row r="123" spans="1:13" s="4" customFormat="1" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A123" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B123" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="C123" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="D123" s="10" t="s">
+        <v>182</v>
+      </c>
+      <c r="E123" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="F123" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="G123" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="H123" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="I123" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="J123" s="10"/>
+      <c r="K123" s="10"/>
+      <c r="L123" s="10"/>
+      <c r="M123" s="10"/>
+    </row>
+    <row r="124" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A124" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="B124" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="C124" s="13" t="s">
+        <v>223</v>
+      </c>
+      <c r="D124" s="14">
+        <v>49</v>
+      </c>
+      <c r="E124" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="F124" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="G124" s="14">
+        <v>5</v>
+      </c>
+      <c r="H124" s="14">
+        <v>5</v>
+      </c>
+      <c r="I124" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="J124" s="13"/>
+      <c r="K124" s="13"/>
+      <c r="L124" s="13"/>
+      <c r="M124" s="13"/>
+    </row>
+    <row r="125" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A125" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="B125" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="C125" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="D125" s="12">
+        <v>49</v>
+      </c>
+      <c r="E125" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="F125" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="G125" s="12">
+        <v>5</v>
+      </c>
+      <c r="H125" s="12">
+        <v>5</v>
+      </c>
+      <c r="I125" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="J125" s="11"/>
+      <c r="K125" s="11"/>
+      <c r="L125" s="11"/>
+      <c r="M125" s="11"/>
+    </row>
+    <row r="127" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A127" s="32" t="s">
+        <v>195</v>
+      </c>
+      <c r="B127" s="32"/>
+      <c r="C127" s="32"/>
+      <c r="D127" s="32"/>
+      <c r="E127" s="32"/>
+      <c r="F127" s="32"/>
+      <c r="G127" s="32"/>
+      <c r="H127" s="32"/>
+      <c r="I127" s="32"/>
+      <c r="J127" s="32"/>
+      <c r="K127" s="32"/>
+      <c r="L127" s="32"/>
+      <c r="M127" s="32"/>
+    </row>
+    <row r="128" spans="1:13" s="3" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A128" s="31" t="s">
+        <v>193</v>
+      </c>
+      <c r="B128" s="31"/>
+      <c r="C128" s="31"/>
+      <c r="D128" s="31"/>
+      <c r="E128" s="31"/>
+      <c r="F128" s="31"/>
+      <c r="G128" s="31"/>
+      <c r="H128" s="31"/>
+      <c r="I128" s="31"/>
+      <c r="J128" s="31"/>
+      <c r="K128" s="31"/>
+      <c r="L128" s="31"/>
+      <c r="M128" s="31"/>
+    </row>
+    <row r="129" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A129" s="26" t="s">
+        <v>189</v>
+      </c>
+      <c r="B129" s="26"/>
+      <c r="C129" s="26"/>
+      <c r="D129" s="26"/>
+      <c r="E129" s="26"/>
+      <c r="F129" s="26"/>
+      <c r="G129" s="26"/>
+      <c r="H129" s="26"/>
+      <c r="I129" s="26"/>
+      <c r="J129" s="26"/>
+      <c r="K129" s="26"/>
+      <c r="L129" s="26"/>
+      <c r="M129" s="26"/>
+    </row>
+    <row r="130" spans="1:13" s="4" customFormat="1" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A130" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B130" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C130" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="D130" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="E130" s="8"/>
+      <c r="F130" s="8"/>
+      <c r="G130" s="8"/>
+      <c r="H130" s="8"/>
+      <c r="I130" s="8"/>
+      <c r="J130" s="8"/>
+      <c r="K130" s="8"/>
+      <c r="L130" s="8"/>
+      <c r="M130" s="8"/>
+    </row>
+    <row r="131" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A131" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="B131" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="C60" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="D60" s="14"/>
-      <c r="E60" s="13"/>
-      <c r="F60" s="13"/>
-      <c r="G60" s="14"/>
-      <c r="H60" s="14"/>
-      <c r="I60" s="13"/>
-      <c r="J60" s="13"/>
-      <c r="K60" s="13"/>
-      <c r="L60" s="13"/>
-      <c r="M60" s="13"/>
-    </row>
-    <row r="61" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="B61" s="11" t="s">
-        <v>152</v>
-      </c>
-      <c r="C61" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="D61" s="12"/>
-      <c r="E61" s="11"/>
-      <c r="F61" s="11"/>
-      <c r="G61" s="12"/>
-      <c r="H61" s="12"/>
-      <c r="I61" s="11"/>
-      <c r="J61" s="11"/>
-      <c r="K61" s="11"/>
-      <c r="L61" s="11"/>
-      <c r="M61" s="11"/>
-    </row>
-    <row r="63" spans="1:16" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="43" t="s">
-        <v>148</v>
-      </c>
-      <c r="B63" s="43"/>
-      <c r="C63" s="43"/>
-      <c r="D63" s="43"/>
-      <c r="E63" s="43"/>
-      <c r="F63" s="43"/>
-      <c r="G63" s="43"/>
-      <c r="H63" s="43"/>
-      <c r="I63" s="43"/>
-      <c r="J63" s="43"/>
-      <c r="K63" s="43"/>
-      <c r="L63" s="43"/>
-      <c r="M63" s="43"/>
-      <c r="N63" s="43"/>
-      <c r="O63" s="43"/>
-      <c r="P63" s="43"/>
-    </row>
-    <row r="64" spans="1:16" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="22" t="s">
-        <v>170</v>
-      </c>
-      <c r="B64" s="22"/>
-      <c r="C64" s="22"/>
-      <c r="D64" s="22"/>
-      <c r="E64" s="22"/>
-      <c r="F64" s="22"/>
-      <c r="G64" s="22"/>
-      <c r="H64" s="22"/>
-      <c r="I64" s="22"/>
-      <c r="J64" s="22"/>
-      <c r="K64" s="22"/>
-      <c r="L64" s="22"/>
-      <c r="M64" s="22"/>
-      <c r="N64" s="22"/>
-      <c r="O64" s="22"/>
-      <c r="P64" s="22"/>
-    </row>
-    <row r="65" spans="1:16" s="3" customFormat="1" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B65" s="8" t="s">
-        <v>160</v>
-      </c>
-      <c r="C65" s="8" t="s">
-        <v>161</v>
-      </c>
-      <c r="D65" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="E65" s="23" t="s">
-        <v>162</v>
-      </c>
-      <c r="F65" s="24"/>
-      <c r="G65" s="23" t="s">
-        <v>163</v>
-      </c>
-      <c r="H65" s="24"/>
-      <c r="I65" s="23" t="s">
-        <v>164</v>
-      </c>
-      <c r="J65" s="24"/>
-      <c r="K65" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="L65" s="8" t="s">
-        <v>216</v>
-      </c>
-      <c r="M65" s="18" t="s">
-        <v>166</v>
-      </c>
-      <c r="N65" s="8" t="s">
-        <v>167</v>
-      </c>
-      <c r="O65" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="P65" s="8" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="66" spans="1:16" s="4" customFormat="1" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="B66" s="13">
-        <v>25</v>
-      </c>
-      <c r="C66" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="D66" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="E66" s="46" t="s">
-        <v>37</v>
-      </c>
-      <c r="F66" s="47"/>
-      <c r="G66" s="25" t="s">
-        <v>38</v>
-      </c>
-      <c r="H66" s="26"/>
-      <c r="I66" s="25" t="s">
-        <v>38</v>
-      </c>
-      <c r="J66" s="26"/>
-      <c r="K66" s="14" t="s">
-        <v>100</v>
-      </c>
-      <c r="L66" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="M66" s="19" t="s">
-        <v>217</v>
-      </c>
-      <c r="N66" s="13">
-        <v>5555555</v>
-      </c>
-      <c r="O66" s="13">
-        <v>5555555</v>
-      </c>
-      <c r="P66" s="13">
-        <v>555555</v>
-      </c>
-    </row>
-    <row r="67" spans="1:16" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="68" spans="1:16" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="33" t="s">
-        <v>154</v>
-      </c>
-      <c r="B68" s="33"/>
-      <c r="C68" s="33"/>
-      <c r="D68" s="33"/>
-      <c r="E68" s="33"/>
-      <c r="F68" s="33"/>
-      <c r="G68" s="33"/>
-      <c r="H68" s="33"/>
-      <c r="I68" s="33"/>
-      <c r="J68" s="33"/>
-      <c r="K68" s="33"/>
-      <c r="L68" s="33"/>
-      <c r="M68" s="33"/>
-    </row>
-    <row r="69" spans="1:16" s="3" customFormat="1" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B69" s="8" t="s">
-        <v>171</v>
-      </c>
-      <c r="C69" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D69" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="E69" s="8"/>
-      <c r="F69" s="8"/>
-      <c r="G69" s="8"/>
-      <c r="H69" s="8"/>
-      <c r="I69" s="8"/>
-      <c r="J69" s="8"/>
-      <c r="K69" s="8"/>
-      <c r="L69" s="8"/>
-      <c r="M69" s="8"/>
-    </row>
-    <row r="70" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="B70" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="C70" s="13" t="s">
-        <v>150</v>
-      </c>
-      <c r="D70" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="E70" s="13"/>
-      <c r="F70" s="13"/>
-      <c r="G70" s="14"/>
-      <c r="H70" s="14"/>
-      <c r="I70" s="13"/>
-      <c r="J70" s="13"/>
-      <c r="K70" s="13"/>
-      <c r="L70" s="13"/>
-      <c r="M70" s="13"/>
-    </row>
-    <row r="71" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="B71" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="C71" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="D71" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="E71" s="11"/>
-      <c r="F71" s="11"/>
-      <c r="G71" s="12"/>
-      <c r="H71" s="12"/>
-      <c r="I71" s="11"/>
-      <c r="J71" s="11"/>
-      <c r="K71" s="11"/>
-      <c r="L71" s="11"/>
-      <c r="M71" s="11"/>
-    </row>
-    <row r="73" spans="1:16" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="33" t="s">
-        <v>155</v>
-      </c>
-      <c r="B73" s="33"/>
-      <c r="C73" s="33"/>
-      <c r="D73" s="33"/>
-      <c r="E73" s="33"/>
-      <c r="F73" s="33"/>
-      <c r="G73" s="33"/>
-      <c r="H73" s="33"/>
-      <c r="I73" s="33"/>
-      <c r="J73" s="33"/>
-      <c r="K73" s="33"/>
-      <c r="L73" s="33"/>
-      <c r="M73" s="33"/>
-    </row>
-    <row r="74" spans="1:16" s="3" customFormat="1" ht="31.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B74" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="C74" s="29"/>
-      <c r="D74" s="27" t="s">
-        <v>156</v>
-      </c>
-      <c r="E74" s="29"/>
-      <c r="F74" s="8"/>
-      <c r="G74" s="8"/>
-      <c r="H74" s="8"/>
-      <c r="I74" s="8"/>
-      <c r="J74" s="8"/>
-      <c r="K74" s="8"/>
-      <c r="L74" s="8"/>
-      <c r="M74" s="8"/>
-    </row>
-    <row r="75" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="B75" s="40" t="s">
-        <v>43</v>
-      </c>
-      <c r="C75" s="41"/>
-      <c r="D75" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="E75" s="35"/>
-      <c r="F75" s="13"/>
-      <c r="G75" s="14"/>
-      <c r="H75" s="14"/>
-      <c r="I75" s="13"/>
-      <c r="J75" s="13"/>
-      <c r="K75" s="13"/>
-      <c r="L75" s="13"/>
-      <c r="M75" s="13"/>
-    </row>
-    <row r="76" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="B76" s="30" t="s">
-        <v>159</v>
-      </c>
-      <c r="C76" s="32"/>
-      <c r="D76" s="36" t="s">
-        <v>33</v>
-      </c>
-      <c r="E76" s="37"/>
-      <c r="F76" s="11"/>
-      <c r="G76" s="12"/>
-      <c r="H76" s="12"/>
-      <c r="I76" s="11"/>
-      <c r="J76" s="11"/>
-      <c r="K76" s="11"/>
-      <c r="L76" s="11"/>
-      <c r="M76" s="11"/>
-    </row>
-    <row r="78" spans="1:16" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="33" t="s">
-        <v>157</v>
-      </c>
-      <c r="B78" s="33"/>
-      <c r="C78" s="33"/>
-      <c r="D78" s="33"/>
-      <c r="E78" s="33"/>
-      <c r="F78" s="33"/>
-      <c r="G78" s="33"/>
-      <c r="H78" s="33"/>
-      <c r="I78" s="33"/>
-      <c r="J78" s="33"/>
-      <c r="K78" s="33"/>
-      <c r="L78" s="33"/>
-      <c r="M78" s="33"/>
-    </row>
-    <row r="79" spans="1:16" s="3" customFormat="1" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B79" s="8" t="s">
-        <v>207</v>
-      </c>
-      <c r="C79" s="8" t="s">
-        <v>208</v>
-      </c>
-      <c r="D79" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="E79" s="8"/>
-      <c r="F79" s="8"/>
-      <c r="G79" s="8"/>
-      <c r="H79" s="8"/>
-      <c r="I79" s="8"/>
-      <c r="J79" s="8"/>
-      <c r="K79" s="8"/>
-      <c r="L79" s="8"/>
-      <c r="M79" s="8"/>
-    </row>
-    <row r="80" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="B80" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="C80" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="D80" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="E80" s="13"/>
-      <c r="F80" s="13"/>
-      <c r="G80" s="14"/>
-      <c r="H80" s="14"/>
-      <c r="I80" s="13"/>
-      <c r="J80" s="13"/>
-      <c r="K80" s="13"/>
-      <c r="L80" s="13"/>
-      <c r="M80" s="13"/>
-    </row>
-    <row r="81" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="B81" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="C81" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="D81" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="E81" s="11"/>
-      <c r="F81" s="11"/>
-      <c r="G81" s="12"/>
-      <c r="H81" s="12"/>
-      <c r="I81" s="11"/>
-      <c r="J81" s="11"/>
-      <c r="K81" s="11"/>
-      <c r="L81" s="11"/>
-      <c r="M81" s="11"/>
-    </row>
-    <row r="83" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="33" t="s">
-        <v>180</v>
-      </c>
-      <c r="B83" s="33"/>
-      <c r="C83" s="33"/>
-      <c r="D83" s="33"/>
-      <c r="E83" s="33"/>
-      <c r="F83" s="33"/>
-      <c r="G83" s="33"/>
-      <c r="H83" s="33"/>
-      <c r="I83" s="33"/>
-      <c r="J83" s="33"/>
-      <c r="K83" s="33"/>
-      <c r="L83" s="33"/>
-      <c r="M83" s="33"/>
-    </row>
-    <row r="84" spans="1:13" s="3" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A84" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B84" s="28" t="s">
-        <v>178</v>
-      </c>
-      <c r="C84" s="28"/>
-      <c r="D84" s="27" t="s">
-        <v>179</v>
-      </c>
-      <c r="E84" s="28"/>
-      <c r="F84" s="29"/>
-      <c r="G84" s="8"/>
-      <c r="H84" s="8"/>
-      <c r="I84" s="8"/>
-      <c r="J84" s="8"/>
-      <c r="K84" s="8"/>
-      <c r="L84" s="8"/>
-      <c r="M84" s="8"/>
-    </row>
-    <row r="85" spans="1:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="B85" s="40" t="s">
-        <v>38</v>
-      </c>
-      <c r="C85" s="41"/>
-      <c r="D85" s="34" t="s">
-        <v>50</v>
-      </c>
-      <c r="E85" s="44"/>
-      <c r="F85" s="35"/>
-      <c r="G85" s="14"/>
-      <c r="H85" s="14"/>
-      <c r="I85" s="13"/>
-      <c r="J85" s="13"/>
-      <c r="K85" s="13"/>
-      <c r="L85" s="13"/>
-      <c r="M85" s="13"/>
-    </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B86" s="7"/>
-    </row>
-    <row r="87" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="33" t="s">
-        <v>172</v>
-      </c>
-      <c r="B87" s="33"/>
-      <c r="C87" s="33"/>
-      <c r="D87" s="33"/>
-      <c r="E87" s="33"/>
-      <c r="F87" s="33"/>
-      <c r="G87" s="33"/>
-      <c r="H87" s="33"/>
-      <c r="I87" s="33"/>
-      <c r="J87" s="33"/>
-      <c r="K87" s="33"/>
-      <c r="L87" s="33"/>
-      <c r="M87" s="33"/>
-    </row>
-    <row r="88" spans="1:13" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="42" t="s">
-        <v>173</v>
-      </c>
-      <c r="B88" s="42"/>
-      <c r="C88" s="42"/>
-      <c r="D88" s="42"/>
-      <c r="E88" s="42"/>
-      <c r="F88" s="42"/>
-      <c r="G88" s="42"/>
-      <c r="H88" s="42"/>
-      <c r="I88" s="42"/>
-      <c r="J88" s="42"/>
-      <c r="K88" s="42"/>
-      <c r="L88" s="42"/>
-      <c r="M88" s="42"/>
-    </row>
-    <row r="89" spans="1:13" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A89" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B89" s="8" t="s">
-        <v>209</v>
-      </c>
-      <c r="C89" s="27" t="s">
-        <v>51</v>
-      </c>
-      <c r="D89" s="28"/>
-      <c r="E89" s="29"/>
-      <c r="F89" s="8"/>
-      <c r="G89" s="8"/>
-      <c r="H89" s="8"/>
-      <c r="I89" s="8"/>
-      <c r="J89" s="8"/>
-      <c r="K89" s="8"/>
-      <c r="L89" s="8"/>
-      <c r="M89" s="8"/>
-    </row>
-    <row r="90" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="B90" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="C90" s="40" t="s">
-        <v>219</v>
-      </c>
-      <c r="D90" s="45"/>
-      <c r="E90" s="41"/>
-      <c r="F90" s="13"/>
-      <c r="G90" s="14"/>
-      <c r="H90" s="14"/>
-      <c r="I90" s="13"/>
-      <c r="J90" s="13"/>
-      <c r="K90" s="13"/>
-      <c r="L90" s="13"/>
-      <c r="M90" s="13"/>
-    </row>
-    <row r="91" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A91" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="B91" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="C91" s="30"/>
-      <c r="D91" s="31"/>
-      <c r="E91" s="32"/>
-      <c r="F91" s="11"/>
-      <c r="G91" s="12"/>
-      <c r="H91" s="12"/>
-      <c r="I91" s="11"/>
-      <c r="J91" s="11"/>
-      <c r="K91" s="11"/>
-      <c r="L91" s="11"/>
-      <c r="M91" s="11"/>
-    </row>
-    <row r="92" spans="1:13" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="93" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A93" s="43" t="s">
-        <v>181</v>
-      </c>
-      <c r="B93" s="43"/>
-      <c r="C93" s="43"/>
-      <c r="D93" s="43"/>
-      <c r="E93" s="43"/>
-      <c r="F93" s="43"/>
-      <c r="G93" s="43"/>
-      <c r="H93" s="43"/>
-      <c r="I93" s="43"/>
-      <c r="J93" s="43"/>
-      <c r="K93" s="43"/>
-      <c r="L93" s="43"/>
-      <c r="M93" s="43"/>
-    </row>
-    <row r="94" spans="1:13" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A94" s="42" t="s">
-        <v>185</v>
-      </c>
-      <c r="B94" s="42"/>
-      <c r="C94" s="42"/>
-      <c r="D94" s="42"/>
-      <c r="E94" s="42"/>
-      <c r="F94" s="42"/>
-      <c r="G94" s="42"/>
-      <c r="H94" s="42"/>
-      <c r="I94" s="42"/>
-      <c r="J94" s="42"/>
-      <c r="K94" s="42"/>
-      <c r="L94" s="42"/>
-      <c r="M94" s="42"/>
-    </row>
-    <row r="95" spans="1:13" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A95" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B95" s="8" t="s">
-        <v>175</v>
-      </c>
-      <c r="C95" s="8" t="s">
-        <v>174</v>
-      </c>
-      <c r="D95" s="8" t="s">
-        <v>176</v>
-      </c>
-      <c r="E95" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="F95" s="8" t="s">
-        <v>177</v>
-      </c>
-      <c r="G95" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="H95" s="8"/>
-      <c r="I95" s="8"/>
-      <c r="J95" s="8"/>
-      <c r="K95" s="8"/>
-      <c r="L95" s="8"/>
-      <c r="M95" s="8"/>
-    </row>
-    <row r="96" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A96" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="B96" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="C96" s="13">
-        <v>162</v>
-      </c>
-      <c r="D96" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="E96" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="F96" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="G96" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="H96" s="14"/>
-      <c r="I96" s="13"/>
-      <c r="J96" s="13"/>
-      <c r="K96" s="13"/>
-      <c r="L96" s="13"/>
-      <c r="M96" s="13"/>
-    </row>
-    <row r="97" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A97" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="B97" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="C97" s="11">
-        <v>162</v>
-      </c>
-      <c r="D97" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="E97" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="F97" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="G97" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="H97" s="12"/>
-      <c r="I97" s="11"/>
-      <c r="J97" s="11"/>
-      <c r="K97" s="11"/>
-      <c r="L97" s="11"/>
-      <c r="M97" s="11"/>
-    </row>
-    <row r="98" spans="1:13" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="99" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A99" s="33" t="s">
-        <v>182</v>
-      </c>
-      <c r="B99" s="33"/>
-      <c r="C99" s="33"/>
-      <c r="D99" s="33"/>
-      <c r="E99" s="33"/>
-      <c r="F99" s="33"/>
-      <c r="G99" s="33"/>
-      <c r="H99" s="33"/>
-      <c r="I99" s="33"/>
-      <c r="J99" s="33"/>
-      <c r="K99" s="33"/>
-      <c r="L99" s="33"/>
-      <c r="M99" s="33"/>
-    </row>
-    <row r="100" spans="1:13" s="3" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A100" s="42" t="s">
-        <v>183</v>
-      </c>
-      <c r="B100" s="42"/>
-      <c r="C100" s="42"/>
-      <c r="D100" s="42"/>
-      <c r="E100" s="42"/>
-      <c r="F100" s="42"/>
-      <c r="G100" s="42"/>
-      <c r="H100" s="42"/>
-      <c r="I100" s="42"/>
-      <c r="J100" s="42"/>
-      <c r="K100" s="42"/>
-      <c r="L100" s="42"/>
-      <c r="M100" s="42"/>
-    </row>
-    <row r="101" spans="1:13" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A101" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B101" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="C101" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="D101" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="E101" s="8" t="s">
-        <v>184</v>
-      </c>
-      <c r="F101" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="G101" s="8"/>
-      <c r="H101" s="8"/>
-      <c r="I101" s="8"/>
-      <c r="J101" s="8"/>
-      <c r="K101" s="8"/>
-      <c r="L101" s="8"/>
-      <c r="M101" s="8"/>
-    </row>
-    <row r="102" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A102" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="B102" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="C102" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="D102" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="E102" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="F102" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="G102" s="14"/>
-      <c r="H102" s="14"/>
-      <c r="I102" s="13"/>
-      <c r="J102" s="13"/>
-      <c r="K102" s="13"/>
-      <c r="L102" s="13"/>
-      <c r="M102" s="13"/>
-    </row>
-    <row r="103" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A103" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="B103" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="C103" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="D103" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="E103" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="F103" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="G103" s="12"/>
-      <c r="H103" s="12"/>
-      <c r="I103" s="11"/>
-      <c r="J103" s="11"/>
-      <c r="K103" s="11"/>
-      <c r="L103" s="11"/>
-      <c r="M103" s="11"/>
-    </row>
-    <row r="104" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A104" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="B104" s="13" t="s">
+      <c r="C131" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="D131" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="C104" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="D104" s="14"/>
-      <c r="E104" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="F104" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="G104" s="14"/>
-      <c r="H104" s="14"/>
-      <c r="I104" s="13"/>
-      <c r="J104" s="13"/>
-      <c r="K104" s="13"/>
-      <c r="L104" s="13"/>
-      <c r="M104" s="13"/>
-    </row>
-    <row r="105" spans="1:13" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="106" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A106" s="33" t="s">
-        <v>186</v>
-      </c>
-      <c r="B106" s="33"/>
-      <c r="C106" s="33"/>
-      <c r="D106" s="33"/>
-      <c r="E106" s="33"/>
-      <c r="F106" s="33"/>
-      <c r="G106" s="33"/>
-      <c r="H106" s="33"/>
-      <c r="I106" s="33"/>
-      <c r="J106" s="33"/>
-      <c r="K106" s="33"/>
-      <c r="L106" s="33"/>
-      <c r="M106" s="33"/>
-    </row>
-    <row r="107" spans="1:13" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A107" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B107" s="8" t="s">
-        <v>193</v>
-      </c>
-      <c r="C107" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="D107" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="E107" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="F107" s="8" t="s">
-        <v>192</v>
-      </c>
-      <c r="G107" s="8" t="s">
-        <v>191</v>
-      </c>
-      <c r="H107" s="8" t="s">
-        <v>190</v>
-      </c>
-      <c r="I107" s="8" t="s">
-        <v>189</v>
-      </c>
-      <c r="J107" s="8" t="s">
-        <v>188</v>
-      </c>
-      <c r="K107" s="8"/>
-      <c r="L107" s="8"/>
-      <c r="M107" s="8"/>
-    </row>
-    <row r="108" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A108" s="13" t="s">
+      <c r="E131" s="16"/>
+      <c r="F131" s="16"/>
+      <c r="G131" s="16"/>
+      <c r="H131" s="16"/>
+      <c r="I131" s="16"/>
+      <c r="J131" s="16"/>
+      <c r="K131" s="16"/>
+      <c r="L131" s="16"/>
+      <c r="M131" s="16"/>
+    </row>
+    <row r="132" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A132" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="B108" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="C108" s="13">
-        <v>514</v>
-      </c>
-      <c r="D108" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="E108" s="13" t="s">
+      <c r="B132" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="F108" s="13" t="s">
+      <c r="C132" s="17"/>
+      <c r="D132" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="G108" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="H108" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="I108" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="J108" s="13" t="s">
-        <v>187</v>
-      </c>
-      <c r="K108" s="13"/>
-      <c r="L108" s="13"/>
-      <c r="M108" s="13"/>
-    </row>
-    <row r="109" spans="1:13" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="110" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A110" s="33" t="s">
-        <v>194</v>
-      </c>
-      <c r="B110" s="33"/>
-      <c r="C110" s="33"/>
-      <c r="D110" s="33"/>
-      <c r="E110" s="33"/>
-      <c r="F110" s="33"/>
-      <c r="G110" s="33"/>
-      <c r="H110" s="33"/>
-      <c r="I110" s="33"/>
-      <c r="J110" s="33"/>
-      <c r="K110" s="33"/>
-      <c r="L110" s="33"/>
-      <c r="M110" s="33"/>
-    </row>
-    <row r="111" spans="1:13" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="39" t="s">
-        <v>200</v>
-      </c>
-      <c r="B111" s="39"/>
-      <c r="C111" s="39"/>
-      <c r="D111" s="39"/>
-      <c r="E111" s="39"/>
-      <c r="F111" s="39"/>
-      <c r="G111" s="39"/>
-      <c r="H111" s="39"/>
-      <c r="I111" s="39"/>
-      <c r="J111" s="39"/>
-      <c r="K111" s="39"/>
-      <c r="L111" s="39"/>
-      <c r="M111" s="39"/>
-    </row>
-    <row r="112" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="22" t="s">
-        <v>108</v>
-      </c>
-      <c r="B112" s="22"/>
-      <c r="C112" s="22"/>
-      <c r="D112" s="22"/>
-      <c r="E112" s="22"/>
-      <c r="F112" s="22"/>
-      <c r="G112" s="22"/>
-      <c r="H112" s="22"/>
-      <c r="I112" s="22"/>
-      <c r="J112" s="22"/>
-      <c r="K112" s="22"/>
-      <c r="L112" s="22"/>
-      <c r="M112" s="22"/>
-    </row>
-    <row r="113" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A113" s="48" t="s">
-        <v>201</v>
-      </c>
-      <c r="B113" s="48"/>
-      <c r="C113" s="48"/>
-      <c r="D113" s="48"/>
-      <c r="E113" s="48"/>
-      <c r="F113" s="48"/>
-      <c r="G113" s="48"/>
-      <c r="H113" s="48"/>
-      <c r="I113" s="48"/>
-      <c r="J113" s="48"/>
-      <c r="K113" s="48"/>
-      <c r="L113" s="48"/>
-      <c r="M113" s="48"/>
-    </row>
-    <row r="114" spans="1:13" s="4" customFormat="1" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A114" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B114" s="8" t="s">
-        <v>197</v>
-      </c>
-      <c r="C114" s="8" t="s">
-        <v>198</v>
-      </c>
-      <c r="D114" s="8" t="s">
-        <v>199</v>
-      </c>
-      <c r="E114" s="8" t="s">
-        <v>206</v>
-      </c>
-      <c r="F114" s="8" t="s">
-        <v>196</v>
-      </c>
-      <c r="G114" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="H114" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="I114" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="J114" s="8"/>
-      <c r="K114" s="8"/>
-      <c r="L114" s="8"/>
-      <c r="M114" s="8"/>
-    </row>
-    <row r="115" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A115" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="B115" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="C115" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="D115" s="14">
-        <v>1812</v>
-      </c>
-      <c r="E115" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="F115" s="13" t="s">
-        <v>195</v>
-      </c>
-      <c r="G115" s="14">
-        <v>5</v>
-      </c>
-      <c r="H115" s="14">
-        <v>5</v>
-      </c>
-      <c r="I115" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="J115" s="13"/>
-      <c r="K115" s="13"/>
-      <c r="L115" s="13"/>
-      <c r="M115" s="13"/>
-    </row>
-    <row r="116" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A116" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="B116" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="C116" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="D116" s="12">
-        <v>1812</v>
-      </c>
-      <c r="E116" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="F116" s="11" t="s">
-        <v>195</v>
-      </c>
-      <c r="G116" s="12">
-        <v>5</v>
-      </c>
-      <c r="H116" s="12">
-        <v>5</v>
-      </c>
-      <c r="I116" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="J116" s="11"/>
-      <c r="K116" s="11"/>
-      <c r="L116" s="11"/>
-      <c r="M116" s="11"/>
-    </row>
-    <row r="117" spans="1:13" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="118" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A118" s="33" t="s">
-        <v>210</v>
-      </c>
-      <c r="B118" s="33"/>
-      <c r="C118" s="33"/>
-      <c r="D118" s="33"/>
-      <c r="E118" s="33"/>
-      <c r="F118" s="33"/>
-      <c r="G118" s="33"/>
-      <c r="H118" s="33"/>
-      <c r="I118" s="33"/>
-      <c r="J118" s="33"/>
-      <c r="K118" s="33"/>
-      <c r="L118" s="33"/>
-      <c r="M118" s="33"/>
-    </row>
-    <row r="119" spans="1:13" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="39" t="s">
-        <v>200</v>
-      </c>
-      <c r="B119" s="39"/>
-      <c r="C119" s="39"/>
-      <c r="D119" s="39"/>
-      <c r="E119" s="39"/>
-      <c r="F119" s="39"/>
-      <c r="G119" s="39"/>
-      <c r="H119" s="39"/>
-      <c r="I119" s="39"/>
-      <c r="J119" s="39"/>
-      <c r="K119" s="39"/>
-      <c r="L119" s="39"/>
-      <c r="M119" s="39"/>
-    </row>
-    <row r="120" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="22" t="s">
-        <v>108</v>
-      </c>
-      <c r="B120" s="22"/>
-      <c r="C120" s="22"/>
-      <c r="D120" s="22"/>
-      <c r="E120" s="22"/>
-      <c r="F120" s="22"/>
-      <c r="G120" s="22"/>
-      <c r="H120" s="22"/>
-      <c r="I120" s="22"/>
-      <c r="J120" s="22"/>
-      <c r="K120" s="22"/>
-      <c r="L120" s="22"/>
-      <c r="M120" s="22"/>
-    </row>
-    <row r="121" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A121" s="48" t="s">
-        <v>202</v>
-      </c>
-      <c r="B121" s="48"/>
-      <c r="C121" s="48"/>
-      <c r="D121" s="48"/>
-      <c r="E121" s="48"/>
-      <c r="F121" s="48"/>
-      <c r="G121" s="48"/>
-      <c r="H121" s="48"/>
-      <c r="I121" s="48"/>
-      <c r="J121" s="48"/>
-      <c r="K121" s="48"/>
-      <c r="L121" s="48"/>
-      <c r="M121" s="48"/>
-    </row>
-    <row r="122" spans="1:13" s="4" customFormat="1" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A122" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B122" s="10" t="s">
-        <v>197</v>
-      </c>
-      <c r="C122" s="10" t="s">
-        <v>205</v>
-      </c>
-      <c r="D122" s="10" t="s">
-        <v>204</v>
-      </c>
-      <c r="E122" s="10" t="s">
-        <v>206</v>
-      </c>
-      <c r="F122" s="10" t="s">
-        <v>203</v>
-      </c>
-      <c r="G122" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="H122" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="I122" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="J122" s="10"/>
-      <c r="K122" s="10"/>
-      <c r="L122" s="10"/>
-      <c r="M122" s="10"/>
-    </row>
-    <row r="123" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A123" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="B123" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="C123" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="D123" s="14">
-        <v>49</v>
-      </c>
-      <c r="E123" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="F123" s="13" t="s">
-        <v>195</v>
-      </c>
-      <c r="G123" s="14">
-        <v>5</v>
-      </c>
-      <c r="H123" s="14">
-        <v>5</v>
-      </c>
-      <c r="I123" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="J123" s="13"/>
-      <c r="K123" s="13"/>
-      <c r="L123" s="13"/>
-      <c r="M123" s="13"/>
-    </row>
-    <row r="124" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A124" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="B124" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="C124" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="D124" s="12">
-        <v>49</v>
-      </c>
-      <c r="E124" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="F124" s="11" t="s">
-        <v>195</v>
-      </c>
-      <c r="G124" s="12">
-        <v>5</v>
-      </c>
-      <c r="H124" s="12">
-        <v>5</v>
-      </c>
-      <c r="I124" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="J124" s="11"/>
-      <c r="K124" s="11"/>
-      <c r="L124" s="11"/>
-      <c r="M124" s="11"/>
-    </row>
-    <row r="126" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A126" s="38" t="s">
-        <v>218</v>
-      </c>
-      <c r="B126" s="38"/>
-      <c r="C126" s="38"/>
-      <c r="D126" s="38"/>
-      <c r="E126" s="38"/>
-      <c r="F126" s="38"/>
-      <c r="G126" s="38"/>
-      <c r="H126" s="38"/>
-      <c r="I126" s="38"/>
-      <c r="J126" s="38"/>
-      <c r="K126" s="38"/>
-      <c r="L126" s="38"/>
-      <c r="M126" s="38"/>
-    </row>
-    <row r="127" spans="1:13" s="3" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A127" s="39" t="s">
-        <v>215</v>
-      </c>
-      <c r="B127" s="39"/>
-      <c r="C127" s="39"/>
-      <c r="D127" s="39"/>
-      <c r="E127" s="39"/>
-      <c r="F127" s="39"/>
-      <c r="G127" s="39"/>
-      <c r="H127" s="39"/>
-      <c r="I127" s="39"/>
-      <c r="J127" s="39"/>
-      <c r="K127" s="39"/>
-      <c r="L127" s="39"/>
-      <c r="M127" s="39"/>
-    </row>
-    <row r="128" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A128" s="22" t="s">
-        <v>211</v>
-      </c>
-      <c r="B128" s="22"/>
-      <c r="C128" s="22"/>
-      <c r="D128" s="22"/>
-      <c r="E128" s="22"/>
-      <c r="F128" s="22"/>
-      <c r="G128" s="22"/>
-      <c r="H128" s="22"/>
-      <c r="I128" s="22"/>
-      <c r="J128" s="22"/>
-      <c r="K128" s="22"/>
-      <c r="L128" s="22"/>
-      <c r="M128" s="22"/>
-    </row>
-    <row r="129" spans="1:13" s="4" customFormat="1" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A129" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B129" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="C129" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="D129" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="E129" s="8"/>
-      <c r="F129" s="8"/>
-      <c r="G129" s="8"/>
-      <c r="H129" s="8"/>
-      <c r="I129" s="8"/>
-      <c r="J129" s="8"/>
-      <c r="K129" s="8"/>
-      <c r="L129" s="8"/>
-      <c r="M129" s="8"/>
-    </row>
-    <row r="130" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A130" s="16" t="s">
-        <v>95</v>
-      </c>
-      <c r="B130" s="16" t="s">
-        <v>96</v>
-      </c>
-      <c r="C130" s="16" t="s">
-        <v>92</v>
-      </c>
-      <c r="D130" s="16" t="s">
-        <v>91</v>
-      </c>
-      <c r="E130" s="16"/>
-      <c r="F130" s="16"/>
-      <c r="G130" s="16"/>
-      <c r="H130" s="16"/>
-      <c r="I130" s="16"/>
-      <c r="J130" s="16"/>
-      <c r="K130" s="16"/>
-      <c r="L130" s="16"/>
-      <c r="M130" s="16"/>
-    </row>
-    <row r="131" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A131" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="B131" s="17" t="s">
-        <v>97</v>
-      </c>
-      <c r="C131" s="17"/>
-      <c r="D131" s="17" t="s">
-        <v>98</v>
-      </c>
-      <c r="E131" s="17"/>
-      <c r="F131" s="17"/>
-      <c r="G131" s="17"/>
-      <c r="H131" s="17"/>
-      <c r="I131" s="17"/>
-      <c r="J131" s="17"/>
-      <c r="K131" s="17"/>
-      <c r="L131" s="17"/>
-      <c r="M131" s="17"/>
+      <c r="E132" s="17"/>
+      <c r="F132" s="17"/>
+      <c r="G132" s="17"/>
+      <c r="H132" s="17"/>
+      <c r="I132" s="17"/>
+      <c r="J132" s="17"/>
+      <c r="K132" s="17"/>
+      <c r="L132" s="17"/>
+      <c r="M132" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="55">
+    <mergeCell ref="I66:J66"/>
+    <mergeCell ref="I67:J67"/>
+    <mergeCell ref="C90:E90"/>
+    <mergeCell ref="C92:E92"/>
+    <mergeCell ref="A84:M84"/>
+    <mergeCell ref="A69:M69"/>
+    <mergeCell ref="A74:M74"/>
+    <mergeCell ref="A79:M79"/>
+    <mergeCell ref="B77:C77"/>
+    <mergeCell ref="G66:H66"/>
+    <mergeCell ref="G67:H67"/>
+    <mergeCell ref="D76:E76"/>
+    <mergeCell ref="D77:E77"/>
+    <mergeCell ref="E66:F66"/>
+    <mergeCell ref="E67:F67"/>
+    <mergeCell ref="A127:M127"/>
+    <mergeCell ref="A128:M128"/>
+    <mergeCell ref="A129:M129"/>
+    <mergeCell ref="B85:C85"/>
+    <mergeCell ref="B86:C86"/>
+    <mergeCell ref="A89:M89"/>
+    <mergeCell ref="A94:M94"/>
+    <mergeCell ref="A100:M100"/>
+    <mergeCell ref="A101:M101"/>
+    <mergeCell ref="A95:M95"/>
+    <mergeCell ref="D85:F85"/>
+    <mergeCell ref="D86:F86"/>
+    <mergeCell ref="C91:E91"/>
+    <mergeCell ref="A120:M120"/>
+    <mergeCell ref="A122:M122"/>
+    <mergeCell ref="A121:M121"/>
+    <mergeCell ref="A114:M114"/>
+    <mergeCell ref="A119:M119"/>
+    <mergeCell ref="A88:M88"/>
+    <mergeCell ref="A49:M49"/>
+    <mergeCell ref="A58:M58"/>
+    <mergeCell ref="A59:M59"/>
+    <mergeCell ref="A64:P64"/>
+    <mergeCell ref="A54:M54"/>
+    <mergeCell ref="A113:M113"/>
+    <mergeCell ref="D75:E75"/>
+    <mergeCell ref="B75:C75"/>
+    <mergeCell ref="B76:C76"/>
+    <mergeCell ref="A107:M107"/>
+    <mergeCell ref="A111:M111"/>
+    <mergeCell ref="A112:M112"/>
+    <mergeCell ref="A65:P65"/>
     <mergeCell ref="A5:M5"/>
     <mergeCell ref="A1:M1"/>
     <mergeCell ref="A33:M33"/>
@@ -4572,53 +4645,6 @@
     <mergeCell ref="A6:M6"/>
     <mergeCell ref="A34:M34"/>
     <mergeCell ref="A23:M23"/>
-    <mergeCell ref="A113:M113"/>
-    <mergeCell ref="A118:M118"/>
-    <mergeCell ref="A87:M87"/>
-    <mergeCell ref="A49:M49"/>
-    <mergeCell ref="A57:M57"/>
-    <mergeCell ref="A58:M58"/>
-    <mergeCell ref="A63:P63"/>
-    <mergeCell ref="A53:M53"/>
-    <mergeCell ref="A112:M112"/>
-    <mergeCell ref="D74:E74"/>
-    <mergeCell ref="B74:C74"/>
-    <mergeCell ref="B75:C75"/>
-    <mergeCell ref="A106:M106"/>
-    <mergeCell ref="A110:M110"/>
-    <mergeCell ref="A111:M111"/>
-    <mergeCell ref="A126:M126"/>
-    <mergeCell ref="A127:M127"/>
-    <mergeCell ref="A128:M128"/>
-    <mergeCell ref="B84:C84"/>
-    <mergeCell ref="B85:C85"/>
-    <mergeCell ref="A88:M88"/>
-    <mergeCell ref="A93:M93"/>
-    <mergeCell ref="A99:M99"/>
-    <mergeCell ref="A100:M100"/>
-    <mergeCell ref="A94:M94"/>
-    <mergeCell ref="D84:F84"/>
-    <mergeCell ref="D85:F85"/>
-    <mergeCell ref="C90:E90"/>
-    <mergeCell ref="A119:M119"/>
-    <mergeCell ref="A121:M121"/>
-    <mergeCell ref="A120:M120"/>
-    <mergeCell ref="A64:P64"/>
-    <mergeCell ref="I65:J65"/>
-    <mergeCell ref="I66:J66"/>
-    <mergeCell ref="C89:E89"/>
-    <mergeCell ref="C91:E91"/>
-    <mergeCell ref="A83:M83"/>
-    <mergeCell ref="A68:M68"/>
-    <mergeCell ref="A73:M73"/>
-    <mergeCell ref="A78:M78"/>
-    <mergeCell ref="B76:C76"/>
-    <mergeCell ref="G65:H65"/>
-    <mergeCell ref="G66:H66"/>
-    <mergeCell ref="D75:E75"/>
-    <mergeCell ref="D76:E76"/>
-    <mergeCell ref="E65:F65"/>
-    <mergeCell ref="E66:F66"/>
   </mergeCells>
   <dataValidations count="52">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A3" xr:uid="{00000000-0002-0000-0000-000000000000}">
@@ -4637,7 +4663,7 @@
       <formula1>5</formula1>
       <formula2>3097</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Node ID" error="Valid Node ID is between 101 and 4000" sqref="C51 D8:D21 D25:E31" xr:uid="{00000000-0002-0000-0000-000005000000}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Node ID" error="Valid Node ID is between 101 and 4000" sqref="D25:E31 D8:D21 C51:C52" xr:uid="{00000000-0002-0000-0000-000005000000}">
       <formula1>101</formula1>
       <formula2>4000</formula2>
     </dataValidation>
@@ -4662,129 +4688,129 @@
       <formula1>1</formula1>
       <formula2>7</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A51" xr:uid="{00000000-0002-0000-0000-00000C000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A51:A52" xr:uid="{00000000-0002-0000-0000-00000C000000}">
       <formula1>"bgp_rr"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B55 D70:D71 D80:D81 G96:G97 D108 I115:I116 I123:I124 D66" xr:uid="{00000000-0002-0000-0000-00000D000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B56 D71:D72 D81:D82 G97:G98 D109 I116:I117 I124:I125 D67" xr:uid="{00000000-0002-0000-0000-00000D000000}">
       <formula1>"inband,oob"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A55" xr:uid="{00000000-0002-0000-0000-00000E000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A56" xr:uid="{00000000-0002-0000-0000-00000E000000}">
       <formula1>"dns_mgmt"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A60:A61" xr:uid="{00000000-0002-0000-0000-00000F000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A61:A62" xr:uid="{00000000-0002-0000-0000-00000F000000}">
       <formula1>"dns"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C60:C61 D75:D76" xr:uid="{00000000-0002-0000-0000-000010000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C61:C62 D76:D77" xr:uid="{00000000-0002-0000-0000-000010000000}">
       <formula1>"no,yes"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A66" xr:uid="{00000000-0002-0000-0000-000011000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A67" xr:uid="{00000000-0002-0000-0000-000011000000}">
       <formula1>"smartcallhome"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C70:C71" xr:uid="{00000000-0002-0000-0000-000012000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C71:C72" xr:uid="{00000000-0002-0000-0000-000012000000}">
       <formula1>"false,true"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A75:A76" xr:uid="{00000000-0002-0000-0000-000013000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A76:A77" xr:uid="{00000000-0002-0000-0000-000013000000}">
       <formula1>"search_domain"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A70:A71" xr:uid="{00000000-0002-0000-0000-000014000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A71:A72" xr:uid="{00000000-0002-0000-0000-000014000000}">
       <formula1>"ntp"</formula1>
     </dataValidation>
-    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Community String" error="The SNMP Community can be 1 to 32 characters and contain letters, numbers, and [.\-]. No other special characters" sqref="B90:B91" xr:uid="{00000000-0002-0000-0000-000015000000}">
+    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Community String" error="The SNMP Community can be 1 to 32 characters and contain letters, numbers, and [.\-]. No other special characters" sqref="B91:B92" xr:uid="{00000000-0002-0000-0000-000015000000}">
       <formula1>1</formula1>
       <formula2>32</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A85" xr:uid="{00000000-0002-0000-0000-000016000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A86" xr:uid="{00000000-0002-0000-0000-000016000000}">
       <formula1>"snmp_info"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A90:A91" xr:uid="{00000000-0002-0000-0000-000017000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A91:A92" xr:uid="{00000000-0002-0000-0000-000017000000}">
       <formula1>"snmp_comm"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C102:C104" xr:uid="{00000000-0002-0000-0000-000018000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C103:C105" xr:uid="{00000000-0002-0000-0000-000018000000}">
       <formula1>"aes-128,des,none"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E102:E104" xr:uid="{00000000-0002-0000-0000-000019000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E103:E105" xr:uid="{00000000-0002-0000-0000-000019000000}">
       <formula1>"md5,sha1"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D96:D97" xr:uid="{00000000-0002-0000-0000-00001A000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D97:D98" xr:uid="{00000000-0002-0000-0000-00001A000000}">
       <formula1>"v1,v2c,v3"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A102:A104" xr:uid="{00000000-0002-0000-0000-00001B000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A103:A105" xr:uid="{00000000-0002-0000-0000-00001B000000}">
       <formula1>"snmp_user"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E108 H108" xr:uid="{00000000-0002-0000-0000-00001C000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E109 H109" xr:uid="{00000000-0002-0000-0000-00001C000000}">
       <formula1>"emergencies,alerts,critical,errors,warnings,notifications,information,debugging"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F108" xr:uid="{00000000-0002-0000-0000-00001D000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F109" xr:uid="{00000000-0002-0000-0000-00001D000000}">
       <formula1>"local0,local1,local2,local3,local4,local5,local6,local7"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G108 I108" xr:uid="{00000000-0002-0000-0000-00001E000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G109 I109" xr:uid="{00000000-0002-0000-0000-00001E000000}">
       <formula1>"enabled,disabled"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J108" xr:uid="{00000000-0002-0000-0000-00001F000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J109" xr:uid="{00000000-0002-0000-0000-00001F000000}">
       <formula1>"emergencies,alerts,critical"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A108" xr:uid="{00000000-0002-0000-0000-000020000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A109" xr:uid="{00000000-0002-0000-0000-000020000000}">
       <formula1>"syslog"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F115:F116 F123:F124" xr:uid="{00000000-0002-0000-0000-000021000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F116:F117 F124:F125" xr:uid="{00000000-0002-0000-0000-000021000000}">
       <formula1>"chap,mschap,pap"</formula1>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="RADIUS Timeout" error="Timeout should be between 5 and 60 and be a Factor of 5.  Default is 5" sqref="G115:G116" xr:uid="{00000000-0002-0000-0000-000022000000}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="RADIUS Timeout" error="Timeout should be between 5 and 60 and be a Factor of 5.  Default is 5" sqref="G116:G117" xr:uid="{00000000-0002-0000-0000-000022000000}">
       <formula1>5</formula1>
       <formula2>60</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="RADIUS Retry" error="Retry should be a number between 1 and 5.  Default is 1" sqref="H115:H116" xr:uid="{00000000-0002-0000-0000-000023000000}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="RADIUS Retry" error="Retry should be a number between 1 and 5.  Default is 1" sqref="H116:H117" xr:uid="{00000000-0002-0000-0000-000023000000}">
       <formula1>1</formula1>
       <formula2>5</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="TACACS Timeout" error="Timeout should be between 5 and 60 and be a Factor of 5.  Default is 5" sqref="G123:G124" xr:uid="{00000000-0002-0000-0000-000024000000}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="TACACS Timeout" error="Timeout should be between 5 and 60 and be a Factor of 5.  Default is 5" sqref="G124:G125" xr:uid="{00000000-0002-0000-0000-000024000000}">
       <formula1>5</formula1>
       <formula2>60</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="TACACS Retry" error="Retry should be a number between 1 and 5.  Default is 1" sqref="H123:H124" xr:uid="{00000000-0002-0000-0000-000025000000}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="TACACS Retry" error="Retry should be a number between 1 and 5.  Default is 1" sqref="H124:H125" xr:uid="{00000000-0002-0000-0000-000025000000}">
       <formula1>1</formula1>
       <formula2>5</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Syslog Port" error="Valid Port Range is between 1 and 65535.  Default is 514" sqref="C108" xr:uid="{00000000-0002-0000-0000-000026000000}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Syslog Port" error="Valid Port Range is between 1 and 65535.  Default is 514" sqref="C109" xr:uid="{00000000-0002-0000-0000-000026000000}">
       <formula1>1</formula1>
       <formula2>65535</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="RADIUS Port" error="Valid Port Range is between 1 and 65535. Default is 1812" sqref="D115:D116" xr:uid="{00000000-0002-0000-0000-000027000000}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="RADIUS Port" error="Valid Port Range is between 1 and 65535. Default is 1812" sqref="D116:D117" xr:uid="{00000000-0002-0000-0000-000027000000}">
       <formula1>1</formula1>
       <formula2>65535</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="TACACS Port" error="Valid Port Range is between 1 and 65535. Default is 49" sqref="D123:D124" xr:uid="{00000000-0002-0000-0000-000028000000}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="TACACS Port" error="Valid Port Range is between 1 and 65535. Default is 49" sqref="D124:D125" xr:uid="{00000000-0002-0000-0000-000028000000}">
       <formula1>1</formula1>
       <formula2>65535</formula2>
     </dataValidation>
-    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Login Domain" error="Maximum length is 10 Alpha Numberic Characters or an underscore &quot;_&quot;.  But it must not begin with a underscore &quot;_&quot;." sqref="B123:B124" xr:uid="{00000000-0002-0000-0000-000029000000}">
+    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Login Domain" error="Maximum length is 10 Alpha Numberic Characters or an underscore &quot;_&quot;.  But it must not begin with a underscore &quot;_&quot;." sqref="B124:B125" xr:uid="{00000000-0002-0000-0000-000029000000}">
       <formula1>1</formula1>
       <formula2>10</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A123:A124" xr:uid="{00000000-0002-0000-0000-00002A000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A124:A125" xr:uid="{00000000-0002-0000-0000-00002A000000}">
       <formula1>"tacacs"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A115:A116" xr:uid="{00000000-0002-0000-0000-00002B000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A116:A117" xr:uid="{00000000-0002-0000-0000-00002B000000}">
       <formula1>"radius"</formula1>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SNMP Trap Port" error="Valid Port Range is between 1 and 65535.  Default is 162" sqref="C96:C97" xr:uid="{00000000-0002-0000-0000-00002C000000}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SNMP Trap Port" error="Valid Port Range is between 1 and 65535.  Default is 162" sqref="C97:C98" xr:uid="{00000000-0002-0000-0000-00002C000000}">
       <formula1>1</formula1>
       <formula2>65535</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A96:A97" xr:uid="{00000000-0002-0000-0000-00002D000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A97:A98" xr:uid="{00000000-0002-0000-0000-00002D000000}">
       <formula1>"snmp_trap"</formula1>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SMTP Port" error="Valid Port Range is between 1 and 65535.  Default is 25" sqref="B66" xr:uid="{00000000-0002-0000-0000-00002E000000}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SMTP Port" error="Valid Port Range is between 1 and 65535.  Default is 25" sqref="B67" xr:uid="{00000000-0002-0000-0000-00002E000000}">
       <formula1>1</formula1>
       <formula2>65535</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Login Domain Type" error="The Login Domain Type can be [local|ldap|radius|tacacs|rsa|saml].  SAML is not supported for Console Authentication" sqref="D130:D131" xr:uid="{00000000-0002-0000-0000-00002F000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Login Domain Type" error="The Login Domain Type can be [local|ldap|radius|tacacs|rsa|saml].  SAML is not supported for Console Authentication" sqref="D131:D132" xr:uid="{00000000-0002-0000-0000-00002F000000}">
       <formula1>"local,ldap,radius,tacacs,rsa,saml"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B130:B131" xr:uid="{00000000-0002-0000-0000-000030000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B131:B132" xr:uid="{00000000-0002-0000-0000-000030000000}">
       <formula1>"console,default"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A130:A131" xr:uid="{00000000-0002-0000-0000-000031000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A131:A132" xr:uid="{00000000-0002-0000-0000-000031000000}">
       <formula1>"realm"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A25:A31" xr:uid="{A2F55667-432D-4009-90B0-3CBF96713B99}">
@@ -4795,8 +4821,13 @@
       <formula2>1000</formula2>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="E67" r:id="rId1" xr:uid="{47B0C783-B08F-4E70-8365-F66BC2D1DC4E}"/>
+    <hyperlink ref="G67" r:id="rId2" xr:uid="{ECB49B35-5BD8-4A7F-88FF-240597E5B135}"/>
+    <hyperlink ref="I67" r:id="rId3" xr:uid="{F5D689CB-3F4A-4EED-ADA0-F02A0EBD47A7}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -4818,13 +4849,13 @@
   <sheetData>
     <row r="1" spans="1:3" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>129</v>
+        <v>110</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -4832,66 +4863,66 @@
         <v>8</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>111</v>
+        <v>92</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>112</v>
+        <v>93</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>127</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
-        <v>113</v>
+        <v>94</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>120</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>128</v>
+        <v>109</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>115</v>
+        <v>96</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>124</v>
+        <v>105</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>116</v>
+        <v>97</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>125</v>
+        <v>106</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>117</v>
+        <v>98</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>126</v>
+        <v>107</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>118</v>
+        <v>99</v>
       </c>
       <c r="C9" s="1">
         <v>9504</v>
@@ -4899,7 +4930,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
       <c r="C10" s="1">
         <v>9508</v>
@@ -4907,7 +4938,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>120</v>
+        <v>101</v>
       </c>
       <c r="C11" s="1">
         <v>9516</v>
@@ -4915,37 +4946,37 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>121</v>
+        <v>102</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>123</v>
+        <v>104</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>124</v>
+        <v>105</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
-        <v>125</v>
+        <v>106</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
-        <v>126</v>
+        <v>107</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
-        <v>130</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Configuration Backup Resources
</commit_message>
<xml_diff>
--- a/Terraform/aci/base-configs/aci-fabric-deploy-Input-Spreadsheet.xlsx
+++ b/Terraform/aci/base-configs/aci-fabric-deploy-Input-Spreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\tyscott\terraform-aci-fabric-deploy\Terraform\aci\base-configs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5022D74E-BB54-4AC8-8681-F7AB03CE8651}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CD6433E-4684-4E3B-89CC-2317396C39F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="User Input" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="244">
   <si>
     <t>Type</t>
   </si>
@@ -887,6 +887,63 @@
   </si>
   <si>
     <t>198.18.1.72</t>
+  </si>
+  <si>
+    <t>Fabric Backup</t>
+  </si>
+  <si>
+    <t>backup</t>
+  </si>
+  <si>
+    <t>Encryption Key</t>
+  </si>
+  <si>
+    <t>Backup Hour</t>
+  </si>
+  <si>
+    <t>Backup Minute</t>
+  </si>
+  <si>
+    <t>Remote Host</t>
+  </si>
+  <si>
+    <t>cisco123cisco123</t>
+  </si>
+  <si>
+    <t>lnx2.example.com</t>
+  </si>
+  <si>
+    <t>Protocol</t>
+  </si>
+  <si>
+    <t>sftp</t>
+  </si>
+  <si>
+    <t>Remote Path</t>
+  </si>
+  <si>
+    <t>Remote Port</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Auth Type</t>
+  </si>
+  <si>
+    <t>Password or SSH Passphrase</t>
+  </si>
+  <si>
+    <t>SSH Key (If Using ssh-key)</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>The Encryption Key is used to encrypt the backup files.  The Backup Hour and Minute are used to create a triggered schedule once per day for configuration backups.  Make sure to select either password or ssh-key based authentication.  If it is ssh-key you need to provide the ssh-private-key and passphrase that you have created using some type of ssh-key generation utility like ssh-keygen.</t>
   </si>
 </sst>
 </file>
@@ -1660,7 +1717,7 @@
     <xf numFmtId="0" fontId="3" fillId="35" borderId="8" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="17" fillId="33" borderId="8" xfId="2" applyNumberFormat="1"/>
@@ -1715,67 +1772,25 @@
     <xf numFmtId="49" fontId="20" fillId="34" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="17" fillId="33" borderId="8" xfId="2" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="33" borderId="8" xfId="2" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="34" borderId="8" xfId="3" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="34" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="34" borderId="8" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="33" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="34" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="16" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="20" fillId="34" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="20" fillId="34" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="34" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="36" borderId="8" xfId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="11" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="20" fillId="34" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="20" fillId="34" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="20" fillId="34" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="20" fillId="34" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="18" fillId="0" borderId="25" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="18" fillId="0" borderId="26" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="21" fillId="34" borderId="22" xfId="43" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="1" fontId="20" fillId="34" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="11" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="16" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="20" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1787,20 +1802,83 @@
     <xf numFmtId="49" fontId="20" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="17" fillId="33" borderId="8" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="20" fillId="34" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="20" fillId="34" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="1" fontId="20" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="20" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="21" fillId="34" borderId="22" xfId="43" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="20" fillId="34" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="21" fillId="34" borderId="22" xfId="43" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="17" fillId="36" borderId="8" xfId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="21" fillId="34" borderId="22" xfId="43" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="18" fillId="34" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="34" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="20" fillId="34" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="20" fillId="34" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="34" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="33" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="20" fillId="34" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="20" fillId="34" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="34" borderId="8" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="33" borderId="8" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="34" borderId="8" xfId="3" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="22" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="23" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="24" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="20" fillId="34" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="20" fillId="34" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="33" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="44">
@@ -2159,10 +2237,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P132"/>
+  <dimension ref="A1:P137"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D125" sqref="D125"/>
+      <selection activeCell="A6" sqref="A6:P6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2186,24 +2264,24 @@
     <col min="17" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="6" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="20" t="s">
+    <row r="1" spans="1:16" s="6" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="47" t="s">
         <v>81</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
-      <c r="L1" s="20"/>
-      <c r="M1" s="20"/>
-    </row>
-    <row r="2" spans="1:13" s="3" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="47"/>
+      <c r="K1" s="47"/>
+      <c r="L1" s="47"/>
+      <c r="M1" s="47"/>
+    </row>
+    <row r="2" spans="1:16" s="3" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
@@ -2222,7 +2300,7 @@
       <c r="L2" s="8"/>
       <c r="M2" s="8"/>
     </row>
-    <row r="3" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
         <v>1</v>
       </c>
@@ -2241,420 +2319,464 @@
       <c r="L3" s="13"/>
       <c r="M3" s="13"/>
     </row>
-    <row r="5" spans="1:13" s="6" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="20" t="s">
-        <v>90</v>
-      </c>
-      <c r="B5" s="20"/>
-      <c r="C5" s="20"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="20"/>
-      <c r="I5" s="20"/>
-      <c r="J5" s="20"/>
-      <c r="K5" s="20"/>
-      <c r="L5" s="20"/>
-      <c r="M5" s="20"/>
-    </row>
-    <row r="6" spans="1:13" s="6" customFormat="1" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="22" t="s">
-        <v>203</v>
-      </c>
-      <c r="B6" s="22"/>
-      <c r="C6" s="22"/>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
-      <c r="F6" s="22"/>
-      <c r="G6" s="22"/>
-      <c r="H6" s="22"/>
-      <c r="I6" s="22"/>
-      <c r="J6" s="22"/>
-      <c r="K6" s="22"/>
-      <c r="L6" s="22"/>
-      <c r="M6" s="22"/>
-    </row>
-    <row r="7" spans="1:13" s="3" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="55" t="s">
+        <v>225</v>
+      </c>
+      <c r="B5" s="55"/>
+      <c r="C5" s="55"/>
+      <c r="D5" s="55"/>
+      <c r="E5" s="55"/>
+      <c r="F5" s="55"/>
+      <c r="G5" s="55"/>
+      <c r="H5" s="55"/>
+      <c r="I5" s="55"/>
+      <c r="J5" s="55"/>
+      <c r="K5" s="55"/>
+      <c r="L5" s="55"/>
+      <c r="M5" s="55"/>
+      <c r="N5" s="55"/>
+      <c r="O5" s="55"/>
+      <c r="P5" s="55"/>
+    </row>
+    <row r="6" spans="1:16" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="54" t="s">
+        <v>243</v>
+      </c>
+      <c r="B6" s="54"/>
+      <c r="C6" s="54"/>
+      <c r="D6" s="54"/>
+      <c r="E6" s="54"/>
+      <c r="F6" s="54"/>
+      <c r="G6" s="54"/>
+      <c r="H6" s="54"/>
+      <c r="I6" s="54"/>
+      <c r="J6" s="54"/>
+      <c r="K6" s="54"/>
+      <c r="L6" s="54"/>
+      <c r="M6" s="54"/>
+      <c r="N6" s="54"/>
+      <c r="O6" s="54"/>
+      <c r="P6" s="54"/>
+    </row>
+    <row r="7" spans="1:16" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B7" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>228</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>229</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>233</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>235</v>
+      </c>
+      <c r="I7" s="8" t="s">
+        <v>236</v>
+      </c>
+      <c r="J7" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="K7" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="L7" s="8" t="s">
+        <v>239</v>
+      </c>
+      <c r="M7" s="8" t="s">
+        <v>240</v>
+      </c>
+      <c r="N7" s="49" t="s">
+        <v>36</v>
+      </c>
+      <c r="O7" s="50"/>
+      <c r="P7" s="51"/>
+    </row>
+    <row r="8" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="13" t="s">
+        <v>226</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>231</v>
+      </c>
+      <c r="C8" s="14">
+        <v>0</v>
+      </c>
+      <c r="D8" s="14">
+        <v>0</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>232</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" s="14" t="s">
+        <v>234</v>
+      </c>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14">
+        <v>22</v>
+      </c>
+      <c r="J8" s="13" t="s">
+        <v>241</v>
+      </c>
+      <c r="K8" s="13" t="s">
+        <v>242</v>
+      </c>
+      <c r="L8" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="M8" s="13"/>
+      <c r="N8" s="52"/>
+      <c r="O8" s="53"/>
+      <c r="P8" s="36"/>
+    </row>
+    <row r="10" spans="1:16" s="6" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="47" t="s">
+        <v>90</v>
+      </c>
+      <c r="B10" s="47"/>
+      <c r="C10" s="47"/>
+      <c r="D10" s="47"/>
+      <c r="E10" s="47"/>
+      <c r="F10" s="47"/>
+      <c r="G10" s="47"/>
+      <c r="H10" s="47"/>
+      <c r="I10" s="47"/>
+      <c r="J10" s="47"/>
+      <c r="K10" s="47"/>
+      <c r="L10" s="47"/>
+      <c r="M10" s="47"/>
+    </row>
+    <row r="11" spans="1:16" s="6" customFormat="1" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="48" t="s">
+        <v>203</v>
+      </c>
+      <c r="B11" s="48"/>
+      <c r="C11" s="48"/>
+      <c r="D11" s="48"/>
+      <c r="E11" s="48"/>
+      <c r="F11" s="48"/>
+      <c r="G11" s="48"/>
+      <c r="H11" s="48"/>
+      <c r="I11" s="48"/>
+      <c r="J11" s="48"/>
+      <c r="K11" s="48"/>
+      <c r="L11" s="48"/>
+      <c r="M11" s="48"/>
+    </row>
+    <row r="12" spans="1:16" s="3" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C12" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D12" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="E12" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="F12" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="G7" s="8" t="s">
+      <c r="G12" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="H7" s="8" t="s">
+      <c r="H12" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="I7" s="8" t="s">
+      <c r="I12" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="J7" s="8" t="s">
+      <c r="J12" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="K7" s="8" t="s">
+      <c r="K12" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="L7" s="8" t="s">
+      <c r="L12" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="M7" s="8"/>
-    </row>
-    <row r="8" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="13" t="s">
+      <c r="M12" s="8"/>
+    </row>
+    <row r="13" spans="1:16" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B13" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C13" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="14">
+      <c r="D13" s="14">
         <v>201</v>
       </c>
-      <c r="E8" s="13" t="s">
+      <c r="E13" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="F8" s="14">
+      <c r="F13" s="14">
         <v>1</v>
       </c>
-      <c r="G8" s="14" t="s">
+      <c r="G13" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="H8" s="14" t="s">
+      <c r="H13" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="I8" s="13" t="s">
+      <c r="I13" s="13" t="s">
         <v>210</v>
       </c>
-      <c r="J8" s="13" t="s">
+      <c r="J13" s="13" t="s">
         <v>211</v>
       </c>
-      <c r="K8" s="13" t="s">
+      <c r="K13" s="13" t="s">
         <v>212</v>
       </c>
-      <c r="L8" s="13" t="s">
+      <c r="L13" s="13" t="s">
         <v>213</v>
       </c>
-      <c r="M8" s="13"/>
-    </row>
-    <row r="9" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="11" t="s">
+      <c r="M13" s="13"/>
+    </row>
+    <row r="14" spans="1:16" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B14" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C14" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="12">
+      <c r="D14" s="12">
         <v>202</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="E14" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="F9" s="12">
+      <c r="F14" s="12">
         <v>1</v>
       </c>
-      <c r="G9" s="12" t="s">
+      <c r="G14" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="H9" s="12" t="s">
+      <c r="H14" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="I9" s="11" t="s">
+      <c r="I14" s="11" t="s">
         <v>214</v>
       </c>
-      <c r="J9" s="11" t="s">
+      <c r="J14" s="11" t="s">
         <v>211</v>
       </c>
-      <c r="K9" s="11" t="s">
+      <c r="K14" s="11" t="s">
         <v>215</v>
       </c>
-      <c r="L9" s="11" t="s">
+      <c r="L14" s="11" t="s">
         <v>213</v>
       </c>
-      <c r="M9" s="11"/>
-    </row>
-    <row r="10" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="13" t="s">
+      <c r="M14" s="11"/>
+    </row>
+    <row r="15" spans="1:16" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="B15" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C15" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="14">
+      <c r="D15" s="14">
         <v>101</v>
       </c>
-      <c r="E10" s="13" t="s">
+      <c r="E15" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="F10" s="14">
+      <c r="F15" s="14">
         <v>1</v>
       </c>
-      <c r="G10" s="14" t="s">
+      <c r="G15" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="H10" s="14">
+      <c r="H15" s="14">
         <v>9508</v>
       </c>
-      <c r="I10" s="13" t="s">
+      <c r="I15" s="13" t="s">
         <v>216</v>
       </c>
-      <c r="J10" s="13" t="s">
+      <c r="J15" s="13" t="s">
         <v>211</v>
       </c>
-      <c r="K10" s="13" t="s">
+      <c r="K15" s="13" t="s">
         <v>217</v>
       </c>
-      <c r="L10" s="13" t="s">
+      <c r="L15" s="13" t="s">
         <v>213</v>
       </c>
-      <c r="M10" s="13"/>
-    </row>
-    <row r="11" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="11"/>
-      <c r="B11" s="11"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="11"/>
-      <c r="K11" s="11"/>
-      <c r="L11" s="11"/>
-      <c r="M11" s="11"/>
-    </row>
-    <row r="12" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="13"/>
-      <c r="B12" s="13"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="13"/>
-      <c r="J12" s="13"/>
-      <c r="K12" s="13"/>
-      <c r="L12" s="13"/>
-      <c r="M12" s="13"/>
-    </row>
-    <row r="13" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="11"/>
-      <c r="B13" s="11"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="11"/>
-      <c r="J13" s="11"/>
-      <c r="K13" s="11"/>
-      <c r="L13" s="11"/>
-      <c r="M13" s="11"/>
-    </row>
-    <row r="14" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="13"/>
-      <c r="B14" s="13"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="13"/>
-      <c r="J14" s="13"/>
-      <c r="K14" s="13"/>
-      <c r="L14" s="13"/>
-      <c r="M14" s="13"/>
-    </row>
-    <row r="15" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="11"/>
-      <c r="B15" s="11"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="11"/>
-      <c r="J15" s="11"/>
-      <c r="K15" s="11"/>
-      <c r="L15" s="11"/>
-      <c r="M15" s="11"/>
-    </row>
-    <row r="16" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="13"/>
-      <c r="B16" s="13"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="13"/>
-      <c r="J16" s="13"/>
-      <c r="K16" s="13"/>
-      <c r="L16" s="13"/>
-      <c r="M16" s="13"/>
+      <c r="M15" s="13"/>
+    </row>
+    <row r="16" spans="1:16" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="11"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="11"/>
+      <c r="L16" s="11"/>
+      <c r="M16" s="11"/>
     </row>
     <row r="17" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="11"/>
-      <c r="B17" s="11"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="11"/>
-      <c r="J17" s="11"/>
-      <c r="K17" s="11"/>
-      <c r="L17" s="11"/>
-      <c r="M17" s="11"/>
+      <c r="A17" s="13"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="13"/>
+      <c r="K17" s="13"/>
+      <c r="L17" s="13"/>
+      <c r="M17" s="13"/>
     </row>
     <row r="18" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="13"/>
-      <c r="B18" s="13"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="14"/>
-      <c r="I18" s="13"/>
-      <c r="J18" s="13"/>
-      <c r="K18" s="13"/>
-      <c r="L18" s="13"/>
-      <c r="M18" s="13"/>
+      <c r="A18" s="11"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="11"/>
+      <c r="K18" s="11"/>
+      <c r="L18" s="11"/>
+      <c r="M18" s="11"/>
     </row>
     <row r="19" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="11"/>
-      <c r="B19" s="11"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="12"/>
-      <c r="H19" s="12"/>
-      <c r="I19" s="11"/>
-      <c r="J19" s="11"/>
-      <c r="K19" s="11"/>
-      <c r="L19" s="11"/>
-      <c r="M19" s="11"/>
+      <c r="A19" s="13"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="13"/>
+      <c r="J19" s="13"/>
+      <c r="K19" s="13"/>
+      <c r="L19" s="13"/>
+      <c r="M19" s="13"/>
     </row>
     <row r="20" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="13"/>
-      <c r="B20" s="13"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="14"/>
-      <c r="I20" s="13"/>
-      <c r="J20" s="13"/>
-      <c r="K20" s="13"/>
-      <c r="L20" s="13"/>
-      <c r="M20" s="13"/>
+      <c r="A20" s="11"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="11"/>
+      <c r="J20" s="11"/>
+      <c r="K20" s="11"/>
+      <c r="L20" s="11"/>
+      <c r="M20" s="11"/>
     </row>
     <row r="21" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="11"/>
-      <c r="B21" s="11"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="12"/>
-      <c r="H21" s="12"/>
-      <c r="I21" s="11"/>
-      <c r="J21" s="11"/>
-      <c r="K21" s="11"/>
-      <c r="L21" s="11"/>
-      <c r="M21" s="11"/>
-    </row>
-    <row r="23" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="20" t="s">
-        <v>202</v>
-      </c>
-      <c r="B23" s="20"/>
-      <c r="C23" s="20"/>
-      <c r="D23" s="20"/>
-      <c r="E23" s="20"/>
-      <c r="F23" s="20"/>
-      <c r="G23" s="20"/>
-      <c r="H23" s="20"/>
-      <c r="I23" s="20"/>
-      <c r="J23" s="20"/>
-      <c r="K23" s="20"/>
-      <c r="L23" s="20"/>
-      <c r="M23" s="20"/>
-    </row>
-    <row r="24" spans="1:13" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B24" s="8" t="s">
-        <v>198</v>
-      </c>
-      <c r="C24" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="D24" s="8" t="s">
-        <v>199</v>
-      </c>
-      <c r="E24" s="8" t="s">
-        <v>200</v>
-      </c>
-      <c r="F24" s="8"/>
-      <c r="G24" s="8"/>
-      <c r="H24" s="8"/>
-      <c r="I24" s="8"/>
-      <c r="J24" s="8"/>
-      <c r="K24" s="8"/>
-      <c r="L24" s="8"/>
-      <c r="M24" s="8"/>
-    </row>
-    <row r="25" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="13" t="s">
-        <v>197</v>
-      </c>
-      <c r="B25" s="14">
-        <v>201</v>
-      </c>
-      <c r="C25" s="13" t="s">
-        <v>201</v>
-      </c>
-      <c r="D25" s="14">
-        <v>201</v>
-      </c>
-      <c r="E25" s="14">
-        <v>202</v>
-      </c>
-      <c r="F25" s="13"/>
+      <c r="A21" s="13"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="13"/>
+      <c r="J21" s="13"/>
+      <c r="K21" s="13"/>
+      <c r="L21" s="13"/>
+      <c r="M21" s="13"/>
+    </row>
+    <row r="22" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="11"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="11"/>
+      <c r="J22" s="11"/>
+      <c r="K22" s="11"/>
+      <c r="L22" s="11"/>
+      <c r="M22" s="11"/>
+    </row>
+    <row r="23" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="13"/>
+      <c r="B23" s="13"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="14"/>
+      <c r="I23" s="13"/>
+      <c r="J23" s="13"/>
+      <c r="K23" s="13"/>
+      <c r="L23" s="13"/>
+      <c r="M23" s="13"/>
+    </row>
+    <row r="24" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="11"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="12"/>
+      <c r="I24" s="11"/>
+      <c r="J24" s="11"/>
+      <c r="K24" s="11"/>
+      <c r="L24" s="11"/>
+      <c r="M24" s="11"/>
+    </row>
+    <row r="25" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="13"/>
+      <c r="B25" s="13"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="14"/>
       <c r="G25" s="14"/>
       <c r="H25" s="14"/>
       <c r="I25" s="13"/>
@@ -2663,13 +2785,13 @@
       <c r="L25" s="13"/>
       <c r="M25" s="13"/>
     </row>
-    <row r="26" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="11"/>
-      <c r="B26" s="12"/>
+      <c r="B26" s="11"/>
       <c r="C26" s="11"/>
       <c r="D26" s="12"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="11"/>
+      <c r="E26" s="11"/>
+      <c r="F26" s="12"/>
       <c r="G26" s="12"/>
       <c r="H26" s="12"/>
       <c r="I26" s="11"/>
@@ -2678,374 +2800,382 @@
       <c r="L26" s="11"/>
       <c r="M26" s="11"/>
     </row>
-    <row r="27" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="13"/>
-      <c r="B27" s="14"/>
-      <c r="C27" s="13"/>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="14"/>
-      <c r="H27" s="14"/>
-      <c r="I27" s="13"/>
-      <c r="J27" s="13"/>
-      <c r="K27" s="13"/>
-      <c r="L27" s="13"/>
-      <c r="M27" s="13"/>
-    </row>
-    <row r="28" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="11"/>
-      <c r="B28" s="12"/>
-      <c r="C28" s="11"/>
-      <c r="D28" s="12"/>
-      <c r="E28" s="12"/>
-      <c r="F28" s="11"/>
-      <c r="G28" s="12"/>
-      <c r="H28" s="12"/>
-      <c r="I28" s="11"/>
-      <c r="J28" s="11"/>
-      <c r="K28" s="11"/>
-      <c r="L28" s="11"/>
-      <c r="M28" s="11"/>
-    </row>
-    <row r="29" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="13"/>
-      <c r="B29" s="14"/>
-      <c r="C29" s="13"/>
-      <c r="D29" s="14"/>
-      <c r="E29" s="14"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="14"/>
-      <c r="H29" s="14"/>
-      <c r="I29" s="13"/>
-      <c r="J29" s="13"/>
-      <c r="K29" s="13"/>
-      <c r="L29" s="13"/>
-      <c r="M29" s="13"/>
+    <row r="28" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="47" t="s">
+        <v>202</v>
+      </c>
+      <c r="B28" s="47"/>
+      <c r="C28" s="47"/>
+      <c r="D28" s="47"/>
+      <c r="E28" s="47"/>
+      <c r="F28" s="47"/>
+      <c r="G28" s="47"/>
+      <c r="H28" s="47"/>
+      <c r="I28" s="47"/>
+      <c r="J28" s="47"/>
+      <c r="K28" s="47"/>
+      <c r="L28" s="47"/>
+      <c r="M28" s="47"/>
+    </row>
+    <row r="29" spans="1:13" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>200</v>
+      </c>
+      <c r="F29" s="8"/>
+      <c r="G29" s="8"/>
+      <c r="H29" s="8"/>
+      <c r="I29" s="8"/>
+      <c r="J29" s="8"/>
+      <c r="K29" s="8"/>
+      <c r="L29" s="8"/>
+      <c r="M29" s="8"/>
     </row>
     <row r="30" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="11"/>
-      <c r="B30" s="12"/>
-      <c r="C30" s="11"/>
-      <c r="D30" s="12"/>
-      <c r="E30" s="12"/>
-      <c r="F30" s="11"/>
-      <c r="G30" s="12"/>
-      <c r="H30" s="12"/>
-      <c r="I30" s="11"/>
-      <c r="J30" s="11"/>
-      <c r="K30" s="11"/>
-      <c r="L30" s="11"/>
-      <c r="M30" s="11"/>
+      <c r="A30" s="13" t="s">
+        <v>197</v>
+      </c>
+      <c r="B30" s="14">
+        <v>201</v>
+      </c>
+      <c r="C30" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="D30" s="14">
+        <v>201</v>
+      </c>
+      <c r="E30" s="14">
+        <v>202</v>
+      </c>
+      <c r="F30" s="13"/>
+      <c r="G30" s="14"/>
+      <c r="H30" s="14"/>
+      <c r="I30" s="13"/>
+      <c r="J30" s="13"/>
+      <c r="K30" s="13"/>
+      <c r="L30" s="13"/>
+      <c r="M30" s="13"/>
     </row>
     <row r="31" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="13"/>
-      <c r="B31" s="14"/>
-      <c r="C31" s="13"/>
-      <c r="D31" s="14"/>
-      <c r="E31" s="14"/>
-      <c r="F31" s="13"/>
-      <c r="G31" s="14"/>
-      <c r="H31" s="14"/>
-      <c r="I31" s="13"/>
-      <c r="J31" s="13"/>
-      <c r="K31" s="13"/>
-      <c r="L31" s="13"/>
-      <c r="M31" s="13"/>
-    </row>
-    <row r="33" spans="1:13" s="6" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="20" t="s">
-        <v>122</v>
-      </c>
-      <c r="B33" s="20"/>
-      <c r="C33" s="20"/>
-      <c r="D33" s="20"/>
-      <c r="E33" s="20"/>
-      <c r="F33" s="20"/>
-      <c r="G33" s="20"/>
-      <c r="H33" s="20"/>
-      <c r="I33" s="20"/>
-      <c r="J33" s="20"/>
-      <c r="K33" s="20"/>
-      <c r="L33" s="20"/>
-      <c r="M33" s="20"/>
-    </row>
-    <row r="34" spans="1:13" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="23" t="s">
-        <v>124</v>
-      </c>
-      <c r="B34" s="23"/>
-      <c r="C34" s="23"/>
-      <c r="D34" s="23"/>
-      <c r="E34" s="23"/>
-      <c r="F34" s="23"/>
-      <c r="G34" s="23"/>
-      <c r="H34" s="23"/>
-      <c r="I34" s="23"/>
-      <c r="J34" s="23"/>
-      <c r="K34" s="23"/>
-      <c r="L34" s="23"/>
-      <c r="M34" s="23"/>
-    </row>
-    <row r="35" spans="1:13" s="3" customFormat="1" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B35" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="C35" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="D35" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="E35" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="F35" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="G35" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="H35" s="8" t="s">
-        <v>190</v>
-      </c>
-      <c r="I35" s="8" t="s">
-        <v>192</v>
-      </c>
-      <c r="J35" s="8" t="s">
-        <v>191</v>
-      </c>
-      <c r="K35" s="8"/>
-      <c r="L35" s="8"/>
-      <c r="M35" s="8"/>
-    </row>
-    <row r="36" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B36" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="C36" s="14">
-        <v>1</v>
-      </c>
-      <c r="D36" s="14">
-        <v>1</v>
-      </c>
-      <c r="E36" s="13" t="s">
-        <v>218</v>
-      </c>
-      <c r="F36" s="13" t="s">
-        <v>213</v>
-      </c>
-      <c r="G36" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="H36" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="I36" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="J36" s="13" t="s">
-        <v>88</v>
-      </c>
+      <c r="A31" s="11"/>
+      <c r="B31" s="12"/>
+      <c r="C31" s="11"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="12"/>
+      <c r="F31" s="11"/>
+      <c r="G31" s="12"/>
+      <c r="H31" s="12"/>
+      <c r="I31" s="11"/>
+      <c r="J31" s="11"/>
+      <c r="K31" s="11"/>
+      <c r="L31" s="11"/>
+      <c r="M31" s="11"/>
+    </row>
+    <row r="32" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="13"/>
+      <c r="B32" s="14"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="14"/>
+      <c r="E32" s="14"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="14"/>
+      <c r="H32" s="14"/>
+      <c r="I32" s="13"/>
+      <c r="J32" s="13"/>
+      <c r="K32" s="13"/>
+      <c r="L32" s="13"/>
+      <c r="M32" s="13"/>
+    </row>
+    <row r="33" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="11"/>
+      <c r="B33" s="12"/>
+      <c r="C33" s="11"/>
+      <c r="D33" s="12"/>
+      <c r="E33" s="12"/>
+      <c r="F33" s="11"/>
+      <c r="G33" s="12"/>
+      <c r="H33" s="12"/>
+      <c r="I33" s="11"/>
+      <c r="J33" s="11"/>
+      <c r="K33" s="11"/>
+      <c r="L33" s="11"/>
+      <c r="M33" s="11"/>
+    </row>
+    <row r="34" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="13"/>
+      <c r="B34" s="14"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="14"/>
+      <c r="E34" s="14"/>
+      <c r="F34" s="13"/>
+      <c r="G34" s="14"/>
+      <c r="H34" s="14"/>
+      <c r="I34" s="13"/>
+      <c r="J34" s="13"/>
+      <c r="K34" s="13"/>
+      <c r="L34" s="13"/>
+      <c r="M34" s="13"/>
+    </row>
+    <row r="35" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="11"/>
+      <c r="B35" s="12"/>
+      <c r="C35" s="11"/>
+      <c r="D35" s="12"/>
+      <c r="E35" s="12"/>
+      <c r="F35" s="11"/>
+      <c r="G35" s="12"/>
+      <c r="H35" s="12"/>
+      <c r="I35" s="11"/>
+      <c r="J35" s="11"/>
+      <c r="K35" s="11"/>
+      <c r="L35" s="11"/>
+      <c r="M35" s="11"/>
+    </row>
+    <row r="36" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="13"/>
+      <c r="B36" s="14"/>
+      <c r="C36" s="13"/>
+      <c r="D36" s="14"/>
+      <c r="E36" s="14"/>
+      <c r="F36" s="13"/>
+      <c r="G36" s="14"/>
+      <c r="H36" s="14"/>
+      <c r="I36" s="13"/>
+      <c r="J36" s="13"/>
       <c r="K36" s="13"/>
       <c r="L36" s="13"/>
       <c r="M36" s="13"/>
     </row>
-    <row r="37" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="11"/>
-      <c r="B37" s="11"/>
-      <c r="C37" s="12"/>
-      <c r="D37" s="12"/>
-      <c r="E37" s="11"/>
-      <c r="F37" s="11"/>
-      <c r="G37" s="12"/>
-      <c r="H37" s="12"/>
-      <c r="I37" s="11"/>
-      <c r="J37" s="11"/>
-      <c r="K37" s="11"/>
-      <c r="L37" s="11"/>
-      <c r="M37" s="11"/>
-    </row>
-    <row r="38" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="13"/>
-      <c r="B38" s="13"/>
-      <c r="C38" s="14"/>
-      <c r="D38" s="14"/>
-      <c r="E38" s="13"/>
-      <c r="F38" s="13"/>
-      <c r="G38" s="14"/>
-      <c r="H38" s="14"/>
-      <c r="I38" s="13"/>
-      <c r="J38" s="13"/>
-      <c r="K38" s="13"/>
-      <c r="L38" s="13"/>
-      <c r="M38" s="13"/>
-    </row>
-    <row r="39" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="11"/>
-      <c r="B39" s="11"/>
-      <c r="C39" s="12"/>
-      <c r="D39" s="12"/>
-      <c r="E39" s="11"/>
-      <c r="F39" s="11"/>
-      <c r="G39" s="12"/>
-      <c r="H39" s="12"/>
-      <c r="I39" s="11"/>
-      <c r="J39" s="11"/>
-      <c r="K39" s="11"/>
-      <c r="L39" s="11"/>
-      <c r="M39" s="11"/>
-    </row>
-    <row r="40" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="13"/>
-      <c r="B40" s="13"/>
-      <c r="C40" s="14"/>
-      <c r="D40" s="14"/>
-      <c r="E40" s="13"/>
-      <c r="F40" s="13"/>
-      <c r="G40" s="14"/>
-      <c r="H40" s="14"/>
-      <c r="I40" s="13"/>
-      <c r="J40" s="13"/>
-      <c r="K40" s="13"/>
-      <c r="L40" s="13"/>
-      <c r="M40" s="13"/>
-    </row>
-    <row r="41" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="11"/>
-      <c r="B41" s="11"/>
-      <c r="C41" s="12"/>
-      <c r="D41" s="12"/>
-      <c r="E41" s="11"/>
-      <c r="F41" s="11"/>
-      <c r="G41" s="12"/>
-      <c r="H41" s="12"/>
-      <c r="I41" s="11"/>
-      <c r="J41" s="11"/>
-      <c r="K41" s="11"/>
-      <c r="L41" s="11"/>
-      <c r="M41" s="11"/>
-    </row>
-    <row r="42" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="13"/>
-      <c r="B42" s="13"/>
-      <c r="C42" s="14"/>
-      <c r="D42" s="14"/>
-      <c r="E42" s="13"/>
-      <c r="F42" s="13"/>
-      <c r="G42" s="14"/>
-      <c r="H42" s="14"/>
-      <c r="I42" s="13"/>
-      <c r="J42" s="13"/>
-      <c r="K42" s="13"/>
-      <c r="L42" s="13"/>
-      <c r="M42" s="13"/>
-    </row>
-    <row r="44" spans="1:13" s="6" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="20" t="s">
+    <row r="38" spans="1:13" s="6" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="47" t="s">
+        <v>122</v>
+      </c>
+      <c r="B38" s="47"/>
+      <c r="C38" s="47"/>
+      <c r="D38" s="47"/>
+      <c r="E38" s="47"/>
+      <c r="F38" s="47"/>
+      <c r="G38" s="47"/>
+      <c r="H38" s="47"/>
+      <c r="I38" s="47"/>
+      <c r="J38" s="47"/>
+      <c r="K38" s="47"/>
+      <c r="L38" s="47"/>
+      <c r="M38" s="47"/>
+    </row>
+    <row r="39" spans="1:13" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="42" t="s">
+        <v>124</v>
+      </c>
+      <c r="B39" s="42"/>
+      <c r="C39" s="42"/>
+      <c r="D39" s="42"/>
+      <c r="E39" s="42"/>
+      <c r="F39" s="42"/>
+      <c r="G39" s="42"/>
+      <c r="H39" s="42"/>
+      <c r="I39" s="42"/>
+      <c r="J39" s="42"/>
+      <c r="K39" s="42"/>
+      <c r="L39" s="42"/>
+      <c r="M39" s="42"/>
+    </row>
+    <row r="40" spans="1:13" s="3" customFormat="1" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="D40" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="E40" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="F40" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="G40" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="H40" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="I40" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="J40" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="K40" s="8"/>
+      <c r="L40" s="8"/>
+      <c r="M40" s="8"/>
+    </row>
+    <row r="41" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B41" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C41" s="14">
+        <v>1</v>
+      </c>
+      <c r="D41" s="14">
+        <v>1</v>
+      </c>
+      <c r="E41" s="13" t="s">
+        <v>218</v>
+      </c>
+      <c r="F41" s="13" t="s">
+        <v>213</v>
+      </c>
+      <c r="G41" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="H41" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="I41" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="J41" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="K41" s="13"/>
+      <c r="L41" s="13"/>
+      <c r="M41" s="13"/>
+    </row>
+    <row r="42" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="11"/>
+      <c r="B42" s="11"/>
+      <c r="C42" s="12"/>
+      <c r="D42" s="12"/>
+      <c r="E42" s="11"/>
+      <c r="F42" s="11"/>
+      <c r="G42" s="12"/>
+      <c r="H42" s="12"/>
+      <c r="I42" s="11"/>
+      <c r="J42" s="11"/>
+      <c r="K42" s="11"/>
+      <c r="L42" s="11"/>
+      <c r="M42" s="11"/>
+    </row>
+    <row r="43" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="13"/>
+      <c r="B43" s="13"/>
+      <c r="C43" s="14"/>
+      <c r="D43" s="14"/>
+      <c r="E43" s="13"/>
+      <c r="F43" s="13"/>
+      <c r="G43" s="14"/>
+      <c r="H43" s="14"/>
+      <c r="I43" s="13"/>
+      <c r="J43" s="13"/>
+      <c r="K43" s="13"/>
+      <c r="L43" s="13"/>
+      <c r="M43" s="13"/>
+    </row>
+    <row r="44" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="11"/>
+      <c r="B44" s="11"/>
+      <c r="C44" s="12"/>
+      <c r="D44" s="12"/>
+      <c r="E44" s="11"/>
+      <c r="F44" s="11"/>
+      <c r="G44" s="12"/>
+      <c r="H44" s="12"/>
+      <c r="I44" s="11"/>
+      <c r="J44" s="11"/>
+      <c r="K44" s="11"/>
+      <c r="L44" s="11"/>
+      <c r="M44" s="11"/>
+    </row>
+    <row r="45" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="13"/>
+      <c r="B45" s="13"/>
+      <c r="C45" s="14"/>
+      <c r="D45" s="14"/>
+      <c r="E45" s="13"/>
+      <c r="F45" s="13"/>
+      <c r="G45" s="14"/>
+      <c r="H45" s="14"/>
+      <c r="I45" s="13"/>
+      <c r="J45" s="13"/>
+      <c r="K45" s="13"/>
+      <c r="L45" s="13"/>
+      <c r="M45" s="13"/>
+    </row>
+    <row r="46" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="11"/>
+      <c r="B46" s="11"/>
+      <c r="C46" s="12"/>
+      <c r="D46" s="12"/>
+      <c r="E46" s="11"/>
+      <c r="F46" s="11"/>
+      <c r="G46" s="12"/>
+      <c r="H46" s="12"/>
+      <c r="I46" s="11"/>
+      <c r="J46" s="11"/>
+      <c r="K46" s="11"/>
+      <c r="L46" s="11"/>
+      <c r="M46" s="11"/>
+    </row>
+    <row r="47" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="13"/>
+      <c r="B47" s="13"/>
+      <c r="C47" s="14"/>
+      <c r="D47" s="14"/>
+      <c r="E47" s="13"/>
+      <c r="F47" s="13"/>
+      <c r="G47" s="14"/>
+      <c r="H47" s="14"/>
+      <c r="I47" s="13"/>
+      <c r="J47" s="13"/>
+      <c r="K47" s="13"/>
+      <c r="L47" s="13"/>
+      <c r="M47" s="13"/>
+    </row>
+    <row r="49" spans="1:13" s="6" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="47" t="s">
         <v>121</v>
       </c>
-      <c r="B44" s="20"/>
-      <c r="C44" s="20"/>
-      <c r="D44" s="20"/>
-      <c r="E44" s="20"/>
-      <c r="F44" s="20"/>
-      <c r="G44" s="20"/>
-      <c r="H44" s="20"/>
-      <c r="I44" s="20"/>
-      <c r="J44" s="20"/>
-      <c r="K44" s="20"/>
-      <c r="L44" s="20"/>
-      <c r="M44" s="20"/>
-    </row>
-    <row r="45" spans="1:13" s="3" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B45" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C45" s="8"/>
-      <c r="D45" s="8"/>
-      <c r="E45" s="8"/>
-      <c r="F45" s="8"/>
-      <c r="G45" s="8"/>
-      <c r="H45" s="8"/>
-      <c r="I45" s="8"/>
-      <c r="J45" s="8"/>
-      <c r="K45" s="8"/>
-      <c r="L45" s="8"/>
-      <c r="M45" s="8"/>
-    </row>
-    <row r="46" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="B46" s="14">
-        <v>65513</v>
-      </c>
-      <c r="C46" s="13"/>
-      <c r="D46" s="14"/>
-      <c r="E46" s="13"/>
-      <c r="F46" s="13"/>
-      <c r="G46" s="14"/>
-      <c r="H46" s="14"/>
-      <c r="I46" s="13"/>
-      <c r="J46" s="13"/>
-      <c r="K46" s="13"/>
-      <c r="L46" s="13"/>
-      <c r="M46" s="13"/>
-    </row>
-    <row r="48" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="21" t="s">
-        <v>123</v>
-      </c>
-      <c r="B48" s="21"/>
-      <c r="C48" s="21"/>
-      <c r="D48" s="21"/>
-      <c r="E48" s="21"/>
-      <c r="F48" s="21"/>
-      <c r="G48" s="21"/>
-      <c r="H48" s="21"/>
-      <c r="I48" s="21"/>
-      <c r="J48" s="21"/>
-      <c r="K48" s="21"/>
-      <c r="L48" s="21"/>
-      <c r="M48" s="21"/>
-    </row>
-    <row r="49" spans="1:16" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="23" t="s">
-        <v>125</v>
-      </c>
-      <c r="B49" s="23"/>
-      <c r="C49" s="23"/>
-      <c r="D49" s="23"/>
-      <c r="E49" s="23"/>
-      <c r="F49" s="23"/>
-      <c r="G49" s="23"/>
-      <c r="H49" s="23"/>
-      <c r="I49" s="23"/>
-      <c r="J49" s="23"/>
-      <c r="K49" s="23"/>
-      <c r="L49" s="23"/>
-      <c r="M49" s="23"/>
-    </row>
-    <row r="50" spans="1:16" s="3" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B49" s="47"/>
+      <c r="C49" s="47"/>
+      <c r="D49" s="47"/>
+      <c r="E49" s="47"/>
+      <c r="F49" s="47"/>
+      <c r="G49" s="47"/>
+      <c r="H49" s="47"/>
+      <c r="I49" s="47"/>
+      <c r="J49" s="47"/>
+      <c r="K49" s="47"/>
+      <c r="L49" s="47"/>
+      <c r="M49" s="47"/>
+    </row>
+    <row r="50" spans="1:13" s="3" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="C50" s="8" t="s">
-        <v>114</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="C50" s="8"/>
       <c r="D50" s="8"/>
       <c r="E50" s="8"/>
       <c r="F50" s="8"/>
@@ -3057,16 +3187,14 @@
       <c r="L50" s="8"/>
       <c r="M50" s="8"/>
     </row>
-    <row r="51" spans="1:16" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="B51" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="C51" s="14">
-        <v>101</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="B51" s="14">
+        <v>65513</v>
+      </c>
+      <c r="C51" s="13"/>
       <c r="D51" s="14"/>
       <c r="E51" s="13"/>
       <c r="F51" s="13"/>
@@ -3078,46 +3206,50 @@
       <c r="L51" s="13"/>
       <c r="M51" s="13"/>
     </row>
-    <row r="52" spans="1:16" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="11"/>
-      <c r="B52" s="11"/>
-      <c r="C52" s="12"/>
-      <c r="D52" s="12"/>
-      <c r="E52" s="11"/>
-      <c r="F52" s="11"/>
-      <c r="G52" s="12"/>
-      <c r="H52" s="12"/>
-      <c r="I52" s="11"/>
-      <c r="J52" s="11"/>
-      <c r="K52" s="11"/>
-      <c r="L52" s="11"/>
-      <c r="M52" s="11"/>
-    </row>
-    <row r="54" spans="1:16" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="21" t="s">
-        <v>126</v>
-      </c>
-      <c r="B54" s="21"/>
-      <c r="C54" s="21"/>
-      <c r="D54" s="21"/>
-      <c r="E54" s="21"/>
-      <c r="F54" s="21"/>
-      <c r="G54" s="21"/>
-      <c r="H54" s="21"/>
-      <c r="I54" s="21"/>
-      <c r="J54" s="21"/>
-      <c r="K54" s="21"/>
-      <c r="L54" s="21"/>
-      <c r="M54" s="21"/>
-    </row>
-    <row r="55" spans="1:16" s="3" customFormat="1" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="30" t="s">
+        <v>123</v>
+      </c>
+      <c r="B53" s="30"/>
+      <c r="C53" s="30"/>
+      <c r="D53" s="30"/>
+      <c r="E53" s="30"/>
+      <c r="F53" s="30"/>
+      <c r="G53" s="30"/>
+      <c r="H53" s="30"/>
+      <c r="I53" s="30"/>
+      <c r="J53" s="30"/>
+      <c r="K53" s="30"/>
+      <c r="L53" s="30"/>
+      <c r="M53" s="30"/>
+    </row>
+    <row r="54" spans="1:13" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="42" t="s">
+        <v>125</v>
+      </c>
+      <c r="B54" s="42"/>
+      <c r="C54" s="42"/>
+      <c r="D54" s="42"/>
+      <c r="E54" s="42"/>
+      <c r="F54" s="42"/>
+      <c r="G54" s="42"/>
+      <c r="H54" s="42"/>
+      <c r="I54" s="42"/>
+      <c r="J54" s="42"/>
+      <c r="K54" s="42"/>
+      <c r="L54" s="42"/>
+      <c r="M54" s="42"/>
+    </row>
+    <row r="55" spans="1:13" s="3" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B55" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="C55" s="8"/>
+      <c r="B55" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="C55" s="8" t="s">
+        <v>114</v>
+      </c>
       <c r="D55" s="8"/>
       <c r="E55" s="8"/>
       <c r="F55" s="8"/>
@@ -3129,14 +3261,16 @@
       <c r="L55" s="8"/>
       <c r="M55" s="8"/>
     </row>
-    <row r="56" spans="1:16" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="B56" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="C56" s="14"/>
+        <v>18</v>
+      </c>
+      <c r="B56" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C56" s="14">
+        <v>101</v>
+      </c>
       <c r="D56" s="14"/>
       <c r="E56" s="13"/>
       <c r="F56" s="13"/>
@@ -3148,50 +3282,46 @@
       <c r="L56" s="13"/>
       <c r="M56" s="13"/>
     </row>
-    <row r="58" spans="1:16" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="B58" s="21"/>
-      <c r="C58" s="21"/>
-      <c r="D58" s="21"/>
-      <c r="E58" s="21"/>
-      <c r="F58" s="21"/>
-      <c r="G58" s="21"/>
-      <c r="H58" s="21"/>
-      <c r="I58" s="21"/>
-      <c r="J58" s="21"/>
-      <c r="K58" s="21"/>
-      <c r="L58" s="21"/>
-      <c r="M58" s="21"/>
-    </row>
-    <row r="59" spans="1:16" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="23" t="s">
-        <v>128</v>
-      </c>
-      <c r="B59" s="23"/>
-      <c r="C59" s="23"/>
-      <c r="D59" s="23"/>
-      <c r="E59" s="23"/>
-      <c r="F59" s="23"/>
-      <c r="G59" s="23"/>
-      <c r="H59" s="23"/>
-      <c r="I59" s="23"/>
-      <c r="J59" s="23"/>
-      <c r="K59" s="23"/>
-      <c r="L59" s="23"/>
-      <c r="M59" s="23"/>
-    </row>
-    <row r="60" spans="1:16" s="3" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="11"/>
+      <c r="B57" s="11"/>
+      <c r="C57" s="12"/>
+      <c r="D57" s="12"/>
+      <c r="E57" s="11"/>
+      <c r="F57" s="11"/>
+      <c r="G57" s="12"/>
+      <c r="H57" s="12"/>
+      <c r="I57" s="11"/>
+      <c r="J57" s="11"/>
+      <c r="K57" s="11"/>
+      <c r="L57" s="11"/>
+      <c r="M57" s="11"/>
+    </row>
+    <row r="59" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="30" t="s">
+        <v>126</v>
+      </c>
+      <c r="B59" s="30"/>
+      <c r="C59" s="30"/>
+      <c r="D59" s="30"/>
+      <c r="E59" s="30"/>
+      <c r="F59" s="30"/>
+      <c r="G59" s="30"/>
+      <c r="H59" s="30"/>
+      <c r="I59" s="30"/>
+      <c r="J59" s="30"/>
+      <c r="K59" s="30"/>
+      <c r="L59" s="30"/>
+      <c r="M59" s="30"/>
+    </row>
+    <row r="60" spans="1:13" s="3" customFormat="1" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B60" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="C60" s="8" t="s">
-        <v>21</v>
-      </c>
+      <c r="B60" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="C60" s="8"/>
       <c r="D60" s="8"/>
       <c r="E60" s="8"/>
       <c r="F60" s="8"/>
@@ -3203,16 +3333,14 @@
       <c r="L60" s="8"/>
       <c r="M60" s="8"/>
     </row>
-    <row r="61" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="B61" s="13" t="s">
-        <v>219</v>
-      </c>
-      <c r="C61" s="13" t="s">
-        <v>23</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="B61" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C61" s="14"/>
       <c r="D61" s="14"/>
       <c r="E61" s="13"/>
       <c r="F61" s="13"/>
@@ -3224,271 +3352,263 @@
       <c r="L61" s="13"/>
       <c r="M61" s="13"/>
     </row>
-    <row r="62" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="11" t="s">
+    <row r="63" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="30" t="s">
+        <v>127</v>
+      </c>
+      <c r="B63" s="30"/>
+      <c r="C63" s="30"/>
+      <c r="D63" s="30"/>
+      <c r="E63" s="30"/>
+      <c r="F63" s="30"/>
+      <c r="G63" s="30"/>
+      <c r="H63" s="30"/>
+      <c r="I63" s="30"/>
+      <c r="J63" s="30"/>
+      <c r="K63" s="30"/>
+      <c r="L63" s="30"/>
+      <c r="M63" s="30"/>
+    </row>
+    <row r="64" spans="1:13" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="42" t="s">
+        <v>128</v>
+      </c>
+      <c r="B64" s="42"/>
+      <c r="C64" s="42"/>
+      <c r="D64" s="42"/>
+      <c r="E64" s="42"/>
+      <c r="F64" s="42"/>
+      <c r="G64" s="42"/>
+      <c r="H64" s="42"/>
+      <c r="I64" s="42"/>
+      <c r="J64" s="42"/>
+      <c r="K64" s="42"/>
+      <c r="L64" s="42"/>
+      <c r="M64" s="42"/>
+    </row>
+    <row r="65" spans="1:16" s="3" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B65" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="C65" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D65" s="8"/>
+      <c r="E65" s="8"/>
+      <c r="F65" s="8"/>
+      <c r="G65" s="8"/>
+      <c r="H65" s="8"/>
+      <c r="I65" s="8"/>
+      <c r="J65" s="8"/>
+      <c r="K65" s="8"/>
+      <c r="L65" s="8"/>
+      <c r="M65" s="8"/>
+    </row>
+    <row r="66" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B62" s="11" t="s">
+      <c r="B66" s="13" t="s">
+        <v>219</v>
+      </c>
+      <c r="C66" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D66" s="14"/>
+      <c r="E66" s="13"/>
+      <c r="F66" s="13"/>
+      <c r="G66" s="14"/>
+      <c r="H66" s="14"/>
+      <c r="I66" s="13"/>
+      <c r="J66" s="13"/>
+      <c r="K66" s="13"/>
+      <c r="L66" s="13"/>
+      <c r="M66" s="13"/>
+    </row>
+    <row r="67" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B67" s="11" t="s">
         <v>220</v>
       </c>
-      <c r="C62" s="11" t="s">
+      <c r="C67" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="D62" s="12"/>
-      <c r="E62" s="11"/>
-      <c r="F62" s="11"/>
-      <c r="G62" s="12"/>
-      <c r="H62" s="12"/>
-      <c r="I62" s="11"/>
-      <c r="J62" s="11"/>
-      <c r="K62" s="11"/>
-      <c r="L62" s="11"/>
-      <c r="M62" s="11"/>
-    </row>
-    <row r="64" spans="1:16" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="25" t="s">
+      <c r="D67" s="12"/>
+      <c r="E67" s="11"/>
+      <c r="F67" s="11"/>
+      <c r="G67" s="12"/>
+      <c r="H67" s="12"/>
+      <c r="I67" s="11"/>
+      <c r="J67" s="11"/>
+      <c r="K67" s="11"/>
+      <c r="L67" s="11"/>
+      <c r="M67" s="11"/>
+    </row>
+    <row r="69" spans="1:16" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="43" t="s">
         <v>129</v>
       </c>
-      <c r="B64" s="25"/>
-      <c r="C64" s="25"/>
-      <c r="D64" s="25"/>
-      <c r="E64" s="25"/>
-      <c r="F64" s="25"/>
-      <c r="G64" s="25"/>
-      <c r="H64" s="25"/>
-      <c r="I64" s="25"/>
-      <c r="J64" s="25"/>
-      <c r="K64" s="25"/>
-      <c r="L64" s="25"/>
-      <c r="M64" s="25"/>
-      <c r="N64" s="25"/>
-      <c r="O64" s="25"/>
-      <c r="P64" s="25"/>
-    </row>
-    <row r="65" spans="1:16" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="26" t="s">
+      <c r="B69" s="43"/>
+      <c r="C69" s="43"/>
+      <c r="D69" s="43"/>
+      <c r="E69" s="43"/>
+      <c r="F69" s="43"/>
+      <c r="G69" s="43"/>
+      <c r="H69" s="43"/>
+      <c r="I69" s="43"/>
+      <c r="J69" s="43"/>
+      <c r="K69" s="43"/>
+      <c r="L69" s="43"/>
+      <c r="M69" s="43"/>
+      <c r="N69" s="43"/>
+      <c r="O69" s="43"/>
+      <c r="P69" s="43"/>
+    </row>
+    <row r="70" spans="1:16" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="39" t="s">
         <v>148</v>
       </c>
-      <c r="B65" s="26"/>
-      <c r="C65" s="26"/>
-      <c r="D65" s="26"/>
-      <c r="E65" s="26"/>
-      <c r="F65" s="26"/>
-      <c r="G65" s="26"/>
-      <c r="H65" s="26"/>
-      <c r="I65" s="26"/>
-      <c r="J65" s="26"/>
-      <c r="K65" s="26"/>
-      <c r="L65" s="26"/>
-      <c r="M65" s="26"/>
-      <c r="N65" s="26"/>
-      <c r="O65" s="26"/>
-      <c r="P65" s="26"/>
-    </row>
-    <row r="66" spans="1:16" s="3" customFormat="1" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="8" t="s">
+      <c r="B70" s="39"/>
+      <c r="C70" s="39"/>
+      <c r="D70" s="39"/>
+      <c r="E70" s="39"/>
+      <c r="F70" s="39"/>
+      <c r="G70" s="39"/>
+      <c r="H70" s="39"/>
+      <c r="I70" s="39"/>
+      <c r="J70" s="39"/>
+      <c r="K70" s="39"/>
+      <c r="L70" s="39"/>
+      <c r="M70" s="39"/>
+      <c r="N70" s="39"/>
+      <c r="O70" s="39"/>
+      <c r="P70" s="39"/>
+    </row>
+    <row r="71" spans="1:16" s="3" customFormat="1" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B66" s="8" t="s">
+      <c r="B71" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="C66" s="8" t="s">
+      <c r="C71" s="8" t="s">
         <v>139</v>
       </c>
-      <c r="D66" s="8" t="s">
+      <c r="D71" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="E66" s="38" t="s">
+      <c r="E71" s="20" t="s">
         <v>140</v>
       </c>
-      <c r="F66" s="39"/>
-      <c r="G66" s="38" t="s">
+      <c r="F71" s="21"/>
+      <c r="G71" s="20" t="s">
         <v>141</v>
       </c>
-      <c r="H66" s="39"/>
-      <c r="I66" s="38" t="s">
+      <c r="H71" s="21"/>
+      <c r="I71" s="20" t="s">
         <v>142</v>
       </c>
-      <c r="J66" s="39"/>
-      <c r="K66" s="8" t="s">
+      <c r="J71" s="21"/>
+      <c r="K71" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="L66" s="8" t="s">
+      <c r="L71" s="8" t="s">
         <v>194</v>
       </c>
-      <c r="M66" s="18" t="s">
+      <c r="M71" s="18" t="s">
         <v>144</v>
       </c>
-      <c r="N66" s="8" t="s">
+      <c r="N71" s="8" t="s">
         <v>145</v>
       </c>
-      <c r="O66" s="8" t="s">
+      <c r="O71" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="P66" s="8" t="s">
+      <c r="P71" s="8" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="67" spans="1:16" s="4" customFormat="1" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="13" t="s">
+    <row r="72" spans="1:16" s="4" customFormat="1" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="B67" s="14">
+      <c r="B72" s="14">
         <v>25</v>
       </c>
-      <c r="C67" s="13" t="s">
+      <c r="C72" s="13" t="s">
         <v>204</v>
       </c>
-      <c r="D67" s="14" t="s">
+      <c r="D72" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="E67" s="47" t="s">
+      <c r="E72" s="35" t="s">
         <v>205</v>
       </c>
-      <c r="F67" s="46"/>
-      <c r="G67" s="48" t="s">
+      <c r="F72" s="36"/>
+      <c r="G72" s="22" t="s">
         <v>206</v>
       </c>
-      <c r="H67" s="40"/>
-      <c r="I67" s="48" t="s">
+      <c r="H72" s="23"/>
+      <c r="I72" s="22" t="s">
         <v>206</v>
       </c>
-      <c r="J67" s="40"/>
-      <c r="K67" s="13" t="s">
+      <c r="J72" s="23"/>
+      <c r="K72" s="13" t="s">
         <v>207</v>
       </c>
-      <c r="L67" s="14" t="s">
+      <c r="L72" s="14" t="s">
         <v>208</v>
       </c>
-      <c r="M67" s="19" t="s">
+      <c r="M72" s="19" t="s">
         <v>209</v>
       </c>
-      <c r="N67" s="13">
+      <c r="N72" s="13">
         <v>5555555</v>
       </c>
-      <c r="O67" s="13">
+      <c r="O72" s="13">
         <v>5555555</v>
       </c>
-      <c r="P67" s="13">
+      <c r="P72" s="13">
         <v>555555</v>
       </c>
     </row>
-    <row r="68" spans="1:16" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="69" spans="1:16" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="21" t="s">
+    <row r="73" spans="1:16" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
+    <row r="74" spans="1:16" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="30" t="s">
         <v>132</v>
       </c>
-      <c r="B69" s="21"/>
-      <c r="C69" s="21"/>
-      <c r="D69" s="21"/>
-      <c r="E69" s="21"/>
-      <c r="F69" s="21"/>
-      <c r="G69" s="21"/>
-      <c r="H69" s="21"/>
-      <c r="I69" s="21"/>
-      <c r="J69" s="21"/>
-      <c r="K69" s="21"/>
-      <c r="L69" s="21"/>
-      <c r="M69" s="21"/>
-    </row>
-    <row r="70" spans="1:16" s="3" customFormat="1" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B70" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="C70" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D70" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="E70" s="8"/>
-      <c r="F70" s="8"/>
-      <c r="G70" s="8"/>
-      <c r="H70" s="8"/>
-      <c r="I70" s="8"/>
-      <c r="J70" s="8"/>
-      <c r="K70" s="8"/>
-      <c r="L70" s="8"/>
-      <c r="M70" s="8"/>
-    </row>
-    <row r="71" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="B71" s="13" t="s">
-        <v>219</v>
-      </c>
-      <c r="C71" s="13" t="s">
-        <v>130</v>
-      </c>
-      <c r="D71" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="E71" s="13"/>
-      <c r="F71" s="13"/>
-      <c r="G71" s="14"/>
-      <c r="H71" s="14"/>
-      <c r="I71" s="13"/>
-      <c r="J71" s="13"/>
-      <c r="K71" s="13"/>
-      <c r="L71" s="13"/>
-      <c r="M71" s="13"/>
-    </row>
-    <row r="72" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="B72" s="11" t="s">
-        <v>220</v>
-      </c>
-      <c r="C72" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="D72" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="E72" s="11"/>
-      <c r="F72" s="11"/>
-      <c r="G72" s="12"/>
-      <c r="H72" s="12"/>
-      <c r="I72" s="11"/>
-      <c r="J72" s="11"/>
-      <c r="K72" s="11"/>
-      <c r="L72" s="11"/>
-      <c r="M72" s="11"/>
-    </row>
-    <row r="74" spans="1:16" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="21" t="s">
-        <v>133</v>
-      </c>
-      <c r="B74" s="21"/>
-      <c r="C74" s="21"/>
-      <c r="D74" s="21"/>
-      <c r="E74" s="21"/>
-      <c r="F74" s="21"/>
-      <c r="G74" s="21"/>
-      <c r="H74" s="21"/>
-      <c r="I74" s="21"/>
-      <c r="J74" s="21"/>
-      <c r="K74" s="21"/>
-      <c r="L74" s="21"/>
-      <c r="M74" s="21"/>
-    </row>
-    <row r="75" spans="1:16" s="3" customFormat="1" ht="31.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B74" s="30"/>
+      <c r="C74" s="30"/>
+      <c r="D74" s="30"/>
+      <c r="E74" s="30"/>
+      <c r="F74" s="30"/>
+      <c r="G74" s="30"/>
+      <c r="H74" s="30"/>
+      <c r="I74" s="30"/>
+      <c r="J74" s="30"/>
+      <c r="K74" s="30"/>
+      <c r="L74" s="30"/>
+      <c r="M74" s="30"/>
+    </row>
+    <row r="75" spans="1:16" s="3" customFormat="1" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B75" s="27" t="s">
-        <v>28</v>
-      </c>
-      <c r="C75" s="28"/>
-      <c r="D75" s="27" t="s">
-        <v>134</v>
-      </c>
-      <c r="E75" s="28"/>
+      <c r="B75" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="C75" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D75" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="E75" s="8"/>
       <c r="F75" s="8"/>
       <c r="G75" s="8"/>
       <c r="H75" s="8"/>
@@ -3500,16 +3620,18 @@
     </row>
     <row r="76" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B76" s="29" t="s">
-        <v>30</v>
-      </c>
-      <c r="C76" s="30"/>
-      <c r="D76" s="34" t="s">
-        <v>24</v>
-      </c>
-      <c r="E76" s="36"/>
+        <v>27</v>
+      </c>
+      <c r="B76" s="13" t="s">
+        <v>219</v>
+      </c>
+      <c r="C76" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="D76" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E76" s="13"/>
       <c r="F76" s="13"/>
       <c r="G76" s="14"/>
       <c r="H76" s="14"/>
@@ -3521,16 +3643,18 @@
     </row>
     <row r="77" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="B77" s="41" t="s">
-        <v>137</v>
-      </c>
-      <c r="C77" s="43"/>
-      <c r="D77" s="44" t="s">
-        <v>23</v>
-      </c>
-      <c r="E77" s="45"/>
+        <v>27</v>
+      </c>
+      <c r="B77" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="C77" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="D77" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="E77" s="11"/>
       <c r="F77" s="11"/>
       <c r="G77" s="12"/>
       <c r="H77" s="12"/>
@@ -3541,36 +3665,34 @@
       <c r="M77" s="11"/>
     </row>
     <row r="79" spans="1:16" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="21" t="s">
-        <v>135</v>
-      </c>
-      <c r="B79" s="21"/>
-      <c r="C79" s="21"/>
-      <c r="D79" s="21"/>
-      <c r="E79" s="21"/>
-      <c r="F79" s="21"/>
-      <c r="G79" s="21"/>
-      <c r="H79" s="21"/>
-      <c r="I79" s="21"/>
-      <c r="J79" s="21"/>
-      <c r="K79" s="21"/>
-      <c r="L79" s="21"/>
-      <c r="M79" s="21"/>
-    </row>
-    <row r="80" spans="1:16" s="3" customFormat="1" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A79" s="30" t="s">
+        <v>133</v>
+      </c>
+      <c r="B79" s="30"/>
+      <c r="C79" s="30"/>
+      <c r="D79" s="30"/>
+      <c r="E79" s="30"/>
+      <c r="F79" s="30"/>
+      <c r="G79" s="30"/>
+      <c r="H79" s="30"/>
+      <c r="I79" s="30"/>
+      <c r="J79" s="30"/>
+      <c r="K79" s="30"/>
+      <c r="L79" s="30"/>
+      <c r="M79" s="30"/>
+    </row>
+    <row r="80" spans="1:16" s="3" customFormat="1" ht="31.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B80" s="8" t="s">
-        <v>185</v>
-      </c>
-      <c r="C80" s="8" t="s">
-        <v>186</v>
-      </c>
-      <c r="D80" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="E80" s="8"/>
+      <c r="B80" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="C80" s="26"/>
+      <c r="D80" s="24" t="s">
+        <v>134</v>
+      </c>
+      <c r="E80" s="26"/>
       <c r="F80" s="8"/>
       <c r="G80" s="8"/>
       <c r="H80" s="8"/>
@@ -3582,18 +3704,16 @@
     </row>
     <row r="81" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="B81" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="C81" s="13" t="s">
-        <v>221</v>
-      </c>
-      <c r="D81" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="E81" s="13"/>
+        <v>29</v>
+      </c>
+      <c r="B81" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="C81" s="41"/>
+      <c r="D81" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="E81" s="32"/>
       <c r="F81" s="13"/>
       <c r="G81" s="14"/>
       <c r="H81" s="14"/>
@@ -3605,18 +3725,16 @@
     </row>
     <row r="82" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A82" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="B82" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="C82" s="11" t="s">
-        <v>222</v>
-      </c>
-      <c r="D82" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="E82" s="11"/>
+        <v>29</v>
+      </c>
+      <c r="B82" s="27" t="s">
+        <v>137</v>
+      </c>
+      <c r="C82" s="29"/>
+      <c r="D82" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="E82" s="34"/>
       <c r="F82" s="11"/>
       <c r="G82" s="12"/>
       <c r="H82" s="12"/>
@@ -3627,35 +3745,37 @@
       <c r="M82" s="11"/>
     </row>
     <row r="84" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A84" s="21" t="s">
-        <v>158</v>
-      </c>
-      <c r="B84" s="21"/>
-      <c r="C84" s="21"/>
-      <c r="D84" s="21"/>
-      <c r="E84" s="21"/>
-      <c r="F84" s="21"/>
-      <c r="G84" s="21"/>
-      <c r="H84" s="21"/>
-      <c r="I84" s="21"/>
-      <c r="J84" s="21"/>
-      <c r="K84" s="21"/>
-      <c r="L84" s="21"/>
-      <c r="M84" s="21"/>
-    </row>
-    <row r="85" spans="1:13" s="3" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A84" s="30" t="s">
+        <v>135</v>
+      </c>
+      <c r="B84" s="30"/>
+      <c r="C84" s="30"/>
+      <c r="D84" s="30"/>
+      <c r="E84" s="30"/>
+      <c r="F84" s="30"/>
+      <c r="G84" s="30"/>
+      <c r="H84" s="30"/>
+      <c r="I84" s="30"/>
+      <c r="J84" s="30"/>
+      <c r="K84" s="30"/>
+      <c r="L84" s="30"/>
+      <c r="M84" s="30"/>
+    </row>
+    <row r="85" spans="1:13" s="3" customFormat="1" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A85" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B85" s="33" t="s">
-        <v>156</v>
-      </c>
-      <c r="C85" s="33"/>
-      <c r="D85" s="27" t="s">
-        <v>157</v>
-      </c>
-      <c r="E85" s="33"/>
-      <c r="F85" s="28"/>
+      <c r="B85" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="C85" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="D85" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="E85" s="8"/>
+      <c r="F85" s="8"/>
       <c r="G85" s="8"/>
       <c r="H85" s="8"/>
       <c r="I85" s="8"/>
@@ -3664,19 +3784,21 @@
       <c r="L85" s="8"/>
       <c r="M85" s="8"/>
     </row>
-    <row r="86" spans="1:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A86" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="B86" s="29" t="s">
-        <v>26</v>
-      </c>
-      <c r="C86" s="30"/>
-      <c r="D86" s="34" t="s">
-        <v>35</v>
-      </c>
-      <c r="E86" s="35"/>
-      <c r="F86" s="36"/>
+        <v>31</v>
+      </c>
+      <c r="B86" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C86" s="13" t="s">
+        <v>221</v>
+      </c>
+      <c r="D86" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E86" s="13"/>
+      <c r="F86" s="13"/>
       <c r="G86" s="14"/>
       <c r="H86" s="14"/>
       <c r="I86" s="13"/>
@@ -3685,56 +3807,59 @@
       <c r="L86" s="13"/>
       <c r="M86" s="13"/>
     </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B87" s="7"/>
-    </row>
-    <row r="88" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="21" t="s">
-        <v>150</v>
-      </c>
-      <c r="B88" s="21"/>
-      <c r="C88" s="21"/>
-      <c r="D88" s="21"/>
-      <c r="E88" s="21"/>
-      <c r="F88" s="21"/>
-      <c r="G88" s="21"/>
-      <c r="H88" s="21"/>
-      <c r="I88" s="21"/>
-      <c r="J88" s="21"/>
-      <c r="K88" s="21"/>
-      <c r="L88" s="21"/>
-      <c r="M88" s="21"/>
-    </row>
-    <row r="89" spans="1:13" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A89" s="23" t="s">
-        <v>151</v>
-      </c>
-      <c r="B89" s="23"/>
-      <c r="C89" s="23"/>
-      <c r="D89" s="23"/>
-      <c r="E89" s="23"/>
-      <c r="F89" s="23"/>
-      <c r="G89" s="23"/>
-      <c r="H89" s="23"/>
-      <c r="I89" s="23"/>
-      <c r="J89" s="23"/>
-      <c r="K89" s="23"/>
-      <c r="L89" s="23"/>
-      <c r="M89" s="23"/>
-    </row>
-    <row r="90" spans="1:13" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A87" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B87" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C87" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="D87" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="E87" s="11"/>
+      <c r="F87" s="11"/>
+      <c r="G87" s="12"/>
+      <c r="H87" s="12"/>
+      <c r="I87" s="11"/>
+      <c r="J87" s="11"/>
+      <c r="K87" s="11"/>
+      <c r="L87" s="11"/>
+      <c r="M87" s="11"/>
+    </row>
+    <row r="89" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A89" s="30" t="s">
+        <v>158</v>
+      </c>
+      <c r="B89" s="30"/>
+      <c r="C89" s="30"/>
+      <c r="D89" s="30"/>
+      <c r="E89" s="30"/>
+      <c r="F89" s="30"/>
+      <c r="G89" s="30"/>
+      <c r="H89" s="30"/>
+      <c r="I89" s="30"/>
+      <c r="J89" s="30"/>
+      <c r="K89" s="30"/>
+      <c r="L89" s="30"/>
+      <c r="M89" s="30"/>
+    </row>
+    <row r="90" spans="1:13" s="3" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A90" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B90" s="8" t="s">
-        <v>187</v>
-      </c>
-      <c r="C90" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="D90" s="33"/>
-      <c r="E90" s="28"/>
-      <c r="F90" s="8"/>
+      <c r="B90" s="25" t="s">
+        <v>156</v>
+      </c>
+      <c r="C90" s="25"/>
+      <c r="D90" s="24" t="s">
+        <v>157</v>
+      </c>
+      <c r="E90" s="25"/>
+      <c r="F90" s="26"/>
       <c r="G90" s="8"/>
       <c r="H90" s="8"/>
       <c r="I90" s="8"/>
@@ -3743,19 +3868,19 @@
       <c r="L90" s="8"/>
       <c r="M90" s="8"/>
     </row>
-    <row r="91" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A91" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="B91" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="C91" s="29" t="s">
-        <v>196</v>
-      </c>
-      <c r="D91" s="37"/>
-      <c r="E91" s="30"/>
-      <c r="F91" s="13"/>
+        <v>34</v>
+      </c>
+      <c r="B91" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="C91" s="41"/>
+      <c r="D91" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="E91" s="44"/>
+      <c r="F91" s="32"/>
       <c r="G91" s="14"/>
       <c r="H91" s="14"/>
       <c r="I91" s="13"/>
@@ -3764,1067 +3889,1175 @@
       <c r="L91" s="13"/>
       <c r="M91" s="13"/>
     </row>
-    <row r="92" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A92" s="11" t="s">
+    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B92" s="7"/>
+    </row>
+    <row r="93" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A93" s="30" t="s">
+        <v>150</v>
+      </c>
+      <c r="B93" s="30"/>
+      <c r="C93" s="30"/>
+      <c r="D93" s="30"/>
+      <c r="E93" s="30"/>
+      <c r="F93" s="30"/>
+      <c r="G93" s="30"/>
+      <c r="H93" s="30"/>
+      <c r="I93" s="30"/>
+      <c r="J93" s="30"/>
+      <c r="K93" s="30"/>
+      <c r="L93" s="30"/>
+      <c r="M93" s="30"/>
+    </row>
+    <row r="94" spans="1:13" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A94" s="42" t="s">
+        <v>151</v>
+      </c>
+      <c r="B94" s="42"/>
+      <c r="C94" s="42"/>
+      <c r="D94" s="42"/>
+      <c r="E94" s="42"/>
+      <c r="F94" s="42"/>
+      <c r="G94" s="42"/>
+      <c r="H94" s="42"/>
+      <c r="I94" s="42"/>
+      <c r="J94" s="42"/>
+      <c r="K94" s="42"/>
+      <c r="L94" s="42"/>
+      <c r="M94" s="42"/>
+    </row>
+    <row r="95" spans="1:13" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A95" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B95" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="C95" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="D95" s="25"/>
+      <c r="E95" s="26"/>
+      <c r="F95" s="8"/>
+      <c r="G95" s="8"/>
+      <c r="H95" s="8"/>
+      <c r="I95" s="8"/>
+      <c r="J95" s="8"/>
+      <c r="K95" s="8"/>
+      <c r="L95" s="8"/>
+      <c r="M95" s="8"/>
+    </row>
+    <row r="96" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A96" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="B92" s="11" t="s">
+      <c r="B96" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C96" s="40" t="s">
+        <v>196</v>
+      </c>
+      <c r="D96" s="45"/>
+      <c r="E96" s="41"/>
+      <c r="F96" s="13"/>
+      <c r="G96" s="14"/>
+      <c r="H96" s="14"/>
+      <c r="I96" s="13"/>
+      <c r="J96" s="13"/>
+      <c r="K96" s="13"/>
+      <c r="L96" s="13"/>
+      <c r="M96" s="13"/>
+    </row>
+    <row r="97" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A97" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B97" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="C92" s="41"/>
-      <c r="D92" s="42"/>
-      <c r="E92" s="43"/>
-      <c r="F92" s="11"/>
-      <c r="G92" s="12"/>
-      <c r="H92" s="12"/>
-      <c r="I92" s="11"/>
-      <c r="J92" s="11"/>
-      <c r="K92" s="11"/>
-      <c r="L92" s="11"/>
-      <c r="M92" s="11"/>
-    </row>
-    <row r="93" spans="1:13" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="94" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A94" s="25" t="s">
+      <c r="C97" s="27"/>
+      <c r="D97" s="28"/>
+      <c r="E97" s="29"/>
+      <c r="F97" s="11"/>
+      <c r="G97" s="12"/>
+      <c r="H97" s="12"/>
+      <c r="I97" s="11"/>
+      <c r="J97" s="11"/>
+      <c r="K97" s="11"/>
+      <c r="L97" s="11"/>
+      <c r="M97" s="11"/>
+    </row>
+    <row r="98" spans="1:13" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
+    <row r="99" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A99" s="43" t="s">
         <v>159</v>
       </c>
-      <c r="B94" s="25"/>
-      <c r="C94" s="25"/>
-      <c r="D94" s="25"/>
-      <c r="E94" s="25"/>
-      <c r="F94" s="25"/>
-      <c r="G94" s="25"/>
-      <c r="H94" s="25"/>
-      <c r="I94" s="25"/>
-      <c r="J94" s="25"/>
-      <c r="K94" s="25"/>
-      <c r="L94" s="25"/>
-      <c r="M94" s="25"/>
-    </row>
-    <row r="95" spans="1:13" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A95" s="23" t="s">
+      <c r="B99" s="43"/>
+      <c r="C99" s="43"/>
+      <c r="D99" s="43"/>
+      <c r="E99" s="43"/>
+      <c r="F99" s="43"/>
+      <c r="G99" s="43"/>
+      <c r="H99" s="43"/>
+      <c r="I99" s="43"/>
+      <c r="J99" s="43"/>
+      <c r="K99" s="43"/>
+      <c r="L99" s="43"/>
+      <c r="M99" s="43"/>
+    </row>
+    <row r="100" spans="1:13" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A100" s="42" t="s">
         <v>163</v>
       </c>
-      <c r="B95" s="23"/>
-      <c r="C95" s="23"/>
-      <c r="D95" s="23"/>
-      <c r="E95" s="23"/>
-      <c r="F95" s="23"/>
-      <c r="G95" s="23"/>
-      <c r="H95" s="23"/>
-      <c r="I95" s="23"/>
-      <c r="J95" s="23"/>
-      <c r="K95" s="23"/>
-      <c r="L95" s="23"/>
-      <c r="M95" s="23"/>
-    </row>
-    <row r="96" spans="1:13" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A96" s="8" t="s">
+      <c r="B100" s="42"/>
+      <c r="C100" s="42"/>
+      <c r="D100" s="42"/>
+      <c r="E100" s="42"/>
+      <c r="F100" s="42"/>
+      <c r="G100" s="42"/>
+      <c r="H100" s="42"/>
+      <c r="I100" s="42"/>
+      <c r="J100" s="42"/>
+      <c r="K100" s="42"/>
+      <c r="L100" s="42"/>
+      <c r="M100" s="42"/>
+    </row>
+    <row r="101" spans="1:13" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A101" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B96" s="8" t="s">
+      <c r="B101" s="8" t="s">
         <v>153</v>
       </c>
-      <c r="C96" s="8" t="s">
+      <c r="C101" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="D96" s="8" t="s">
+      <c r="D101" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="E96" s="8" t="s">
+      <c r="E101" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="F96" s="8" t="s">
+      <c r="F101" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="G96" s="8" t="s">
+      <c r="G101" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="H96" s="8"/>
-      <c r="I96" s="8"/>
-      <c r="J96" s="8"/>
-      <c r="K96" s="8"/>
-      <c r="L96" s="8"/>
-      <c r="M96" s="8"/>
-    </row>
-    <row r="97" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A97" s="13" t="s">
+      <c r="H101" s="8"/>
+      <c r="I101" s="8"/>
+      <c r="J101" s="8"/>
+      <c r="K101" s="8"/>
+      <c r="L101" s="8"/>
+      <c r="M101" s="8"/>
+    </row>
+    <row r="102" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A102" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="B97" s="13" t="s">
+      <c r="B102" s="13" t="s">
         <v>221</v>
       </c>
-      <c r="C97" s="14">
+      <c r="C102" s="14">
         <v>162</v>
       </c>
-      <c r="D97" s="14" t="s">
+      <c r="D102" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="E97" s="13" t="s">
+      <c r="E102" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="F97" s="13" t="s">
+      <c r="F102" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="G97" s="14" t="s">
+      <c r="G102" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="H97" s="14"/>
-      <c r="I97" s="13"/>
-      <c r="J97" s="13"/>
-      <c r="K97" s="13"/>
-      <c r="L97" s="13"/>
-      <c r="M97" s="13"/>
-    </row>
-    <row r="98" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="11" t="s">
+      <c r="H102" s="14"/>
+      <c r="I102" s="13"/>
+      <c r="J102" s="13"/>
+      <c r="K102" s="13"/>
+      <c r="L102" s="13"/>
+      <c r="M102" s="13"/>
+    </row>
+    <row r="103" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A103" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="B98" s="11" t="s">
+      <c r="B103" s="11" t="s">
         <v>222</v>
       </c>
-      <c r="C98" s="12">
+      <c r="C103" s="12">
         <v>162</v>
       </c>
-      <c r="D98" s="12" t="s">
+      <c r="D103" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="E98" s="11" t="s">
+      <c r="E103" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="F98" s="11" t="s">
+      <c r="F103" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="G98" s="12" t="s">
+      <c r="G103" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="H98" s="12"/>
-      <c r="I98" s="11"/>
-      <c r="J98" s="11"/>
-      <c r="K98" s="11"/>
-      <c r="L98" s="11"/>
-      <c r="M98" s="11"/>
-    </row>
-    <row r="99" spans="1:13" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="100" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A100" s="21" t="s">
+      <c r="H103" s="12"/>
+      <c r="I103" s="11"/>
+      <c r="J103" s="11"/>
+      <c r="K103" s="11"/>
+      <c r="L103" s="11"/>
+      <c r="M103" s="11"/>
+    </row>
+    <row r="104" spans="1:13" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
+    <row r="105" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A105" s="30" t="s">
         <v>160</v>
       </c>
-      <c r="B100" s="21"/>
-      <c r="C100" s="21"/>
-      <c r="D100" s="21"/>
-      <c r="E100" s="21"/>
-      <c r="F100" s="21"/>
-      <c r="G100" s="21"/>
-      <c r="H100" s="21"/>
-      <c r="I100" s="21"/>
-      <c r="J100" s="21"/>
-      <c r="K100" s="21"/>
-      <c r="L100" s="21"/>
-      <c r="M100" s="21"/>
-    </row>
-    <row r="101" spans="1:13" s="3" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A101" s="23" t="s">
+      <c r="B105" s="30"/>
+      <c r="C105" s="30"/>
+      <c r="D105" s="30"/>
+      <c r="E105" s="30"/>
+      <c r="F105" s="30"/>
+      <c r="G105" s="30"/>
+      <c r="H105" s="30"/>
+      <c r="I105" s="30"/>
+      <c r="J105" s="30"/>
+      <c r="K105" s="30"/>
+      <c r="L105" s="30"/>
+      <c r="M105" s="30"/>
+    </row>
+    <row r="106" spans="1:13" s="3" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A106" s="42" t="s">
         <v>161</v>
       </c>
-      <c r="B101" s="23"/>
-      <c r="C101" s="23"/>
-      <c r="D101" s="23"/>
-      <c r="E101" s="23"/>
-      <c r="F101" s="23"/>
-      <c r="G101" s="23"/>
-      <c r="H101" s="23"/>
-      <c r="I101" s="23"/>
-      <c r="J101" s="23"/>
-      <c r="K101" s="23"/>
-      <c r="L101" s="23"/>
-      <c r="M101" s="23"/>
-    </row>
-    <row r="102" spans="1:13" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A102" s="8" t="s">
+      <c r="B106" s="42"/>
+      <c r="C106" s="42"/>
+      <c r="D106" s="42"/>
+      <c r="E106" s="42"/>
+      <c r="F106" s="42"/>
+      <c r="G106" s="42"/>
+      <c r="H106" s="42"/>
+      <c r="I106" s="42"/>
+      <c r="J106" s="42"/>
+      <c r="K106" s="42"/>
+      <c r="L106" s="42"/>
+      <c r="M106" s="42"/>
+    </row>
+    <row r="107" spans="1:13" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A107" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B102" s="8" t="s">
+      <c r="B107" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="C102" s="8" t="s">
+      <c r="C107" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="D102" s="8" t="s">
+      <c r="D107" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="E102" s="8" t="s">
+      <c r="E107" s="8" t="s">
         <v>162</v>
       </c>
-      <c r="F102" s="8" t="s">
+      <c r="F107" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="G102" s="8"/>
-      <c r="H102" s="8"/>
-      <c r="I102" s="8"/>
-      <c r="J102" s="8"/>
-      <c r="K102" s="8"/>
-      <c r="L102" s="8"/>
-      <c r="M102" s="8"/>
-    </row>
-    <row r="103" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A103" s="13" t="s">
+      <c r="G107" s="8"/>
+      <c r="H107" s="8"/>
+      <c r="I107" s="8"/>
+      <c r="J107" s="8"/>
+      <c r="K107" s="8"/>
+      <c r="L107" s="8"/>
+      <c r="M107" s="8"/>
+    </row>
+    <row r="108" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A108" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="B103" s="13" t="s">
+      <c r="B108" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="C103" s="13" t="s">
+      <c r="C108" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="D103" s="14" t="s">
+      <c r="D108" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="E103" s="13" t="s">
+      <c r="E108" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="F103" s="13" t="s">
+      <c r="F108" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="G103" s="14"/>
-      <c r="H103" s="14"/>
-      <c r="I103" s="13"/>
-      <c r="J103" s="13"/>
-      <c r="K103" s="13"/>
-      <c r="L103" s="13"/>
-      <c r="M103" s="13"/>
-    </row>
-    <row r="104" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A104" s="11" t="s">
+      <c r="G108" s="14"/>
+      <c r="H108" s="14"/>
+      <c r="I108" s="13"/>
+      <c r="J108" s="13"/>
+      <c r="K108" s="13"/>
+      <c r="L108" s="13"/>
+      <c r="M108" s="13"/>
+    </row>
+    <row r="109" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A109" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="B104" s="11" t="s">
+      <c r="B109" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="C104" s="11" t="s">
+      <c r="C109" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="D104" s="12" t="s">
+      <c r="D109" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="E104" s="11" t="s">
+      <c r="E109" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="F104" s="11" t="s">
+      <c r="F109" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="G104" s="12"/>
-      <c r="H104" s="12"/>
-      <c r="I104" s="11"/>
-      <c r="J104" s="11"/>
-      <c r="K104" s="11"/>
-      <c r="L104" s="11"/>
-      <c r="M104" s="11"/>
-    </row>
-    <row r="105" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A105" s="13" t="s">
+      <c r="G109" s="12"/>
+      <c r="H109" s="12"/>
+      <c r="I109" s="11"/>
+      <c r="J109" s="11"/>
+      <c r="K109" s="11"/>
+      <c r="L109" s="11"/>
+      <c r="M109" s="11"/>
+    </row>
+    <row r="110" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A110" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="B105" s="13" t="s">
+      <c r="B110" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="C105" s="13" t="s">
+      <c r="C110" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="D105" s="14"/>
-      <c r="E105" s="13" t="s">
+      <c r="D110" s="14"/>
+      <c r="E110" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="F105" s="13" t="s">
+      <c r="F110" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="G105" s="14"/>
-      <c r="H105" s="14"/>
-      <c r="I105" s="13"/>
-      <c r="J105" s="13"/>
-      <c r="K105" s="13"/>
-      <c r="L105" s="13"/>
-      <c r="M105" s="13"/>
-    </row>
-    <row r="106" spans="1:13" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="107" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A107" s="21" t="s">
+      <c r="G110" s="14"/>
+      <c r="H110" s="14"/>
+      <c r="I110" s="13"/>
+      <c r="J110" s="13"/>
+      <c r="K110" s="13"/>
+      <c r="L110" s="13"/>
+      <c r="M110" s="13"/>
+    </row>
+    <row r="111" spans="1:13" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
+    <row r="112" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A112" s="30" t="s">
         <v>164</v>
       </c>
-      <c r="B107" s="21"/>
-      <c r="C107" s="21"/>
-      <c r="D107" s="21"/>
-      <c r="E107" s="21"/>
-      <c r="F107" s="21"/>
-      <c r="G107" s="21"/>
-      <c r="H107" s="21"/>
-      <c r="I107" s="21"/>
-      <c r="J107" s="21"/>
-      <c r="K107" s="21"/>
-      <c r="L107" s="21"/>
-      <c r="M107" s="21"/>
-    </row>
-    <row r="108" spans="1:13" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A108" s="8" t="s">
+      <c r="B112" s="30"/>
+      <c r="C112" s="30"/>
+      <c r="D112" s="30"/>
+      <c r="E112" s="30"/>
+      <c r="F112" s="30"/>
+      <c r="G112" s="30"/>
+      <c r="H112" s="30"/>
+      <c r="I112" s="30"/>
+      <c r="J112" s="30"/>
+      <c r="K112" s="30"/>
+      <c r="L112" s="30"/>
+      <c r="M112" s="30"/>
+    </row>
+    <row r="113" spans="1:13" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A113" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B108" s="8" t="s">
+      <c r="B113" s="8" t="s">
         <v>171</v>
       </c>
-      <c r="C108" s="8" t="s">
+      <c r="C113" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="D108" s="8" t="s">
+      <c r="D113" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="E108" s="8" t="s">
+      <c r="E113" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="F108" s="8" t="s">
+      <c r="F113" s="8" t="s">
         <v>170</v>
       </c>
-      <c r="G108" s="8" t="s">
+      <c r="G113" s="8" t="s">
         <v>169</v>
       </c>
-      <c r="H108" s="8" t="s">
+      <c r="H113" s="8" t="s">
         <v>168</v>
       </c>
-      <c r="I108" s="8" t="s">
+      <c r="I113" s="8" t="s">
         <v>167</v>
       </c>
-      <c r="J108" s="8" t="s">
+      <c r="J113" s="8" t="s">
         <v>166</v>
       </c>
-      <c r="K108" s="8"/>
-      <c r="L108" s="8"/>
-      <c r="M108" s="8"/>
-    </row>
-    <row r="109" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A109" s="13" t="s">
+      <c r="K113" s="8"/>
+      <c r="L113" s="8"/>
+      <c r="M113" s="8"/>
+    </row>
+    <row r="114" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A114" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="B109" s="13" t="s">
+      <c r="B114" s="13" t="s">
         <v>221</v>
       </c>
-      <c r="C109" s="14">
+      <c r="C114" s="14">
         <v>514</v>
       </c>
-      <c r="D109" s="14" t="s">
+      <c r="D114" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="E109" s="13" t="s">
+      <c r="E114" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="F109" s="13" t="s">
+      <c r="F114" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="G109" s="14" t="s">
+      <c r="G114" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="H109" s="14" t="s">
+      <c r="H114" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="I109" s="13" t="s">
+      <c r="I114" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="J109" s="13" t="s">
+      <c r="J114" s="13" t="s">
         <v>165</v>
       </c>
-      <c r="K109" s="13"/>
-      <c r="L109" s="13"/>
-      <c r="M109" s="13"/>
-    </row>
-    <row r="110" spans="1:13" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="111" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A111" s="21" t="s">
+      <c r="K114" s="13"/>
+      <c r="L114" s="13"/>
+      <c r="M114" s="13"/>
+    </row>
+    <row r="115" spans="1:13" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
+    <row r="116" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A116" s="30" t="s">
         <v>172</v>
       </c>
-      <c r="B111" s="21"/>
-      <c r="C111" s="21"/>
-      <c r="D111" s="21"/>
-      <c r="E111" s="21"/>
-      <c r="F111" s="21"/>
-      <c r="G111" s="21"/>
-      <c r="H111" s="21"/>
-      <c r="I111" s="21"/>
-      <c r="J111" s="21"/>
-      <c r="K111" s="21"/>
-      <c r="L111" s="21"/>
-      <c r="M111" s="21"/>
-    </row>
-    <row r="112" spans="1:13" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="31" t="s">
+      <c r="B116" s="30"/>
+      <c r="C116" s="30"/>
+      <c r="D116" s="30"/>
+      <c r="E116" s="30"/>
+      <c r="F116" s="30"/>
+      <c r="G116" s="30"/>
+      <c r="H116" s="30"/>
+      <c r="I116" s="30"/>
+      <c r="J116" s="30"/>
+      <c r="K116" s="30"/>
+      <c r="L116" s="30"/>
+      <c r="M116" s="30"/>
+    </row>
+    <row r="117" spans="1:13" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A117" s="38" t="s">
         <v>178</v>
       </c>
-      <c r="B112" s="31"/>
-      <c r="C112" s="31"/>
-      <c r="D112" s="31"/>
-      <c r="E112" s="31"/>
-      <c r="F112" s="31"/>
-      <c r="G112" s="31"/>
-      <c r="H112" s="31"/>
-      <c r="I112" s="31"/>
-      <c r="J112" s="31"/>
-      <c r="K112" s="31"/>
-      <c r="L112" s="31"/>
-      <c r="M112" s="31"/>
-    </row>
-    <row r="113" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="26" t="s">
+      <c r="B117" s="38"/>
+      <c r="C117" s="38"/>
+      <c r="D117" s="38"/>
+      <c r="E117" s="38"/>
+      <c r="F117" s="38"/>
+      <c r="G117" s="38"/>
+      <c r="H117" s="38"/>
+      <c r="I117" s="38"/>
+      <c r="J117" s="38"/>
+      <c r="K117" s="38"/>
+      <c r="L117" s="38"/>
+      <c r="M117" s="38"/>
+    </row>
+    <row r="118" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A118" s="39" t="s">
         <v>89</v>
       </c>
-      <c r="B113" s="26"/>
-      <c r="C113" s="26"/>
-      <c r="D113" s="26"/>
-      <c r="E113" s="26"/>
-      <c r="F113" s="26"/>
-      <c r="G113" s="26"/>
-      <c r="H113" s="26"/>
-      <c r="I113" s="26"/>
-      <c r="J113" s="26"/>
-      <c r="K113" s="26"/>
-      <c r="L113" s="26"/>
-      <c r="M113" s="26"/>
-    </row>
-    <row r="114" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A114" s="24" t="s">
+      <c r="B118" s="39"/>
+      <c r="C118" s="39"/>
+      <c r="D118" s="39"/>
+      <c r="E118" s="39"/>
+      <c r="F118" s="39"/>
+      <c r="G118" s="39"/>
+      <c r="H118" s="39"/>
+      <c r="I118" s="39"/>
+      <c r="J118" s="39"/>
+      <c r="K118" s="39"/>
+      <c r="L118" s="39"/>
+      <c r="M118" s="39"/>
+    </row>
+    <row r="119" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A119" s="46" t="s">
         <v>179</v>
       </c>
-      <c r="B114" s="24"/>
-      <c r="C114" s="24"/>
-      <c r="D114" s="24"/>
-      <c r="E114" s="24"/>
-      <c r="F114" s="24"/>
-      <c r="G114" s="24"/>
-      <c r="H114" s="24"/>
-      <c r="I114" s="24"/>
-      <c r="J114" s="24"/>
-      <c r="K114" s="24"/>
-      <c r="L114" s="24"/>
-      <c r="M114" s="24"/>
-    </row>
-    <row r="115" spans="1:13" s="4" customFormat="1" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A115" s="8" t="s">
+      <c r="B119" s="46"/>
+      <c r="C119" s="46"/>
+      <c r="D119" s="46"/>
+      <c r="E119" s="46"/>
+      <c r="F119" s="46"/>
+      <c r="G119" s="46"/>
+      <c r="H119" s="46"/>
+      <c r="I119" s="46"/>
+      <c r="J119" s="46"/>
+      <c r="K119" s="46"/>
+      <c r="L119" s="46"/>
+      <c r="M119" s="46"/>
+    </row>
+    <row r="120" spans="1:13" s="4" customFormat="1" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A120" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B115" s="8" t="s">
+      <c r="B120" s="8" t="s">
         <v>175</v>
       </c>
-      <c r="C115" s="8" t="s">
+      <c r="C120" s="8" t="s">
         <v>176</v>
       </c>
-      <c r="D115" s="8" t="s">
+      <c r="D120" s="8" t="s">
         <v>177</v>
       </c>
-      <c r="E115" s="8" t="s">
+      <c r="E120" s="8" t="s">
         <v>184</v>
       </c>
-      <c r="F115" s="8" t="s">
+      <c r="F120" s="8" t="s">
         <v>174</v>
       </c>
-      <c r="G115" s="8" t="s">
+      <c r="G120" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="H115" s="8" t="s">
+      <c r="H120" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="I115" s="8" t="s">
+      <c r="I120" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="J115" s="8"/>
-      <c r="K115" s="8"/>
-      <c r="L115" s="8"/>
-      <c r="M115" s="8"/>
-    </row>
-    <row r="116" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A116" s="13" t="s">
+      <c r="J120" s="8"/>
+      <c r="K120" s="8"/>
+      <c r="L120" s="8"/>
+      <c r="M120" s="8"/>
+    </row>
+    <row r="121" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A121" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="B116" s="13" t="s">
+      <c r="B121" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="C116" s="13" t="s">
+      <c r="C121" s="13" t="s">
         <v>223</v>
       </c>
-      <c r="D116" s="14">
+      <c r="D121" s="14">
         <v>1812</v>
       </c>
-      <c r="E116" s="13" t="s">
+      <c r="E121" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="F116" s="13" t="s">
+      <c r="F121" s="13" t="s">
         <v>173</v>
       </c>
-      <c r="G116" s="14">
+      <c r="G121" s="14">
         <v>5</v>
       </c>
-      <c r="H116" s="14">
+      <c r="H121" s="14">
         <v>5</v>
       </c>
-      <c r="I116" s="13" t="s">
+      <c r="I121" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="J116" s="13"/>
-      <c r="K116" s="13"/>
-      <c r="L116" s="13"/>
-      <c r="M116" s="13"/>
-    </row>
-    <row r="117" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A117" s="11" t="s">
+      <c r="J121" s="13"/>
+      <c r="K121" s="13"/>
+      <c r="L121" s="13"/>
+      <c r="M121" s="13"/>
+    </row>
+    <row r="122" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A122" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="B117" s="11" t="s">
+      <c r="B122" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="C117" s="11" t="s">
+      <c r="C122" s="11" t="s">
         <v>224</v>
       </c>
-      <c r="D117" s="12">
+      <c r="D122" s="12">
         <v>1812</v>
       </c>
-      <c r="E117" s="11" t="s">
+      <c r="E122" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="F117" s="11" t="s">
+      <c r="F122" s="11" t="s">
         <v>173</v>
       </c>
-      <c r="G117" s="12">
+      <c r="G122" s="12">
         <v>5</v>
       </c>
-      <c r="H117" s="12">
+      <c r="H122" s="12">
         <v>5</v>
       </c>
-      <c r="I117" s="11" t="s">
+      <c r="I122" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="J117" s="11"/>
-      <c r="K117" s="11"/>
-      <c r="L117" s="11"/>
-      <c r="M117" s="11"/>
-    </row>
-    <row r="118" spans="1:13" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="119" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A119" s="21" t="s">
+      <c r="J122" s="11"/>
+      <c r="K122" s="11"/>
+      <c r="L122" s="11"/>
+      <c r="M122" s="11"/>
+    </row>
+    <row r="123" spans="1:13" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
+    <row r="124" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A124" s="30" t="s">
         <v>188</v>
       </c>
-      <c r="B119" s="21"/>
-      <c r="C119" s="21"/>
-      <c r="D119" s="21"/>
-      <c r="E119" s="21"/>
-      <c r="F119" s="21"/>
-      <c r="G119" s="21"/>
-      <c r="H119" s="21"/>
-      <c r="I119" s="21"/>
-      <c r="J119" s="21"/>
-      <c r="K119" s="21"/>
-      <c r="L119" s="21"/>
-      <c r="M119" s="21"/>
-    </row>
-    <row r="120" spans="1:13" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="31" t="s">
+      <c r="B124" s="30"/>
+      <c r="C124" s="30"/>
+      <c r="D124" s="30"/>
+      <c r="E124" s="30"/>
+      <c r="F124" s="30"/>
+      <c r="G124" s="30"/>
+      <c r="H124" s="30"/>
+      <c r="I124" s="30"/>
+      <c r="J124" s="30"/>
+      <c r="K124" s="30"/>
+      <c r="L124" s="30"/>
+      <c r="M124" s="30"/>
+    </row>
+    <row r="125" spans="1:13" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A125" s="38" t="s">
         <v>178</v>
       </c>
-      <c r="B120" s="31"/>
-      <c r="C120" s="31"/>
-      <c r="D120" s="31"/>
-      <c r="E120" s="31"/>
-      <c r="F120" s="31"/>
-      <c r="G120" s="31"/>
-      <c r="H120" s="31"/>
-      <c r="I120" s="31"/>
-      <c r="J120" s="31"/>
-      <c r="K120" s="31"/>
-      <c r="L120" s="31"/>
-      <c r="M120" s="31"/>
-    </row>
-    <row r="121" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="26" t="s">
+      <c r="B125" s="38"/>
+      <c r="C125" s="38"/>
+      <c r="D125" s="38"/>
+      <c r="E125" s="38"/>
+      <c r="F125" s="38"/>
+      <c r="G125" s="38"/>
+      <c r="H125" s="38"/>
+      <c r="I125" s="38"/>
+      <c r="J125" s="38"/>
+      <c r="K125" s="38"/>
+      <c r="L125" s="38"/>
+      <c r="M125" s="38"/>
+    </row>
+    <row r="126" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A126" s="39" t="s">
         <v>89</v>
       </c>
-      <c r="B121" s="26"/>
-      <c r="C121" s="26"/>
-      <c r="D121" s="26"/>
-      <c r="E121" s="26"/>
-      <c r="F121" s="26"/>
-      <c r="G121" s="26"/>
-      <c r="H121" s="26"/>
-      <c r="I121" s="26"/>
-      <c r="J121" s="26"/>
-      <c r="K121" s="26"/>
-      <c r="L121" s="26"/>
-      <c r="M121" s="26"/>
-    </row>
-    <row r="122" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A122" s="24" t="s">
+      <c r="B126" s="39"/>
+      <c r="C126" s="39"/>
+      <c r="D126" s="39"/>
+      <c r="E126" s="39"/>
+      <c r="F126" s="39"/>
+      <c r="G126" s="39"/>
+      <c r="H126" s="39"/>
+      <c r="I126" s="39"/>
+      <c r="J126" s="39"/>
+      <c r="K126" s="39"/>
+      <c r="L126" s="39"/>
+      <c r="M126" s="39"/>
+    </row>
+    <row r="127" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A127" s="46" t="s">
         <v>180</v>
       </c>
-      <c r="B122" s="24"/>
-      <c r="C122" s="24"/>
-      <c r="D122" s="24"/>
-      <c r="E122" s="24"/>
-      <c r="F122" s="24"/>
-      <c r="G122" s="24"/>
-      <c r="H122" s="24"/>
-      <c r="I122" s="24"/>
-      <c r="J122" s="24"/>
-      <c r="K122" s="24"/>
-      <c r="L122" s="24"/>
-      <c r="M122" s="24"/>
-    </row>
-    <row r="123" spans="1:13" s="4" customFormat="1" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A123" s="10" t="s">
+      <c r="B127" s="46"/>
+      <c r="C127" s="46"/>
+      <c r="D127" s="46"/>
+      <c r="E127" s="46"/>
+      <c r="F127" s="46"/>
+      <c r="G127" s="46"/>
+      <c r="H127" s="46"/>
+      <c r="I127" s="46"/>
+      <c r="J127" s="46"/>
+      <c r="K127" s="46"/>
+      <c r="L127" s="46"/>
+      <c r="M127" s="46"/>
+    </row>
+    <row r="128" spans="1:13" s="4" customFormat="1" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A128" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B123" s="10" t="s">
+      <c r="B128" s="10" t="s">
         <v>175</v>
       </c>
-      <c r="C123" s="10" t="s">
+      <c r="C128" s="10" t="s">
         <v>183</v>
       </c>
-      <c r="D123" s="10" t="s">
+      <c r="D128" s="10" t="s">
         <v>182</v>
       </c>
-      <c r="E123" s="10" t="s">
+      <c r="E128" s="10" t="s">
         <v>184</v>
       </c>
-      <c r="F123" s="10" t="s">
+      <c r="F128" s="10" t="s">
         <v>181</v>
       </c>
-      <c r="G123" s="10" t="s">
+      <c r="G128" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="H123" s="10" t="s">
+      <c r="H128" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="I123" s="10" t="s">
+      <c r="I128" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="J123" s="10"/>
-      <c r="K123" s="10"/>
-      <c r="L123" s="10"/>
-      <c r="M123" s="10"/>
-    </row>
-    <row r="124" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A124" s="13" t="s">
+      <c r="J128" s="10"/>
+      <c r="K128" s="10"/>
+      <c r="L128" s="10"/>
+      <c r="M128" s="10"/>
+    </row>
+    <row r="129" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A129" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="B124" s="13" t="s">
+      <c r="B129" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="C124" s="13" t="s">
+      <c r="C129" s="13" t="s">
         <v>223</v>
       </c>
-      <c r="D124" s="14">
+      <c r="D129" s="14">
         <v>49</v>
       </c>
-      <c r="E124" s="13" t="s">
+      <c r="E129" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="F124" s="13" t="s">
+      <c r="F129" s="13" t="s">
         <v>173</v>
       </c>
-      <c r="G124" s="14">
+      <c r="G129" s="14">
         <v>5</v>
       </c>
-      <c r="H124" s="14">
+      <c r="H129" s="14">
         <v>5</v>
       </c>
-      <c r="I124" s="13" t="s">
+      <c r="I129" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="J124" s="13"/>
-      <c r="K124" s="13"/>
-      <c r="L124" s="13"/>
-      <c r="M124" s="13"/>
-    </row>
-    <row r="125" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A125" s="11" t="s">
+      <c r="J129" s="13"/>
+      <c r="K129" s="13"/>
+      <c r="L129" s="13"/>
+      <c r="M129" s="13"/>
+    </row>
+    <row r="130" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A130" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="B125" s="11" t="s">
+      <c r="B130" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="C125" s="11" t="s">
+      <c r="C130" s="11" t="s">
         <v>224</v>
       </c>
-      <c r="D125" s="12">
+      <c r="D130" s="12">
         <v>49</v>
       </c>
-      <c r="E125" s="11" t="s">
+      <c r="E130" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="F125" s="11" t="s">
+      <c r="F130" s="11" t="s">
         <v>173</v>
       </c>
-      <c r="G125" s="12">
+      <c r="G130" s="12">
         <v>5</v>
       </c>
-      <c r="H125" s="12">
+      <c r="H130" s="12">
         <v>5</v>
       </c>
-      <c r="I125" s="11" t="s">
+      <c r="I130" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="J125" s="11"/>
-      <c r="K125" s="11"/>
-      <c r="L125" s="11"/>
-      <c r="M125" s="11"/>
-    </row>
-    <row r="127" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A127" s="32" t="s">
+      <c r="J130" s="11"/>
+      <c r="K130" s="11"/>
+      <c r="L130" s="11"/>
+      <c r="M130" s="11"/>
+    </row>
+    <row r="132" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A132" s="37" t="s">
         <v>195</v>
       </c>
-      <c r="B127" s="32"/>
-      <c r="C127" s="32"/>
-      <c r="D127" s="32"/>
-      <c r="E127" s="32"/>
-      <c r="F127" s="32"/>
-      <c r="G127" s="32"/>
-      <c r="H127" s="32"/>
-      <c r="I127" s="32"/>
-      <c r="J127" s="32"/>
-      <c r="K127" s="32"/>
-      <c r="L127" s="32"/>
-      <c r="M127" s="32"/>
-    </row>
-    <row r="128" spans="1:13" s="3" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A128" s="31" t="s">
+      <c r="B132" s="37"/>
+      <c r="C132" s="37"/>
+      <c r="D132" s="37"/>
+      <c r="E132" s="37"/>
+      <c r="F132" s="37"/>
+      <c r="G132" s="37"/>
+      <c r="H132" s="37"/>
+      <c r="I132" s="37"/>
+      <c r="J132" s="37"/>
+      <c r="K132" s="37"/>
+      <c r="L132" s="37"/>
+      <c r="M132" s="37"/>
+    </row>
+    <row r="133" spans="1:13" s="3" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A133" s="38" t="s">
         <v>193</v>
       </c>
-      <c r="B128" s="31"/>
-      <c r="C128" s="31"/>
-      <c r="D128" s="31"/>
-      <c r="E128" s="31"/>
-      <c r="F128" s="31"/>
-      <c r="G128" s="31"/>
-      <c r="H128" s="31"/>
-      <c r="I128" s="31"/>
-      <c r="J128" s="31"/>
-      <c r="K128" s="31"/>
-      <c r="L128" s="31"/>
-      <c r="M128" s="31"/>
-    </row>
-    <row r="129" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A129" s="26" t="s">
+      <c r="B133" s="38"/>
+      <c r="C133" s="38"/>
+      <c r="D133" s="38"/>
+      <c r="E133" s="38"/>
+      <c r="F133" s="38"/>
+      <c r="G133" s="38"/>
+      <c r="H133" s="38"/>
+      <c r="I133" s="38"/>
+      <c r="J133" s="38"/>
+      <c r="K133" s="38"/>
+      <c r="L133" s="38"/>
+      <c r="M133" s="38"/>
+    </row>
+    <row r="134" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A134" s="39" t="s">
         <v>189</v>
       </c>
-      <c r="B129" s="26"/>
-      <c r="C129" s="26"/>
-      <c r="D129" s="26"/>
-      <c r="E129" s="26"/>
-      <c r="F129" s="26"/>
-      <c r="G129" s="26"/>
-      <c r="H129" s="26"/>
-      <c r="I129" s="26"/>
-      <c r="J129" s="26"/>
-      <c r="K129" s="26"/>
-      <c r="L129" s="26"/>
-      <c r="M129" s="26"/>
-    </row>
-    <row r="130" spans="1:13" s="4" customFormat="1" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A130" s="8" t="s">
+      <c r="B134" s="39"/>
+      <c r="C134" s="39"/>
+      <c r="D134" s="39"/>
+      <c r="E134" s="39"/>
+      <c r="F134" s="39"/>
+      <c r="G134" s="39"/>
+      <c r="H134" s="39"/>
+      <c r="I134" s="39"/>
+      <c r="J134" s="39"/>
+      <c r="K134" s="39"/>
+      <c r="L134" s="39"/>
+      <c r="M134" s="39"/>
+    </row>
+    <row r="135" spans="1:13" s="4" customFormat="1" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A135" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B130" s="8" t="s">
+      <c r="B135" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="C130" s="8" t="s">
+      <c r="C135" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="D130" s="8" t="s">
+      <c r="D135" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="E130" s="8"/>
-      <c r="F130" s="8"/>
-      <c r="G130" s="8"/>
-      <c r="H130" s="8"/>
-      <c r="I130" s="8"/>
-      <c r="J130" s="8"/>
-      <c r="K130" s="8"/>
-      <c r="L130" s="8"/>
-      <c r="M130" s="8"/>
-    </row>
-    <row r="131" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A131" s="16" t="s">
+      <c r="E135" s="8"/>
+      <c r="F135" s="8"/>
+      <c r="G135" s="8"/>
+      <c r="H135" s="8"/>
+      <c r="I135" s="8"/>
+      <c r="J135" s="8"/>
+      <c r="K135" s="8"/>
+      <c r="L135" s="8"/>
+      <c r="M135" s="8"/>
+    </row>
+    <row r="136" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A136" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="B131" s="16" t="s">
+      <c r="B136" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="C131" s="16" t="s">
+      <c r="C136" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="D131" s="16" t="s">
+      <c r="D136" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="E131" s="16"/>
-      <c r="F131" s="16"/>
-      <c r="G131" s="16"/>
-      <c r="H131" s="16"/>
-      <c r="I131" s="16"/>
-      <c r="J131" s="16"/>
-      <c r="K131" s="16"/>
-      <c r="L131" s="16"/>
-      <c r="M131" s="16"/>
-    </row>
-    <row r="132" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A132" s="17" t="s">
+      <c r="E136" s="16"/>
+      <c r="F136" s="16"/>
+      <c r="G136" s="16"/>
+      <c r="H136" s="16"/>
+      <c r="I136" s="16"/>
+      <c r="J136" s="16"/>
+      <c r="K136" s="16"/>
+      <c r="L136" s="16"/>
+      <c r="M136" s="16"/>
+    </row>
+    <row r="137" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A137" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="B132" s="17" t="s">
+      <c r="B137" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="C132" s="17"/>
-      <c r="D132" s="17" t="s">
+      <c r="C137" s="17"/>
+      <c r="D137" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="E132" s="17"/>
-      <c r="F132" s="17"/>
-      <c r="G132" s="17"/>
-      <c r="H132" s="17"/>
-      <c r="I132" s="17"/>
-      <c r="J132" s="17"/>
-      <c r="K132" s="17"/>
-      <c r="L132" s="17"/>
-      <c r="M132" s="17"/>
+      <c r="E137" s="17"/>
+      <c r="F137" s="17"/>
+      <c r="G137" s="17"/>
+      <c r="H137" s="17"/>
+      <c r="I137" s="17"/>
+      <c r="J137" s="17"/>
+      <c r="K137" s="17"/>
+      <c r="L137" s="17"/>
+      <c r="M137" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="55">
-    <mergeCell ref="I66:J66"/>
-    <mergeCell ref="I67:J67"/>
-    <mergeCell ref="C90:E90"/>
-    <mergeCell ref="C92:E92"/>
-    <mergeCell ref="A84:M84"/>
-    <mergeCell ref="A69:M69"/>
+  <mergeCells count="59">
+    <mergeCell ref="N7:P7"/>
+    <mergeCell ref="N8:P8"/>
+    <mergeCell ref="A6:P6"/>
+    <mergeCell ref="A5:P5"/>
+    <mergeCell ref="A10:M10"/>
+    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="A38:M38"/>
+    <mergeCell ref="A49:M49"/>
+    <mergeCell ref="A53:M53"/>
+    <mergeCell ref="A11:M11"/>
+    <mergeCell ref="A39:M39"/>
+    <mergeCell ref="A28:M28"/>
+    <mergeCell ref="A119:M119"/>
+    <mergeCell ref="A124:M124"/>
+    <mergeCell ref="A93:M93"/>
+    <mergeCell ref="A54:M54"/>
+    <mergeCell ref="A63:M63"/>
+    <mergeCell ref="A64:M64"/>
+    <mergeCell ref="A69:P69"/>
+    <mergeCell ref="A59:M59"/>
+    <mergeCell ref="A118:M118"/>
+    <mergeCell ref="D80:E80"/>
+    <mergeCell ref="B80:C80"/>
+    <mergeCell ref="B81:C81"/>
+    <mergeCell ref="A112:M112"/>
+    <mergeCell ref="A116:M116"/>
+    <mergeCell ref="A117:M117"/>
+    <mergeCell ref="A70:P70"/>
+    <mergeCell ref="A132:M132"/>
+    <mergeCell ref="A133:M133"/>
+    <mergeCell ref="A134:M134"/>
+    <mergeCell ref="B90:C90"/>
+    <mergeCell ref="B91:C91"/>
+    <mergeCell ref="A94:M94"/>
+    <mergeCell ref="A99:M99"/>
+    <mergeCell ref="A105:M105"/>
+    <mergeCell ref="A106:M106"/>
+    <mergeCell ref="A100:M100"/>
+    <mergeCell ref="D90:F90"/>
+    <mergeCell ref="D91:F91"/>
+    <mergeCell ref="C96:E96"/>
+    <mergeCell ref="A125:M125"/>
+    <mergeCell ref="A127:M127"/>
+    <mergeCell ref="A126:M126"/>
+    <mergeCell ref="I71:J71"/>
+    <mergeCell ref="I72:J72"/>
+    <mergeCell ref="C95:E95"/>
+    <mergeCell ref="C97:E97"/>
+    <mergeCell ref="A89:M89"/>
     <mergeCell ref="A74:M74"/>
     <mergeCell ref="A79:M79"/>
-    <mergeCell ref="B77:C77"/>
-    <mergeCell ref="G66:H66"/>
-    <mergeCell ref="G67:H67"/>
-    <mergeCell ref="D76:E76"/>
-    <mergeCell ref="D77:E77"/>
-    <mergeCell ref="E66:F66"/>
-    <mergeCell ref="E67:F67"/>
-    <mergeCell ref="A127:M127"/>
-    <mergeCell ref="A128:M128"/>
-    <mergeCell ref="A129:M129"/>
-    <mergeCell ref="B85:C85"/>
-    <mergeCell ref="B86:C86"/>
-    <mergeCell ref="A89:M89"/>
-    <mergeCell ref="A94:M94"/>
-    <mergeCell ref="A100:M100"/>
-    <mergeCell ref="A101:M101"/>
-    <mergeCell ref="A95:M95"/>
-    <mergeCell ref="D85:F85"/>
-    <mergeCell ref="D86:F86"/>
-    <mergeCell ref="C91:E91"/>
-    <mergeCell ref="A120:M120"/>
-    <mergeCell ref="A122:M122"/>
-    <mergeCell ref="A121:M121"/>
-    <mergeCell ref="A114:M114"/>
-    <mergeCell ref="A119:M119"/>
-    <mergeCell ref="A88:M88"/>
-    <mergeCell ref="A49:M49"/>
-    <mergeCell ref="A58:M58"/>
-    <mergeCell ref="A59:M59"/>
-    <mergeCell ref="A64:P64"/>
-    <mergeCell ref="A54:M54"/>
-    <mergeCell ref="A113:M113"/>
-    <mergeCell ref="D75:E75"/>
-    <mergeCell ref="B75:C75"/>
-    <mergeCell ref="B76:C76"/>
-    <mergeCell ref="A107:M107"/>
-    <mergeCell ref="A111:M111"/>
-    <mergeCell ref="A112:M112"/>
-    <mergeCell ref="A65:P65"/>
-    <mergeCell ref="A5:M5"/>
-    <mergeCell ref="A1:M1"/>
-    <mergeCell ref="A33:M33"/>
-    <mergeCell ref="A44:M44"/>
-    <mergeCell ref="A48:M48"/>
-    <mergeCell ref="A6:M6"/>
-    <mergeCell ref="A34:M34"/>
-    <mergeCell ref="A23:M23"/>
+    <mergeCell ref="A84:M84"/>
+    <mergeCell ref="B82:C82"/>
+    <mergeCell ref="G71:H71"/>
+    <mergeCell ref="G72:H72"/>
+    <mergeCell ref="D81:E81"/>
+    <mergeCell ref="D82:E82"/>
+    <mergeCell ref="E71:F71"/>
+    <mergeCell ref="E72:F72"/>
   </mergeCells>
-  <dataValidations count="52">
+  <dataValidations count="59">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A3" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"inband_vlan"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E8:E21" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E13:E26" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"unspecified,remote-leaf-wan"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G8:G21 G25:G31" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G13:G26 G30:G36" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>switch_role</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H8:H21 H25:H31" xr:uid="{00000000-0002-0000-0000-000003000000}">
-      <formula1>INDIRECT(G8)</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H13:H26 H30:H36" xr:uid="{00000000-0002-0000-0000-000003000000}">
+      <formula1>INDIRECT(G13)</formula1>
     </dataValidation>
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Inband VLAN" error="VLAN must be between 5 and 3097" sqref="B3" xr:uid="{00000000-0002-0000-0000-000004000000}">
       <formula1>5</formula1>
       <formula2>3097</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Node ID" error="Valid Node ID is between 101 and 4000" sqref="D25:E31 D8:D21 C51:C52" xr:uid="{00000000-0002-0000-0000-000005000000}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Node ID" error="Valid Node ID is between 101 and 4000" sqref="D30:E36 D13:D26 C56:C57" xr:uid="{00000000-0002-0000-0000-000005000000}">
       <formula1>101</formula1>
       <formula2>4000</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A8:A21" xr:uid="{00000000-0002-0000-0000-000006000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A13:A26" xr:uid="{00000000-0002-0000-0000-000006000000}">
       <formula1>"switch"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A36:A42" xr:uid="{00000000-0002-0000-0000-000007000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A41:A47" xr:uid="{00000000-0002-0000-0000-000007000000}">
       <formula1>"apic_inb"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A46" xr:uid="{00000000-0002-0000-0000-000008000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A51" xr:uid="{00000000-0002-0000-0000-000008000000}">
       <formula1>"bgp_as"</formula1>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="BGP ASN" error="BGP ASN Must be between 1 and 4294967295" sqref="B46" xr:uid="{00000000-0002-0000-0000-000009000000}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="BGP ASN" error="BGP ASN Must be between 1 and 4294967295" sqref="B51" xr:uid="{00000000-0002-0000-0000-000009000000}">
       <formula1>1</formula1>
       <formula2>4294967295</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Pod ID" error="Pod Id must be between 1 and 12!" sqref="D36:D42 F8:F21 F25:F31" xr:uid="{00000000-0002-0000-0000-00000A000000}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Pod ID" error="Pod Id must be between 1 and 12!" sqref="D41:D47 F13:F26 F30:F36" xr:uid="{00000000-0002-0000-0000-00000A000000}">
       <formula1>1</formula1>
       <formula2>12</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="APIC Node ID" error="APIC Node ID must be between 1 and 7" sqref="C36:C42" xr:uid="{00000000-0002-0000-0000-00000B000000}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="APIC Node ID" error="APIC Node ID must be between 1 and 7" sqref="C41:C47" xr:uid="{00000000-0002-0000-0000-00000B000000}">
       <formula1>1</formula1>
       <formula2>7</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A51:A52" xr:uid="{00000000-0002-0000-0000-00000C000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A56:A57" xr:uid="{00000000-0002-0000-0000-00000C000000}">
       <formula1>"bgp_rr"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B56 D71:D72 D81:D82 G97:G98 D109 I116:I117 I124:I125 D67" xr:uid="{00000000-0002-0000-0000-00000D000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B61 D76:D77 D86:D87 G102:G103 D114 I121:I122 I129:I130 D72 F8" xr:uid="{00000000-0002-0000-0000-00000D000000}">
       <formula1>"inband,oob"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A56" xr:uid="{00000000-0002-0000-0000-00000E000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A61" xr:uid="{00000000-0002-0000-0000-00000E000000}">
       <formula1>"dns_mgmt"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A61:A62" xr:uid="{00000000-0002-0000-0000-00000F000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A66:A67" xr:uid="{00000000-0002-0000-0000-00000F000000}">
       <formula1>"dns"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C61:C62 D76:D77" xr:uid="{00000000-0002-0000-0000-000010000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C66:C67 D81:D82" xr:uid="{00000000-0002-0000-0000-000010000000}">
       <formula1>"no,yes"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A67" xr:uid="{00000000-0002-0000-0000-000011000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A72" xr:uid="{00000000-0002-0000-0000-000011000000}">
       <formula1>"smartcallhome"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C71:C72" xr:uid="{00000000-0002-0000-0000-000012000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C76:C77" xr:uid="{00000000-0002-0000-0000-000012000000}">
       <formula1>"false,true"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A76:A77" xr:uid="{00000000-0002-0000-0000-000013000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A81:A82" xr:uid="{00000000-0002-0000-0000-000013000000}">
       <formula1>"search_domain"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A71:A72" xr:uid="{00000000-0002-0000-0000-000014000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A76:A77" xr:uid="{00000000-0002-0000-0000-000014000000}">
       <formula1>"ntp"</formula1>
     </dataValidation>
-    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Community String" error="The SNMP Community can be 1 to 32 characters and contain letters, numbers, and [.\-]. No other special characters" sqref="B91:B92" xr:uid="{00000000-0002-0000-0000-000015000000}">
+    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Community String" error="The SNMP Community can be 1 to 32 characters and contain letters, numbers, and [.\-]. No other special characters" sqref="B96:B97" xr:uid="{00000000-0002-0000-0000-000015000000}">
       <formula1>1</formula1>
       <formula2>32</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A86" xr:uid="{00000000-0002-0000-0000-000016000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A91" xr:uid="{00000000-0002-0000-0000-000016000000}">
       <formula1>"snmp_info"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A91:A92" xr:uid="{00000000-0002-0000-0000-000017000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A96:A97" xr:uid="{00000000-0002-0000-0000-000017000000}">
       <formula1>"snmp_comm"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C103:C105" xr:uid="{00000000-0002-0000-0000-000018000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C108:C110" xr:uid="{00000000-0002-0000-0000-000018000000}">
       <formula1>"aes-128,des,none"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E103:E105" xr:uid="{00000000-0002-0000-0000-000019000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E108:E110" xr:uid="{00000000-0002-0000-0000-000019000000}">
       <formula1>"md5,sha1"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D97:D98" xr:uid="{00000000-0002-0000-0000-00001A000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D102:D103" xr:uid="{00000000-0002-0000-0000-00001A000000}">
       <formula1>"v1,v2c,v3"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A103:A105" xr:uid="{00000000-0002-0000-0000-00001B000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A108:A110" xr:uid="{00000000-0002-0000-0000-00001B000000}">
       <formula1>"snmp_user"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E109 H109" xr:uid="{00000000-0002-0000-0000-00001C000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E114 H114" xr:uid="{00000000-0002-0000-0000-00001C000000}">
       <formula1>"emergencies,alerts,critical,errors,warnings,notifications,information,debugging"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F109" xr:uid="{00000000-0002-0000-0000-00001D000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F114" xr:uid="{00000000-0002-0000-0000-00001D000000}">
       <formula1>"local0,local1,local2,local3,local4,local5,local6,local7"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G109 I109" xr:uid="{00000000-0002-0000-0000-00001E000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G114 I114" xr:uid="{00000000-0002-0000-0000-00001E000000}">
       <formula1>"enabled,disabled"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J109" xr:uid="{00000000-0002-0000-0000-00001F000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J114" xr:uid="{00000000-0002-0000-0000-00001F000000}">
       <formula1>"emergencies,alerts,critical"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A109" xr:uid="{00000000-0002-0000-0000-000020000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A114" xr:uid="{00000000-0002-0000-0000-000020000000}">
       <formula1>"syslog"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F116:F117 F124:F125" xr:uid="{00000000-0002-0000-0000-000021000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F121:F122 F129:F130" xr:uid="{00000000-0002-0000-0000-000021000000}">
       <formula1>"chap,mschap,pap"</formula1>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="RADIUS Timeout" error="Timeout should be between 5 and 60 and be a Factor of 5.  Default is 5" sqref="G116:G117" xr:uid="{00000000-0002-0000-0000-000022000000}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="RADIUS Timeout" error="Timeout should be between 5 and 60 and be a Factor of 5.  Default is 5" sqref="G121:G122" xr:uid="{00000000-0002-0000-0000-000022000000}">
       <formula1>5</formula1>
       <formula2>60</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="RADIUS Retry" error="Retry should be a number between 1 and 5.  Default is 1" sqref="H116:H117" xr:uid="{00000000-0002-0000-0000-000023000000}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="RADIUS Retry" error="Retry should be a number between 1 and 5.  Default is 1" sqref="H121:H122" xr:uid="{00000000-0002-0000-0000-000023000000}">
       <formula1>1</formula1>
       <formula2>5</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="TACACS Timeout" error="Timeout should be between 5 and 60 and be a Factor of 5.  Default is 5" sqref="G124:G125" xr:uid="{00000000-0002-0000-0000-000024000000}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="TACACS Timeout" error="Timeout should be between 5 and 60 and be a Factor of 5.  Default is 5" sqref="G129:G130" xr:uid="{00000000-0002-0000-0000-000024000000}">
       <formula1>5</formula1>
       <formula2>60</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="TACACS Retry" error="Retry should be a number between 1 and 5.  Default is 1" sqref="H124:H125" xr:uid="{00000000-0002-0000-0000-000025000000}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="TACACS Retry" error="Retry should be a number between 1 and 5.  Default is 1" sqref="H129:H130" xr:uid="{00000000-0002-0000-0000-000025000000}">
       <formula1>1</formula1>
       <formula2>5</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Syslog Port" error="Valid Port Range is between 1 and 65535.  Default is 514" sqref="C109" xr:uid="{00000000-0002-0000-0000-000026000000}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Syslog Port" error="Valid Port Range is between 1 and 65535.  Default is 514" sqref="C114" xr:uid="{00000000-0002-0000-0000-000026000000}">
       <formula1>1</formula1>
       <formula2>65535</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="RADIUS Port" error="Valid Port Range is between 1 and 65535. Default is 1812" sqref="D116:D117" xr:uid="{00000000-0002-0000-0000-000027000000}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="RADIUS Port" error="Valid Port Range is between 1 and 65535. Default is 1812" sqref="D121:D122" xr:uid="{00000000-0002-0000-0000-000027000000}">
       <formula1>1</formula1>
       <formula2>65535</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="TACACS Port" error="Valid Port Range is between 1 and 65535. Default is 49" sqref="D124:D125" xr:uid="{00000000-0002-0000-0000-000028000000}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="TACACS Port" error="Valid Port Range is between 1 and 65535. Default is 49" sqref="D129:D130" xr:uid="{00000000-0002-0000-0000-000028000000}">
       <formula1>1</formula1>
       <formula2>65535</formula2>
     </dataValidation>
-    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Login Domain" error="Maximum length is 10 Alpha Numberic Characters or an underscore &quot;_&quot;.  But it must not begin with a underscore &quot;_&quot;." sqref="B124:B125" xr:uid="{00000000-0002-0000-0000-000029000000}">
+    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Login Domain" error="Maximum length is 10 Alpha Numberic Characters or an underscore &quot;_&quot;.  But it must not begin with a underscore &quot;_&quot;." sqref="B129:B130" xr:uid="{00000000-0002-0000-0000-000029000000}">
       <formula1>1</formula1>
       <formula2>10</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A124:A125" xr:uid="{00000000-0002-0000-0000-00002A000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A129:A130" xr:uid="{00000000-0002-0000-0000-00002A000000}">
       <formula1>"tacacs"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A116:A117" xr:uid="{00000000-0002-0000-0000-00002B000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A121:A122" xr:uid="{00000000-0002-0000-0000-00002B000000}">
       <formula1>"radius"</formula1>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SNMP Trap Port" error="Valid Port Range is between 1 and 65535.  Default is 162" sqref="C97:C98" xr:uid="{00000000-0002-0000-0000-00002C000000}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SNMP Trap Port" error="Valid Port Range is between 1 and 65535.  Default is 162" sqref="C102:C103" xr:uid="{00000000-0002-0000-0000-00002C000000}">
       <formula1>1</formula1>
       <formula2>65535</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A97:A98" xr:uid="{00000000-0002-0000-0000-00002D000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A102:A103" xr:uid="{00000000-0002-0000-0000-00002D000000}">
       <formula1>"snmp_trap"</formula1>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SMTP Port" error="Valid Port Range is between 1 and 65535.  Default is 25" sqref="B67" xr:uid="{00000000-0002-0000-0000-00002E000000}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SMTP Port" error="Valid Port Range is between 1 and 65535.  Default is 25" sqref="B72" xr:uid="{00000000-0002-0000-0000-00002E000000}">
       <formula1>1</formula1>
       <formula2>65535</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Login Domain Type" error="The Login Domain Type can be [local|ldap|radius|tacacs|rsa|saml].  SAML is not supported for Console Authentication" sqref="D131:D132" xr:uid="{00000000-0002-0000-0000-00002F000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Login Domain Type" error="The Login Domain Type can be [local|ldap|radius|tacacs|rsa|saml].  SAML is not supported for Console Authentication" sqref="D136:D137" xr:uid="{00000000-0002-0000-0000-00002F000000}">
       <formula1>"local,ldap,radius,tacacs,rsa,saml"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B131:B132" xr:uid="{00000000-0002-0000-0000-000030000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B136:B137" xr:uid="{00000000-0002-0000-0000-000030000000}">
       <formula1>"console,default"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A131:A132" xr:uid="{00000000-0002-0000-0000-000031000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A136:A137" xr:uid="{00000000-0002-0000-0000-000031000000}">
       <formula1>"realm"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A25:A31" xr:uid="{A2F55667-432D-4009-90B0-3CBF96713B99}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A30:A36" xr:uid="{A2F55667-432D-4009-90B0-3CBF96713B99}">
       <formula1>"vpc_pair"</formula1>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="VPC ID" error="The VPC ID must be a number between 1 and 1000" sqref="B25:B31" xr:uid="{2DB049D3-4D1F-4770-AA8C-B1564D6B004B}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="VPC ID" error="The VPC ID must be a number between 1 and 1000" sqref="B30:B36" xr:uid="{2DB049D3-4D1F-4770-AA8C-B1564D6B004B}">
       <formula1>1</formula1>
       <formula2>1000</formula2>
     </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A8" xr:uid="{F1D834FB-B49E-4782-9CC5-3D1041DE88B7}">
+      <formula1>"backup"</formula1>
+    </dataValidation>
+    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8" xr:uid="{DB8C1ADF-D3F1-4510-9008-6655A2311A3D}">
+      <formula1>16</formula1>
+      <formula2>32</formula2>
+    </dataValidation>
+    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" errorTitle="Backup Hour" error="Valid Hour is between 0 and 23" sqref="C8" xr:uid="{60A7E17B-12FB-4EFD-A780-8B3F75235F60}">
+      <formula1>0</formula1>
+      <formula2>23</formula2>
+    </dataValidation>
+    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" errorTitle="Backup Minute" error="Valid Hour is between 0 and 59" sqref="D8" xr:uid="{089F4D15-6FA0-494C-AD4D-FCA3D13980CF}">
+      <formula1>0</formula1>
+      <formula2>59</formula2>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G8" xr:uid="{BFEC7590-08FB-4199-9BF5-8BEEFDB98E9E}">
+      <formula1>"ftp,scp,sftp"</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I8" xr:uid="{2A556DCD-DAE6-4033-9656-114D3F66275C}">
+      <formula1>0</formula1>
+      <formula2>65535</formula2>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J8" xr:uid="{EF451635-7AEA-41B7-80CF-916EDF399679}">
+      <formula1>"password,ssh-key"</formula1>
+    </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="E67" r:id="rId1" xr:uid="{47B0C783-B08F-4E70-8365-F66BC2D1DC4E}"/>
-    <hyperlink ref="G67" r:id="rId2" xr:uid="{ECB49B35-5BD8-4A7F-88FF-240597E5B135}"/>
-    <hyperlink ref="I67" r:id="rId3" xr:uid="{F5D689CB-3F4A-4EED-ADA0-F02A0EBD47A7}"/>
+    <hyperlink ref="E72" r:id="rId1" xr:uid="{47B0C783-B08F-4E70-8365-F66BC2D1DC4E}"/>
+    <hyperlink ref="G72" r:id="rId2" xr:uid="{ECB49B35-5BD8-4A7F-88FF-240597E5B135}"/>
+    <hyperlink ref="I72" r:id="rId3" xr:uid="{F5D689CB-3F4A-4EED-ADA0-F02A0EBD47A7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>

</xml_diff>